<commit_message>
1125655 - XSD updates - OrderReference
</commit_message>
<xml_diff>
--- a/specification/excel/Pagero Universal Format.xlsx
+++ b/specification/excel/Pagero Universal Format.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\development\format\puf-billing\specification\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B04DCE1-2E79-4E24-8CDF-9CD35F741EF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3F4C7A4-7676-4CA2-8392-B516697FFCE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="8" r:id="rId1"/>
@@ -4016,8 +4016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDB56CEA-A5F9-42A4-9956-612B841F9EA3}">
   <dimension ref="A1:F492"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A290" workbookViewId="0">
-      <selection activeCell="I301" sqref="I301"/>
+    <sheetView tabSelected="1" topLeftCell="A380" workbookViewId="0">
+      <selection activeCell="B390" sqref="B390"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -10372,7 +10372,7 @@
         <v>13</v>
       </c>
       <c r="B390" s="18" t="s">
-        <v>286</v>
+        <v>39</v>
       </c>
       <c r="C390" s="22" t="s">
         <v>591</v>
@@ -12420,6 +12420,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008296D2E9439BF946A1501D3A497E974E" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9a8df56671683c60572e05043457fa7c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="222206e9-2590-4389-ac08-92b39e79291a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7a8e40c0b678fce4b7614ca76454760e" ns2:_="">
     <xsd:import namespace="222206e9-2590-4389-ac08-92b39e79291a"/>
@@ -12565,35 +12580,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58840883-6350-4B75-8993-54B5916E5251}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97BB75A6-1832-49A3-9C38-BF9FC8430A95}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="222206e9-2590-4389-ac08-92b39e79291a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -12615,9 +12605,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97BB75A6-1832-49A3-9C38-BF9FC8430A95}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58840883-6350-4B75-8993-54B5916E5251}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="222206e9-2590-4389-ac08-92b39e79291a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
934709 - US examples, Tax Type Name
</commit_message>
<xml_diff>
--- a/specification/excel/Pagero Universal Format.xlsx
+++ b/specification/excel/Pagero Universal Format.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\development\format\puf-billing\specification\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3F4C7A4-7676-4CA2-8392-B516697FFCE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9FBD7DB-CDE0-4692-A9C0-101EAAC718EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="0" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="8" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Test Cases" sheetId="4" state="hidden" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Base PUF (no extensions)'!$A$1:$F$492</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Base PUF (no extensions)'!$A$1:$F$495</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2004" uniqueCount="708">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2019" uniqueCount="711">
   <si>
     <t>Comments</t>
   </si>
@@ -2592,6 +2592,15 @@
   </si>
   <si>
     <t>The currency in which the Financial Account is held expressed as a code</t>
+  </si>
+  <si>
+    <t>IAO</t>
+  </si>
+  <si>
+    <t>Standard</t>
+  </si>
+  <si>
+    <t>The name of this taxation scheme.</t>
   </si>
 </sst>
 </file>
@@ -3898,7 +3907,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFC8AF48-A32B-49A1-A68C-71E5B6F7A240}">
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A19" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
@@ -4014,10 +4023,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDB56CEA-A5F9-42A4-9956-612B841F9EA3}">
-  <dimension ref="A1:F492"/>
+  <dimension ref="A1:F495"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A380" workbookViewId="0">
-      <selection activeCell="B390" sqref="B390"/>
+    <sheetView tabSelected="1" topLeftCell="A243" workbookViewId="0">
+      <selection activeCell="C326" sqref="C326"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4951,7 +4960,7 @@
         <v>53</v>
       </c>
       <c r="B57" s="18" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C57" s="22" t="s">
         <v>438</v>
@@ -4969,7 +4978,7 @@
         <v>41</v>
       </c>
       <c r="B58" s="18" t="s">
-        <v>45</v>
+        <v>286</v>
       </c>
       <c r="C58" s="22" t="s">
         <v>412</v>
@@ -4997,7 +5006,7 @@
         <v>13</v>
       </c>
       <c r="B60" s="18" t="s">
-        <v>45</v>
+        <v>286</v>
       </c>
       <c r="C60" s="22" t="s">
         <v>413</v>
@@ -5015,7 +5024,7 @@
         <v>41</v>
       </c>
       <c r="B61" s="18" t="s">
-        <v>45</v>
+        <v>286</v>
       </c>
       <c r="C61" s="22" t="s">
         <v>414</v>
@@ -5391,7 +5400,7 @@
         <v>70</v>
       </c>
       <c r="B84" s="103" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C84" s="104"/>
       <c r="D84" s="104"/>
@@ -5403,7 +5412,7 @@
         <v>71</v>
       </c>
       <c r="B85" s="18" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C85" s="22" t="s">
         <v>309</v>
@@ -5421,7 +5430,7 @@
         <v>68</v>
       </c>
       <c r="B86" s="18" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C86" s="22" t="s">
         <v>310</v>
@@ -5439,7 +5448,7 @@
         <v>452</v>
       </c>
       <c r="B87" s="18" t="s">
-        <v>45</v>
+        <v>286</v>
       </c>
       <c r="C87" s="22" t="s">
         <v>453</v>
@@ -5769,7 +5778,7 @@
         <v>53</v>
       </c>
       <c r="B108" s="18" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C108" s="22" t="s">
         <v>461</v>
@@ -5787,7 +5796,7 @@
         <v>41</v>
       </c>
       <c r="B109" s="18" t="s">
-        <v>45</v>
+        <v>286</v>
       </c>
       <c r="C109" s="22" t="s">
         <v>462</v>
@@ -5815,7 +5824,7 @@
         <v>13</v>
       </c>
       <c r="B111" s="18" t="s">
-        <v>45</v>
+        <v>286</v>
       </c>
       <c r="C111" s="22" t="s">
         <v>318</v>
@@ -5833,7 +5842,7 @@
         <v>41</v>
       </c>
       <c r="B112" s="18" t="s">
-        <v>45</v>
+        <v>286</v>
       </c>
       <c r="C112" s="22" t="s">
         <v>463</v>
@@ -6495,7 +6504,7 @@
         <v>54</v>
       </c>
       <c r="B153" s="25" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C153" s="57"/>
       <c r="D153" s="23"/>
@@ -6507,7 +6516,7 @@
         <v>13</v>
       </c>
       <c r="B154" s="18" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C154" s="22" t="s">
         <v>327</v>
@@ -6571,7 +6580,7 @@
         <v>70</v>
       </c>
       <c r="B158" s="25" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C158" s="57" t="s">
         <v>329</v>
@@ -6585,7 +6594,7 @@
         <v>68</v>
       </c>
       <c r="B159" s="18" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C159" s="22" t="s">
         <v>330</v>
@@ -6681,7 +6690,7 @@
         <v>53</v>
       </c>
       <c r="B166" s="18" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C166" s="22" t="s">
         <v>461</v>
@@ -6699,7 +6708,7 @@
         <v>41</v>
       </c>
       <c r="B167" s="18" t="s">
-        <v>45</v>
+        <v>286</v>
       </c>
       <c r="C167" s="22" t="s">
         <v>462</v>
@@ -7070,7 +7079,7 @@
         <v>68</v>
       </c>
       <c r="B190" s="18" t="s">
-        <v>45</v>
+        <v>286</v>
       </c>
       <c r="C190" s="22" t="s">
         <v>323</v>
@@ -7100,7 +7109,7 @@
         <v>13</v>
       </c>
       <c r="B192" s="18" t="s">
-        <v>45</v>
+        <v>286</v>
       </c>
       <c r="C192" s="22" t="s">
         <v>697</v>
@@ -9356,502 +9365,502 @@
       <c r="F329" s="17"/>
     </row>
     <row r="330" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A330" s="129" t="s">
+      <c r="A330" s="125" t="s">
+        <v>56</v>
+      </c>
+      <c r="B330" s="18" t="s">
+        <v>708</v>
+      </c>
+      <c r="C330" s="22" t="s">
+        <v>710</v>
+      </c>
+      <c r="D330" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="E330" s="17" t="s">
+        <v>709</v>
+      </c>
+      <c r="F330" s="17"/>
+    </row>
+    <row r="331" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A331" s="129" t="s">
         <v>115</v>
       </c>
-      <c r="B330" s="25" t="s">
+      <c r="B331" s="25" t="s">
         <v>285</v>
       </c>
-      <c r="C330" s="57"/>
-      <c r="D330" s="23"/>
-      <c r="E330" s="36"/>
-      <c r="F330" s="23"/>
-    </row>
-    <row r="331" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A331" s="92" t="s">
-        <v>116</v>
-      </c>
-      <c r="B331" s="18" t="s">
-        <v>285</v>
-      </c>
-      <c r="C331" s="22" t="s">
-        <v>550</v>
-      </c>
-      <c r="D331" s="17" t="s">
-        <v>224</v>
-      </c>
-      <c r="E331" s="34">
-        <v>250</v>
-      </c>
-      <c r="F331" s="17"/>
+      <c r="C331" s="57"/>
+      <c r="D331" s="23"/>
+      <c r="E331" s="36"/>
+      <c r="F331" s="23"/>
     </row>
     <row r="332" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A332" s="92" t="s">
+        <v>116</v>
+      </c>
+      <c r="B332" s="18" t="s">
+        <v>285</v>
+      </c>
+      <c r="C332" s="22" t="s">
+        <v>550</v>
+      </c>
+      <c r="D332" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="E332" s="34">
+        <v>250</v>
+      </c>
+      <c r="F332" s="17"/>
+    </row>
+    <row r="333" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A333" s="92" t="s">
         <v>111</v>
       </c>
-      <c r="B332" s="18" t="s">
+      <c r="B333" s="18" t="s">
         <v>286</v>
       </c>
-      <c r="C332" s="22" t="s">
+      <c r="C333" s="22" t="s">
         <v>549</v>
       </c>
-      <c r="D332" s="17" t="s">
+      <c r="D333" s="17" t="s">
         <v>164</v>
       </c>
-      <c r="E332" s="34" t="s">
+      <c r="E333" s="34" t="s">
         <v>225</v>
       </c>
-      <c r="F332" s="17"/>
-    </row>
-    <row r="333" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A333" s="100" t="s">
+      <c r="F333" s="17"/>
+    </row>
+    <row r="334" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A334" s="100" t="s">
         <v>253</v>
       </c>
-      <c r="B333" s="62" t="s">
+      <c r="B334" s="62" t="s">
         <v>276</v>
       </c>
-      <c r="C333" s="28" t="s">
+      <c r="C334" s="28" t="s">
         <v>555</v>
       </c>
-      <c r="D333" s="21"/>
-      <c r="E333" s="32"/>
-      <c r="F333" s="32"/>
-    </row>
-    <row r="334" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A334" s="92" t="s">
-        <v>254</v>
-      </c>
-      <c r="B334" s="18" t="s">
-        <v>288</v>
-      </c>
-      <c r="C334" s="22" t="s">
-        <v>556</v>
-      </c>
-      <c r="D334" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="E334" s="17" t="s">
-        <v>225</v>
-      </c>
-      <c r="F334" s="17"/>
+      <c r="D334" s="21"/>
+      <c r="E334" s="32"/>
+      <c r="F334" s="32"/>
     </row>
     <row r="335" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A335" s="92" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B335" s="18" t="s">
         <v>288</v>
       </c>
       <c r="C335" s="22" t="s">
-        <v>553</v>
+        <v>556</v>
       </c>
       <c r="D335" s="17" t="s">
         <v>164</v>
       </c>
       <c r="E335" s="17" t="s">
-        <v>557</v>
+        <v>225</v>
       </c>
       <c r="F335" s="17"/>
     </row>
     <row r="336" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A336" s="92" t="s">
+        <v>255</v>
+      </c>
+      <c r="B336" s="18" t="s">
+        <v>288</v>
+      </c>
+      <c r="C336" s="22" t="s">
+        <v>553</v>
+      </c>
+      <c r="D336" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="E336" s="17" t="s">
+        <v>557</v>
+      </c>
+      <c r="F336" s="17"/>
+    </row>
+    <row r="337" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A337" s="92" t="s">
         <v>256</v>
       </c>
-      <c r="B336" s="18" t="s">
+      <c r="B337" s="18" t="s">
         <v>290</v>
       </c>
-      <c r="C336" s="22" t="s">
+      <c r="C337" s="22" t="s">
         <v>554</v>
       </c>
-      <c r="D336" s="17" t="s">
+      <c r="D337" s="17" t="s">
         <v>538</v>
       </c>
-      <c r="E336" s="17" t="s">
+      <c r="E337" s="17" t="s">
         <v>558</v>
       </c>
-      <c r="F336" s="17"/>
-    </row>
-    <row r="337" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A337" s="92" t="s">
+      <c r="F337" s="17"/>
+    </row>
+    <row r="338" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A338" s="92" t="s">
         <v>257</v>
       </c>
-      <c r="B337" s="18" t="s">
+      <c r="B338" s="18" t="s">
         <v>289</v>
       </c>
-      <c r="C337" s="22" t="s">
+      <c r="C338" s="22" t="s">
         <v>361</v>
       </c>
-      <c r="D337" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="E337" s="34" t="s">
+      <c r="D338" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="E338" s="34" t="s">
         <v>258</v>
       </c>
-      <c r="F337" s="34" t="s">
+      <c r="F338" s="34" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="338" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A338" s="133" t="s">
+    <row r="339" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A339" s="133" t="s">
         <v>259</v>
       </c>
-      <c r="B338" s="18" t="s">
+      <c r="B339" s="18" t="s">
         <v>290</v>
       </c>
-      <c r="C338" s="29" t="s">
+      <c r="C339" s="29" t="s">
         <v>362</v>
       </c>
-      <c r="D338" s="17" t="s">
+      <c r="D339" s="17" t="s">
         <v>163</v>
       </c>
-      <c r="E338" s="35">
+      <c r="E339" s="35">
         <v>43466</v>
       </c>
-      <c r="F338" s="17"/>
-    </row>
-    <row r="339" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A339" s="100" t="s">
+      <c r="F339" s="17"/>
+    </row>
+    <row r="340" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A340" s="100" t="s">
         <v>115</v>
       </c>
-      <c r="B339" s="62" t="s">
+      <c r="B340" s="62" t="s">
         <v>45</v>
       </c>
-      <c r="C339" s="28" t="s">
+      <c r="C340" s="28" t="s">
         <v>363</v>
       </c>
-      <c r="D339" s="21"/>
-      <c r="E339" s="32"/>
-      <c r="F339" s="21"/>
-    </row>
-    <row r="340" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A340" s="92" t="s">
-        <v>116</v>
-      </c>
-      <c r="B340" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="C340" s="22" t="s">
-        <v>559</v>
-      </c>
-      <c r="D340" s="17" t="s">
-        <v>224</v>
-      </c>
-      <c r="E340" s="34" t="s">
-        <v>226</v>
-      </c>
-      <c r="F340" s="17"/>
+      <c r="D340" s="21"/>
+      <c r="E340" s="32"/>
+      <c r="F340" s="21"/>
     </row>
     <row r="341" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A341" s="92" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B341" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="C341" s="56" t="s">
+      <c r="C341" s="22" t="s">
+        <v>559</v>
+      </c>
+      <c r="D341" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="E341" s="34" t="s">
+        <v>226</v>
+      </c>
+      <c r="F341" s="17"/>
+    </row>
+    <row r="342" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A342" s="92" t="s">
+        <v>111</v>
+      </c>
+      <c r="B342" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C342" s="56" t="s">
         <v>560</v>
       </c>
-      <c r="D341" s="17" t="s">
+      <c r="D342" s="17" t="s">
         <v>164</v>
       </c>
-      <c r="E341" s="34" t="s">
+      <c r="E342" s="34" t="s">
         <v>225</v>
       </c>
-      <c r="F341" s="17"/>
-    </row>
-    <row r="342" spans="1:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="A342" s="129" t="s">
+      <c r="F342" s="17"/>
+    </row>
+    <row r="343" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A343" s="129" t="s">
         <v>117</v>
       </c>
-      <c r="B342" s="25" t="s">
+      <c r="B343" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="C342" s="57" t="s">
+      <c r="C343" s="57" t="s">
         <v>388</v>
       </c>
-      <c r="D342" s="23"/>
-      <c r="E342" s="36"/>
-      <c r="F342" s="36"/>
-    </row>
-    <row r="343" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A343" s="117" t="s">
-        <v>416</v>
-      </c>
-      <c r="B343" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="C343" s="22" t="s">
-        <v>417</v>
-      </c>
-      <c r="D343" s="22"/>
-      <c r="E343" s="22"/>
-      <c r="F343" s="22"/>
+      <c r="D343" s="23"/>
+      <c r="E343" s="36"/>
+      <c r="F343" s="36"/>
     </row>
     <row r="344" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A344" s="117" t="s">
-        <v>118</v>
+        <v>416</v>
       </c>
       <c r="B344" s="18" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C344" s="22" t="s">
-        <v>561</v>
-      </c>
-      <c r="D344" s="17" t="s">
-        <v>224</v>
-      </c>
-      <c r="E344" s="22" t="s">
-        <v>227</v>
-      </c>
-      <c r="F344" s="17"/>
+        <v>417</v>
+      </c>
+      <c r="D344" s="22"/>
+      <c r="E344" s="22"/>
+      <c r="F344" s="22"/>
     </row>
     <row r="345" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A345" s="117" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="B345" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="C345" s="56" t="s">
-        <v>562</v>
+      <c r="C345" s="22" t="s">
+        <v>561</v>
       </c>
       <c r="D345" s="17" t="s">
-        <v>164</v>
+        <v>224</v>
       </c>
       <c r="E345" s="22" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="F345" s="17"/>
     </row>
-    <row r="346" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A346" s="117" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B346" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="C346" s="22" t="s">
-        <v>563</v>
+      <c r="C346" s="56" t="s">
+        <v>562</v>
       </c>
       <c r="D346" s="17" t="s">
-        <v>224</v>
+        <v>164</v>
       </c>
       <c r="E346" s="22" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F346" s="17"/>
     </row>
-    <row r="347" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A347" s="117" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B347" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="C347" s="56" t="s">
+      <c r="C347" s="22" t="s">
+        <v>563</v>
+      </c>
+      <c r="D347" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="E347" s="22" t="s">
+        <v>226</v>
+      </c>
+      <c r="F347" s="17"/>
+    </row>
+    <row r="348" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A348" s="117" t="s">
+        <v>111</v>
+      </c>
+      <c r="B348" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C348" s="56" t="s">
         <v>564</v>
       </c>
-      <c r="D347" s="17" t="s">
+      <c r="D348" s="17" t="s">
         <v>164</v>
       </c>
-      <c r="E347" s="34" t="s">
+      <c r="E348" s="34" t="s">
         <v>225</v>
       </c>
-      <c r="F347" s="17"/>
-    </row>
-    <row r="348" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A348" s="122" t="s">
+      <c r="F348" s="17"/>
+    </row>
+    <row r="349" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A349" s="122" t="s">
         <v>113</v>
       </c>
-      <c r="B348" s="103" t="s">
+      <c r="B349" s="103" t="s">
         <v>45</v>
       </c>
-      <c r="C348" s="112"/>
-      <c r="D348" s="104"/>
-      <c r="E348" s="105"/>
-      <c r="F348" s="61"/>
-    </row>
-    <row r="349" spans="1:6" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A349" s="119" t="s">
+      <c r="C349" s="112"/>
+      <c r="D349" s="104"/>
+      <c r="E349" s="105"/>
+      <c r="F349" s="61"/>
+    </row>
+    <row r="350" spans="1:6" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A350" s="119" t="s">
         <v>13</v>
-      </c>
-      <c r="B349" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="C349" s="22" t="s">
-        <v>565</v>
-      </c>
-      <c r="D349" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="E349" s="34" t="s">
-        <v>184</v>
-      </c>
-      <c r="F349" s="17"/>
-    </row>
-    <row r="350" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A350" s="119" t="s">
-        <v>114</v>
       </c>
       <c r="B350" s="18" t="s">
         <v>45</v>
       </c>
       <c r="C350" s="22" t="s">
+        <v>565</v>
+      </c>
+      <c r="D350" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="E350" s="34" t="s">
+        <v>184</v>
+      </c>
+      <c r="F350" s="17"/>
+    </row>
+    <row r="351" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A351" s="119" t="s">
+        <v>114</v>
+      </c>
+      <c r="B351" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C351" s="22" t="s">
         <v>364</v>
       </c>
-      <c r="D350" s="17" t="s">
+      <c r="D351" s="17" t="s">
         <v>223</v>
       </c>
-      <c r="E350" s="34">
+      <c r="E351" s="34">
         <v>25</v>
       </c>
-      <c r="F350" s="17"/>
-    </row>
-    <row r="351" spans="1:6" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A351" s="119" t="s">
+      <c r="F351" s="17"/>
+    </row>
+    <row r="352" spans="1:6" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A352" s="119" t="s">
         <v>119</v>
-      </c>
-      <c r="B351" s="18" t="s">
-        <v>283</v>
-      </c>
-      <c r="C351" s="22" t="s">
-        <v>566</v>
-      </c>
-      <c r="D351" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="E351" s="34" t="s">
-        <v>567</v>
-      </c>
-      <c r="F351" s="17"/>
-    </row>
-    <row r="352" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A352" s="119" t="s">
-        <v>120</v>
       </c>
       <c r="B352" s="18" t="s">
         <v>283</v>
       </c>
       <c r="C352" s="22" t="s">
+        <v>566</v>
+      </c>
+      <c r="D352" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="E352" s="34" t="s">
+        <v>567</v>
+      </c>
+      <c r="F352" s="17"/>
+    </row>
+    <row r="353" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A353" s="119" t="s">
+        <v>120</v>
+      </c>
+      <c r="B353" s="18" t="s">
+        <v>283</v>
+      </c>
+      <c r="C353" s="22" t="s">
         <v>365</v>
       </c>
-      <c r="D352" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="E352" s="34" t="s">
+      <c r="D353" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="E353" s="34" t="s">
         <v>228</v>
       </c>
-      <c r="F352" s="17"/>
-    </row>
-    <row r="353" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A353" s="124" t="s">
+      <c r="F353" s="17"/>
+    </row>
+    <row r="354" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A354" s="124" t="s">
         <v>69</v>
       </c>
-      <c r="B353" s="106" t="s">
+      <c r="B354" s="106" t="s">
         <v>45</v>
       </c>
-      <c r="C353" s="113"/>
-      <c r="D353" s="107"/>
-      <c r="E353" s="108"/>
-      <c r="F353" s="67"/>
-    </row>
-    <row r="354" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A354" s="125" t="s">
+      <c r="C354" s="113"/>
+      <c r="D354" s="107"/>
+      <c r="E354" s="108"/>
+      <c r="F354" s="67"/>
+    </row>
+    <row r="355" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A355" s="125" t="s">
         <v>13</v>
       </c>
-      <c r="B354" s="18" t="s">
+      <c r="B355" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="C354" s="22" t="s">
+      <c r="C355" s="22" t="s">
         <v>548</v>
       </c>
-      <c r="D354" s="17" t="s">
+      <c r="D355" s="17" t="s">
         <v>164</v>
       </c>
-      <c r="E354" s="17" t="s">
+      <c r="E355" s="17" t="s">
         <v>192</v>
       </c>
-      <c r="F354" s="17"/>
-    </row>
-    <row r="355" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A355" s="100" t="s">
+      <c r="F355" s="17"/>
+    </row>
+    <row r="356" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A356" s="125" t="s">
+        <v>56</v>
+      </c>
+      <c r="B356" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C356" s="22" t="s">
+        <v>710</v>
+      </c>
+      <c r="D356" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="E356" s="17" t="s">
+        <v>709</v>
+      </c>
+      <c r="F356" s="17"/>
+    </row>
+    <row r="357" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A357" s="100" t="s">
         <v>121</v>
       </c>
-      <c r="B355" s="62" t="s">
+      <c r="B357" s="62" t="s">
         <v>45</v>
       </c>
-      <c r="C355" s="28" t="s">
+      <c r="C357" s="28" t="s">
         <v>122</v>
       </c>
-      <c r="D355" s="21"/>
-      <c r="E355" s="32"/>
-      <c r="F355" s="32"/>
-    </row>
-    <row r="356" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A356" s="92" t="s">
-        <v>416</v>
-      </c>
-      <c r="B356" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="C356" s="22" t="s">
-        <v>417</v>
-      </c>
-      <c r="D356" s="22"/>
-      <c r="E356" s="22"/>
-      <c r="F356" s="22"/>
-    </row>
-    <row r="357" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A357" s="92" t="s">
-        <v>123</v>
-      </c>
-      <c r="B357" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="C357" s="22" t="s">
-        <v>568</v>
-      </c>
-      <c r="D357" s="17" t="s">
-        <v>224</v>
-      </c>
-      <c r="E357" s="41" t="s">
-        <v>245</v>
-      </c>
-      <c r="F357" s="17"/>
+      <c r="D357" s="21"/>
+      <c r="E357" s="32"/>
+      <c r="F357" s="32"/>
     </row>
     <row r="358" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A358" s="92" t="s">
-        <v>111</v>
+        <v>416</v>
       </c>
       <c r="B358" s="18" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C358" s="22" t="s">
-        <v>569</v>
-      </c>
-      <c r="D358" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="E358" s="34" t="s">
-        <v>225</v>
-      </c>
-      <c r="F358" s="17"/>
-    </row>
-    <row r="359" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+        <v>417</v>
+      </c>
+      <c r="D358" s="22"/>
+      <c r="E358" s="22"/>
+      <c r="F358" s="22"/>
+    </row>
+    <row r="359" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A359" s="92" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B359" s="18" t="s">
         <v>45</v>
       </c>
       <c r="C359" s="22" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="D359" s="17" t="s">
         <v>224</v>
       </c>
       <c r="E359" s="41" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F359" s="17"/>
     </row>
@@ -9863,7 +9872,7 @@
         <v>45</v>
       </c>
       <c r="C360" s="22" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="D360" s="17" t="s">
         <v>164</v>
@@ -9875,19 +9884,19 @@
     </row>
     <row r="361" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A361" s="92" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B361" s="18" t="s">
         <v>45</v>
       </c>
       <c r="C361" s="22" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="D361" s="17" t="s">
         <v>224</v>
       </c>
       <c r="E361" s="41" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F361" s="17"/>
     </row>
@@ -9899,7 +9908,7 @@
         <v>45</v>
       </c>
       <c r="C362" s="22" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="D362" s="17" t="s">
         <v>164</v>
@@ -9909,21 +9918,21 @@
       </c>
       <c r="F362" s="17"/>
     </row>
-    <row r="363" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="363" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A363" s="92" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B363" s="18" t="s">
-        <v>283</v>
+        <v>45</v>
       </c>
       <c r="C363" s="22" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="D363" s="17" t="s">
         <v>224</v>
       </c>
-      <c r="E363" s="34" t="s">
-        <v>248</v>
+      <c r="E363" s="41" t="s">
+        <v>247</v>
       </c>
       <c r="F363" s="17"/>
     </row>
@@ -9932,10 +9941,10 @@
         <v>111</v>
       </c>
       <c r="B364" s="18" t="s">
-        <v>285</v>
+        <v>45</v>
       </c>
       <c r="C364" s="22" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="D364" s="17" t="s">
         <v>164</v>
@@ -9947,19 +9956,19 @@
     </row>
     <row r="365" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A365" s="92" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B365" s="18" t="s">
         <v>283</v>
       </c>
       <c r="C365" s="22" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="D365" s="17" t="s">
         <v>224</v>
       </c>
-      <c r="E365" s="41" t="s">
-        <v>249</v>
+      <c r="E365" s="34" t="s">
+        <v>248</v>
       </c>
       <c r="F365" s="17"/>
     </row>
@@ -9971,7 +9980,7 @@
         <v>285</v>
       </c>
       <c r="C366" s="22" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="D366" s="17" t="s">
         <v>164</v>
@@ -9981,21 +9990,21 @@
       </c>
       <c r="F366" s="17"/>
     </row>
-    <row r="367" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="367" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A367" s="92" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B367" s="18" t="s">
         <v>283</v>
       </c>
       <c r="C367" s="22" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="D367" s="17" t="s">
         <v>224</v>
       </c>
       <c r="E367" s="41" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F367" s="17"/>
     </row>
@@ -10007,7 +10016,7 @@
         <v>285</v>
       </c>
       <c r="C368" s="22" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="D368" s="17" t="s">
         <v>164</v>
@@ -10017,21 +10026,21 @@
       </c>
       <c r="F368" s="17"/>
     </row>
-    <row r="369" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="369" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A369" s="92" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B369" s="18" t="s">
         <v>283</v>
       </c>
       <c r="C369" s="22" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="D369" s="17" t="s">
         <v>224</v>
       </c>
       <c r="E369" s="41" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="F369" s="17"/>
     </row>
@@ -10043,7 +10052,7 @@
         <v>285</v>
       </c>
       <c r="C370" s="22" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="D370" s="17" t="s">
         <v>164</v>
@@ -10053,21 +10062,21 @@
       </c>
       <c r="F370" s="17"/>
     </row>
-    <row r="371" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="371" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A371" s="92" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B371" s="18" t="s">
-        <v>45</v>
+        <v>283</v>
       </c>
       <c r="C371" s="22" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="D371" s="17" t="s">
         <v>224</v>
       </c>
       <c r="E371" s="41" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="F371" s="17"/>
     </row>
@@ -10076,10 +10085,10 @@
         <v>111</v>
       </c>
       <c r="B372" s="18" t="s">
-        <v>45</v>
+        <v>285</v>
       </c>
       <c r="C372" s="22" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="D372" s="17" t="s">
         <v>164</v>
@@ -10089,727 +10098,731 @@
       </c>
       <c r="F372" s="17"/>
     </row>
-    <row r="373" spans="1:6" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A373" s="100" t="s">
+    <row r="373" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A373" s="92" t="s">
+        <v>130</v>
+      </c>
+      <c r="B373" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C373" s="22" t="s">
+        <v>582</v>
+      </c>
+      <c r="D373" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="E373" s="41" t="s">
+        <v>251</v>
+      </c>
+      <c r="F373" s="17"/>
+    </row>
+    <row r="374" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A374" s="92" t="s">
+        <v>111</v>
+      </c>
+      <c r="B374" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C374" s="22" t="s">
+        <v>583</v>
+      </c>
+      <c r="D374" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="E374" s="34" t="s">
+        <v>225</v>
+      </c>
+      <c r="F374" s="17"/>
+    </row>
+    <row r="375" spans="1:6" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A375" s="100" t="s">
         <v>131</v>
       </c>
-      <c r="B373" s="62" t="s">
+      <c r="B375" s="62" t="s">
         <v>45</v>
       </c>
-      <c r="C373" s="28" t="s">
+      <c r="C375" s="28" t="s">
         <v>584</v>
       </c>
-      <c r="D373" s="21"/>
-      <c r="E373" s="32"/>
-      <c r="F373" s="32"/>
-    </row>
-    <row r="374" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A374" s="134" t="s">
+      <c r="D375" s="21"/>
+      <c r="E375" s="32"/>
+      <c r="F375" s="32"/>
+    </row>
+    <row r="376" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A376" s="134" t="s">
         <v>416</v>
       </c>
-      <c r="B374" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="C374" s="22" t="s">
+      <c r="B376" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C376" s="22" t="s">
         <v>585</v>
       </c>
-      <c r="D374" s="22"/>
-      <c r="E374" s="22"/>
-      <c r="F374" s="22"/>
-    </row>
-    <row r="375" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A375" s="134" t="s">
+      <c r="D376" s="22"/>
+      <c r="E376" s="22"/>
+      <c r="F376" s="22"/>
+    </row>
+    <row r="377" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A377" s="134" t="s">
         <v>13</v>
-      </c>
-      <c r="B375" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="C375" s="22" t="s">
-        <v>366</v>
-      </c>
-      <c r="D375" s="17" t="s">
-        <v>166</v>
-      </c>
-      <c r="E375" s="34">
-        <v>1</v>
-      </c>
-      <c r="F375" s="17"/>
-    </row>
-    <row r="376" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A376" s="134" t="s">
-        <v>19</v>
-      </c>
-      <c r="B376" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="C376" s="22" t="s">
-        <v>586</v>
-      </c>
-      <c r="D376" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="E376" s="34" t="s">
-        <v>229</v>
-      </c>
-      <c r="F376" s="34"/>
-    </row>
-    <row r="377" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A377" s="134" t="s">
-        <v>133</v>
       </c>
       <c r="B377" s="18" t="s">
         <v>45</v>
       </c>
       <c r="C377" s="22" t="s">
-        <v>701</v>
+        <v>366</v>
       </c>
       <c r="D377" s="17" t="s">
-        <v>230</v>
+        <v>166</v>
       </c>
       <c r="E377" s="34">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="F377" s="17"/>
     </row>
-    <row r="378" spans="1:6" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A378" s="92" t="s">
-        <v>134</v>
+    <row r="378" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A378" s="134" t="s">
+        <v>19</v>
       </c>
       <c r="B378" s="18" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C378" s="22" t="s">
-        <v>702</v>
+        <v>586</v>
       </c>
       <c r="D378" s="17" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="E378" s="34" t="s">
-        <v>231</v>
-      </c>
-      <c r="F378" s="17"/>
-    </row>
-    <row r="379" spans="1:6" x14ac:dyDescent="0.2">
+        <v>229</v>
+      </c>
+      <c r="F378" s="34"/>
+    </row>
+    <row r="379" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A379" s="134" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="B379" s="18" t="s">
         <v>45</v>
       </c>
       <c r="C379" s="22" t="s">
-        <v>587</v>
+        <v>701</v>
       </c>
       <c r="D379" s="17" t="s">
-        <v>224</v>
-      </c>
-      <c r="E379" s="41" t="s">
-        <v>252</v>
+        <v>230</v>
+      </c>
+      <c r="E379" s="34">
+        <v>100</v>
       </c>
       <c r="F379" s="17"/>
     </row>
-    <row r="380" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="380" spans="1:6" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A380" s="92" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="B380" s="18" t="s">
         <v>45</v>
       </c>
       <c r="C380" s="22" t="s">
-        <v>588</v>
+        <v>702</v>
       </c>
       <c r="D380" s="17" t="s">
         <v>164</v>
       </c>
       <c r="E380" s="34" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="F380" s="17"/>
     </row>
     <row r="381" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A381" s="134" t="s">
+        <v>123</v>
+      </c>
+      <c r="B381" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C381" s="22" t="s">
+        <v>587</v>
+      </c>
+      <c r="D381" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="E381" s="41" t="s">
+        <v>252</v>
+      </c>
+      <c r="F381" s="17"/>
+    </row>
+    <row r="382" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A382" s="92" t="s">
+        <v>111</v>
+      </c>
+      <c r="B382" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C382" s="22" t="s">
+        <v>588</v>
+      </c>
+      <c r="D382" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="E382" s="34" t="s">
+        <v>225</v>
+      </c>
+      <c r="F382" s="17"/>
+    </row>
+    <row r="383" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A383" s="134" t="s">
         <v>22</v>
       </c>
-      <c r="B381" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="C381" s="22" t="s">
+      <c r="B383" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C383" s="22" t="s">
         <v>367</v>
       </c>
-      <c r="D381" s="17" t="s">
+      <c r="D383" s="17" t="s">
         <v>166</v>
       </c>
-      <c r="E381" s="34" t="s">
+      <c r="E383" s="34" t="s">
         <v>232</v>
       </c>
-      <c r="F381" s="17"/>
-    </row>
-    <row r="382" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A382" s="135" t="s">
+      <c r="F383" s="17"/>
+    </row>
+    <row r="384" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A384" s="135" t="s">
         <v>24</v>
       </c>
-      <c r="B382" s="25" t="s">
+      <c r="B384" s="25" t="s">
         <v>283</v>
       </c>
-      <c r="C382" s="57" t="s">
+      <c r="C384" s="57" t="s">
         <v>135</v>
       </c>
-      <c r="D382" s="23"/>
-      <c r="E382" s="36"/>
-      <c r="F382" s="36"/>
-    </row>
-    <row r="383" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A383" s="117" t="s">
+      <c r="D384" s="23"/>
+      <c r="E384" s="36"/>
+      <c r="F384" s="36"/>
+    </row>
+    <row r="385" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A385" s="117" t="s">
         <v>25</v>
       </c>
-      <c r="B383" s="18" t="s">
+      <c r="B385" s="18" t="s">
         <v>285</v>
       </c>
-      <c r="C383" s="22" t="s">
+      <c r="C385" s="22" t="s">
         <v>368</v>
       </c>
-      <c r="D383" s="17" t="s">
+      <c r="D385" s="17" t="s">
         <v>163</v>
       </c>
-      <c r="E383" s="35">
+      <c r="E385" s="35">
         <v>43013</v>
       </c>
-      <c r="F383" s="17"/>
-    </row>
-    <row r="384" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A384" s="117" t="s">
+      <c r="F385" s="17"/>
+    </row>
+    <row r="386" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A386" s="117" t="s">
         <v>26</v>
       </c>
-      <c r="B384" s="18" t="s">
+      <c r="B386" s="18" t="s">
         <v>285</v>
       </c>
-      <c r="C384" s="22" t="s">
+      <c r="C386" s="22" t="s">
         <v>369</v>
       </c>
-      <c r="D384" s="17" t="s">
+      <c r="D386" s="17" t="s">
         <v>163</v>
       </c>
-      <c r="E384" s="35">
+      <c r="E386" s="35">
         <v>43023</v>
       </c>
-      <c r="F384" s="17"/>
-    </row>
-    <row r="385" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A385" s="135" t="s">
+      <c r="F386" s="17"/>
+    </row>
+    <row r="387" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A387" s="135" t="s">
         <v>136</v>
       </c>
-      <c r="B385" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="C385" s="57"/>
-      <c r="D385" s="23"/>
-      <c r="E385" s="36"/>
-      <c r="F385" s="36"/>
-    </row>
-    <row r="386" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A386" s="136" t="s">
+      <c r="B387" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="C387" s="57"/>
+      <c r="D387" s="23"/>
+      <c r="E387" s="36"/>
+      <c r="F387" s="36"/>
+    </row>
+    <row r="388" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A388" s="136" t="s">
         <v>416</v>
       </c>
-      <c r="B386" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="C386" s="22" t="s">
+      <c r="B388" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C388" s="22" t="s">
         <v>585</v>
       </c>
-      <c r="D386" s="22"/>
-      <c r="E386" s="22"/>
-      <c r="F386" s="22"/>
-    </row>
-    <row r="387" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A387" s="117" t="s">
+      <c r="D388" s="22"/>
+      <c r="E388" s="22"/>
+      <c r="F388" s="22"/>
+    </row>
+    <row r="389" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A389" s="117" t="s">
         <v>137</v>
       </c>
-      <c r="B387" s="18" t="s">
+      <c r="B389" s="18" t="s">
         <v>286</v>
       </c>
-      <c r="C387" s="22" t="s">
+      <c r="C389" s="22" t="s">
         <v>370</v>
       </c>
-      <c r="D387" s="17" t="s">
+      <c r="D389" s="17" t="s">
         <v>166</v>
       </c>
-      <c r="E387" s="34">
+      <c r="E389" s="34">
         <v>10</v>
       </c>
-      <c r="F387" s="17"/>
-    </row>
-    <row r="388" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A388" s="117" t="s">
+      <c r="F389" s="17"/>
+    </row>
+    <row r="390" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A390" s="117" t="s">
         <v>589</v>
       </c>
-      <c r="B388" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="C388" s="22" t="s">
+      <c r="B390" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C390" s="22" t="s">
         <v>590</v>
       </c>
-      <c r="D388" s="17" t="s">
+      <c r="D390" s="17" t="s">
         <v>166</v>
       </c>
-      <c r="E388" s="34">
+      <c r="E390" s="34">
         <v>1</v>
       </c>
-      <c r="F388" s="17"/>
-    </row>
-    <row r="389" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A389" s="122" t="s">
+      <c r="F390" s="17"/>
+    </row>
+    <row r="391" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A391" s="122" t="s">
         <v>27</v>
       </c>
-      <c r="B389" s="103" t="s">
-        <v>39</v>
-      </c>
-      <c r="C389" s="112"/>
-      <c r="D389" s="104"/>
-      <c r="E389" s="105"/>
-      <c r="F389" s="61"/>
-    </row>
-    <row r="390" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A390" s="119" t="s">
-        <v>13</v>
-      </c>
-      <c r="B390" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="C390" s="22" t="s">
-        <v>591</v>
-      </c>
-      <c r="D390" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="E390" s="34" t="s">
-        <v>592</v>
-      </c>
-      <c r="F390" s="17"/>
-    </row>
-    <row r="391" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A391" s="119" t="s">
-        <v>28</v>
-      </c>
-      <c r="B391" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="C391" s="22" t="s">
-        <v>593</v>
-      </c>
-      <c r="D391" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="E391" s="34" t="s">
-        <v>594</v>
-      </c>
-      <c r="F391" s="17"/>
+      <c r="B391" s="103" t="s">
+        <v>39</v>
+      </c>
+      <c r="C391" s="112"/>
+      <c r="D391" s="104"/>
+      <c r="E391" s="105"/>
+      <c r="F391" s="61"/>
     </row>
     <row r="392" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A392" s="119" t="s">
+        <v>13</v>
+      </c>
+      <c r="B392" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C392" s="22" t="s">
+        <v>591</v>
+      </c>
+      <c r="D392" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="E392" s="34" t="s">
+        <v>592</v>
+      </c>
+      <c r="F392" s="17"/>
+    </row>
+    <row r="393" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A393" s="119" t="s">
+        <v>28</v>
+      </c>
+      <c r="B393" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C393" s="22" t="s">
+        <v>593</v>
+      </c>
+      <c r="D393" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="E393" s="34" t="s">
+        <v>594</v>
+      </c>
+      <c r="F393" s="17"/>
+    </row>
+    <row r="394" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A394" s="119" t="s">
         <v>14</v>
       </c>
-      <c r="B392" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="C392" s="22" t="s">
+      <c r="B394" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C394" s="22" t="s">
         <v>595</v>
       </c>
-      <c r="D392" s="17" t="s">
+      <c r="D394" s="17" t="s">
         <v>163</v>
       </c>
-      <c r="E392" s="35">
+      <c r="E394" s="35">
         <v>36161</v>
       </c>
-      <c r="F392" s="17"/>
-    </row>
-    <row r="393" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A393" s="135" t="s">
+      <c r="F394" s="17"/>
+    </row>
+    <row r="395" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A395" s="135" t="s">
         <v>596</v>
       </c>
-      <c r="B393" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="C393" s="57"/>
-      <c r="D393" s="23"/>
-      <c r="E393" s="36"/>
-      <c r="F393" s="36"/>
-    </row>
-    <row r="394" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A394" s="117" t="s">
+      <c r="B395" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="C395" s="57"/>
+      <c r="D395" s="23"/>
+      <c r="E395" s="36"/>
+      <c r="F395" s="36"/>
+    </row>
+    <row r="396" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A396" s="117" t="s">
         <v>137</v>
-      </c>
-      <c r="B394" s="18" t="s">
-        <v>286</v>
-      </c>
-      <c r="C394" s="22" t="s">
-        <v>597</v>
-      </c>
-      <c r="D394" s="17" t="s">
-        <v>166</v>
-      </c>
-      <c r="E394" s="34">
-        <v>10</v>
-      </c>
-      <c r="F394" s="17"/>
-    </row>
-    <row r="395" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A395" s="122" t="s">
-        <v>598</v>
-      </c>
-      <c r="B395" s="103" t="s">
-        <v>39</v>
-      </c>
-      <c r="C395" s="112"/>
-      <c r="D395" s="104"/>
-      <c r="E395" s="105"/>
-      <c r="F395" s="61"/>
-    </row>
-    <row r="396" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A396" s="119" t="s">
-        <v>13</v>
       </c>
       <c r="B396" s="18" t="s">
         <v>286</v>
       </c>
       <c r="C396" s="22" t="s">
+        <v>597</v>
+      </c>
+      <c r="D396" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="E396" s="34">
+        <v>10</v>
+      </c>
+      <c r="F396" s="17"/>
+    </row>
+    <row r="397" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A397" s="122" t="s">
+        <v>598</v>
+      </c>
+      <c r="B397" s="103" t="s">
+        <v>39</v>
+      </c>
+      <c r="C397" s="112"/>
+      <c r="D397" s="104"/>
+      <c r="E397" s="105"/>
+      <c r="F397" s="61"/>
+    </row>
+    <row r="398" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A398" s="119" t="s">
+        <v>13</v>
+      </c>
+      <c r="B398" s="18" t="s">
+        <v>286</v>
+      </c>
+      <c r="C398" s="22" t="s">
         <v>599</v>
       </c>
-      <c r="D396" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="E396" s="95">
+      <c r="D398" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="E398" s="95">
         <v>23421</v>
       </c>
-      <c r="F396" s="17"/>
-    </row>
-    <row r="397" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A397" s="119" t="s">
+      <c r="F398" s="17"/>
+    </row>
+    <row r="399" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A399" s="119" t="s">
         <v>14</v>
       </c>
-      <c r="B397" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="C397" s="22" t="s">
+      <c r="B399" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C399" s="22" t="s">
         <v>600</v>
       </c>
-      <c r="D397" s="17" t="s">
+      <c r="D399" s="17" t="s">
         <v>163</v>
       </c>
-      <c r="E397" s="95" t="s">
+      <c r="E399" s="95" t="s">
         <v>601</v>
       </c>
-      <c r="F397" s="17"/>
-    </row>
-    <row r="398" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A398" s="135" t="s">
+      <c r="F399" s="17"/>
+    </row>
+    <row r="400" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A400" s="135" t="s">
         <v>598</v>
       </c>
-      <c r="B398" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="C398" s="57"/>
-      <c r="D398" s="23"/>
-      <c r="E398" s="36"/>
-      <c r="F398" s="36"/>
-    </row>
-    <row r="399" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A399" s="117" t="s">
-        <v>13</v>
-      </c>
-      <c r="B399" s="18" t="s">
-        <v>286</v>
-      </c>
-      <c r="C399" s="22" t="s">
-        <v>602</v>
-      </c>
-      <c r="D399" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="E399" s="95" t="s">
-        <v>603</v>
-      </c>
-      <c r="F399" s="17"/>
-    </row>
-    <row r="400" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A400" s="117" t="s">
-        <v>428</v>
-      </c>
-      <c r="B400" s="18" t="s">
-        <v>286</v>
-      </c>
-      <c r="C400" s="22" t="s">
-        <v>604</v>
-      </c>
-      <c r="D400" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="E400" s="95" t="s">
-        <v>605</v>
-      </c>
-      <c r="F400" s="17"/>
+      <c r="B400" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="C400" s="57"/>
+      <c r="D400" s="23"/>
+      <c r="E400" s="36"/>
+      <c r="F400" s="36"/>
     </row>
     <row r="401" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A401" s="117" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B401" s="18" t="s">
-        <v>39</v>
+        <v>286</v>
       </c>
       <c r="C401" s="22" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
       <c r="D401" s="17" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="E401" s="95" t="s">
-        <v>601</v>
+        <v>603</v>
       </c>
       <c r="F401" s="17"/>
     </row>
     <row r="402" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A402" s="117" t="s">
-        <v>263</v>
+        <v>428</v>
       </c>
       <c r="B402" s="18" t="s">
-        <v>39</v>
+        <v>286</v>
       </c>
       <c r="C402" s="22" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="D402" s="17" t="s">
-        <v>609</v>
+        <v>164</v>
       </c>
       <c r="E402" s="95" t="s">
-        <v>610</v>
+        <v>605</v>
       </c>
       <c r="F402" s="17"/>
     </row>
     <row r="403" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A403" s="117" t="s">
+        <v>14</v>
+      </c>
+      <c r="B403" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C403" s="22" t="s">
+        <v>606</v>
+      </c>
+      <c r="D403" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="E403" s="95" t="s">
+        <v>601</v>
+      </c>
+      <c r="F403" s="17"/>
+    </row>
+    <row r="404" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A404" s="117" t="s">
+        <v>263</v>
+      </c>
+      <c r="B404" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C404" s="22" t="s">
+        <v>607</v>
+      </c>
+      <c r="D404" s="17" t="s">
+        <v>609</v>
+      </c>
+      <c r="E404" s="95" t="s">
+        <v>610</v>
+      </c>
+      <c r="F404" s="17"/>
+    </row>
+    <row r="405" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A405" s="117" t="s">
         <v>40</v>
       </c>
-      <c r="B403" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="C403" s="22" t="s">
+      <c r="B405" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C405" s="22" t="s">
         <v>608</v>
       </c>
-      <c r="D403" s="17" t="s">
+      <c r="D405" s="17" t="s">
         <v>164</v>
       </c>
-      <c r="E403" s="95" t="s">
+      <c r="E405" s="95" t="s">
         <v>611</v>
       </c>
-      <c r="F403" s="96">
+      <c r="F405" s="96">
         <v>130</v>
       </c>
     </row>
-    <row r="404" spans="1:6" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A404" s="135" t="s">
+    <row r="406" spans="1:6" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A406" s="135" t="s">
         <v>82</v>
       </c>
-      <c r="B404" s="25" t="s">
+      <c r="B406" s="25" t="s">
         <v>276</v>
       </c>
-      <c r="C404" s="57" t="s">
+      <c r="C406" s="57" t="s">
         <v>395</v>
       </c>
-      <c r="D404" s="23"/>
-      <c r="E404" s="36"/>
-      <c r="F404" s="36"/>
-    </row>
-    <row r="405" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A405" s="117" t="s">
+      <c r="D406" s="23"/>
+      <c r="E406" s="36"/>
+      <c r="F406" s="36"/>
+    </row>
+    <row r="407" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A407" s="117" t="s">
         <v>394</v>
-      </c>
-      <c r="B405" s="54" t="s">
-        <v>289</v>
-      </c>
-      <c r="C405" s="22" t="s">
-        <v>612</v>
-      </c>
-      <c r="D405" s="22" t="s">
-        <v>230</v>
-      </c>
-      <c r="E405" s="97">
-        <v>1</v>
-      </c>
-      <c r="F405" s="17"/>
-    </row>
-    <row r="406" spans="1:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="A406" s="117" t="s">
-        <v>134</v>
-      </c>
-      <c r="B406" s="54" t="s">
-        <v>289</v>
-      </c>
-      <c r="C406" s="22" t="s">
-        <v>613</v>
-      </c>
-      <c r="D406" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="E406" s="34" t="s">
-        <v>231</v>
-      </c>
-      <c r="F406" s="17"/>
-    </row>
-    <row r="407" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A407" s="117" t="s">
-        <v>84</v>
       </c>
       <c r="B407" s="54" t="s">
         <v>289</v>
       </c>
       <c r="C407" s="22" t="s">
+        <v>612</v>
+      </c>
+      <c r="D407" s="22" t="s">
+        <v>230</v>
+      </c>
+      <c r="E407" s="97">
+        <v>1</v>
+      </c>
+      <c r="F407" s="17"/>
+    </row>
+    <row r="408" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A408" s="117" t="s">
+        <v>134</v>
+      </c>
+      <c r="B408" s="54" t="s">
+        <v>289</v>
+      </c>
+      <c r="C408" s="22" t="s">
+        <v>613</v>
+      </c>
+      <c r="D408" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="E408" s="34" t="s">
+        <v>231</v>
+      </c>
+      <c r="F408" s="17"/>
+    </row>
+    <row r="409" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A409" s="117" t="s">
+        <v>84</v>
+      </c>
+      <c r="B409" s="54" t="s">
+        <v>289</v>
+      </c>
+      <c r="C409" s="22" t="s">
         <v>614</v>
       </c>
-      <c r="D407" s="17" t="s">
+      <c r="D409" s="17" t="s">
         <v>163</v>
       </c>
-      <c r="E407" s="35">
+      <c r="E409" s="35">
         <v>43070</v>
       </c>
-      <c r="F407" s="17"/>
-    </row>
-    <row r="408" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A408" s="122" t="s">
+      <c r="F409" s="17"/>
+    </row>
+    <row r="410" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A410" s="122" t="s">
         <v>86</v>
       </c>
-      <c r="B408" s="103" t="s">
+      <c r="B410" s="103" t="s">
         <v>276</v>
       </c>
-      <c r="C408" s="112"/>
-      <c r="D408" s="104"/>
-      <c r="E408" s="105"/>
-      <c r="F408" s="61"/>
-    </row>
-    <row r="409" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A409" s="119" t="s">
+      <c r="C410" s="112"/>
+      <c r="D410" s="104"/>
+      <c r="E410" s="105"/>
+      <c r="F410" s="61"/>
+    </row>
+    <row r="411" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A411" s="119" t="s">
         <v>13</v>
       </c>
-      <c r="B409" s="18" t="s">
+      <c r="B411" s="18" t="s">
         <v>276</v>
       </c>
-      <c r="C409" s="22" t="s">
+      <c r="C411" s="22" t="s">
         <v>340</v>
       </c>
-      <c r="D409" s="17" t="s">
+      <c r="D411" s="17" t="s">
         <v>166</v>
       </c>
-      <c r="E409" s="44">
+      <c r="E411" s="44">
         <v>83745498753497</v>
       </c>
-      <c r="F409" s="17"/>
-    </row>
-    <row r="410" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A410" s="119" t="s">
+      <c r="F411" s="17"/>
+    </row>
+    <row r="412" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A412" s="119" t="s">
         <v>41</v>
       </c>
-      <c r="B410" s="18" t="s">
+      <c r="B412" s="18" t="s">
         <v>288</v>
       </c>
-      <c r="C410" s="22" t="s">
+      <c r="C412" s="22" t="s">
         <v>615</v>
       </c>
-      <c r="D410" s="17" t="s">
+      <c r="D412" s="17" t="s">
         <v>164</v>
       </c>
-      <c r="E410" s="41" t="s">
+      <c r="E412" s="41" t="s">
         <v>194</v>
       </c>
-      <c r="F410" s="17"/>
-    </row>
-    <row r="411" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A411" s="122" t="s">
+      <c r="F412" s="17"/>
+    </row>
+    <row r="413" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A413" s="122" t="s">
         <v>87</v>
       </c>
-      <c r="B411" s="103" t="s">
+      <c r="B413" s="103" t="s">
         <v>289</v>
       </c>
-      <c r="C411" s="112" t="s">
+      <c r="C413" s="112" t="s">
         <v>341</v>
       </c>
-      <c r="D411" s="104"/>
-      <c r="E411" s="105"/>
-      <c r="F411" s="61"/>
-    </row>
-    <row r="412" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A412" s="119" t="s">
-        <v>58</v>
-      </c>
-      <c r="B412" s="18" t="s">
-        <v>289</v>
-      </c>
-      <c r="C412" s="22" t="s">
-        <v>342</v>
-      </c>
-      <c r="D412" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="E412" s="34" t="s">
-        <v>210</v>
-      </c>
-      <c r="F412" s="17"/>
-    </row>
-    <row r="413" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A413" s="119" t="s">
-        <v>59</v>
-      </c>
-      <c r="B413" s="18" t="s">
-        <v>289</v>
-      </c>
-      <c r="C413" s="22" t="s">
-        <v>343</v>
-      </c>
-      <c r="D413" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="E413" s="34" t="s">
-        <v>211</v>
-      </c>
-      <c r="F413" s="17"/>
+      <c r="D413" s="104"/>
+      <c r="E413" s="105"/>
+      <c r="F413" s="61"/>
     </row>
     <row r="414" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A414" s="119" t="s">
-        <v>265</v>
+        <v>58</v>
       </c>
       <c r="B414" s="18" t="s">
         <v>289</v>
       </c>
       <c r="C414" s="22" t="s">
-        <v>495</v>
+        <v>342</v>
       </c>
       <c r="D414" s="17" t="s">
         <v>167</v>
       </c>
-      <c r="E414" s="34"/>
+      <c r="E414" s="34" t="s">
+        <v>210</v>
+      </c>
       <c r="F414" s="17"/>
     </row>
-    <row r="415" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="415" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A415" s="119" t="s">
-        <v>266</v>
+        <v>59</v>
       </c>
       <c r="B415" s="18" t="s">
         <v>289</v>
       </c>
       <c r="C415" s="22" t="s">
-        <v>616</v>
+        <v>343</v>
       </c>
       <c r="D415" s="17" t="s">
         <v>167</v>
       </c>
-      <c r="E415" s="34"/>
+      <c r="E415" s="34" t="s">
+        <v>211</v>
+      </c>
       <c r="F415" s="17"/>
     </row>
-    <row r="416" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="416" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A416" s="119" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B416" s="18" t="s">
         <v>289</v>
       </c>
       <c r="C416" s="22" t="s">
-        <v>617</v>
+        <v>495</v>
       </c>
       <c r="D416" s="17" t="s">
         <v>167</v>
@@ -10817,249 +10830,245 @@
       <c r="E416" s="34"/>
       <c r="F416" s="17"/>
     </row>
-    <row r="417" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="417" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A417" s="119" t="s">
-        <v>60</v>
+        <v>266</v>
       </c>
       <c r="B417" s="18" t="s">
         <v>289</v>
       </c>
       <c r="C417" s="22" t="s">
-        <v>344</v>
+        <v>616</v>
       </c>
       <c r="D417" s="17" t="s">
         <v>167</v>
       </c>
-      <c r="E417" s="34" t="s">
-        <v>212</v>
-      </c>
+      <c r="E417" s="34"/>
       <c r="F417" s="17"/>
     </row>
-    <row r="418" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="418" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A418" s="119" t="s">
-        <v>61</v>
+        <v>267</v>
       </c>
       <c r="B418" s="18" t="s">
         <v>289</v>
       </c>
       <c r="C418" s="22" t="s">
-        <v>345</v>
+        <v>617</v>
       </c>
       <c r="D418" s="17" t="s">
         <v>167</v>
       </c>
-      <c r="E418" s="34">
-        <v>86756</v>
-      </c>
+      <c r="E418" s="34"/>
       <c r="F418" s="17"/>
     </row>
     <row r="419" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A419" s="119" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B419" s="18" t="s">
         <v>289</v>
       </c>
       <c r="C419" s="22" t="s">
+        <v>344</v>
+      </c>
+      <c r="D419" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="E419" s="34" t="s">
+        <v>212</v>
+      </c>
+      <c r="F419" s="17"/>
+    </row>
+    <row r="420" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A420" s="119" t="s">
+        <v>61</v>
+      </c>
+      <c r="B420" s="18" t="s">
+        <v>289</v>
+      </c>
+      <c r="C420" s="22" t="s">
+        <v>345</v>
+      </c>
+      <c r="D420" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="E420" s="34">
+        <v>86756</v>
+      </c>
+      <c r="F420" s="17"/>
+    </row>
+    <row r="421" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A421" s="119" t="s">
+        <v>62</v>
+      </c>
+      <c r="B421" s="18" t="s">
+        <v>289</v>
+      </c>
+      <c r="C421" s="22" t="s">
         <v>618</v>
       </c>
-      <c r="D419" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="E419" s="34" t="s">
+      <c r="D421" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="E421" s="34" t="s">
         <v>213</v>
       </c>
-      <c r="F419" s="17"/>
-    </row>
-    <row r="420" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A420" s="131" t="s">
+      <c r="F421" s="17"/>
+    </row>
+    <row r="422" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A422" s="131" t="s">
         <v>65</v>
       </c>
-      <c r="B420" s="115" t="s">
+      <c r="B422" s="115" t="s">
         <v>289</v>
       </c>
-      <c r="C420" s="113"/>
-      <c r="D420" s="107"/>
-      <c r="E420" s="108"/>
-      <c r="F420" s="67"/>
-    </row>
-    <row r="421" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A421" s="125" t="s">
+      <c r="C422" s="113"/>
+      <c r="D422" s="107"/>
+      <c r="E422" s="108"/>
+      <c r="F422" s="67"/>
+    </row>
+    <row r="423" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A423" s="125" t="s">
         <v>66</v>
       </c>
-      <c r="B421" s="18" t="s">
+      <c r="B423" s="18" t="s">
         <v>288</v>
       </c>
-      <c r="C421" s="22" t="s">
+      <c r="C423" s="22" t="s">
         <v>619</v>
       </c>
-      <c r="D421" s="17" t="s">
+      <c r="D423" s="17" t="s">
         <v>164</v>
       </c>
-      <c r="E421" s="34" t="s">
+      <c r="E423" s="34" t="s">
         <v>200</v>
       </c>
-      <c r="F421" s="17"/>
-    </row>
-    <row r="422" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A422" s="125" t="s">
+      <c r="F423" s="17"/>
+    </row>
+    <row r="424" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A424" s="125" t="s">
         <v>56</v>
       </c>
-      <c r="B422" s="18" t="s">
+      <c r="B424" s="18" t="s">
         <v>289</v>
       </c>
-      <c r="C422" s="22" t="s">
+      <c r="C424" s="22" t="s">
         <v>620</v>
       </c>
-      <c r="D422" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="E422" s="34" t="s">
+      <c r="D424" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="E424" s="34" t="s">
         <v>485</v>
       </c>
-      <c r="F422" s="17"/>
-    </row>
-    <row r="423" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A423" s="135" t="s">
+      <c r="F424" s="17"/>
+    </row>
+    <row r="425" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A425" s="135" t="s">
         <v>104</v>
       </c>
-      <c r="B423" s="25" t="s">
+      <c r="B425" s="25" t="s">
         <v>283</v>
       </c>
-      <c r="C423" s="57" t="s">
+      <c r="C425" s="57" t="s">
         <v>371</v>
       </c>
-      <c r="D423" s="23"/>
-      <c r="E423" s="36"/>
-      <c r="F423" s="36"/>
-    </row>
-    <row r="424" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A424" s="117" t="s">
+      <c r="D425" s="23"/>
+      <c r="E425" s="36"/>
+      <c r="F425" s="36"/>
+    </row>
+    <row r="426" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A426" s="117" t="s">
         <v>105</v>
-      </c>
-      <c r="B424" s="18" t="s">
-        <v>283</v>
-      </c>
-      <c r="C424" s="22" t="s">
-        <v>621</v>
-      </c>
-      <c r="D424" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="E424" s="22" t="s">
-        <v>622</v>
-      </c>
-      <c r="F424" s="17"/>
-    </row>
-    <row r="425" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A425" s="117" t="s">
-        <v>106</v>
-      </c>
-      <c r="B425" s="18" t="s">
-        <v>283</v>
-      </c>
-      <c r="C425" s="22" t="s">
-        <v>623</v>
-      </c>
-      <c r="D425" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="E425" s="34">
-        <v>95</v>
-      </c>
-      <c r="F425" s="17"/>
-    </row>
-    <row r="426" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A426" s="117" t="s">
-        <v>107</v>
       </c>
       <c r="B426" s="18" t="s">
         <v>283</v>
       </c>
       <c r="C426" s="22" t="s">
-        <v>372</v>
+        <v>621</v>
       </c>
       <c r="D426" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="E426" s="34" t="s">
-        <v>222</v>
+        <v>164</v>
+      </c>
+      <c r="E426" s="22" t="s">
+        <v>622</v>
       </c>
       <c r="F426" s="17"/>
     </row>
-    <row r="427" spans="1:6" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="427" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A427" s="117" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B427" s="18" t="s">
         <v>283</v>
       </c>
       <c r="C427" s="22" t="s">
-        <v>373</v>
+        <v>623</v>
       </c>
       <c r="D427" s="17" t="s">
-        <v>223</v>
+        <v>164</v>
       </c>
       <c r="E427" s="34">
-        <v>20</v>
+        <v>95</v>
       </c>
       <c r="F427" s="17"/>
     </row>
     <row r="428" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A428" s="117" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B428" s="18" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C428" s="22" t="s">
-        <v>624</v>
+        <v>372</v>
       </c>
       <c r="D428" s="17" t="s">
-        <v>224</v>
+        <v>167</v>
       </c>
       <c r="E428" s="34" t="s">
-        <v>248</v>
+        <v>222</v>
       </c>
       <c r="F428" s="17"/>
     </row>
-    <row r="429" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="429" spans="1:6" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A429" s="117" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B429" s="18" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C429" s="22" t="s">
-        <v>625</v>
+        <v>373</v>
       </c>
       <c r="D429" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="E429" s="34" t="s">
-        <v>225</v>
+        <v>223</v>
+      </c>
+      <c r="E429" s="34">
+        <v>20</v>
       </c>
       <c r="F429" s="17"/>
     </row>
     <row r="430" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A430" s="117" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B430" s="18" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="C430" s="22" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="D430" s="17" t="s">
         <v>224</v>
       </c>
       <c r="E430" s="34" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="F430" s="17"/>
     </row>
-    <row r="431" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="431" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A431" s="117" t="s">
         <v>111</v>
       </c>
@@ -11067,7 +11076,7 @@
         <v>285</v>
       </c>
       <c r="C431" s="22" t="s">
-        <v>543</v>
+        <v>625</v>
       </c>
       <c r="D431" s="17" t="s">
         <v>164</v>
@@ -11075,124 +11084,124 @@
       <c r="E431" s="34" t="s">
         <v>225</v>
       </c>
+      <c r="F431" s="17"/>
     </row>
     <row r="432" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A432" s="135" t="s">
+      <c r="A432" s="117" t="s">
+        <v>112</v>
+      </c>
+      <c r="B432" s="18" t="s">
+        <v>283</v>
+      </c>
+      <c r="C432" s="22" t="s">
+        <v>626</v>
+      </c>
+      <c r="D432" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="E432" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F432" s="17"/>
+    </row>
+    <row r="433" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A433" s="117" t="s">
+        <v>111</v>
+      </c>
+      <c r="B433" s="18" t="s">
+        <v>285</v>
+      </c>
+      <c r="C433" s="22" t="s">
+        <v>543</v>
+      </c>
+      <c r="D433" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="E433" s="34" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="434" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A434" s="135" t="s">
         <v>115</v>
       </c>
-      <c r="B432" s="25" t="s">
+      <c r="B434" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="C432" s="57"/>
-      <c r="D432" s="23"/>
-      <c r="E432" s="36"/>
-      <c r="F432" s="23"/>
-    </row>
-    <row r="433" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A433" s="117" t="s">
+      <c r="C434" s="57"/>
+      <c r="D434" s="23"/>
+      <c r="E434" s="36"/>
+      <c r="F434" s="23"/>
+    </row>
+    <row r="435" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A435" s="117" t="s">
         <v>116</v>
       </c>
-      <c r="B433" s="18" t="s">
+      <c r="B435" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="C433" s="22" t="s">
+      <c r="C435" s="22" t="s">
         <v>628</v>
       </c>
-      <c r="D433" s="17" t="s">
+      <c r="D435" s="17" t="s">
         <v>224</v>
       </c>
-      <c r="E433" s="34" t="s">
+      <c r="E435" s="34" t="s">
         <v>226</v>
       </c>
-      <c r="F433" s="22"/>
-    </row>
-    <row r="434" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A434" s="117" t="s">
+      <c r="F435" s="22"/>
+    </row>
+    <row r="436" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A436" s="117" t="s">
         <v>111</v>
-      </c>
-      <c r="B434" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="C434" s="56" t="s">
-        <v>629</v>
-      </c>
-      <c r="D434" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="E434" s="34" t="s">
-        <v>225</v>
-      </c>
-      <c r="F434" s="17"/>
-    </row>
-    <row r="435" spans="1:6" ht="77.25" x14ac:dyDescent="0.25">
-      <c r="A435" s="122" t="s">
-        <v>117</v>
-      </c>
-      <c r="B435" s="103" t="s">
-        <v>45</v>
-      </c>
-      <c r="C435" s="112" t="s">
-        <v>627</v>
-      </c>
-      <c r="D435" s="104"/>
-      <c r="E435" s="105"/>
-      <c r="F435" s="59"/>
-    </row>
-    <row r="436" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A436" s="119" t="s">
-        <v>118</v>
       </c>
       <c r="B436" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="C436" s="22" t="s">
-        <v>630</v>
+      <c r="C436" s="56" t="s">
+        <v>629</v>
       </c>
       <c r="D436" s="17" t="s">
-        <v>224</v>
-      </c>
-      <c r="E436" s="22" t="s">
-        <v>227</v>
+        <v>164</v>
+      </c>
+      <c r="E436" s="34" t="s">
+        <v>225</v>
       </c>
       <c r="F436" s="17"/>
     </row>
-    <row r="437" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A437" s="119" t="s">
-        <v>111</v>
-      </c>
-      <c r="B437" s="18" t="s">
+    <row r="437" spans="1:6" ht="77.25" x14ac:dyDescent="0.25">
+      <c r="A437" s="122" t="s">
+        <v>117</v>
+      </c>
+      <c r="B437" s="103" t="s">
         <v>45</v>
       </c>
-      <c r="C437" s="56" t="s">
-        <v>631</v>
-      </c>
-      <c r="D437" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="E437" s="22" t="s">
-        <v>225</v>
-      </c>
-      <c r="F437" s="17"/>
-    </row>
-    <row r="438" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C437" s="112" t="s">
+        <v>627</v>
+      </c>
+      <c r="D437" s="104"/>
+      <c r="E437" s="105"/>
+      <c r="F437" s="59"/>
+    </row>
+    <row r="438" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A438" s="119" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B438" s="18" t="s">
         <v>45</v>
       </c>
       <c r="C438" s="22" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="D438" s="17" t="s">
         <v>224</v>
       </c>
       <c r="E438" s="22" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="F438" s="17"/>
     </row>
-    <row r="439" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="439" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A439" s="119" t="s">
         <v>111</v>
       </c>
@@ -11200,331 +11209,339 @@
         <v>45</v>
       </c>
       <c r="C439" s="56" t="s">
-        <v>358</v>
+        <v>631</v>
       </c>
       <c r="D439" s="17" t="s">
         <v>164</v>
       </c>
-      <c r="E439" s="34" t="s">
+      <c r="E439" s="22" t="s">
         <v>225</v>
       </c>
       <c r="F439" s="17"/>
     </row>
-    <row r="440" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A440" s="124" t="s">
-        <v>113</v>
-      </c>
-      <c r="B440" s="106" t="s">
+    <row r="440" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A440" s="119" t="s">
+        <v>116</v>
+      </c>
+      <c r="B440" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="C440" s="113"/>
-      <c r="D440" s="107"/>
-      <c r="E440" s="108"/>
-      <c r="F440" s="67"/>
-    </row>
-    <row r="441" spans="1:6" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="C440" s="22" t="s">
+        <v>632</v>
+      </c>
+      <c r="D440" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="E440" s="22" t="s">
+        <v>226</v>
+      </c>
+      <c r="F440" s="17"/>
+    </row>
+    <row r="441" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A441" s="119" t="s">
-        <v>13</v>
+        <v>111</v>
       </c>
       <c r="B441" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="C441" s="22" t="s">
-        <v>703</v>
+      <c r="C441" s="56" t="s">
+        <v>358</v>
       </c>
       <c r="D441" s="17" t="s">
         <v>164</v>
       </c>
       <c r="E441" s="34" t="s">
+        <v>225</v>
+      </c>
+      <c r="F441" s="17"/>
+    </row>
+    <row r="442" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A442" s="124" t="s">
+        <v>113</v>
+      </c>
+      <c r="B442" s="106" t="s">
+        <v>45</v>
+      </c>
+      <c r="C442" s="113"/>
+      <c r="D442" s="107"/>
+      <c r="E442" s="108"/>
+      <c r="F442" s="67"/>
+    </row>
+    <row r="443" spans="1:6" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A443" s="119" t="s">
+        <v>13</v>
+      </c>
+      <c r="B443" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C443" s="22" t="s">
+        <v>703</v>
+      </c>
+      <c r="D443" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="E443" s="34" t="s">
         <v>184</v>
       </c>
-      <c r="F441" s="17"/>
-    </row>
-    <row r="442" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A442" s="119" t="s">
+      <c r="F443" s="17"/>
+    </row>
+    <row r="444" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A444" s="119" t="s">
         <v>114</v>
       </c>
-      <c r="B442" s="18" t="s">
+      <c r="B444" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="C442" s="22" t="s">
+      <c r="C444" s="22" t="s">
         <v>364</v>
       </c>
-      <c r="D442" s="17" t="s">
+      <c r="D444" s="17" t="s">
         <v>223</v>
       </c>
-      <c r="E442" s="34">
+      <c r="E444" s="34">
         <v>25</v>
       </c>
-      <c r="F442" s="17"/>
-    </row>
-    <row r="443" spans="1:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="A443" s="119" t="s">
+      <c r="F444" s="17"/>
+    </row>
+    <row r="445" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A445" s="119" t="s">
         <v>119</v>
       </c>
-      <c r="B443" s="18" t="s">
+      <c r="B445" s="18" t="s">
         <v>283</v>
       </c>
-      <c r="C443" s="22" t="s">
+      <c r="C445" s="22" t="s">
         <v>633</v>
       </c>
-      <c r="D443" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="E443" s="34"/>
-      <c r="F443" s="17"/>
-    </row>
-    <row r="444" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A444" s="119" t="s">
+      <c r="D445" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="E445" s="34"/>
+      <c r="F445" s="17"/>
+    </row>
+    <row r="446" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A446" s="119" t="s">
         <v>120</v>
       </c>
-      <c r="B444" s="18" t="s">
+      <c r="B446" s="18" t="s">
         <v>283</v>
       </c>
-      <c r="C444" s="22" t="s">
+      <c r="C446" s="22" t="s">
         <v>634</v>
       </c>
-      <c r="D444" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="E444" s="34" t="s">
+      <c r="D446" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="E446" s="34" t="s">
         <v>228</v>
       </c>
-      <c r="F444" s="17"/>
-    </row>
-    <row r="445" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A445" s="124" t="s">
+      <c r="F446" s="17"/>
+    </row>
+    <row r="447" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A447" s="124" t="s">
         <v>69</v>
       </c>
-      <c r="B445" s="106" t="s">
+      <c r="B447" s="106" t="s">
         <v>45</v>
       </c>
-      <c r="C445" s="113"/>
-      <c r="D445" s="107"/>
-      <c r="E445" s="108"/>
-      <c r="F445" s="67"/>
-    </row>
-    <row r="446" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A446" s="125" t="s">
+      <c r="C447" s="113"/>
+      <c r="D447" s="107"/>
+      <c r="E447" s="108"/>
+      <c r="F447" s="67"/>
+    </row>
+    <row r="448" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A448" s="125" t="s">
         <v>13</v>
       </c>
-      <c r="B446" s="18" t="s">
+      <c r="B448" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="C446" s="22" t="s">
+      <c r="C448" s="22" t="s">
         <v>548</v>
       </c>
-      <c r="D446" s="17" t="s">
+      <c r="D448" s="17" t="s">
         <v>164</v>
       </c>
-      <c r="E446" s="17" t="s">
+      <c r="E448" s="17" t="s">
         <v>192</v>
       </c>
-      <c r="F446" s="17"/>
-    </row>
-    <row r="447" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A447" s="135" t="s">
+      <c r="F448" s="17"/>
+    </row>
+    <row r="449" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A449" s="125" t="s">
+        <v>56</v>
+      </c>
+      <c r="B449" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C449" s="22" t="s">
+        <v>710</v>
+      </c>
+      <c r="D449" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="E449" s="17" t="s">
+        <v>709</v>
+      </c>
+      <c r="F449" s="17"/>
+    </row>
+    <row r="450" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A450" s="135" t="s">
         <v>139</v>
       </c>
-      <c r="B447" s="25" t="s">
+      <c r="B450" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="C447" s="57" t="s">
+      <c r="C450" s="57" t="s">
         <v>374</v>
       </c>
-      <c r="D447" s="23"/>
-      <c r="E447" s="36"/>
-      <c r="F447" s="36"/>
-    </row>
-    <row r="448" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A448" s="136" t="s">
+      <c r="D450" s="23"/>
+      <c r="E450" s="36"/>
+      <c r="F450" s="36"/>
+    </row>
+    <row r="451" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A451" s="136" t="s">
         <v>416</v>
       </c>
-      <c r="B448" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="C448" s="22" t="s">
+      <c r="B451" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C451" s="22" t="s">
         <v>585</v>
       </c>
-      <c r="D448" s="22"/>
-      <c r="E448" s="22"/>
-      <c r="F448" s="22"/>
-    </row>
-    <row r="449" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A449" s="117" t="s">
+      <c r="D451" s="22"/>
+      <c r="E451" s="22"/>
+      <c r="F451" s="22"/>
+    </row>
+    <row r="452" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A452" s="117" t="s">
         <v>140</v>
       </c>
-      <c r="B449" s="18" t="s">
+      <c r="B452" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="C449" s="22" t="s">
+      <c r="C452" s="22" t="s">
         <v>375</v>
       </c>
-      <c r="D449" s="22" t="s">
-        <v>167</v>
-      </c>
-      <c r="E449" s="33" t="s">
+      <c r="D452" s="22" t="s">
+        <v>167</v>
+      </c>
+      <c r="E452" s="33" t="s">
         <v>233</v>
       </c>
-      <c r="F449" s="22"/>
-    </row>
-    <row r="450" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A450" s="117" t="s">
+      <c r="F452" s="22"/>
+    </row>
+    <row r="453" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A453" s="117" t="s">
         <v>56</v>
       </c>
-      <c r="B450" s="18" t="s">
+      <c r="B453" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="C450" s="22" t="s">
+      <c r="C453" s="22" t="s">
         <v>376</v>
       </c>
-      <c r="D450" s="22" t="s">
-        <v>167</v>
-      </c>
-      <c r="E450" s="34" t="s">
+      <c r="D453" s="22" t="s">
+        <v>167</v>
+      </c>
+      <c r="E453" s="34" t="s">
         <v>141</v>
       </c>
-      <c r="F450" s="17"/>
-    </row>
-    <row r="451" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A451" s="122" t="s">
+      <c r="F453" s="17"/>
+    </row>
+    <row r="454" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A454" s="122" t="s">
         <v>142</v>
       </c>
-      <c r="B451" s="103" t="s">
-        <v>39</v>
-      </c>
-      <c r="C451" s="112"/>
-      <c r="D451" s="104"/>
-      <c r="E451" s="105"/>
-      <c r="F451" s="61"/>
-    </row>
-    <row r="452" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A452" s="119" t="s">
+      <c r="B454" s="103" t="s">
+        <v>39</v>
+      </c>
+      <c r="C454" s="112"/>
+      <c r="D454" s="104"/>
+      <c r="E454" s="105"/>
+      <c r="F454" s="61"/>
+    </row>
+    <row r="455" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A455" s="119" t="s">
         <v>13</v>
       </c>
-      <c r="B452" s="18" t="s">
+      <c r="B455" s="18" t="s">
         <v>286</v>
       </c>
-      <c r="C452" s="22" t="s">
+      <c r="C455" s="22" t="s">
         <v>377</v>
       </c>
-      <c r="D452" s="17" t="s">
+      <c r="D455" s="17" t="s">
         <v>166</v>
       </c>
-      <c r="E452" s="34">
+      <c r="E455" s="34">
         <v>123455</v>
       </c>
-      <c r="F452" s="17"/>
-    </row>
-    <row r="453" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A453" s="122" t="s">
+      <c r="F455" s="17"/>
+    </row>
+    <row r="456" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A456" s="122" t="s">
         <v>143</v>
       </c>
-      <c r="B453" s="103" t="s">
-        <v>39</v>
-      </c>
-      <c r="C453" s="112"/>
-      <c r="D453" s="104"/>
-      <c r="E453" s="105"/>
-      <c r="F453" s="61"/>
-    </row>
-    <row r="454" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A454" s="119" t="s">
+      <c r="B456" s="103" t="s">
+        <v>39</v>
+      </c>
+      <c r="C456" s="112"/>
+      <c r="D456" s="104"/>
+      <c r="E456" s="105"/>
+      <c r="F456" s="61"/>
+    </row>
+    <row r="457" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A457" s="119" t="s">
         <v>13</v>
       </c>
-      <c r="B454" s="18" t="s">
+      <c r="B457" s="18" t="s">
         <v>286</v>
       </c>
-      <c r="C454" s="22" t="s">
+      <c r="C457" s="22" t="s">
         <v>378</v>
       </c>
-      <c r="D454" s="17" t="s">
+      <c r="D457" s="17" t="s">
         <v>166</v>
       </c>
-      <c r="E454" s="34">
+      <c r="E457" s="34">
         <v>987342</v>
       </c>
-      <c r="F454" s="17"/>
-    </row>
-    <row r="455" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A455" s="122" t="s">
+      <c r="F457" s="17"/>
+    </row>
+    <row r="458" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A458" s="122" t="s">
         <v>635</v>
       </c>
-      <c r="B455" s="103" t="s">
-        <v>39</v>
-      </c>
-      <c r="C455" s="112"/>
-      <c r="D455" s="104"/>
-      <c r="E455" s="105"/>
-      <c r="F455" s="61"/>
-    </row>
-    <row r="456" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A456" s="119" t="s">
+      <c r="B458" s="103" t="s">
+        <v>39</v>
+      </c>
+      <c r="C458" s="112"/>
+      <c r="D458" s="104"/>
+      <c r="E458" s="105"/>
+      <c r="F458" s="61"/>
+    </row>
+    <row r="459" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A459" s="119" t="s">
         <v>13</v>
-      </c>
-      <c r="B456" s="18" t="s">
-        <v>286</v>
-      </c>
-      <c r="C456" s="22" t="s">
-        <v>636</v>
-      </c>
-      <c r="D456" s="17" t="s">
-        <v>166</v>
-      </c>
-      <c r="E456" s="34" t="s">
-        <v>637</v>
-      </c>
-      <c r="F456" s="17"/>
-    </row>
-    <row r="457" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A457" s="122" t="s">
-        <v>144</v>
-      </c>
-      <c r="B457" s="103" t="s">
-        <v>39</v>
-      </c>
-      <c r="C457" s="112"/>
-      <c r="D457" s="104"/>
-      <c r="E457" s="105"/>
-      <c r="F457" s="61"/>
-    </row>
-    <row r="458" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A458" s="119" t="s">
-        <v>13</v>
-      </c>
-      <c r="B458" s="18" t="s">
-        <v>286</v>
-      </c>
-      <c r="C458" s="22" t="s">
-        <v>379</v>
-      </c>
-      <c r="D458" s="17" t="s">
-        <v>166</v>
-      </c>
-      <c r="E458" s="34">
-        <v>10986700</v>
-      </c>
-      <c r="F458" s="17"/>
-    </row>
-    <row r="459" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A459" s="119" t="s">
-        <v>41</v>
       </c>
       <c r="B459" s="18" t="s">
         <v>286</v>
       </c>
       <c r="C459" s="22" t="s">
-        <v>638</v>
-      </c>
-      <c r="D459" s="17"/>
-      <c r="E459" s="41" t="s">
-        <v>234</v>
+        <v>636</v>
+      </c>
+      <c r="D459" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="E459" s="34" t="s">
+        <v>637</v>
       </c>
       <c r="F459" s="17"/>
     </row>
     <row r="460" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A460" s="122" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B460" s="103" t="s">
         <v>39</v>
@@ -11536,223 +11553,219 @@
     </row>
     <row r="461" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A461" s="119" t="s">
+        <v>13</v>
+      </c>
+      <c r="B461" s="18" t="s">
+        <v>286</v>
+      </c>
+      <c r="C461" s="22" t="s">
+        <v>379</v>
+      </c>
+      <c r="D461" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="E461" s="34">
+        <v>10986700</v>
+      </c>
+      <c r="F461" s="17"/>
+    </row>
+    <row r="462" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A462" s="119" t="s">
+        <v>41</v>
+      </c>
+      <c r="B462" s="18" t="s">
+        <v>286</v>
+      </c>
+      <c r="C462" s="22" t="s">
+        <v>638</v>
+      </c>
+      <c r="D462" s="17"/>
+      <c r="E462" s="41" t="s">
+        <v>234</v>
+      </c>
+      <c r="F462" s="17"/>
+    </row>
+    <row r="463" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A463" s="122" t="s">
+        <v>145</v>
+      </c>
+      <c r="B463" s="103" t="s">
+        <v>39</v>
+      </c>
+      <c r="C463" s="112"/>
+      <c r="D463" s="104"/>
+      <c r="E463" s="105"/>
+      <c r="F463" s="61"/>
+    </row>
+    <row r="464" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A464" s="119" t="s">
         <v>66</v>
       </c>
-      <c r="B461" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="C461" s="22" t="s">
+      <c r="B464" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C464" s="22" t="s">
         <v>380</v>
-      </c>
-      <c r="D461" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="E461" s="34" t="s">
-        <v>191</v>
-      </c>
-      <c r="F461" s="17"/>
-    </row>
-    <row r="462" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A462" s="122" t="s">
-        <v>146</v>
-      </c>
-      <c r="B462" s="103" t="s">
-        <v>39</v>
-      </c>
-      <c r="C462" s="112"/>
-      <c r="D462" s="104"/>
-      <c r="E462" s="105"/>
-      <c r="F462" s="61"/>
-    </row>
-    <row r="463" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A463" s="119" t="s">
-        <v>147</v>
-      </c>
-      <c r="B463" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="C463" s="22" t="s">
-        <v>381</v>
-      </c>
-      <c r="D463" s="17" t="s">
-        <v>166</v>
-      </c>
-      <c r="E463" s="34">
-        <v>9873242</v>
-      </c>
-      <c r="F463" s="17"/>
-    </row>
-    <row r="464" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A464" s="119" t="s">
-        <v>148</v>
-      </c>
-      <c r="B464" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="C464" s="22" t="s">
-        <v>639</v>
       </c>
       <c r="D464" s="17" t="s">
         <v>164</v>
       </c>
       <c r="E464" s="34" t="s">
-        <v>236</v>
+        <v>191</v>
       </c>
       <c r="F464" s="17"/>
     </row>
-    <row r="465" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A465" s="119" t="s">
-        <v>149</v>
-      </c>
-      <c r="B465" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="C465" s="22" t="s">
-        <v>640</v>
-      </c>
-      <c r="D465" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="E465" s="34"/>
-      <c r="F465" s="17"/>
-    </row>
-    <row r="466" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A466" s="122" t="s">
-        <v>150</v>
-      </c>
-      <c r="B466" s="103" t="s">
-        <v>45</v>
-      </c>
-      <c r="C466" s="112" t="s">
-        <v>382</v>
-      </c>
-      <c r="D466" s="104"/>
-      <c r="E466" s="105"/>
-      <c r="F466" s="61"/>
-    </row>
-    <row r="467" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="465" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A465" s="122" t="s">
+        <v>146</v>
+      </c>
+      <c r="B465" s="103" t="s">
+        <v>39</v>
+      </c>
+      <c r="C465" s="112"/>
+      <c r="D465" s="104"/>
+      <c r="E465" s="105"/>
+      <c r="F465" s="61"/>
+    </row>
+    <row r="466" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A466" s="119" t="s">
+        <v>147</v>
+      </c>
+      <c r="B466" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C466" s="22" t="s">
+        <v>381</v>
+      </c>
+      <c r="D466" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="E466" s="34">
+        <v>9873242</v>
+      </c>
+      <c r="F466" s="17"/>
+    </row>
+    <row r="467" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A467" s="119" t="s">
-        <v>13</v>
+        <v>148</v>
       </c>
       <c r="B467" s="18" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C467" s="22" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="D467" s="17" t="s">
         <v>164</v>
       </c>
       <c r="E467" s="34" t="s">
-        <v>184</v>
-      </c>
-      <c r="F467" s="34"/>
+        <v>236</v>
+      </c>
+      <c r="F467" s="17"/>
     </row>
     <row r="468" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A468" s="119" t="s">
-        <v>114</v>
+        <v>149</v>
       </c>
       <c r="B468" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C468" s="22" t="s">
+        <v>640</v>
+      </c>
+      <c r="D468" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="E468" s="34"/>
+      <c r="F468" s="17"/>
+    </row>
+    <row r="469" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A469" s="122" t="s">
+        <v>150</v>
+      </c>
+      <c r="B469" s="103" t="s">
         <v>45</v>
       </c>
-      <c r="C468" s="22" t="s">
-        <v>392</v>
-      </c>
-      <c r="D468" s="17" t="s">
-        <v>223</v>
-      </c>
-      <c r="E468" s="34">
-        <v>25</v>
-      </c>
-      <c r="F468" s="34"/>
-    </row>
-    <row r="469" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A469" s="124" t="s">
-        <v>69</v>
-      </c>
-      <c r="B469" s="106" t="s">
-        <v>45</v>
-      </c>
-      <c r="C469" s="113"/>
-      <c r="D469" s="107"/>
-      <c r="E469" s="108"/>
-      <c r="F469" s="67"/>
-    </row>
-    <row r="470" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A470" s="125" t="s">
+      <c r="C469" s="112" t="s">
+        <v>382</v>
+      </c>
+      <c r="D469" s="104"/>
+      <c r="E469" s="105"/>
+      <c r="F469" s="61"/>
+    </row>
+    <row r="470" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A470" s="119" t="s">
         <v>13</v>
       </c>
       <c r="B470" s="18" t="s">
         <v>45</v>
       </c>
       <c r="C470" s="22" t="s">
+        <v>641</v>
+      </c>
+      <c r="D470" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="E470" s="34" t="s">
+        <v>184</v>
+      </c>
+      <c r="F470" s="34"/>
+    </row>
+    <row r="471" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A471" s="119" t="s">
+        <v>114</v>
+      </c>
+      <c r="B471" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C471" s="22" t="s">
+        <v>392</v>
+      </c>
+      <c r="D471" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="E471" s="34">
+        <v>25</v>
+      </c>
+      <c r="F471" s="34"/>
+    </row>
+    <row r="472" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A472" s="124" t="s">
+        <v>69</v>
+      </c>
+      <c r="B472" s="106" t="s">
+        <v>45</v>
+      </c>
+      <c r="C472" s="113"/>
+      <c r="D472" s="107"/>
+      <c r="E472" s="108"/>
+      <c r="F472" s="67"/>
+    </row>
+    <row r="473" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A473" s="125" t="s">
+        <v>13</v>
+      </c>
+      <c r="B473" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C473" s="22" t="s">
         <v>548</v>
       </c>
-      <c r="D470" s="17"/>
-      <c r="E470" s="34" t="s">
+      <c r="D473" s="17"/>
+      <c r="E473" s="34" t="s">
         <v>192</v>
-      </c>
-      <c r="F470" s="34"/>
-    </row>
-    <row r="471" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A471" s="122" t="s">
-        <v>151</v>
-      </c>
-      <c r="B471" s="103" t="s">
-        <v>39</v>
-      </c>
-      <c r="C471" s="112" t="s">
-        <v>152</v>
-      </c>
-      <c r="D471" s="104"/>
-      <c r="E471" s="105"/>
-      <c r="F471" s="61"/>
-    </row>
-    <row r="472" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A472" s="119" t="s">
-        <v>56</v>
-      </c>
-      <c r="B472" s="18" t="s">
-        <v>286</v>
-      </c>
-      <c r="C472" s="22" t="s">
-        <v>642</v>
-      </c>
-      <c r="D472" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="E472" s="34" t="s">
-        <v>644</v>
-      </c>
-      <c r="F472" s="34"/>
-    </row>
-    <row r="473" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A473" s="119" t="s">
-        <v>153</v>
-      </c>
-      <c r="B473" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="C473" s="22" t="s">
-        <v>643</v>
-      </c>
-      <c r="D473" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="E473" s="34" t="s">
-        <v>645</v>
       </c>
       <c r="F473" s="34"/>
     </row>
     <row r="474" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A474" s="122" t="s">
-        <v>646</v>
+        <v>151</v>
       </c>
       <c r="B474" s="103" t="s">
         <v>39</v>
       </c>
       <c r="C474" s="112" t="s">
-        <v>647</v>
+        <v>152</v>
       </c>
       <c r="D474" s="104"/>
       <c r="E474" s="105"/>
@@ -11760,312 +11773,362 @@
     </row>
     <row r="475" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A475" s="119" t="s">
-        <v>648</v>
+        <v>56</v>
       </c>
       <c r="B475" s="18" t="s">
-        <v>39</v>
+        <v>286</v>
       </c>
       <c r="C475" s="22" t="s">
-        <v>653</v>
+        <v>642</v>
       </c>
       <c r="D475" s="17" t="s">
-        <v>163</v>
-      </c>
-      <c r="E475" s="35">
-        <v>36161</v>
+        <v>167</v>
+      </c>
+      <c r="E475" s="34" t="s">
+        <v>644</v>
       </c>
       <c r="F475" s="34"/>
     </row>
     <row r="476" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A476" s="119" t="s">
+        <v>153</v>
+      </c>
+      <c r="B476" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C476" s="22" t="s">
+        <v>643</v>
+      </c>
+      <c r="D476" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="E476" s="34" t="s">
+        <v>645</v>
+      </c>
+      <c r="F476" s="34"/>
+    </row>
+    <row r="477" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A477" s="122" t="s">
+        <v>646</v>
+      </c>
+      <c r="B477" s="103" t="s">
+        <v>39</v>
+      </c>
+      <c r="C477" s="112" t="s">
+        <v>647</v>
+      </c>
+      <c r="D477" s="104"/>
+      <c r="E477" s="105"/>
+      <c r="F477" s="61"/>
+    </row>
+    <row r="478" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A478" s="119" t="s">
+        <v>648</v>
+      </c>
+      <c r="B478" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C478" s="22" t="s">
+        <v>653</v>
+      </c>
+      <c r="D478" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="E478" s="35">
+        <v>36161</v>
+      </c>
+      <c r="F478" s="34"/>
+    </row>
+    <row r="479" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A479" s="119" t="s">
         <v>649</v>
       </c>
-      <c r="B476" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="C476" s="22" t="s">
+      <c r="B479" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C479" s="22" t="s">
         <v>654</v>
       </c>
-      <c r="D476" s="17" t="s">
+      <c r="D479" s="17" t="s">
         <v>163</v>
       </c>
-      <c r="E476" s="35">
+      <c r="E479" s="35">
         <v>36161</v>
-      </c>
-      <c r="F476" s="34"/>
-    </row>
-    <row r="477" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A477" s="119" t="s">
-        <v>650</v>
-      </c>
-      <c r="B477" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="C477" s="22" t="s">
-        <v>655</v>
-      </c>
-      <c r="D477" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="E477" s="34">
-        <v>123456</v>
-      </c>
-      <c r="F477" s="34"/>
-    </row>
-    <row r="478" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A478" s="124" t="s">
-        <v>651</v>
-      </c>
-      <c r="B478" s="106" t="s">
-        <v>39</v>
-      </c>
-      <c r="C478" s="113"/>
-      <c r="D478" s="107"/>
-      <c r="E478" s="108"/>
-      <c r="F478" s="67"/>
-    </row>
-    <row r="479" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A479" s="119" t="s">
-        <v>652</v>
-      </c>
-      <c r="B479" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="C479" s="22" t="s">
-        <v>656</v>
-      </c>
-      <c r="D479" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="E479" s="34" t="s">
-        <v>603</v>
       </c>
       <c r="F479" s="34"/>
     </row>
     <row r="480" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A480" s="119" t="s">
+        <v>650</v>
+      </c>
+      <c r="B480" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C480" s="22" t="s">
+        <v>655</v>
+      </c>
+      <c r="D480" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="E480" s="34">
+        <v>123456</v>
+      </c>
+      <c r="F480" s="34"/>
+    </row>
+    <row r="481" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A481" s="124" t="s">
+        <v>651</v>
+      </c>
+      <c r="B481" s="106" t="s">
+        <v>39</v>
+      </c>
+      <c r="C481" s="113"/>
+      <c r="D481" s="107"/>
+      <c r="E481" s="108"/>
+      <c r="F481" s="67"/>
+    </row>
+    <row r="482" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A482" s="119" t="s">
+        <v>652</v>
+      </c>
+      <c r="B482" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C482" s="22" t="s">
+        <v>656</v>
+      </c>
+      <c r="D482" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="E482" s="34" t="s">
+        <v>603</v>
+      </c>
+      <c r="F482" s="34"/>
+    </row>
+    <row r="483" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A483" s="119" t="s">
         <v>664</v>
       </c>
-      <c r="B480" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="C480" s="22" t="s">
+      <c r="B483" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C483" s="22" t="s">
         <v>665</v>
       </c>
-      <c r="D480" s="17" t="s">
+      <c r="D483" s="17" t="s">
         <v>163</v>
       </c>
-      <c r="E480" s="35">
+      <c r="E483" s="35">
         <v>44562</v>
       </c>
-      <c r="F480" s="34"/>
-    </row>
-    <row r="481" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A481" s="135" t="s">
+      <c r="F483" s="34"/>
+    </row>
+    <row r="484" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A484" s="135" t="s">
         <v>154</v>
       </c>
-      <c r="B481" s="25" t="s">
+      <c r="B484" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="C481" s="57" t="s">
+      <c r="C484" s="57" t="s">
         <v>155</v>
       </c>
-      <c r="D481" s="23"/>
-      <c r="E481" s="36"/>
-      <c r="F481" s="36"/>
-    </row>
-    <row r="482" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A482" s="136" t="s">
+      <c r="D484" s="23"/>
+      <c r="E484" s="36"/>
+      <c r="F484" s="36"/>
+    </row>
+    <row r="485" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A485" s="136" t="s">
         <v>416</v>
       </c>
-      <c r="B482" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="C482" s="22" t="s">
+      <c r="B485" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C485" s="22" t="s">
         <v>585</v>
       </c>
-      <c r="D482" s="22"/>
-      <c r="E482" s="22"/>
-      <c r="F482" s="22"/>
-    </row>
-    <row r="483" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A483" s="117" t="s">
+      <c r="D485" s="22"/>
+      <c r="E485" s="22"/>
+      <c r="F485" s="22"/>
+    </row>
+    <row r="486" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A486" s="117" t="s">
         <v>156</v>
-      </c>
-      <c r="B483" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="C483" s="22" t="s">
-        <v>393</v>
-      </c>
-      <c r="D483" s="17" t="s">
-        <v>224</v>
-      </c>
-      <c r="E483" s="34" t="s">
-        <v>235</v>
-      </c>
-      <c r="F483" s="34"/>
-    </row>
-    <row r="484" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A484" s="117" t="s">
-        <v>111</v>
-      </c>
-      <c r="B484" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="C484" s="22" t="s">
-        <v>657</v>
-      </c>
-      <c r="D484" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="E484" s="34" t="s">
-        <v>225</v>
-      </c>
-      <c r="F484" s="34"/>
-    </row>
-    <row r="485" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A485" s="117" t="s">
-        <v>157</v>
-      </c>
-      <c r="B485" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="C485" s="22" t="s">
-        <v>158</v>
-      </c>
-      <c r="D485" s="17" t="s">
-        <v>230</v>
-      </c>
-      <c r="E485" s="34">
-        <v>1</v>
-      </c>
-      <c r="F485" s="34"/>
-    </row>
-    <row r="486" spans="1:6" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A486" s="117" t="s">
-        <v>134</v>
       </c>
       <c r="B486" s="18" t="s">
         <v>45</v>
       </c>
       <c r="C486" s="22" t="s">
+        <v>393</v>
+      </c>
+      <c r="D486" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="E486" s="34" t="s">
+        <v>235</v>
+      </c>
+      <c r="F486" s="34"/>
+    </row>
+    <row r="487" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A487" s="117" t="s">
+        <v>111</v>
+      </c>
+      <c r="B487" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C487" s="22" t="s">
+        <v>657</v>
+      </c>
+      <c r="D487" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="E487" s="34" t="s">
+        <v>225</v>
+      </c>
+      <c r="F487" s="34"/>
+    </row>
+    <row r="488" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A488" s="117" t="s">
+        <v>157</v>
+      </c>
+      <c r="B488" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C488" s="22" t="s">
+        <v>158</v>
+      </c>
+      <c r="D488" s="17" t="s">
+        <v>230</v>
+      </c>
+      <c r="E488" s="34">
+        <v>1</v>
+      </c>
+      <c r="F488" s="34"/>
+    </row>
+    <row r="489" spans="1:6" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A489" s="117" t="s">
+        <v>134</v>
+      </c>
+      <c r="B489" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C489" s="22" t="s">
         <v>658</v>
       </c>
-      <c r="D486" s="17"/>
-      <c r="E486" s="34" t="s">
+      <c r="D489" s="17"/>
+      <c r="E489" s="34" t="s">
         <v>231</v>
       </c>
-      <c r="F486" s="34"/>
-    </row>
-    <row r="487" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A487" s="122" t="s">
+      <c r="F489" s="34"/>
+    </row>
+    <row r="490" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A490" s="122" t="s">
         <v>104</v>
       </c>
-      <c r="B487" s="103" t="s">
+      <c r="B490" s="103" t="s">
         <v>283</v>
       </c>
-      <c r="C487" s="112" t="s">
+      <c r="C490" s="112" t="s">
         <v>691</v>
       </c>
-      <c r="D487" s="104"/>
-      <c r="E487" s="105"/>
-      <c r="F487" s="61"/>
-    </row>
-    <row r="488" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A488" s="119" t="s">
-        <v>105</v>
-      </c>
-      <c r="B488" s="18" t="s">
-        <v>283</v>
-      </c>
-      <c r="C488" s="22" t="s">
-        <v>659</v>
-      </c>
-      <c r="D488" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="E488" s="22" t="s">
-        <v>622</v>
-      </c>
-      <c r="F488" s="17" t="s">
-        <v>622</v>
-      </c>
-    </row>
-    <row r="489" spans="1:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="A489" s="119" t="s">
-        <v>109</v>
-      </c>
-      <c r="B489" s="18" t="s">
-        <v>285</v>
-      </c>
-      <c r="C489" s="22" t="s">
-        <v>660</v>
-      </c>
-      <c r="D489" s="17" t="s">
-        <v>224</v>
-      </c>
-      <c r="E489" s="34" t="s">
-        <v>248</v>
-      </c>
-      <c r="F489" s="17"/>
-    </row>
-    <row r="490" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A490" s="119" t="s">
-        <v>111</v>
-      </c>
-      <c r="B490" s="18" t="s">
-        <v>285</v>
-      </c>
-      <c r="C490" s="22" t="s">
-        <v>661</v>
-      </c>
-      <c r="D490" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="E490" s="34" t="s">
-        <v>225</v>
-      </c>
-      <c r="F490" s="17"/>
+      <c r="D490" s="104"/>
+      <c r="E490" s="105"/>
+      <c r="F490" s="61"/>
     </row>
     <row r="491" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A491" s="119" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="B491" s="18" t="s">
         <v>283</v>
       </c>
       <c r="C491" s="22" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
       <c r="D491" s="17" t="s">
-        <v>224</v>
-      </c>
-      <c r="E491" s="34" t="s">
-        <v>250</v>
-      </c>
-      <c r="F491" s="17"/>
-    </row>
-    <row r="492" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+        <v>164</v>
+      </c>
+      <c r="E491" s="22" t="s">
+        <v>622</v>
+      </c>
+      <c r="F491" s="17" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="492" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A492" s="119" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B492" s="18" t="s">
         <v>285</v>
       </c>
       <c r="C492" s="22" t="s">
+        <v>660</v>
+      </c>
+      <c r="D492" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="E492" s="34" t="s">
+        <v>248</v>
+      </c>
+      <c r="F492" s="17"/>
+    </row>
+    <row r="493" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A493" s="119" t="s">
+        <v>111</v>
+      </c>
+      <c r="B493" s="18" t="s">
+        <v>285</v>
+      </c>
+      <c r="C493" s="22" t="s">
+        <v>661</v>
+      </c>
+      <c r="D493" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="E493" s="34" t="s">
+        <v>225</v>
+      </c>
+      <c r="F493" s="17"/>
+    </row>
+    <row r="494" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A494" s="119" t="s">
+        <v>112</v>
+      </c>
+      <c r="B494" s="18" t="s">
+        <v>283</v>
+      </c>
+      <c r="C494" s="22" t="s">
+        <v>662</v>
+      </c>
+      <c r="D494" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="E494" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F494" s="17"/>
+    </row>
+    <row r="495" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A495" s="119" t="s">
+        <v>111</v>
+      </c>
+      <c r="B495" s="18" t="s">
+        <v>285</v>
+      </c>
+      <c r="C495" s="22" t="s">
         <v>663</v>
       </c>
-      <c r="D492" s="17" t="s">
+      <c r="D495" s="17" t="s">
         <v>164</v>
       </c>
-      <c r="E492" s="34" t="s">
+      <c r="E495" s="34" t="s">
         <v>225</v>
       </c>
-      <c r="F492" s="17"/>
+      <c r="F495" s="17"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F492" xr:uid="{FDB56CEA-A5F9-42A4-9956-612B841F9EA3}"/>
+  <autoFilter ref="A1:F495" xr:uid="{FDB56CEA-A5F9-42A4-9956-612B841F9EA3}"/>
   <hyperlinks>
     <hyperlink ref="E143" r:id="rId1" xr:uid="{DC86665A-695B-47C7-A818-F422C1F11636}"/>
     <hyperlink ref="A3" r:id="rId2" location="_extublextensions" xr:uid="{9531FFDF-372C-4676-833B-DAB9A8A93F85}"/>
@@ -12102,29 +12165,29 @@
     <hyperlink ref="A287" r:id="rId33" location="_cacpaymentmeans" xr:uid="{3CB911BD-0763-4D38-9F13-9D231802AFCD}"/>
     <hyperlink ref="A306" r:id="rId34" location="_cacpaymentterms" xr:uid="{4A408CD3-720D-4E9B-8F6F-4C6F1F87DDC1}"/>
     <hyperlink ref="A314" r:id="rId35" location="_cacallowancecharge" xr:uid="{80D22635-8F22-45B1-8C34-1716E9E26DE8}"/>
-    <hyperlink ref="A333" r:id="rId36" location="_cactaxexchangerate" xr:uid="{BCD141C2-4004-4CBB-B0BC-78234B52536F}"/>
-    <hyperlink ref="A339" r:id="rId37" location="_cactaxtotal" xr:uid="{F590367A-A414-4836-B877-B45CAAC6831A}"/>
-    <hyperlink ref="A355" r:id="rId38" location="_caclegalmonetarytotal" xr:uid="{8210054B-4866-4E0B-927B-112720F5333A}"/>
-    <hyperlink ref="A373" r:id="rId39" location="_cacinvoiceline" xr:uid="{3369C0DE-B96E-467C-ACCE-5A15AF093960}"/>
-    <hyperlink ref="A374" r:id="rId40" location="line-extension" xr:uid="{B0885766-A5C8-4695-92B2-C7145CD1F1E9}"/>
-    <hyperlink ref="A375" r:id="rId41" location="_cbcid_2" xr:uid="{71781B25-853D-4EFB-8F44-A9D3625850D0}"/>
-    <hyperlink ref="A376" r:id="rId42" location="_cbcnote_2" xr:uid="{98D33551-D2FB-41A5-A4E1-AEE90E145BA9}"/>
-    <hyperlink ref="A377" r:id="rId43" location="_cbcinvoicedquantity" xr:uid="{87EF7BBA-1B13-4007-9095-8AE85F5F1008}"/>
-    <hyperlink ref="A379" r:id="rId44" location="_cbclineextensionamount" xr:uid="{D40231D1-E253-47C4-B5B9-B84EB5F6F50F}"/>
-    <hyperlink ref="A381" r:id="rId45" location="_cbcaccountingcost_2" xr:uid="{309B2CF2-FC9E-489D-8994-EB8FAC53C8FC}"/>
-    <hyperlink ref="A382" r:id="rId46" location="_cacinvoiceperiod_2" xr:uid="{A9EFAE24-A87A-48DF-9825-6EAE0A819597}"/>
-    <hyperlink ref="A385" r:id="rId47" location="_cacorderlinereference" xr:uid="{EA537A80-55AC-4040-AC1B-EAAE9B5C5833}"/>
-    <hyperlink ref="A386" r:id="rId48" location="line-extension" xr:uid="{43385FB3-6E8C-479C-90A3-4E2457151E6A}"/>
-    <hyperlink ref="A393" r:id="rId49" location="_cacdespatchlinereference" xr:uid="{5CA189E3-27B9-45A0-9E5C-68E190ECD76F}"/>
-    <hyperlink ref="A398" r:id="rId50" location="_cacdocumentreference" xr:uid="{A19B217D-77E4-425F-BDA5-5DF30BE8056A}"/>
-    <hyperlink ref="A404" r:id="rId51" location="_cacdelivery_2" xr:uid="{282BE4F7-2F74-4307-BEA0-8B99B6D0D072}"/>
-    <hyperlink ref="A423" r:id="rId52" location="_cacallowancecharge_2" xr:uid="{BBB5AC6A-295D-4CC8-9AB0-23254C334669}"/>
-    <hyperlink ref="A432" r:id="rId53" location="_cactaxtotal_2" xr:uid="{B39E2A67-C6B0-4C2A-BCB9-6F069B44CAE2}"/>
-    <hyperlink ref="A447" r:id="rId54" location="_cacitem" xr:uid="{B64D9D45-3490-4FEE-9419-FD0CA5A56103}"/>
-    <hyperlink ref="A448" r:id="rId55" location="_item" xr:uid="{6A80D8B8-C919-4E6A-BA08-40D3A5648119}"/>
-    <hyperlink ref="A481" r:id="rId56" location="_cacprice" xr:uid="{3BB354D5-3D7E-483C-A9EF-D83745606B59}"/>
-    <hyperlink ref="A482" r:id="rId57" location="_price" xr:uid="{F00AB999-534C-4AB0-AEB7-47167B304468}"/>
-    <hyperlink ref="A487" r:id="rId58" location="_cacallowancecharge_2" xr:uid="{EE4A92E6-5BEF-42BB-95BF-9A7B00B36F90}"/>
+    <hyperlink ref="A334" r:id="rId36" location="_cactaxexchangerate" xr:uid="{BCD141C2-4004-4CBB-B0BC-78234B52536F}"/>
+    <hyperlink ref="A340" r:id="rId37" location="_cactaxtotal" xr:uid="{F590367A-A414-4836-B877-B45CAAC6831A}"/>
+    <hyperlink ref="A357" r:id="rId38" location="_caclegalmonetarytotal" xr:uid="{8210054B-4866-4E0B-927B-112720F5333A}"/>
+    <hyperlink ref="A375" r:id="rId39" location="_cacinvoiceline" xr:uid="{3369C0DE-B96E-467C-ACCE-5A15AF093960}"/>
+    <hyperlink ref="A376" r:id="rId40" location="line-extension" xr:uid="{B0885766-A5C8-4695-92B2-C7145CD1F1E9}"/>
+    <hyperlink ref="A377" r:id="rId41" location="_cbcid_2" xr:uid="{71781B25-853D-4EFB-8F44-A9D3625850D0}"/>
+    <hyperlink ref="A378" r:id="rId42" location="_cbcnote_2" xr:uid="{98D33551-D2FB-41A5-A4E1-AEE90E145BA9}"/>
+    <hyperlink ref="A379" r:id="rId43" location="_cbcinvoicedquantity" xr:uid="{87EF7BBA-1B13-4007-9095-8AE85F5F1008}"/>
+    <hyperlink ref="A381" r:id="rId44" location="_cbclineextensionamount" xr:uid="{D40231D1-E253-47C4-B5B9-B84EB5F6F50F}"/>
+    <hyperlink ref="A383" r:id="rId45" location="_cbcaccountingcost_2" xr:uid="{309B2CF2-FC9E-489D-8994-EB8FAC53C8FC}"/>
+    <hyperlink ref="A384" r:id="rId46" location="_cacinvoiceperiod_2" xr:uid="{A9EFAE24-A87A-48DF-9825-6EAE0A819597}"/>
+    <hyperlink ref="A387" r:id="rId47" location="_cacorderlinereference" xr:uid="{EA537A80-55AC-4040-AC1B-EAAE9B5C5833}"/>
+    <hyperlink ref="A388" r:id="rId48" location="line-extension" xr:uid="{43385FB3-6E8C-479C-90A3-4E2457151E6A}"/>
+    <hyperlink ref="A395" r:id="rId49" location="_cacdespatchlinereference" xr:uid="{5CA189E3-27B9-45A0-9E5C-68E190ECD76F}"/>
+    <hyperlink ref="A400" r:id="rId50" location="_cacdocumentreference" xr:uid="{A19B217D-77E4-425F-BDA5-5DF30BE8056A}"/>
+    <hyperlink ref="A406" r:id="rId51" location="_cacdelivery_2" xr:uid="{282BE4F7-2F74-4307-BEA0-8B99B6D0D072}"/>
+    <hyperlink ref="A425" r:id="rId52" location="_cacallowancecharge_2" xr:uid="{BBB5AC6A-295D-4CC8-9AB0-23254C334669}"/>
+    <hyperlink ref="A434" r:id="rId53" location="_cactaxtotal_2" xr:uid="{B39E2A67-C6B0-4C2A-BCB9-6F069B44CAE2}"/>
+    <hyperlink ref="A450" r:id="rId54" location="_cacitem" xr:uid="{B64D9D45-3490-4FEE-9419-FD0CA5A56103}"/>
+    <hyperlink ref="A451" r:id="rId55" location="_item" xr:uid="{6A80D8B8-C919-4E6A-BA08-40D3A5648119}"/>
+    <hyperlink ref="A484" r:id="rId56" location="_cacprice" xr:uid="{3BB354D5-3D7E-483C-A9EF-D83745606B59}"/>
+    <hyperlink ref="A485" r:id="rId57" location="_price" xr:uid="{F00AB999-534C-4AB0-AEB7-47167B304468}"/>
+    <hyperlink ref="A490" r:id="rId58" location="_cacallowancecharge_2" xr:uid="{EE4A92E6-5BEF-42BB-95BF-9A7B00B36F90}"/>
     <hyperlink ref="A310" r:id="rId59" location="_cacprepaidpayment" display="https://pagero.github.io/puf-billing/ - _cacprepaidpayment" xr:uid="{93904BDA-31E1-4B82-992D-F6F1FD7C9DE7}"/>
     <hyperlink ref="E281" r:id="rId60" xr:uid="{96DE9CC8-A74C-4283-88B5-21C225678470}"/>
   </hyperlinks>

</xml_diff>

<commit_message>
1131621 - PUF Excel Specification - Added WithholdingTaxTotal on row and header level
</commit_message>
<xml_diff>
--- a/specification/excel/Pagero Universal Format.xlsx
+++ b/specification/excel/Pagero Universal Format.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\development\format\puf-billing\specification\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7451D5C-4268-4E7E-99D1-EB31B107780E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EFF16C2-08BD-4C44-9345-E6BA623977AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28695" yWindow="-5250" windowWidth="26010" windowHeight="20985" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="54495" yWindow="-5250" windowWidth="26010" windowHeight="20985" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="8" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Test Cases" sheetId="4" state="hidden" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Base PUF (no extensions)'!$A$1:$F$520</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Base PUF (no extensions)'!$A$1:$F$553</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2126" uniqueCount="738">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2264" uniqueCount="745">
   <si>
     <t>Comments</t>
   </si>
@@ -2688,6 +2688,43 @@
   </si>
   <si>
     <t>Bank address country name.</t>
+  </si>
+  <si>
+    <t>cac:WithholdingTaxTotal</t>
+  </si>
+  <si>
+    <t>Document withholding  tax amount
+Documents total withholding tax amount in document currency.
+Summary of all cac:TaxSubTotal/cbc:TaxAmount.</t>
+  </si>
+  <si>
+    <t>Document total withholding tax amount currency
+Document total withholding tax amount currency, must be the same as cbc:DocumentCurrencyCode.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A group of business terms providing information about VAT breakdown by different categories, rates and exemption reasons
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>One segment for each withholding rate on the invoice</t>
+    </r>
+  </si>
+  <si>
+    <t>Placeholder for Extensions.</t>
+  </si>
+  <si>
+    <t>Total taxable amount for each tax category or tax rate.</t>
+  </si>
+  <si>
+    <t>The total withholding tax amount, the sum of the withholding tax subtotals..
+Summary of all TaxSubTotal/TaxAmount.</t>
   </si>
 </sst>
 </file>
@@ -3126,7 +3163,7 @@
     <xf numFmtId="0" fontId="21" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="139">
+  <cellXfs count="142">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3487,6 +3524,16 @@
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -3994,7 +4041,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFC8AF48-A32B-49A1-A68C-71E5B6F7A240}">
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
@@ -4110,10 +4157,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDB56CEA-A5F9-42A4-9956-612B841F9EA3}">
-  <dimension ref="A1:F520"/>
+  <dimension ref="A1:F553"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A296" workbookViewId="0">
-      <selection activeCell="E315" sqref="E315"/>
+    <sheetView tabSelected="1" topLeftCell="A479" workbookViewId="0">
+      <selection activeCell="A501" sqref="A501"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -10333,2317 +10380,2861 @@
       </c>
       <c r="F381" s="17"/>
     </row>
-    <row r="382" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A382" s="100" t="s">
-        <v>121</v>
+    <row r="382" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A382" s="32" t="s">
+        <v>738</v>
       </c>
       <c r="B382" s="62" t="s">
         <v>45</v>
       </c>
       <c r="C382" s="28" t="s">
-        <v>122</v>
+        <v>712</v>
       </c>
       <c r="D382" s="21"/>
       <c r="E382" s="32"/>
-      <c r="F382" s="32"/>
+      <c r="F382" s="21"/>
     </row>
     <row r="383" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A383" s="92" t="s">
-        <v>416</v>
+        <v>116</v>
       </c>
       <c r="B383" s="18" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="C383" s="22" t="s">
-        <v>417</v>
-      </c>
-      <c r="D383" s="22"/>
-      <c r="E383" s="22"/>
-      <c r="F383" s="22"/>
-    </row>
-    <row r="384" spans="1:6" x14ac:dyDescent="0.2">
+        <v>739</v>
+      </c>
+      <c r="D383" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="E383" s="34" t="s">
+        <v>226</v>
+      </c>
+      <c r="F383" s="17"/>
+    </row>
+    <row r="384" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A384" s="92" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="B384" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="C384" s="22" t="s">
-        <v>568</v>
+      <c r="C384" s="56" t="s">
+        <v>740</v>
       </c>
       <c r="D384" s="17" t="s">
-        <v>224</v>
-      </c>
-      <c r="E384" s="41" t="s">
-        <v>245</v>
+        <v>164</v>
+      </c>
+      <c r="E384" s="34" t="s">
+        <v>225</v>
       </c>
       <c r="F384" s="17"/>
     </row>
-    <row r="385" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A385" s="92" t="s">
-        <v>111</v>
-      </c>
-      <c r="B385" s="18" t="s">
+    <row r="385" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A385" s="139" t="s">
+        <v>117</v>
+      </c>
+      <c r="B385" s="140" t="s">
         <v>45</v>
       </c>
-      <c r="C385" s="22" t="s">
-        <v>569</v>
-      </c>
-      <c r="D385" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="E385" s="34" t="s">
-        <v>225</v>
-      </c>
-      <c r="F385" s="17"/>
-    </row>
-    <row r="386" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A386" s="92" t="s">
-        <v>124</v>
+      <c r="C385" s="57" t="s">
+        <v>741</v>
+      </c>
+      <c r="D385" s="58"/>
+      <c r="E385" s="141"/>
+      <c r="F385" s="141"/>
+    </row>
+    <row r="386" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A386" s="117" t="s">
+        <v>416</v>
       </c>
       <c r="B386" s="18" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C386" s="22" t="s">
-        <v>570</v>
-      </c>
-      <c r="D386" s="17" t="s">
-        <v>224</v>
-      </c>
-      <c r="E386" s="41" t="s">
-        <v>246</v>
-      </c>
-      <c r="F386" s="17"/>
-    </row>
-    <row r="387" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A387" s="92" t="s">
-        <v>111</v>
+        <v>742</v>
+      </c>
+      <c r="D386" s="22"/>
+      <c r="E386" s="22"/>
+      <c r="F386" s="22"/>
+    </row>
+    <row r="387" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A387" s="117" t="s">
+        <v>118</v>
       </c>
       <c r="B387" s="18" t="s">
         <v>45</v>
       </c>
       <c r="C387" s="22" t="s">
-        <v>571</v>
+        <v>743</v>
       </c>
       <c r="D387" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="E387" s="34" t="s">
-        <v>225</v>
+        <v>224</v>
+      </c>
+      <c r="E387" s="22" t="s">
+        <v>227</v>
       </c>
       <c r="F387" s="17"/>
     </row>
-    <row r="388" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A388" s="92" t="s">
-        <v>125</v>
+    <row r="388" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A388" s="117" t="s">
+        <v>111</v>
       </c>
       <c r="B388" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="C388" s="22" t="s">
-        <v>572</v>
+      <c r="C388" s="56" t="s">
+        <v>562</v>
       </c>
       <c r="D388" s="17" t="s">
-        <v>224</v>
-      </c>
-      <c r="E388" s="41" t="s">
-        <v>247</v>
+        <v>164</v>
+      </c>
+      <c r="E388" s="22" t="s">
+        <v>225</v>
       </c>
       <c r="F388" s="17"/>
     </row>
-    <row r="389" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A389" s="92" t="s">
-        <v>111</v>
+    <row r="389" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A389" s="117" t="s">
+        <v>116</v>
       </c>
       <c r="B389" s="18" t="s">
         <v>45</v>
       </c>
       <c r="C389" s="22" t="s">
-        <v>573</v>
+        <v>563</v>
       </c>
       <c r="D389" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="E389" s="22" t="s">
+        <v>226</v>
+      </c>
+      <c r="F389" s="17"/>
+    </row>
+    <row r="390" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A390" s="117" t="s">
+        <v>111</v>
+      </c>
+      <c r="B390" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C390" s="56" t="s">
+        <v>564</v>
+      </c>
+      <c r="D390" s="17" t="s">
         <v>164</v>
       </c>
-      <c r="E389" s="34" t="s">
+      <c r="E390" s="34" t="s">
         <v>225</v>
       </c>
-      <c r="F389" s="17"/>
-    </row>
-    <row r="390" spans="1:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="A390" s="92" t="s">
-        <v>126</v>
-      </c>
-      <c r="B390" s="18" t="s">
-        <v>283</v>
-      </c>
-      <c r="C390" s="22" t="s">
-        <v>574</v>
-      </c>
-      <c r="D390" s="17" t="s">
-        <v>224</v>
-      </c>
-      <c r="E390" s="34" t="s">
-        <v>248</v>
-      </c>
       <c r="F390" s="17"/>
     </row>
-    <row r="391" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A391" s="92" t="s">
-        <v>111</v>
-      </c>
-      <c r="B391" s="18" t="s">
-        <v>285</v>
-      </c>
-      <c r="C391" s="22" t="s">
-        <v>575</v>
-      </c>
-      <c r="D391" s="17" t="s">
+    <row r="391" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A391" s="122" t="s">
+        <v>113</v>
+      </c>
+      <c r="B391" s="103" t="s">
+        <v>45</v>
+      </c>
+      <c r="C391" s="112"/>
+      <c r="D391" s="104"/>
+      <c r="E391" s="105"/>
+      <c r="F391" s="61"/>
+    </row>
+    <row r="392" spans="1:6" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A392" s="119" t="s">
+        <v>13</v>
+      </c>
+      <c r="B392" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C392" s="22" t="s">
+        <v>703</v>
+      </c>
+      <c r="D392" s="17" t="s">
         <v>164</v>
       </c>
-      <c r="E391" s="34" t="s">
-        <v>225</v>
-      </c>
-      <c r="F391" s="17"/>
-    </row>
-    <row r="392" spans="1:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="A392" s="92" t="s">
-        <v>127</v>
-      </c>
-      <c r="B392" s="18" t="s">
-        <v>283</v>
-      </c>
-      <c r="C392" s="22" t="s">
-        <v>576</v>
-      </c>
-      <c r="D392" s="17" t="s">
-        <v>224</v>
-      </c>
-      <c r="E392" s="41" t="s">
-        <v>249</v>
+      <c r="E392" s="34" t="s">
+        <v>184</v>
       </c>
       <c r="F392" s="17"/>
     </row>
-    <row r="393" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A393" s="92" t="s">
-        <v>111</v>
+    <row r="393" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A393" s="119" t="s">
+        <v>114</v>
       </c>
       <c r="B393" s="18" t="s">
-        <v>285</v>
+        <v>45</v>
       </c>
       <c r="C393" s="22" t="s">
-        <v>577</v>
+        <v>364</v>
       </c>
       <c r="D393" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="E393" s="34" t="s">
-        <v>225</v>
+        <v>223</v>
+      </c>
+      <c r="E393" s="34">
+        <v>25</v>
       </c>
       <c r="F393" s="17"/>
     </row>
-    <row r="394" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A394" s="92" t="s">
-        <v>128</v>
+    <row r="394" spans="1:6" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A394" s="119" t="s">
+        <v>119</v>
       </c>
       <c r="B394" s="18" t="s">
         <v>283</v>
       </c>
       <c r="C394" s="22" t="s">
-        <v>578</v>
+        <v>566</v>
       </c>
       <c r="D394" s="17" t="s">
-        <v>224</v>
-      </c>
-      <c r="E394" s="41" t="s">
-        <v>250</v>
+        <v>167</v>
+      </c>
+      <c r="E394" s="34" t="s">
+        <v>567</v>
       </c>
       <c r="F394" s="17"/>
     </row>
-    <row r="395" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A395" s="92" t="s">
-        <v>111</v>
+    <row r="395" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A395" s="119" t="s">
+        <v>120</v>
       </c>
       <c r="B395" s="18" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C395" s="22" t="s">
-        <v>579</v>
+        <v>365</v>
       </c>
       <c r="D395" s="17" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="E395" s="34" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="F395" s="17"/>
     </row>
-    <row r="396" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A396" s="92" t="s">
-        <v>129</v>
-      </c>
-      <c r="B396" s="18" t="s">
-        <v>283</v>
-      </c>
-      <c r="C396" s="22" t="s">
-        <v>580</v>
-      </c>
-      <c r="D396" s="17" t="s">
-        <v>224</v>
-      </c>
-      <c r="E396" s="41" t="s">
-        <v>249</v>
-      </c>
-      <c r="F396" s="17"/>
-    </row>
-    <row r="397" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A397" s="92" t="s">
-        <v>111</v>
+    <row r="396" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A396" s="124" t="s">
+        <v>69</v>
+      </c>
+      <c r="B396" s="106" t="s">
+        <v>45</v>
+      </c>
+      <c r="C396" s="113"/>
+      <c r="D396" s="107"/>
+      <c r="E396" s="108"/>
+      <c r="F396" s="67"/>
+    </row>
+    <row r="397" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A397" s="125" t="s">
+        <v>13</v>
       </c>
       <c r="B397" s="18" t="s">
-        <v>285</v>
+        <v>45</v>
       </c>
       <c r="C397" s="22" t="s">
-        <v>581</v>
+        <v>548</v>
       </c>
       <c r="D397" s="17" t="s">
         <v>164</v>
       </c>
-      <c r="E397" s="34" t="s">
-        <v>225</v>
+      <c r="E397" s="17" t="s">
+        <v>192</v>
       </c>
       <c r="F397" s="17"/>
     </row>
-    <row r="398" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A398" s="92" t="s">
-        <v>130</v>
+    <row r="398" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A398" s="125" t="s">
+        <v>56</v>
       </c>
       <c r="B398" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C398" s="22" t="s">
+        <v>710</v>
+      </c>
+      <c r="D398" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="E398" s="17" t="s">
+        <v>709</v>
+      </c>
+      <c r="F398" s="17"/>
+    </row>
+    <row r="399" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A399" s="100" t="s">
+        <v>121</v>
+      </c>
+      <c r="B399" s="62" t="s">
         <v>45</v>
       </c>
-      <c r="C398" s="22" t="s">
-        <v>582</v>
-      </c>
-      <c r="D398" s="17" t="s">
+      <c r="C399" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="D399" s="21"/>
+      <c r="E399" s="32"/>
+      <c r="F399" s="32"/>
+    </row>
+    <row r="400" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A400" s="92" t="s">
+        <v>416</v>
+      </c>
+      <c r="B400" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C400" s="22" t="s">
+        <v>417</v>
+      </c>
+      <c r="D400" s="22"/>
+      <c r="E400" s="22"/>
+      <c r="F400" s="22"/>
+    </row>
+    <row r="401" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A401" s="92" t="s">
+        <v>123</v>
+      </c>
+      <c r="B401" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C401" s="22" t="s">
+        <v>568</v>
+      </c>
+      <c r="D401" s="17" t="s">
         <v>224</v>
       </c>
-      <c r="E398" s="41" t="s">
-        <v>251</v>
-      </c>
-      <c r="F398" s="17"/>
-    </row>
-    <row r="399" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A399" s="92" t="s">
+      <c r="E401" s="41" t="s">
+        <v>245</v>
+      </c>
+      <c r="F401" s="17"/>
+    </row>
+    <row r="402" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A402" s="92" t="s">
         <v>111</v>
-      </c>
-      <c r="B399" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="C399" s="22" t="s">
-        <v>583</v>
-      </c>
-      <c r="D399" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="E399" s="34" t="s">
-        <v>225</v>
-      </c>
-      <c r="F399" s="17"/>
-    </row>
-    <row r="400" spans="1:6" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A400" s="100" t="s">
-        <v>131</v>
-      </c>
-      <c r="B400" s="62" t="s">
-        <v>45</v>
-      </c>
-      <c r="C400" s="28" t="s">
-        <v>584</v>
-      </c>
-      <c r="D400" s="21"/>
-      <c r="E400" s="32"/>
-      <c r="F400" s="32"/>
-    </row>
-    <row r="401" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A401" s="134" t="s">
-        <v>416</v>
-      </c>
-      <c r="B401" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="C401" s="22" t="s">
-        <v>585</v>
-      </c>
-      <c r="D401" s="22"/>
-      <c r="E401" s="22"/>
-      <c r="F401" s="22"/>
-    </row>
-    <row r="402" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A402" s="134" t="s">
-        <v>13</v>
       </c>
       <c r="B402" s="18" t="s">
         <v>45</v>
       </c>
       <c r="C402" s="22" t="s">
-        <v>366</v>
+        <v>569</v>
       </c>
       <c r="D402" s="17" t="s">
-        <v>166</v>
-      </c>
-      <c r="E402" s="34">
-        <v>1</v>
+        <v>164</v>
+      </c>
+      <c r="E402" s="34" t="s">
+        <v>225</v>
       </c>
       <c r="F402" s="17"/>
     </row>
-    <row r="403" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A403" s="134" t="s">
-        <v>19</v>
+    <row r="403" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A403" s="92" t="s">
+        <v>124</v>
       </c>
       <c r="B403" s="18" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="C403" s="22" t="s">
-        <v>586</v>
+        <v>570</v>
       </c>
       <c r="D403" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="E403" s="34" t="s">
-        <v>229</v>
-      </c>
-      <c r="F403" s="34"/>
+        <v>224</v>
+      </c>
+      <c r="E403" s="41" t="s">
+        <v>246</v>
+      </c>
+      <c r="F403" s="17"/>
     </row>
     <row r="404" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A404" s="134" t="s">
-        <v>133</v>
+      <c r="A404" s="92" t="s">
+        <v>111</v>
       </c>
       <c r="B404" s="18" t="s">
         <v>45</v>
       </c>
       <c r="C404" s="22" t="s">
-        <v>701</v>
+        <v>571</v>
       </c>
       <c r="D404" s="17" t="s">
-        <v>230</v>
-      </c>
-      <c r="E404" s="34">
-        <v>100</v>
+        <v>164</v>
+      </c>
+      <c r="E404" s="34" t="s">
+        <v>225</v>
       </c>
       <c r="F404" s="17"/>
     </row>
-    <row r="405" spans="1:6" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="405" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A405" s="92" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="B405" s="18" t="s">
         <v>45</v>
       </c>
       <c r="C405" s="22" t="s">
-        <v>702</v>
+        <v>572</v>
       </c>
       <c r="D405" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="E405" s="34" t="s">
-        <v>231</v>
+        <v>224</v>
+      </c>
+      <c r="E405" s="41" t="s">
+        <v>247</v>
       </c>
       <c r="F405" s="17"/>
     </row>
-    <row r="406" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A406" s="134" t="s">
-        <v>123</v>
+    <row r="406" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A406" s="92" t="s">
+        <v>111</v>
       </c>
       <c r="B406" s="18" t="s">
         <v>45</v>
       </c>
       <c r="C406" s="22" t="s">
-        <v>587</v>
+        <v>573</v>
       </c>
       <c r="D406" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="E406" s="34" t="s">
+        <v>225</v>
+      </c>
+      <c r="F406" s="17"/>
+    </row>
+    <row r="407" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A407" s="92" t="s">
+        <v>126</v>
+      </c>
+      <c r="B407" s="18" t="s">
+        <v>283</v>
+      </c>
+      <c r="C407" s="22" t="s">
+        <v>574</v>
+      </c>
+      <c r="D407" s="17" t="s">
         <v>224</v>
       </c>
-      <c r="E406" s="41" t="s">
-        <v>252</v>
-      </c>
-      <c r="F406" s="17"/>
-    </row>
-    <row r="407" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A407" s="92" t="s">
+      <c r="E407" s="34" t="s">
+        <v>248</v>
+      </c>
+      <c r="F407" s="17"/>
+    </row>
+    <row r="408" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A408" s="92" t="s">
         <v>111</v>
       </c>
-      <c r="B407" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="C407" s="22" t="s">
-        <v>588</v>
-      </c>
-      <c r="D407" s="17" t="s">
+      <c r="B408" s="18" t="s">
+        <v>285</v>
+      </c>
+      <c r="C408" s="22" t="s">
+        <v>575</v>
+      </c>
+      <c r="D408" s="17" t="s">
         <v>164</v>
       </c>
-      <c r="E407" s="34" t="s">
+      <c r="E408" s="34" t="s">
         <v>225</v>
       </c>
-      <c r="F407" s="17"/>
-    </row>
-    <row r="408" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A408" s="134" t="s">
-        <v>22</v>
-      </c>
-      <c r="B408" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="C408" s="22" t="s">
-        <v>367</v>
-      </c>
-      <c r="D408" s="17" t="s">
-        <v>166</v>
-      </c>
-      <c r="E408" s="34" t="s">
-        <v>232</v>
-      </c>
       <c r="F408" s="17"/>
     </row>
-    <row r="409" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A409" s="135" t="s">
-        <v>24</v>
-      </c>
-      <c r="B409" s="25" t="s">
+    <row r="409" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A409" s="92" t="s">
+        <v>127</v>
+      </c>
+      <c r="B409" s="18" t="s">
         <v>283</v>
       </c>
-      <c r="C409" s="57" t="s">
-        <v>135</v>
-      </c>
-      <c r="D409" s="23"/>
-      <c r="E409" s="36"/>
-      <c r="F409" s="36"/>
+      <c r="C409" s="22" t="s">
+        <v>576</v>
+      </c>
+      <c r="D409" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="E409" s="41" t="s">
+        <v>249</v>
+      </c>
+      <c r="F409" s="17"/>
     </row>
     <row r="410" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A410" s="117" t="s">
-        <v>25</v>
+      <c r="A410" s="92" t="s">
+        <v>111</v>
       </c>
       <c r="B410" s="18" t="s">
         <v>285</v>
       </c>
       <c r="C410" s="22" t="s">
-        <v>368</v>
+        <v>577</v>
       </c>
       <c r="D410" s="17" t="s">
-        <v>163</v>
-      </c>
-      <c r="E410" s="35">
-        <v>43013</v>
+        <v>164</v>
+      </c>
+      <c r="E410" s="34" t="s">
+        <v>225</v>
       </c>
       <c r="F410" s="17"/>
     </row>
     <row r="411" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A411" s="117" t="s">
-        <v>26</v>
+      <c r="A411" s="92" t="s">
+        <v>128</v>
       </c>
       <c r="B411" s="18" t="s">
+        <v>283</v>
+      </c>
+      <c r="C411" s="22" t="s">
+        <v>578</v>
+      </c>
+      <c r="D411" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="E411" s="41" t="s">
+        <v>250</v>
+      </c>
+      <c r="F411" s="17"/>
+    </row>
+    <row r="412" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A412" s="92" t="s">
+        <v>111</v>
+      </c>
+      <c r="B412" s="18" t="s">
         <v>285</v>
       </c>
-      <c r="C411" s="22" t="s">
-        <v>369</v>
-      </c>
-      <c r="D411" s="17" t="s">
-        <v>163</v>
-      </c>
-      <c r="E411" s="35">
-        <v>43023</v>
-      </c>
-      <c r="F411" s="17"/>
-    </row>
-    <row r="412" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A412" s="135" t="s">
-        <v>136</v>
-      </c>
-      <c r="B412" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="C412" s="57"/>
-      <c r="D412" s="23"/>
-      <c r="E412" s="36"/>
-      <c r="F412" s="36"/>
-    </row>
-    <row r="413" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A413" s="136" t="s">
+      <c r="C412" s="22" t="s">
+        <v>579</v>
+      </c>
+      <c r="D412" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="E412" s="34" t="s">
+        <v>225</v>
+      </c>
+      <c r="F412" s="17"/>
+    </row>
+    <row r="413" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A413" s="92" t="s">
+        <v>129</v>
+      </c>
+      <c r="B413" s="18" t="s">
+        <v>283</v>
+      </c>
+      <c r="C413" s="22" t="s">
+        <v>580</v>
+      </c>
+      <c r="D413" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="E413" s="41" t="s">
+        <v>249</v>
+      </c>
+      <c r="F413" s="17"/>
+    </row>
+    <row r="414" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A414" s="92" t="s">
+        <v>111</v>
+      </c>
+      <c r="B414" s="18" t="s">
+        <v>285</v>
+      </c>
+      <c r="C414" s="22" t="s">
+        <v>581</v>
+      </c>
+      <c r="D414" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="E414" s="34" t="s">
+        <v>225</v>
+      </c>
+      <c r="F414" s="17"/>
+    </row>
+    <row r="415" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A415" s="92" t="s">
+        <v>130</v>
+      </c>
+      <c r="B415" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C415" s="22" t="s">
+        <v>582</v>
+      </c>
+      <c r="D415" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="E415" s="41" t="s">
+        <v>251</v>
+      </c>
+      <c r="F415" s="17"/>
+    </row>
+    <row r="416" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A416" s="92" t="s">
+        <v>111</v>
+      </c>
+      <c r="B416" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C416" s="22" t="s">
+        <v>583</v>
+      </c>
+      <c r="D416" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="E416" s="34" t="s">
+        <v>225</v>
+      </c>
+      <c r="F416" s="17"/>
+    </row>
+    <row r="417" spans="1:6" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A417" s="100" t="s">
+        <v>131</v>
+      </c>
+      <c r="B417" s="62" t="s">
+        <v>45</v>
+      </c>
+      <c r="C417" s="28" t="s">
+        <v>584</v>
+      </c>
+      <c r="D417" s="21"/>
+      <c r="E417" s="32"/>
+      <c r="F417" s="32"/>
+    </row>
+    <row r="418" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A418" s="134" t="s">
         <v>416</v>
       </c>
-      <c r="B413" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="C413" s="22" t="s">
+      <c r="B418" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C418" s="22" t="s">
         <v>585</v>
       </c>
-      <c r="D413" s="22"/>
-      <c r="E413" s="22"/>
-      <c r="F413" s="22"/>
-    </row>
-    <row r="414" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A414" s="117" t="s">
-        <v>137</v>
-      </c>
-      <c r="B414" s="18" t="s">
-        <v>286</v>
-      </c>
-      <c r="C414" s="22" t="s">
-        <v>370</v>
-      </c>
-      <c r="D414" s="17" t="s">
+      <c r="D418" s="22"/>
+      <c r="E418" s="22"/>
+      <c r="F418" s="22"/>
+    </row>
+    <row r="419" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A419" s="134" t="s">
+        <v>13</v>
+      </c>
+      <c r="B419" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C419" s="22" t="s">
+        <v>366</v>
+      </c>
+      <c r="D419" s="17" t="s">
         <v>166</v>
       </c>
-      <c r="E414" s="34">
-        <v>10</v>
-      </c>
-      <c r="F414" s="17"/>
-    </row>
-    <row r="415" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A415" s="117" t="s">
-        <v>589</v>
-      </c>
-      <c r="B415" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="C415" s="22" t="s">
-        <v>590</v>
-      </c>
-      <c r="D415" s="17" t="s">
+      <c r="E419" s="34">
+        <v>1</v>
+      </c>
+      <c r="F419" s="17"/>
+    </row>
+    <row r="420" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A420" s="134" t="s">
+        <v>19</v>
+      </c>
+      <c r="B420" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C420" s="22" t="s">
+        <v>586</v>
+      </c>
+      <c r="D420" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="E420" s="34" t="s">
+        <v>229</v>
+      </c>
+      <c r="F420" s="34"/>
+    </row>
+    <row r="421" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A421" s="134" t="s">
+        <v>133</v>
+      </c>
+      <c r="B421" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C421" s="22" t="s">
+        <v>701</v>
+      </c>
+      <c r="D421" s="17" t="s">
+        <v>230</v>
+      </c>
+      <c r="E421" s="34">
+        <v>100</v>
+      </c>
+      <c r="F421" s="17"/>
+    </row>
+    <row r="422" spans="1:6" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A422" s="92" t="s">
+        <v>134</v>
+      </c>
+      <c r="B422" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C422" s="22" t="s">
+        <v>702</v>
+      </c>
+      <c r="D422" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="E422" s="34" t="s">
+        <v>231</v>
+      </c>
+      <c r="F422" s="17"/>
+    </row>
+    <row r="423" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A423" s="134" t="s">
+        <v>123</v>
+      </c>
+      <c r="B423" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C423" s="22" t="s">
+        <v>587</v>
+      </c>
+      <c r="D423" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="E423" s="41" t="s">
+        <v>252</v>
+      </c>
+      <c r="F423" s="17"/>
+    </row>
+    <row r="424" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A424" s="92" t="s">
+        <v>111</v>
+      </c>
+      <c r="B424" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C424" s="22" t="s">
+        <v>588</v>
+      </c>
+      <c r="D424" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="E424" s="34" t="s">
+        <v>225</v>
+      </c>
+      <c r="F424" s="17"/>
+    </row>
+    <row r="425" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A425" s="134" t="s">
+        <v>22</v>
+      </c>
+      <c r="B425" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C425" s="22" t="s">
+        <v>367</v>
+      </c>
+      <c r="D425" s="17" t="s">
         <v>166</v>
       </c>
-      <c r="E415" s="34">
-        <v>1</v>
-      </c>
-      <c r="F415" s="17"/>
-    </row>
-    <row r="416" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A416" s="122" t="s">
-        <v>27</v>
-      </c>
-      <c r="B416" s="103" t="s">
-        <v>39</v>
-      </c>
-      <c r="C416" s="112"/>
-      <c r="D416" s="104"/>
-      <c r="E416" s="105"/>
-      <c r="F416" s="61"/>
-    </row>
-    <row r="417" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A417" s="119" t="s">
-        <v>13</v>
-      </c>
-      <c r="B417" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="C417" s="22" t="s">
-        <v>591</v>
-      </c>
-      <c r="D417" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="E417" s="34" t="s">
-        <v>592</v>
-      </c>
-      <c r="F417" s="17"/>
-    </row>
-    <row r="418" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A418" s="119" t="s">
-        <v>28</v>
-      </c>
-      <c r="B418" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="C418" s="22" t="s">
-        <v>593</v>
-      </c>
-      <c r="D418" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="E418" s="34" t="s">
-        <v>594</v>
-      </c>
-      <c r="F418" s="17"/>
-    </row>
-    <row r="419" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A419" s="119" t="s">
-        <v>14</v>
-      </c>
-      <c r="B419" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="C419" s="22" t="s">
-        <v>595</v>
-      </c>
-      <c r="D419" s="17" t="s">
-        <v>163</v>
-      </c>
-      <c r="E419" s="35">
-        <v>36161</v>
-      </c>
-      <c r="F419" s="17"/>
-    </row>
-    <row r="420" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A420" s="135" t="s">
-        <v>596</v>
-      </c>
-      <c r="B420" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="C420" s="57"/>
-      <c r="D420" s="23"/>
-      <c r="E420" s="36"/>
-      <c r="F420" s="36"/>
-    </row>
-    <row r="421" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A421" s="117" t="s">
-        <v>137</v>
-      </c>
-      <c r="B421" s="18" t="s">
-        <v>286</v>
-      </c>
-      <c r="C421" s="22" t="s">
-        <v>597</v>
-      </c>
-      <c r="D421" s="17" t="s">
-        <v>166</v>
-      </c>
-      <c r="E421" s="34">
-        <v>10</v>
-      </c>
-      <c r="F421" s="17"/>
-    </row>
-    <row r="422" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A422" s="122" t="s">
-        <v>598</v>
-      </c>
-      <c r="B422" s="103" t="s">
-        <v>39</v>
-      </c>
-      <c r="C422" s="112"/>
-      <c r="D422" s="104"/>
-      <c r="E422" s="105"/>
-      <c r="F422" s="61"/>
-    </row>
-    <row r="423" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A423" s="119" t="s">
-        <v>13</v>
-      </c>
-      <c r="B423" s="18" t="s">
-        <v>286</v>
-      </c>
-      <c r="C423" s="22" t="s">
-        <v>599</v>
-      </c>
-      <c r="D423" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="E423" s="95">
-        <v>23421</v>
-      </c>
-      <c r="F423" s="17"/>
-    </row>
-    <row r="424" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A424" s="119" t="s">
-        <v>14</v>
-      </c>
-      <c r="B424" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="C424" s="22" t="s">
-        <v>600</v>
-      </c>
-      <c r="D424" s="17" t="s">
-        <v>163</v>
-      </c>
-      <c r="E424" s="95" t="s">
-        <v>601</v>
-      </c>
-      <c r="F424" s="17"/>
-    </row>
-    <row r="425" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A425" s="135" t="s">
-        <v>598</v>
-      </c>
-      <c r="B425" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="C425" s="57"/>
-      <c r="D425" s="23"/>
-      <c r="E425" s="36"/>
-      <c r="F425" s="36"/>
+      <c r="E425" s="34" t="s">
+        <v>232</v>
+      </c>
+      <c r="F425" s="17"/>
     </row>
     <row r="426" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A426" s="117" t="s">
-        <v>13</v>
-      </c>
-      <c r="B426" s="18" t="s">
-        <v>286</v>
-      </c>
-      <c r="C426" s="22" t="s">
-        <v>602</v>
-      </c>
-      <c r="D426" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="E426" s="95" t="s">
-        <v>603</v>
-      </c>
-      <c r="F426" s="17"/>
+      <c r="A426" s="135" t="s">
+        <v>24</v>
+      </c>
+      <c r="B426" s="25" t="s">
+        <v>283</v>
+      </c>
+      <c r="C426" s="57" t="s">
+        <v>135</v>
+      </c>
+      <c r="D426" s="23"/>
+      <c r="E426" s="36"/>
+      <c r="F426" s="36"/>
     </row>
     <row r="427" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A427" s="117" t="s">
-        <v>428</v>
+        <v>25</v>
       </c>
       <c r="B427" s="18" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C427" s="22" t="s">
-        <v>604</v>
+        <v>368</v>
       </c>
       <c r="D427" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="E427" s="95" t="s">
-        <v>605</v>
+        <v>163</v>
+      </c>
+      <c r="E427" s="35">
+        <v>43013</v>
       </c>
       <c r="F427" s="17"/>
     </row>
-    <row r="428" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="428" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A428" s="117" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="B428" s="18" t="s">
-        <v>39</v>
+        <v>285</v>
       </c>
       <c r="C428" s="22" t="s">
-        <v>606</v>
+        <v>369</v>
       </c>
       <c r="D428" s="17" t="s">
         <v>163</v>
       </c>
-      <c r="E428" s="95" t="s">
-        <v>601</v>
+      <c r="E428" s="35">
+        <v>43023</v>
       </c>
       <c r="F428" s="17"/>
     </row>
-    <row r="429" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A429" s="117" t="s">
-        <v>263</v>
-      </c>
-      <c r="B429" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="C429" s="22" t="s">
-        <v>607</v>
-      </c>
-      <c r="D429" s="17" t="s">
-        <v>609</v>
-      </c>
-      <c r="E429" s="95" t="s">
-        <v>610</v>
-      </c>
-      <c r="F429" s="17"/>
-    </row>
-    <row r="430" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A430" s="117" t="s">
-        <v>40</v>
+    <row r="429" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A429" s="135" t="s">
+        <v>136</v>
+      </c>
+      <c r="B429" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="C429" s="57"/>
+      <c r="D429" s="23"/>
+      <c r="E429" s="36"/>
+      <c r="F429" s="36"/>
+    </row>
+    <row r="430" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A430" s="136" t="s">
+        <v>416</v>
       </c>
       <c r="B430" s="18" t="s">
         <v>39</v>
       </c>
       <c r="C430" s="22" t="s">
-        <v>608</v>
-      </c>
-      <c r="D430" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="E430" s="95" t="s">
-        <v>611</v>
-      </c>
-      <c r="F430" s="96">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="431" spans="1:6" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A431" s="135" t="s">
-        <v>82</v>
-      </c>
-      <c r="B431" s="25" t="s">
-        <v>276</v>
-      </c>
-      <c r="C431" s="57" t="s">
-        <v>395</v>
-      </c>
-      <c r="D431" s="23"/>
-      <c r="E431" s="36"/>
-      <c r="F431" s="36"/>
-    </row>
-    <row r="432" spans="1:6" x14ac:dyDescent="0.2">
+        <v>585</v>
+      </c>
+      <c r="D430" s="22"/>
+      <c r="E430" s="22"/>
+      <c r="F430" s="22"/>
+    </row>
+    <row r="431" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A431" s="117" t="s">
+        <v>137</v>
+      </c>
+      <c r="B431" s="18" t="s">
+        <v>286</v>
+      </c>
+      <c r="C431" s="22" t="s">
+        <v>370</v>
+      </c>
+      <c r="D431" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="E431" s="34">
+        <v>10</v>
+      </c>
+      <c r="F431" s="17"/>
+    </row>
+    <row r="432" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A432" s="117" t="s">
-        <v>394</v>
-      </c>
-      <c r="B432" s="54" t="s">
-        <v>289</v>
+        <v>589</v>
+      </c>
+      <c r="B432" s="18" t="s">
+        <v>39</v>
       </c>
       <c r="C432" s="22" t="s">
-        <v>612</v>
-      </c>
-      <c r="D432" s="22" t="s">
-        <v>230</v>
-      </c>
-      <c r="E432" s="97">
+        <v>590</v>
+      </c>
+      <c r="D432" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="E432" s="34">
         <v>1</v>
       </c>
       <c r="F432" s="17"/>
     </row>
-    <row r="433" spans="1:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="A433" s="117" t="s">
-        <v>134</v>
-      </c>
-      <c r="B433" s="54" t="s">
-        <v>289</v>
-      </c>
-      <c r="C433" s="22" t="s">
-        <v>613</v>
-      </c>
-      <c r="D433" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="E433" s="34" t="s">
-        <v>231</v>
-      </c>
-      <c r="F433" s="17"/>
-    </row>
-    <row r="434" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A434" s="117" t="s">
-        <v>84</v>
-      </c>
-      <c r="B434" s="54" t="s">
-        <v>289</v>
+    <row r="433" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A433" s="122" t="s">
+        <v>27</v>
+      </c>
+      <c r="B433" s="103" t="s">
+        <v>39</v>
+      </c>
+      <c r="C433" s="112"/>
+      <c r="D433" s="104"/>
+      <c r="E433" s="105"/>
+      <c r="F433" s="61"/>
+    </row>
+    <row r="434" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A434" s="119" t="s">
+        <v>13</v>
+      </c>
+      <c r="B434" s="18" t="s">
+        <v>39</v>
       </c>
       <c r="C434" s="22" t="s">
-        <v>614</v>
+        <v>591</v>
       </c>
       <c r="D434" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="E434" s="34" t="s">
+        <v>592</v>
+      </c>
+      <c r="F434" s="17"/>
+    </row>
+    <row r="435" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A435" s="119" t="s">
+        <v>28</v>
+      </c>
+      <c r="B435" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C435" s="22" t="s">
+        <v>593</v>
+      </c>
+      <c r="D435" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="E435" s="34" t="s">
+        <v>594</v>
+      </c>
+      <c r="F435" s="17"/>
+    </row>
+    <row r="436" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A436" s="119" t="s">
+        <v>14</v>
+      </c>
+      <c r="B436" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C436" s="22" t="s">
+        <v>595</v>
+      </c>
+      <c r="D436" s="17" t="s">
         <v>163</v>
       </c>
-      <c r="E434" s="35">
-        <v>43070</v>
-      </c>
-      <c r="F434" s="17"/>
-    </row>
-    <row r="435" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A435" s="122" t="s">
-        <v>86</v>
-      </c>
-      <c r="B435" s="103" t="s">
-        <v>276</v>
-      </c>
-      <c r="C435" s="112"/>
-      <c r="D435" s="104"/>
-      <c r="E435" s="105"/>
-      <c r="F435" s="61"/>
-    </row>
-    <row r="436" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A436" s="119" t="s">
-        <v>13</v>
-      </c>
-      <c r="B436" s="18" t="s">
-        <v>276</v>
-      </c>
-      <c r="C436" s="22" t="s">
-        <v>340</v>
-      </c>
-      <c r="D436" s="17" t="s">
+      <c r="E436" s="35">
+        <v>36161</v>
+      </c>
+      <c r="F436" s="17"/>
+    </row>
+    <row r="437" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A437" s="135" t="s">
+        <v>596</v>
+      </c>
+      <c r="B437" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="C437" s="57"/>
+      <c r="D437" s="23"/>
+      <c r="E437" s="36"/>
+      <c r="F437" s="36"/>
+    </row>
+    <row r="438" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A438" s="117" t="s">
+        <v>137</v>
+      </c>
+      <c r="B438" s="18" t="s">
+        <v>286</v>
+      </c>
+      <c r="C438" s="22" t="s">
+        <v>597</v>
+      </c>
+      <c r="D438" s="17" t="s">
         <v>166</v>
       </c>
-      <c r="E436" s="44">
-        <v>83745498753497</v>
-      </c>
-      <c r="F436" s="17"/>
-    </row>
-    <row r="437" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A437" s="119" t="s">
-        <v>41</v>
-      </c>
-      <c r="B437" s="18" t="s">
-        <v>288</v>
-      </c>
-      <c r="C437" s="22" t="s">
-        <v>615</v>
-      </c>
-      <c r="D437" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="E437" s="41" t="s">
-        <v>194</v>
-      </c>
-      <c r="F437" s="17"/>
-    </row>
-    <row r="438" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A438" s="122" t="s">
-        <v>87</v>
-      </c>
-      <c r="B438" s="103" t="s">
-        <v>289</v>
-      </c>
-      <c r="C438" s="112" t="s">
-        <v>341</v>
-      </c>
-      <c r="D438" s="104"/>
-      <c r="E438" s="105"/>
-      <c r="F438" s="61"/>
-    </row>
-    <row r="439" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A439" s="119" t="s">
-        <v>58</v>
-      </c>
-      <c r="B439" s="18" t="s">
-        <v>289</v>
-      </c>
-      <c r="C439" s="22" t="s">
-        <v>342</v>
-      </c>
-      <c r="D439" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="E439" s="34" t="s">
-        <v>210</v>
-      </c>
-      <c r="F439" s="17"/>
+      <c r="E438" s="34">
+        <v>10</v>
+      </c>
+      <c r="F438" s="17"/>
+    </row>
+    <row r="439" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A439" s="122" t="s">
+        <v>598</v>
+      </c>
+      <c r="B439" s="103" t="s">
+        <v>39</v>
+      </c>
+      <c r="C439" s="112"/>
+      <c r="D439" s="104"/>
+      <c r="E439" s="105"/>
+      <c r="F439" s="61"/>
     </row>
     <row r="440" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A440" s="119" t="s">
-        <v>59</v>
+        <v>13</v>
       </c>
       <c r="B440" s="18" t="s">
+        <v>286</v>
+      </c>
+      <c r="C440" s="22" t="s">
+        <v>599</v>
+      </c>
+      <c r="D440" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="E440" s="95">
+        <v>23421</v>
+      </c>
+      <c r="F440" s="17"/>
+    </row>
+    <row r="441" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A441" s="119" t="s">
+        <v>14</v>
+      </c>
+      <c r="B441" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C441" s="22" t="s">
+        <v>600</v>
+      </c>
+      <c r="D441" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="E441" s="95" t="s">
+        <v>601</v>
+      </c>
+      <c r="F441" s="17"/>
+    </row>
+    <row r="442" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A442" s="135" t="s">
+        <v>598</v>
+      </c>
+      <c r="B442" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="C442" s="57"/>
+      <c r="D442" s="23"/>
+      <c r="E442" s="36"/>
+      <c r="F442" s="36"/>
+    </row>
+    <row r="443" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A443" s="117" t="s">
+        <v>13</v>
+      </c>
+      <c r="B443" s="18" t="s">
+        <v>286</v>
+      </c>
+      <c r="C443" s="22" t="s">
+        <v>602</v>
+      </c>
+      <c r="D443" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="E443" s="95" t="s">
+        <v>603</v>
+      </c>
+      <c r="F443" s="17"/>
+    </row>
+    <row r="444" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A444" s="117" t="s">
+        <v>428</v>
+      </c>
+      <c r="B444" s="18" t="s">
+        <v>286</v>
+      </c>
+      <c r="C444" s="22" t="s">
+        <v>604</v>
+      </c>
+      <c r="D444" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="E444" s="95" t="s">
+        <v>605</v>
+      </c>
+      <c r="F444" s="17"/>
+    </row>
+    <row r="445" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A445" s="117" t="s">
+        <v>14</v>
+      </c>
+      <c r="B445" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C445" s="22" t="s">
+        <v>606</v>
+      </c>
+      <c r="D445" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="E445" s="95" t="s">
+        <v>601</v>
+      </c>
+      <c r="F445" s="17"/>
+    </row>
+    <row r="446" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A446" s="117" t="s">
+        <v>263</v>
+      </c>
+      <c r="B446" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C446" s="22" t="s">
+        <v>607</v>
+      </c>
+      <c r="D446" s="17" t="s">
+        <v>609</v>
+      </c>
+      <c r="E446" s="95" t="s">
+        <v>610</v>
+      </c>
+      <c r="F446" s="17"/>
+    </row>
+    <row r="447" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A447" s="117" t="s">
+        <v>40</v>
+      </c>
+      <c r="B447" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C447" s="22" t="s">
+        <v>608</v>
+      </c>
+      <c r="D447" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="E447" s="95" t="s">
+        <v>611</v>
+      </c>
+      <c r="F447" s="96">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="448" spans="1:6" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A448" s="135" t="s">
+        <v>82</v>
+      </c>
+      <c r="B448" s="25" t="s">
+        <v>276</v>
+      </c>
+      <c r="C448" s="57" t="s">
+        <v>395</v>
+      </c>
+      <c r="D448" s="23"/>
+      <c r="E448" s="36"/>
+      <c r="F448" s="36"/>
+    </row>
+    <row r="449" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A449" s="117" t="s">
+        <v>394</v>
+      </c>
+      <c r="B449" s="54" t="s">
         <v>289</v>
       </c>
-      <c r="C440" s="22" t="s">
-        <v>343</v>
-      </c>
-      <c r="D440" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="E440" s="34" t="s">
-        <v>211</v>
-      </c>
-      <c r="F440" s="17"/>
-    </row>
-    <row r="441" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A441" s="119" t="s">
-        <v>265</v>
-      </c>
-      <c r="B441" s="18" t="s">
+      <c r="C449" s="22" t="s">
+        <v>612</v>
+      </c>
+      <c r="D449" s="22" t="s">
+        <v>230</v>
+      </c>
+      <c r="E449" s="97">
+        <v>1</v>
+      </c>
+      <c r="F449" s="17"/>
+    </row>
+    <row r="450" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A450" s="117" t="s">
+        <v>134</v>
+      </c>
+      <c r="B450" s="54" t="s">
         <v>289</v>
       </c>
-      <c r="C441" s="22" t="s">
-        <v>495</v>
-      </c>
-      <c r="D441" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="E441" s="34"/>
-      <c r="F441" s="17"/>
-    </row>
-    <row r="442" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A442" s="119" t="s">
-        <v>266</v>
-      </c>
-      <c r="B442" s="18" t="s">
-        <v>289</v>
-      </c>
-      <c r="C442" s="22" t="s">
-        <v>616</v>
-      </c>
-      <c r="D442" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="E442" s="34"/>
-      <c r="F442" s="17"/>
-    </row>
-    <row r="443" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A443" s="119" t="s">
-        <v>267</v>
-      </c>
-      <c r="B443" s="18" t="s">
-        <v>289</v>
-      </c>
-      <c r="C443" s="22" t="s">
-        <v>617</v>
-      </c>
-      <c r="D443" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="E443" s="34"/>
-      <c r="F443" s="17"/>
-    </row>
-    <row r="444" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A444" s="119" t="s">
-        <v>60</v>
-      </c>
-      <c r="B444" s="18" t="s">
-        <v>289</v>
-      </c>
-      <c r="C444" s="22" t="s">
-        <v>344</v>
-      </c>
-      <c r="D444" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="E444" s="34" t="s">
-        <v>212</v>
-      </c>
-      <c r="F444" s="17"/>
-    </row>
-    <row r="445" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A445" s="119" t="s">
-        <v>61</v>
-      </c>
-      <c r="B445" s="18" t="s">
-        <v>289</v>
-      </c>
-      <c r="C445" s="22" t="s">
-        <v>345</v>
-      </c>
-      <c r="D445" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="E445" s="34">
-        <v>86756</v>
-      </c>
-      <c r="F445" s="17"/>
-    </row>
-    <row r="446" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A446" s="119" t="s">
-        <v>62</v>
-      </c>
-      <c r="B446" s="18" t="s">
-        <v>289</v>
-      </c>
-      <c r="C446" s="22" t="s">
-        <v>618</v>
-      </c>
-      <c r="D446" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="E446" s="34" t="s">
-        <v>213</v>
-      </c>
-      <c r="F446" s="17"/>
-    </row>
-    <row r="447" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A447" s="131" t="s">
-        <v>65</v>
-      </c>
-      <c r="B447" s="115" t="s">
-        <v>289</v>
-      </c>
-      <c r="C447" s="113"/>
-      <c r="D447" s="107"/>
-      <c r="E447" s="108"/>
-      <c r="F447" s="67"/>
-    </row>
-    <row r="448" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A448" s="125" t="s">
-        <v>66</v>
-      </c>
-      <c r="B448" s="18" t="s">
-        <v>288</v>
-      </c>
-      <c r="C448" s="22" t="s">
-        <v>619</v>
-      </c>
-      <c r="D448" s="17" t="s">
+      <c r="C450" s="22" t="s">
+        <v>613</v>
+      </c>
+      <c r="D450" s="17" t="s">
         <v>164</v>
       </c>
-      <c r="E448" s="34" t="s">
-        <v>200</v>
-      </c>
-      <c r="F448" s="17"/>
-    </row>
-    <row r="449" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A449" s="125" t="s">
-        <v>56</v>
-      </c>
-      <c r="B449" s="18" t="s">
-        <v>289</v>
-      </c>
-      <c r="C449" s="22" t="s">
-        <v>620</v>
-      </c>
-      <c r="D449" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="E449" s="34" t="s">
-        <v>485</v>
-      </c>
-      <c r="F449" s="17"/>
-    </row>
-    <row r="450" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A450" s="135" t="s">
-        <v>104</v>
-      </c>
-      <c r="B450" s="25" t="s">
-        <v>283</v>
-      </c>
-      <c r="C450" s="57" t="s">
-        <v>371</v>
-      </c>
-      <c r="D450" s="23"/>
-      <c r="E450" s="36"/>
-      <c r="F450" s="36"/>
+      <c r="E450" s="34" t="s">
+        <v>231</v>
+      </c>
+      <c r="F450" s="17"/>
     </row>
     <row r="451" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A451" s="117" t="s">
+        <v>84</v>
+      </c>
+      <c r="B451" s="54" t="s">
+        <v>289</v>
+      </c>
+      <c r="C451" s="22" t="s">
+        <v>614</v>
+      </c>
+      <c r="D451" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="E451" s="35">
+        <v>43070</v>
+      </c>
+      <c r="F451" s="17"/>
+    </row>
+    <row r="452" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A452" s="122" t="s">
+        <v>86</v>
+      </c>
+      <c r="B452" s="103" t="s">
+        <v>276</v>
+      </c>
+      <c r="C452" s="112"/>
+      <c r="D452" s="104"/>
+      <c r="E452" s="105"/>
+      <c r="F452" s="61"/>
+    </row>
+    <row r="453" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A453" s="119" t="s">
+        <v>13</v>
+      </c>
+      <c r="B453" s="18" t="s">
+        <v>276</v>
+      </c>
+      <c r="C453" s="22" t="s">
+        <v>340</v>
+      </c>
+      <c r="D453" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="E453" s="44">
+        <v>83745498753497</v>
+      </c>
+      <c r="F453" s="17"/>
+    </row>
+    <row r="454" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A454" s="119" t="s">
+        <v>41</v>
+      </c>
+      <c r="B454" s="18" t="s">
+        <v>288</v>
+      </c>
+      <c r="C454" s="22" t="s">
+        <v>615</v>
+      </c>
+      <c r="D454" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="E454" s="41" t="s">
+        <v>194</v>
+      </c>
+      <c r="F454" s="17"/>
+    </row>
+    <row r="455" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A455" s="122" t="s">
+        <v>87</v>
+      </c>
+      <c r="B455" s="103" t="s">
+        <v>289</v>
+      </c>
+      <c r="C455" s="112" t="s">
+        <v>341</v>
+      </c>
+      <c r="D455" s="104"/>
+      <c r="E455" s="105"/>
+      <c r="F455" s="61"/>
+    </row>
+    <row r="456" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A456" s="119" t="s">
+        <v>58</v>
+      </c>
+      <c r="B456" s="18" t="s">
+        <v>289</v>
+      </c>
+      <c r="C456" s="22" t="s">
+        <v>342</v>
+      </c>
+      <c r="D456" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="E456" s="34" t="s">
+        <v>210</v>
+      </c>
+      <c r="F456" s="17"/>
+    </row>
+    <row r="457" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A457" s="119" t="s">
+        <v>59</v>
+      </c>
+      <c r="B457" s="18" t="s">
+        <v>289</v>
+      </c>
+      <c r="C457" s="22" t="s">
+        <v>343</v>
+      </c>
+      <c r="D457" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="E457" s="34" t="s">
+        <v>211</v>
+      </c>
+      <c r="F457" s="17"/>
+    </row>
+    <row r="458" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A458" s="119" t="s">
+        <v>265</v>
+      </c>
+      <c r="B458" s="18" t="s">
+        <v>289</v>
+      </c>
+      <c r="C458" s="22" t="s">
+        <v>495</v>
+      </c>
+      <c r="D458" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="E458" s="34"/>
+      <c r="F458" s="17"/>
+    </row>
+    <row r="459" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A459" s="119" t="s">
+        <v>266</v>
+      </c>
+      <c r="B459" s="18" t="s">
+        <v>289</v>
+      </c>
+      <c r="C459" s="22" t="s">
+        <v>616</v>
+      </c>
+      <c r="D459" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="E459" s="34"/>
+      <c r="F459" s="17"/>
+    </row>
+    <row r="460" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A460" s="119" t="s">
+        <v>267</v>
+      </c>
+      <c r="B460" s="18" t="s">
+        <v>289</v>
+      </c>
+      <c r="C460" s="22" t="s">
+        <v>617</v>
+      </c>
+      <c r="D460" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="E460" s="34"/>
+      <c r="F460" s="17"/>
+    </row>
+    <row r="461" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A461" s="119" t="s">
+        <v>60</v>
+      </c>
+      <c r="B461" s="18" t="s">
+        <v>289</v>
+      </c>
+      <c r="C461" s="22" t="s">
+        <v>344</v>
+      </c>
+      <c r="D461" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="E461" s="34" t="s">
+        <v>212</v>
+      </c>
+      <c r="F461" s="17"/>
+    </row>
+    <row r="462" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A462" s="119" t="s">
+        <v>61</v>
+      </c>
+      <c r="B462" s="18" t="s">
+        <v>289</v>
+      </c>
+      <c r="C462" s="22" t="s">
+        <v>345</v>
+      </c>
+      <c r="D462" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="E462" s="34">
+        <v>86756</v>
+      </c>
+      <c r="F462" s="17"/>
+    </row>
+    <row r="463" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A463" s="119" t="s">
+        <v>62</v>
+      </c>
+      <c r="B463" s="18" t="s">
+        <v>289</v>
+      </c>
+      <c r="C463" s="22" t="s">
+        <v>618</v>
+      </c>
+      <c r="D463" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="E463" s="34" t="s">
+        <v>213</v>
+      </c>
+      <c r="F463" s="17"/>
+    </row>
+    <row r="464" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A464" s="131" t="s">
+        <v>65</v>
+      </c>
+      <c r="B464" s="115" t="s">
+        <v>289</v>
+      </c>
+      <c r="C464" s="113"/>
+      <c r="D464" s="107"/>
+      <c r="E464" s="108"/>
+      <c r="F464" s="67"/>
+    </row>
+    <row r="465" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A465" s="125" t="s">
+        <v>66</v>
+      </c>
+      <c r="B465" s="18" t="s">
+        <v>288</v>
+      </c>
+      <c r="C465" s="22" t="s">
+        <v>619</v>
+      </c>
+      <c r="D465" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="E465" s="34" t="s">
+        <v>200</v>
+      </c>
+      <c r="F465" s="17"/>
+    </row>
+    <row r="466" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A466" s="125" t="s">
+        <v>56</v>
+      </c>
+      <c r="B466" s="18" t="s">
+        <v>289</v>
+      </c>
+      <c r="C466" s="22" t="s">
+        <v>620</v>
+      </c>
+      <c r="D466" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="E466" s="34" t="s">
+        <v>485</v>
+      </c>
+      <c r="F466" s="17"/>
+    </row>
+    <row r="467" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A467" s="135" t="s">
+        <v>104</v>
+      </c>
+      <c r="B467" s="25" t="s">
+        <v>283</v>
+      </c>
+      <c r="C467" s="57" t="s">
+        <v>371</v>
+      </c>
+      <c r="D467" s="23"/>
+      <c r="E467" s="36"/>
+      <c r="F467" s="36"/>
+    </row>
+    <row r="468" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A468" s="117" t="s">
         <v>105</v>
       </c>
-      <c r="B451" s="18" t="s">
+      <c r="B468" s="18" t="s">
         <v>283</v>
       </c>
-      <c r="C451" s="22" t="s">
+      <c r="C468" s="22" t="s">
         <v>621</v>
-      </c>
-      <c r="D451" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="E451" s="22" t="s">
-        <v>622</v>
-      </c>
-      <c r="F451" s="17"/>
-    </row>
-    <row r="452" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A452" s="117" t="s">
-        <v>106</v>
-      </c>
-      <c r="B452" s="18" t="s">
-        <v>283</v>
-      </c>
-      <c r="C452" s="22" t="s">
-        <v>623</v>
-      </c>
-      <c r="D452" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="E452" s="34">
-        <v>95</v>
-      </c>
-      <c r="F452" s="17"/>
-    </row>
-    <row r="453" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A453" s="117" t="s">
-        <v>107</v>
-      </c>
-      <c r="B453" s="18" t="s">
-        <v>283</v>
-      </c>
-      <c r="C453" s="22" t="s">
-        <v>372</v>
-      </c>
-      <c r="D453" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="E453" s="34" t="s">
-        <v>222</v>
-      </c>
-      <c r="F453" s="17"/>
-    </row>
-    <row r="454" spans="1:6" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A454" s="117" t="s">
-        <v>108</v>
-      </c>
-      <c r="B454" s="18" t="s">
-        <v>283</v>
-      </c>
-      <c r="C454" s="22" t="s">
-        <v>373</v>
-      </c>
-      <c r="D454" s="17" t="s">
-        <v>223</v>
-      </c>
-      <c r="E454" s="34">
-        <v>20</v>
-      </c>
-      <c r="F454" s="17"/>
-    </row>
-    <row r="455" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A455" s="117" t="s">
-        <v>109</v>
-      </c>
-      <c r="B455" s="18" t="s">
-        <v>285</v>
-      </c>
-      <c r="C455" s="22" t="s">
-        <v>624</v>
-      </c>
-      <c r="D455" s="17" t="s">
-        <v>224</v>
-      </c>
-      <c r="E455" s="34" t="s">
-        <v>248</v>
-      </c>
-      <c r="F455" s="17"/>
-    </row>
-    <row r="456" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A456" s="117" t="s">
-        <v>111</v>
-      </c>
-      <c r="B456" s="18" t="s">
-        <v>285</v>
-      </c>
-      <c r="C456" s="22" t="s">
-        <v>625</v>
-      </c>
-      <c r="D456" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="E456" s="34" t="s">
-        <v>225</v>
-      </c>
-      <c r="F456" s="17"/>
-    </row>
-    <row r="457" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A457" s="117" t="s">
-        <v>112</v>
-      </c>
-      <c r="B457" s="18" t="s">
-        <v>283</v>
-      </c>
-      <c r="C457" s="22" t="s">
-        <v>626</v>
-      </c>
-      <c r="D457" s="17" t="s">
-        <v>224</v>
-      </c>
-      <c r="E457" s="34" t="s">
-        <v>250</v>
-      </c>
-      <c r="F457" s="17"/>
-    </row>
-    <row r="458" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A458" s="117" t="s">
-        <v>111</v>
-      </c>
-      <c r="B458" s="18" t="s">
-        <v>285</v>
-      </c>
-      <c r="C458" s="22" t="s">
-        <v>543</v>
-      </c>
-      <c r="D458" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="E458" s="34" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="459" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A459" s="135" t="s">
-        <v>115</v>
-      </c>
-      <c r="B459" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="C459" s="57"/>
-      <c r="D459" s="23"/>
-      <c r="E459" s="36"/>
-      <c r="F459" s="23"/>
-    </row>
-    <row r="460" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A460" s="117" t="s">
-        <v>116</v>
-      </c>
-      <c r="B460" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="C460" s="22" t="s">
-        <v>628</v>
-      </c>
-      <c r="D460" s="17" t="s">
-        <v>224</v>
-      </c>
-      <c r="E460" s="34" t="s">
-        <v>226</v>
-      </c>
-      <c r="F460" s="22"/>
-    </row>
-    <row r="461" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A461" s="117" t="s">
-        <v>111</v>
-      </c>
-      <c r="B461" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="C461" s="56" t="s">
-        <v>629</v>
-      </c>
-      <c r="D461" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="E461" s="34" t="s">
-        <v>225</v>
-      </c>
-      <c r="F461" s="17"/>
-    </row>
-    <row r="462" spans="1:6" ht="77.25" x14ac:dyDescent="0.25">
-      <c r="A462" s="122" t="s">
-        <v>117</v>
-      </c>
-      <c r="B462" s="103" t="s">
-        <v>45</v>
-      </c>
-      <c r="C462" s="112" t="s">
-        <v>627</v>
-      </c>
-      <c r="D462" s="104"/>
-      <c r="E462" s="105"/>
-      <c r="F462" s="59"/>
-    </row>
-    <row r="463" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A463" s="119" t="s">
-        <v>118</v>
-      </c>
-      <c r="B463" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="C463" s="22" t="s">
-        <v>630</v>
-      </c>
-      <c r="D463" s="17" t="s">
-        <v>224</v>
-      </c>
-      <c r="E463" s="22" t="s">
-        <v>227</v>
-      </c>
-      <c r="F463" s="17"/>
-    </row>
-    <row r="464" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A464" s="119" t="s">
-        <v>111</v>
-      </c>
-      <c r="B464" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="C464" s="56" t="s">
-        <v>631</v>
-      </c>
-      <c r="D464" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="E464" s="22" t="s">
-        <v>225</v>
-      </c>
-      <c r="F464" s="17"/>
-    </row>
-    <row r="465" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A465" s="119" t="s">
-        <v>116</v>
-      </c>
-      <c r="B465" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="C465" s="22" t="s">
-        <v>632</v>
-      </c>
-      <c r="D465" s="17" t="s">
-        <v>224</v>
-      </c>
-      <c r="E465" s="22" t="s">
-        <v>226</v>
-      </c>
-      <c r="F465" s="17"/>
-    </row>
-    <row r="466" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A466" s="119" t="s">
-        <v>111</v>
-      </c>
-      <c r="B466" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="C466" s="56" t="s">
-        <v>358</v>
-      </c>
-      <c r="D466" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="E466" s="34" t="s">
-        <v>225</v>
-      </c>
-      <c r="F466" s="17"/>
-    </row>
-    <row r="467" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A467" s="124" t="s">
-        <v>113</v>
-      </c>
-      <c r="B467" s="106" t="s">
-        <v>45</v>
-      </c>
-      <c r="C467" s="113"/>
-      <c r="D467" s="107"/>
-      <c r="E467" s="108"/>
-      <c r="F467" s="67"/>
-    </row>
-    <row r="468" spans="1:6" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A468" s="119" t="s">
-        <v>13</v>
-      </c>
-      <c r="B468" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="C468" s="22" t="s">
-        <v>703</v>
       </c>
       <c r="D468" s="17" t="s">
         <v>164</v>
       </c>
-      <c r="E468" s="34" t="s">
-        <v>184</v>
+      <c r="E468" s="22" t="s">
+        <v>622</v>
       </c>
       <c r="F468" s="17"/>
     </row>
-    <row r="469" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A469" s="119" t="s">
-        <v>114</v>
+    <row r="469" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A469" s="117" t="s">
+        <v>106</v>
       </c>
       <c r="B469" s="18" t="s">
-        <v>45</v>
+        <v>283</v>
       </c>
       <c r="C469" s="22" t="s">
-        <v>364</v>
+        <v>623</v>
       </c>
       <c r="D469" s="17" t="s">
-        <v>223</v>
+        <v>164</v>
       </c>
       <c r="E469" s="34">
-        <v>25</v>
+        <v>95</v>
       </c>
       <c r="F469" s="17"/>
     </row>
-    <row r="470" spans="1:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="A470" s="119" t="s">
-        <v>119</v>
+    <row r="470" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A470" s="117" t="s">
+        <v>107</v>
       </c>
       <c r="B470" s="18" t="s">
         <v>283</v>
       </c>
       <c r="C470" s="22" t="s">
-        <v>633</v>
+        <v>372</v>
       </c>
       <c r="D470" s="17" t="s">
         <v>167</v>
       </c>
-      <c r="E470" s="34"/>
+      <c r="E470" s="34" t="s">
+        <v>222</v>
+      </c>
       <c r="F470" s="17"/>
     </row>
-    <row r="471" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A471" s="119" t="s">
-        <v>120</v>
+    <row r="471" spans="1:6" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A471" s="117" t="s">
+        <v>108</v>
       </c>
       <c r="B471" s="18" t="s">
         <v>283</v>
       </c>
       <c r="C471" s="22" t="s">
-        <v>634</v>
+        <v>373</v>
       </c>
       <c r="D471" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="E471" s="34" t="s">
-        <v>228</v>
+        <v>223</v>
+      </c>
+      <c r="E471" s="34">
+        <v>20</v>
       </c>
       <c r="F471" s="17"/>
     </row>
-    <row r="472" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A472" s="124" t="s">
-        <v>69</v>
-      </c>
-      <c r="B472" s="106" t="s">
-        <v>45</v>
-      </c>
-      <c r="C472" s="113"/>
-      <c r="D472" s="107"/>
-      <c r="E472" s="108"/>
-      <c r="F472" s="67"/>
+    <row r="472" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A472" s="117" t="s">
+        <v>109</v>
+      </c>
+      <c r="B472" s="18" t="s">
+        <v>285</v>
+      </c>
+      <c r="C472" s="22" t="s">
+        <v>624</v>
+      </c>
+      <c r="D472" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="E472" s="34" t="s">
+        <v>248</v>
+      </c>
+      <c r="F472" s="17"/>
     </row>
     <row r="473" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A473" s="125" t="s">
-        <v>13</v>
+      <c r="A473" s="117" t="s">
+        <v>111</v>
       </c>
       <c r="B473" s="18" t="s">
-        <v>45</v>
+        <v>285</v>
       </c>
       <c r="C473" s="22" t="s">
-        <v>548</v>
+        <v>625</v>
       </c>
       <c r="D473" s="17" t="s">
         <v>164</v>
       </c>
-      <c r="E473" s="17" t="s">
-        <v>192</v>
+      <c r="E473" s="34" t="s">
+        <v>225</v>
       </c>
       <c r="F473" s="17"/>
     </row>
     <row r="474" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A474" s="125" t="s">
-        <v>56</v>
+      <c r="A474" s="117" t="s">
+        <v>112</v>
       </c>
       <c r="B474" s="18" t="s">
-        <v>39</v>
+        <v>283</v>
       </c>
       <c r="C474" s="22" t="s">
-        <v>710</v>
+        <v>626</v>
       </c>
       <c r="D474" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="E474" s="17" t="s">
-        <v>709</v>
+        <v>224</v>
+      </c>
+      <c r="E474" s="34" t="s">
+        <v>250</v>
       </c>
       <c r="F474" s="17"/>
     </row>
-    <row r="475" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A475" s="135" t="s">
-        <v>139</v>
-      </c>
-      <c r="B475" s="25" t="s">
+    <row r="475" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A475" s="117" t="s">
+        <v>111</v>
+      </c>
+      <c r="B475" s="18" t="s">
+        <v>285</v>
+      </c>
+      <c r="C475" s="22" t="s">
+        <v>543</v>
+      </c>
+      <c r="D475" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="E475" s="34" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="476" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A476" s="135" t="s">
+        <v>115</v>
+      </c>
+      <c r="B476" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="C475" s="57" t="s">
-        <v>374</v>
-      </c>
-      <c r="D475" s="23"/>
-      <c r="E475" s="36"/>
-      <c r="F475" s="36"/>
-    </row>
-    <row r="476" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A476" s="136" t="s">
-        <v>416</v>
-      </c>
-      <c r="B476" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="C476" s="22" t="s">
-        <v>585</v>
-      </c>
-      <c r="D476" s="22"/>
-      <c r="E476" s="22"/>
-      <c r="F476" s="22"/>
+      <c r="C476" s="57"/>
+      <c r="D476" s="23"/>
+      <c r="E476" s="36"/>
+      <c r="F476" s="23"/>
     </row>
     <row r="477" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A477" s="117" t="s">
-        <v>140</v>
+        <v>116</v>
       </c>
       <c r="B477" s="18" t="s">
         <v>45</v>
       </c>
       <c r="C477" s="22" t="s">
-        <v>375</v>
-      </c>
-      <c r="D477" s="22" t="s">
-        <v>167</v>
-      </c>
-      <c r="E477" s="33" t="s">
-        <v>233</v>
+        <v>628</v>
+      </c>
+      <c r="D477" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="E477" s="34" t="s">
+        <v>226</v>
       </c>
       <c r="F477" s="22"/>
     </row>
-    <row r="478" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="478" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A478" s="117" t="s">
-        <v>56</v>
+        <v>111</v>
       </c>
       <c r="B478" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="C478" s="22" t="s">
-        <v>376</v>
-      </c>
-      <c r="D478" s="22" t="s">
-        <v>167</v>
+      <c r="C478" s="56" t="s">
+        <v>629</v>
+      </c>
+      <c r="D478" s="17" t="s">
+        <v>164</v>
       </c>
       <c r="E478" s="34" t="s">
-        <v>141</v>
+        <v>225</v>
       </c>
       <c r="F478" s="17"/>
     </row>
-    <row r="479" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="479" spans="1:6" ht="77.25" x14ac:dyDescent="0.25">
       <c r="A479" s="122" t="s">
-        <v>142</v>
+        <v>117</v>
       </c>
       <c r="B479" s="103" t="s">
-        <v>39</v>
-      </c>
-      <c r="C479" s="112"/>
+        <v>45</v>
+      </c>
+      <c r="C479" s="112" t="s">
+        <v>627</v>
+      </c>
       <c r="D479" s="104"/>
       <c r="E479" s="105"/>
-      <c r="F479" s="61"/>
-    </row>
-    <row r="480" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F479" s="59"/>
+    </row>
+    <row r="480" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A480" s="119" t="s">
-        <v>13</v>
+        <v>118</v>
       </c>
       <c r="B480" s="18" t="s">
-        <v>286</v>
+        <v>45</v>
       </c>
       <c r="C480" s="22" t="s">
-        <v>377</v>
+        <v>630</v>
       </c>
       <c r="D480" s="17" t="s">
-        <v>166</v>
-      </c>
-      <c r="E480" s="34">
-        <v>123455</v>
+        <v>224</v>
+      </c>
+      <c r="E480" s="22" t="s">
+        <v>227</v>
       </c>
       <c r="F480" s="17"/>
     </row>
-    <row r="481" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A481" s="122" t="s">
-        <v>143</v>
-      </c>
-      <c r="B481" s="103" t="s">
-        <v>39</v>
-      </c>
-      <c r="C481" s="112"/>
-      <c r="D481" s="104"/>
-      <c r="E481" s="105"/>
-      <c r="F481" s="61"/>
+    <row r="481" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A481" s="119" t="s">
+        <v>111</v>
+      </c>
+      <c r="B481" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C481" s="56" t="s">
+        <v>631</v>
+      </c>
+      <c r="D481" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="E481" s="22" t="s">
+        <v>225</v>
+      </c>
+      <c r="F481" s="17"/>
     </row>
     <row r="482" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A482" s="119" t="s">
+        <v>116</v>
+      </c>
+      <c r="B482" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C482" s="22" t="s">
+        <v>632</v>
+      </c>
+      <c r="D482" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="E482" s="22" t="s">
+        <v>226</v>
+      </c>
+      <c r="F482" s="17"/>
+    </row>
+    <row r="483" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A483" s="119" t="s">
+        <v>111</v>
+      </c>
+      <c r="B483" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C483" s="56" t="s">
+        <v>358</v>
+      </c>
+      <c r="D483" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="E483" s="34" t="s">
+        <v>225</v>
+      </c>
+      <c r="F483" s="17"/>
+    </row>
+    <row r="484" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A484" s="124" t="s">
+        <v>113</v>
+      </c>
+      <c r="B484" s="106" t="s">
+        <v>45</v>
+      </c>
+      <c r="C484" s="113"/>
+      <c r="D484" s="107"/>
+      <c r="E484" s="108"/>
+      <c r="F484" s="67"/>
+    </row>
+    <row r="485" spans="1:6" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A485" s="119" t="s">
         <v>13</v>
       </c>
-      <c r="B482" s="18" t="s">
-        <v>286</v>
-      </c>
-      <c r="C482" s="22" t="s">
-        <v>378</v>
-      </c>
-      <c r="D482" s="17" t="s">
-        <v>166</v>
-      </c>
-      <c r="E482" s="34">
-        <v>987342</v>
-      </c>
-      <c r="F482" s="17"/>
-    </row>
-    <row r="483" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A483" s="122" t="s">
-        <v>635</v>
-      </c>
-      <c r="B483" s="103" t="s">
-        <v>39</v>
-      </c>
-      <c r="C483" s="112"/>
-      <c r="D483" s="104"/>
-      <c r="E483" s="105"/>
-      <c r="F483" s="61"/>
-    </row>
-    <row r="484" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A484" s="119" t="s">
-        <v>13</v>
-      </c>
-      <c r="B484" s="18" t="s">
-        <v>286</v>
-      </c>
-      <c r="C484" s="22" t="s">
-        <v>636</v>
-      </c>
-      <c r="D484" s="17" t="s">
-        <v>166</v>
-      </c>
-      <c r="E484" s="34" t="s">
-        <v>637</v>
-      </c>
-      <c r="F484" s="17"/>
-    </row>
-    <row r="485" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A485" s="122" t="s">
-        <v>144</v>
-      </c>
-      <c r="B485" s="103" t="s">
-        <v>39</v>
-      </c>
-      <c r="C485" s="112"/>
-      <c r="D485" s="104"/>
-      <c r="E485" s="105"/>
-      <c r="F485" s="61"/>
+      <c r="B485" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C485" s="22" t="s">
+        <v>703</v>
+      </c>
+      <c r="D485" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="E485" s="34" t="s">
+        <v>184</v>
+      </c>
+      <c r="F485" s="17"/>
     </row>
     <row r="486" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A486" s="119" t="s">
+        <v>114</v>
+      </c>
+      <c r="B486" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C486" s="22" t="s">
+        <v>364</v>
+      </c>
+      <c r="D486" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="E486" s="34">
+        <v>25</v>
+      </c>
+      <c r="F486" s="17"/>
+    </row>
+    <row r="487" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A487" s="119" t="s">
+        <v>119</v>
+      </c>
+      <c r="B487" s="18" t="s">
+        <v>283</v>
+      </c>
+      <c r="C487" s="22" t="s">
+        <v>633</v>
+      </c>
+      <c r="D487" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="E487" s="34"/>
+      <c r="F487" s="17"/>
+    </row>
+    <row r="488" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A488" s="119" t="s">
+        <v>120</v>
+      </c>
+      <c r="B488" s="18" t="s">
+        <v>283</v>
+      </c>
+      <c r="C488" s="22" t="s">
+        <v>634</v>
+      </c>
+      <c r="D488" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="E488" s="34" t="s">
+        <v>228</v>
+      </c>
+      <c r="F488" s="17"/>
+    </row>
+    <row r="489" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A489" s="124" t="s">
+        <v>69</v>
+      </c>
+      <c r="B489" s="106" t="s">
+        <v>45</v>
+      </c>
+      <c r="C489" s="113"/>
+      <c r="D489" s="107"/>
+      <c r="E489" s="108"/>
+      <c r="F489" s="67"/>
+    </row>
+    <row r="490" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A490" s="125" t="s">
         <v>13</v>
       </c>
-      <c r="B486" s="18" t="s">
-        <v>286</v>
-      </c>
-      <c r="C486" s="22" t="s">
-        <v>379</v>
-      </c>
-      <c r="D486" s="17" t="s">
-        <v>166</v>
-      </c>
-      <c r="E486" s="34">
-        <v>10986700</v>
-      </c>
-      <c r="F486" s="17"/>
-    </row>
-    <row r="487" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A487" s="119" t="s">
-        <v>41</v>
-      </c>
-      <c r="B487" s="18" t="s">
-        <v>286</v>
-      </c>
-      <c r="C487" s="22" t="s">
-        <v>638</v>
-      </c>
-      <c r="D487" s="17"/>
-      <c r="E487" s="41" t="s">
-        <v>234</v>
-      </c>
-      <c r="F487" s="17"/>
-    </row>
-    <row r="488" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A488" s="122" t="s">
-        <v>145</v>
-      </c>
-      <c r="B488" s="103" t="s">
-        <v>39</v>
-      </c>
-      <c r="C488" s="112"/>
-      <c r="D488" s="104"/>
-      <c r="E488" s="105"/>
-      <c r="F488" s="61"/>
-    </row>
-    <row r="489" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A489" s="119" t="s">
-        <v>66</v>
-      </c>
-      <c r="B489" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="C489" s="22" t="s">
-        <v>380</v>
-      </c>
-      <c r="D489" s="17" t="s">
+      <c r="B490" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C490" s="22" t="s">
+        <v>548</v>
+      </c>
+      <c r="D490" s="17" t="s">
         <v>164</v>
       </c>
-      <c r="E489" s="34" t="s">
-        <v>191</v>
-      </c>
-      <c r="F489" s="17"/>
-    </row>
-    <row r="490" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A490" s="122" t="s">
-        <v>146</v>
-      </c>
-      <c r="B490" s="103" t="s">
-        <v>39</v>
-      </c>
-      <c r="C490" s="112"/>
-      <c r="D490" s="104"/>
-      <c r="E490" s="105"/>
-      <c r="F490" s="61"/>
+      <c r="E490" s="17" t="s">
+        <v>192</v>
+      </c>
+      <c r="F490" s="17"/>
     </row>
     <row r="491" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A491" s="119" t="s">
-        <v>147</v>
+      <c r="A491" s="125" t="s">
+        <v>56</v>
       </c>
       <c r="B491" s="18" t="s">
         <v>39</v>
       </c>
       <c r="C491" s="22" t="s">
-        <v>381</v>
+        <v>710</v>
       </c>
       <c r="D491" s="17" t="s">
-        <v>166</v>
-      </c>
-      <c r="E491" s="34">
-        <v>9873242</v>
+        <v>167</v>
+      </c>
+      <c r="E491" s="17" t="s">
+        <v>709</v>
       </c>
       <c r="F491" s="17"/>
     </row>
-    <row r="492" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A492" s="119" t="s">
-        <v>148</v>
-      </c>
-      <c r="B492" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="C492" s="22" t="s">
-        <v>639</v>
-      </c>
-      <c r="D492" s="17" t="s">
+    <row r="492" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A492" s="141" t="s">
+        <v>738</v>
+      </c>
+      <c r="B492" s="140" t="s">
+        <v>45</v>
+      </c>
+      <c r="C492" s="57"/>
+      <c r="D492" s="58"/>
+      <c r="E492" s="141"/>
+      <c r="F492" s="58"/>
+    </row>
+    <row r="493" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A493" s="117" t="s">
+        <v>116</v>
+      </c>
+      <c r="B493" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C493" s="22" t="s">
+        <v>744</v>
+      </c>
+      <c r="D493" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="E493" s="34" t="s">
+        <v>226</v>
+      </c>
+      <c r="F493" s="22"/>
+    </row>
+    <row r="494" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A494" s="117" t="s">
+        <v>111</v>
+      </c>
+      <c r="B494" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C494" s="56" t="s">
+        <v>629</v>
+      </c>
+      <c r="D494" s="17" t="s">
         <v>164</v>
       </c>
-      <c r="E492" s="34" t="s">
-        <v>236</v>
-      </c>
-      <c r="F492" s="17"/>
-    </row>
-    <row r="493" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A493" s="119" t="s">
-        <v>149</v>
-      </c>
-      <c r="B493" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="C493" s="22" t="s">
-        <v>640</v>
-      </c>
-      <c r="D493" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="E493" s="34"/>
-      <c r="F493" s="17"/>
-    </row>
-    <row r="494" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A494" s="122" t="s">
-        <v>150</v>
-      </c>
-      <c r="B494" s="103" t="s">
+      <c r="E494" s="34" t="s">
+        <v>225</v>
+      </c>
+      <c r="F494" s="17"/>
+    </row>
+    <row r="495" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A495" s="122" t="s">
+        <v>117</v>
+      </c>
+      <c r="B495" s="103" t="s">
         <v>45</v>
       </c>
-      <c r="C494" s="112" t="s">
-        <v>382</v>
-      </c>
-      <c r="D494" s="104"/>
-      <c r="E494" s="105"/>
-      <c r="F494" s="61"/>
-    </row>
-    <row r="495" spans="1:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="A495" s="119" t="s">
-        <v>13</v>
-      </c>
-      <c r="B495" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="C495" s="22" t="s">
-        <v>641</v>
-      </c>
-      <c r="D495" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="E495" s="34" t="s">
-        <v>184</v>
-      </c>
-      <c r="F495" s="34"/>
-    </row>
-    <row r="496" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C495" s="112"/>
+      <c r="D495" s="104"/>
+      <c r="E495" s="105"/>
+      <c r="F495" s="59"/>
+    </row>
+    <row r="496" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A496" s="119" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="B496" s="18" t="s">
         <v>45</v>
       </c>
       <c r="C496" s="22" t="s">
-        <v>392</v>
+        <v>630</v>
       </c>
       <c r="D496" s="17" t="s">
-        <v>223</v>
-      </c>
-      <c r="E496" s="34">
-        <v>25</v>
-      </c>
-      <c r="F496" s="34"/>
-    </row>
-    <row r="497" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A497" s="124" t="s">
-        <v>69</v>
-      </c>
-      <c r="B497" s="106" t="s">
+        <v>224</v>
+      </c>
+      <c r="E496" s="22" t="s">
+        <v>227</v>
+      </c>
+      <c r="F496" s="17"/>
+    </row>
+    <row r="497" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A497" s="119" t="s">
+        <v>111</v>
+      </c>
+      <c r="B497" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="C497" s="113"/>
-      <c r="D497" s="107"/>
-      <c r="E497" s="108"/>
-      <c r="F497" s="67"/>
-    </row>
-    <row r="498" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A498" s="125" t="s">
-        <v>13</v>
+      <c r="C497" s="56" t="s">
+        <v>631</v>
+      </c>
+      <c r="D497" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="E497" s="22" t="s">
+        <v>225</v>
+      </c>
+      <c r="F497" s="17"/>
+    </row>
+    <row r="498" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A498" s="119" t="s">
+        <v>116</v>
       </c>
       <c r="B498" s="18" t="s">
         <v>45</v>
       </c>
       <c r="C498" s="22" t="s">
+        <v>632</v>
+      </c>
+      <c r="D498" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="E498" s="22" t="s">
+        <v>226</v>
+      </c>
+      <c r="F498" s="17"/>
+    </row>
+    <row r="499" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A499" s="119" t="s">
+        <v>111</v>
+      </c>
+      <c r="B499" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C499" s="56" t="s">
+        <v>358</v>
+      </c>
+      <c r="D499" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="E499" s="34" t="s">
+        <v>225</v>
+      </c>
+      <c r="F499" s="17"/>
+    </row>
+    <row r="500" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A500" s="124" t="s">
+        <v>113</v>
+      </c>
+      <c r="B500" s="106" t="s">
+        <v>45</v>
+      </c>
+      <c r="C500" s="113"/>
+      <c r="D500" s="107"/>
+      <c r="E500" s="108"/>
+      <c r="F500" s="67"/>
+    </row>
+    <row r="501" spans="1:6" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A501" s="119" t="s">
+        <v>13</v>
+      </c>
+      <c r="B501" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C501" s="22" t="s">
+        <v>703</v>
+      </c>
+      <c r="D501" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="E501" s="34" t="s">
+        <v>184</v>
+      </c>
+      <c r="F501" s="17"/>
+    </row>
+    <row r="502" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A502" s="119" t="s">
+        <v>114</v>
+      </c>
+      <c r="B502" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C502" s="22" t="s">
+        <v>364</v>
+      </c>
+      <c r="D502" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="E502" s="34">
+        <v>25</v>
+      </c>
+      <c r="F502" s="17"/>
+    </row>
+    <row r="503" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A503" s="119" t="s">
+        <v>119</v>
+      </c>
+      <c r="B503" s="18" t="s">
+        <v>283</v>
+      </c>
+      <c r="C503" s="22" t="s">
+        <v>633</v>
+      </c>
+      <c r="D503" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="E503" s="34"/>
+      <c r="F503" s="17"/>
+    </row>
+    <row r="504" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A504" s="119" t="s">
+        <v>120</v>
+      </c>
+      <c r="B504" s="18" t="s">
+        <v>283</v>
+      </c>
+      <c r="C504" s="22" t="s">
+        <v>634</v>
+      </c>
+      <c r="D504" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="E504" s="34" t="s">
+        <v>228</v>
+      </c>
+      <c r="F504" s="17"/>
+    </row>
+    <row r="505" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A505" s="124" t="s">
+        <v>69</v>
+      </c>
+      <c r="B505" s="106" t="s">
+        <v>45</v>
+      </c>
+      <c r="C505" s="113"/>
+      <c r="D505" s="107"/>
+      <c r="E505" s="108"/>
+      <c r="F505" s="67"/>
+    </row>
+    <row r="506" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A506" s="125" t="s">
+        <v>13</v>
+      </c>
+      <c r="B506" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C506" s="22" t="s">
         <v>548</v>
       </c>
-      <c r="D498" s="17"/>
-      <c r="E498" s="34" t="s">
+      <c r="D506" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="E506" s="17" t="s">
         <v>192</v>
       </c>
-      <c r="F498" s="34"/>
-    </row>
-    <row r="499" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A499" s="122" t="s">
-        <v>151</v>
-      </c>
-      <c r="B499" s="103" t="s">
-        <v>39</v>
-      </c>
-      <c r="C499" s="112" t="s">
-        <v>152</v>
-      </c>
-      <c r="D499" s="104"/>
-      <c r="E499" s="105"/>
-      <c r="F499" s="61"/>
-    </row>
-    <row r="500" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A500" s="119" t="s">
+      <c r="F506" s="17"/>
+    </row>
+    <row r="507" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A507" s="125" t="s">
         <v>56</v>
       </c>
-      <c r="B500" s="18" t="s">
-        <v>286</v>
-      </c>
-      <c r="C500" s="22" t="s">
-        <v>642</v>
-      </c>
-      <c r="D500" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="E500" s="34" t="s">
-        <v>644</v>
-      </c>
-      <c r="F500" s="34"/>
-    </row>
-    <row r="501" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A501" s="119" t="s">
-        <v>153</v>
-      </c>
-      <c r="B501" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="C501" s="22" t="s">
-        <v>643</v>
-      </c>
-      <c r="D501" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="E501" s="34" t="s">
-        <v>645</v>
-      </c>
-      <c r="F501" s="34"/>
-    </row>
-    <row r="502" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A502" s="122" t="s">
-        <v>646</v>
-      </c>
-      <c r="B502" s="103" t="s">
-        <v>39</v>
-      </c>
-      <c r="C502" s="112" t="s">
-        <v>647</v>
-      </c>
-      <c r="D502" s="104"/>
-      <c r="E502" s="105"/>
-      <c r="F502" s="61"/>
-    </row>
-    <row r="503" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A503" s="119" t="s">
-        <v>648</v>
-      </c>
-      <c r="B503" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="C503" s="22" t="s">
-        <v>653</v>
-      </c>
-      <c r="D503" s="17" t="s">
-        <v>163</v>
-      </c>
-      <c r="E503" s="35">
-        <v>36161</v>
-      </c>
-      <c r="F503" s="34"/>
-    </row>
-    <row r="504" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A504" s="119" t="s">
-        <v>649</v>
-      </c>
-      <c r="B504" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="C504" s="22" t="s">
-        <v>654</v>
-      </c>
-      <c r="D504" s="17" t="s">
-        <v>163</v>
-      </c>
-      <c r="E504" s="35">
-        <v>36161</v>
-      </c>
-      <c r="F504" s="34"/>
-    </row>
-    <row r="505" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A505" s="119" t="s">
-        <v>650</v>
-      </c>
-      <c r="B505" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="C505" s="22" t="s">
-        <v>655</v>
-      </c>
-      <c r="D505" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="E505" s="34">
-        <v>123456</v>
-      </c>
-      <c r="F505" s="34"/>
-    </row>
-    <row r="506" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A506" s="124" t="s">
-        <v>651</v>
-      </c>
-      <c r="B506" s="106" t="s">
-        <v>39</v>
-      </c>
-      <c r="C506" s="113"/>
-      <c r="D506" s="107"/>
-      <c r="E506" s="108"/>
-      <c r="F506" s="67"/>
-    </row>
-    <row r="507" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A507" s="119" t="s">
-        <v>652</v>
-      </c>
       <c r="B507" s="18" t="s">
         <v>39</v>
       </c>
       <c r="C507" s="22" t="s">
-        <v>656</v>
+        <v>710</v>
       </c>
       <c r="D507" s="17" t="s">
         <v>167</v>
       </c>
-      <c r="E507" s="34" t="s">
-        <v>603</v>
-      </c>
-      <c r="F507" s="34"/>
-    </row>
-    <row r="508" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A508" s="119" t="s">
-        <v>664</v>
-      </c>
-      <c r="B508" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="C508" s="22" t="s">
-        <v>665</v>
-      </c>
-      <c r="D508" s="17" t="s">
-        <v>163</v>
-      </c>
-      <c r="E508" s="35">
-        <v>44562</v>
-      </c>
-      <c r="F508" s="34"/>
-    </row>
-    <row r="509" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A509" s="135" t="s">
-        <v>154</v>
-      </c>
-      <c r="B509" s="25" t="s">
+      <c r="E507" s="17" t="s">
+        <v>709</v>
+      </c>
+      <c r="F507" s="17"/>
+    </row>
+    <row r="508" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A508" s="135" t="s">
+        <v>139</v>
+      </c>
+      <c r="B508" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="C509" s="57" t="s">
-        <v>155</v>
-      </c>
-      <c r="D509" s="23"/>
-      <c r="E509" s="36"/>
-      <c r="F509" s="36"/>
-    </row>
-    <row r="510" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A510" s="136" t="s">
+      <c r="C508" s="57" t="s">
+        <v>374</v>
+      </c>
+      <c r="D508" s="23"/>
+      <c r="E508" s="36"/>
+      <c r="F508" s="36"/>
+    </row>
+    <row r="509" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A509" s="136" t="s">
         <v>416</v>
       </c>
+      <c r="B509" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C509" s="22" t="s">
+        <v>585</v>
+      </c>
+      <c r="D509" s="22"/>
+      <c r="E509" s="22"/>
+      <c r="F509" s="22"/>
+    </row>
+    <row r="510" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A510" s="117" t="s">
+        <v>140</v>
+      </c>
       <c r="B510" s="18" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="C510" s="22" t="s">
-        <v>585</v>
-      </c>
-      <c r="D510" s="22"/>
-      <c r="E510" s="22"/>
+        <v>375</v>
+      </c>
+      <c r="D510" s="22" t="s">
+        <v>167</v>
+      </c>
+      <c r="E510" s="33" t="s">
+        <v>233</v>
+      </c>
       <c r="F510" s="22"/>
     </row>
     <row r="511" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A511" s="117" t="s">
-        <v>156</v>
+        <v>56</v>
       </c>
       <c r="B511" s="18" t="s">
         <v>45</v>
       </c>
       <c r="C511" s="22" t="s">
+        <v>376</v>
+      </c>
+      <c r="D511" s="22" t="s">
+        <v>167</v>
+      </c>
+      <c r="E511" s="34" t="s">
+        <v>141</v>
+      </c>
+      <c r="F511" s="17"/>
+    </row>
+    <row r="512" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A512" s="122" t="s">
+        <v>142</v>
+      </c>
+      <c r="B512" s="103" t="s">
+        <v>39</v>
+      </c>
+      <c r="C512" s="112"/>
+      <c r="D512" s="104"/>
+      <c r="E512" s="105"/>
+      <c r="F512" s="61"/>
+    </row>
+    <row r="513" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A513" s="119" t="s">
+        <v>13</v>
+      </c>
+      <c r="B513" s="18" t="s">
+        <v>286</v>
+      </c>
+      <c r="C513" s="22" t="s">
+        <v>377</v>
+      </c>
+      <c r="D513" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="E513" s="34">
+        <v>123455</v>
+      </c>
+      <c r="F513" s="17"/>
+    </row>
+    <row r="514" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A514" s="122" t="s">
+        <v>143</v>
+      </c>
+      <c r="B514" s="103" t="s">
+        <v>39</v>
+      </c>
+      <c r="C514" s="112"/>
+      <c r="D514" s="104"/>
+      <c r="E514" s="105"/>
+      <c r="F514" s="61"/>
+    </row>
+    <row r="515" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A515" s="119" t="s">
+        <v>13</v>
+      </c>
+      <c r="B515" s="18" t="s">
+        <v>286</v>
+      </c>
+      <c r="C515" s="22" t="s">
+        <v>378</v>
+      </c>
+      <c r="D515" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="E515" s="34">
+        <v>987342</v>
+      </c>
+      <c r="F515" s="17"/>
+    </row>
+    <row r="516" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A516" s="122" t="s">
+        <v>635</v>
+      </c>
+      <c r="B516" s="103" t="s">
+        <v>39</v>
+      </c>
+      <c r="C516" s="112"/>
+      <c r="D516" s="104"/>
+      <c r="E516" s="105"/>
+      <c r="F516" s="61"/>
+    </row>
+    <row r="517" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A517" s="119" t="s">
+        <v>13</v>
+      </c>
+      <c r="B517" s="18" t="s">
+        <v>286</v>
+      </c>
+      <c r="C517" s="22" t="s">
+        <v>636</v>
+      </c>
+      <c r="D517" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="E517" s="34" t="s">
+        <v>637</v>
+      </c>
+      <c r="F517" s="17"/>
+    </row>
+    <row r="518" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A518" s="122" t="s">
+        <v>144</v>
+      </c>
+      <c r="B518" s="103" t="s">
+        <v>39</v>
+      </c>
+      <c r="C518" s="112"/>
+      <c r="D518" s="104"/>
+      <c r="E518" s="105"/>
+      <c r="F518" s="61"/>
+    </row>
+    <row r="519" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A519" s="119" t="s">
+        <v>13</v>
+      </c>
+      <c r="B519" s="18" t="s">
+        <v>286</v>
+      </c>
+      <c r="C519" s="22" t="s">
+        <v>379</v>
+      </c>
+      <c r="D519" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="E519" s="34">
+        <v>10986700</v>
+      </c>
+      <c r="F519" s="17"/>
+    </row>
+    <row r="520" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A520" s="119" t="s">
+        <v>41</v>
+      </c>
+      <c r="B520" s="18" t="s">
+        <v>286</v>
+      </c>
+      <c r="C520" s="22" t="s">
+        <v>638</v>
+      </c>
+      <c r="D520" s="17"/>
+      <c r="E520" s="41" t="s">
+        <v>234</v>
+      </c>
+      <c r="F520" s="17"/>
+    </row>
+    <row r="521" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A521" s="122" t="s">
+        <v>145</v>
+      </c>
+      <c r="B521" s="103" t="s">
+        <v>39</v>
+      </c>
+      <c r="C521" s="112"/>
+      <c r="D521" s="104"/>
+      <c r="E521" s="105"/>
+      <c r="F521" s="61"/>
+    </row>
+    <row r="522" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A522" s="119" t="s">
+        <v>66</v>
+      </c>
+      <c r="B522" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C522" s="22" t="s">
+        <v>380</v>
+      </c>
+      <c r="D522" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="E522" s="34" t="s">
+        <v>191</v>
+      </c>
+      <c r="F522" s="17"/>
+    </row>
+    <row r="523" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A523" s="122" t="s">
+        <v>146</v>
+      </c>
+      <c r="B523" s="103" t="s">
+        <v>39</v>
+      </c>
+      <c r="C523" s="112"/>
+      <c r="D523" s="104"/>
+      <c r="E523" s="105"/>
+      <c r="F523" s="61"/>
+    </row>
+    <row r="524" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A524" s="119" t="s">
+        <v>147</v>
+      </c>
+      <c r="B524" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C524" s="22" t="s">
+        <v>381</v>
+      </c>
+      <c r="D524" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="E524" s="34">
+        <v>9873242</v>
+      </c>
+      <c r="F524" s="17"/>
+    </row>
+    <row r="525" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A525" s="119" t="s">
+        <v>148</v>
+      </c>
+      <c r="B525" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C525" s="22" t="s">
+        <v>639</v>
+      </c>
+      <c r="D525" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="E525" s="34" t="s">
+        <v>236</v>
+      </c>
+      <c r="F525" s="17"/>
+    </row>
+    <row r="526" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A526" s="119" t="s">
+        <v>149</v>
+      </c>
+      <c r="B526" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C526" s="22" t="s">
+        <v>640</v>
+      </c>
+      <c r="D526" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="E526" s="34"/>
+      <c r="F526" s="17"/>
+    </row>
+    <row r="527" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A527" s="122" t="s">
+        <v>150</v>
+      </c>
+      <c r="B527" s="103" t="s">
+        <v>45</v>
+      </c>
+      <c r="C527" s="112" t="s">
+        <v>382</v>
+      </c>
+      <c r="D527" s="104"/>
+      <c r="E527" s="105"/>
+      <c r="F527" s="61"/>
+    </row>
+    <row r="528" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A528" s="119" t="s">
+        <v>13</v>
+      </c>
+      <c r="B528" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C528" s="22" t="s">
+        <v>641</v>
+      </c>
+      <c r="D528" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="E528" s="34" t="s">
+        <v>184</v>
+      </c>
+      <c r="F528" s="34"/>
+    </row>
+    <row r="529" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A529" s="119" t="s">
+        <v>114</v>
+      </c>
+      <c r="B529" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C529" s="22" t="s">
+        <v>392</v>
+      </c>
+      <c r="D529" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="E529" s="34">
+        <v>25</v>
+      </c>
+      <c r="F529" s="34"/>
+    </row>
+    <row r="530" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A530" s="124" t="s">
+        <v>69</v>
+      </c>
+      <c r="B530" s="106" t="s">
+        <v>45</v>
+      </c>
+      <c r="C530" s="113"/>
+      <c r="D530" s="107"/>
+      <c r="E530" s="108"/>
+      <c r="F530" s="67"/>
+    </row>
+    <row r="531" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A531" s="125" t="s">
+        <v>13</v>
+      </c>
+      <c r="B531" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C531" s="22" t="s">
+        <v>548</v>
+      </c>
+      <c r="D531" s="17"/>
+      <c r="E531" s="34" t="s">
+        <v>192</v>
+      </c>
+      <c r="F531" s="34"/>
+    </row>
+    <row r="532" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A532" s="122" t="s">
+        <v>151</v>
+      </c>
+      <c r="B532" s="103" t="s">
+        <v>39</v>
+      </c>
+      <c r="C532" s="112" t="s">
+        <v>152</v>
+      </c>
+      <c r="D532" s="104"/>
+      <c r="E532" s="105"/>
+      <c r="F532" s="61"/>
+    </row>
+    <row r="533" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A533" s="119" t="s">
+        <v>56</v>
+      </c>
+      <c r="B533" s="18" t="s">
+        <v>286</v>
+      </c>
+      <c r="C533" s="22" t="s">
+        <v>642</v>
+      </c>
+      <c r="D533" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="E533" s="34" t="s">
+        <v>644</v>
+      </c>
+      <c r="F533" s="34"/>
+    </row>
+    <row r="534" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A534" s="119" t="s">
+        <v>153</v>
+      </c>
+      <c r="B534" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C534" s="22" t="s">
+        <v>643</v>
+      </c>
+      <c r="D534" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="E534" s="34" t="s">
+        <v>645</v>
+      </c>
+      <c r="F534" s="34"/>
+    </row>
+    <row r="535" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A535" s="122" t="s">
+        <v>646</v>
+      </c>
+      <c r="B535" s="103" t="s">
+        <v>39</v>
+      </c>
+      <c r="C535" s="112" t="s">
+        <v>647</v>
+      </c>
+      <c r="D535" s="104"/>
+      <c r="E535" s="105"/>
+      <c r="F535" s="61"/>
+    </row>
+    <row r="536" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A536" s="119" t="s">
+        <v>648</v>
+      </c>
+      <c r="B536" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C536" s="22" t="s">
+        <v>653</v>
+      </c>
+      <c r="D536" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="E536" s="35">
+        <v>36161</v>
+      </c>
+      <c r="F536" s="34"/>
+    </row>
+    <row r="537" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A537" s="119" t="s">
+        <v>649</v>
+      </c>
+      <c r="B537" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C537" s="22" t="s">
+        <v>654</v>
+      </c>
+      <c r="D537" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="E537" s="35">
+        <v>36161</v>
+      </c>
+      <c r="F537" s="34"/>
+    </row>
+    <row r="538" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A538" s="119" t="s">
+        <v>650</v>
+      </c>
+      <c r="B538" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C538" s="22" t="s">
+        <v>655</v>
+      </c>
+      <c r="D538" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="E538" s="34">
+        <v>123456</v>
+      </c>
+      <c r="F538" s="34"/>
+    </row>
+    <row r="539" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A539" s="124" t="s">
+        <v>651</v>
+      </c>
+      <c r="B539" s="106" t="s">
+        <v>39</v>
+      </c>
+      <c r="C539" s="113"/>
+      <c r="D539" s="107"/>
+      <c r="E539" s="108"/>
+      <c r="F539" s="67"/>
+    </row>
+    <row r="540" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A540" s="119" t="s">
+        <v>652</v>
+      </c>
+      <c r="B540" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C540" s="22" t="s">
+        <v>656</v>
+      </c>
+      <c r="D540" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="E540" s="34" t="s">
+        <v>603</v>
+      </c>
+      <c r="F540" s="34"/>
+    </row>
+    <row r="541" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A541" s="119" t="s">
+        <v>664</v>
+      </c>
+      <c r="B541" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C541" s="22" t="s">
+        <v>665</v>
+      </c>
+      <c r="D541" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="E541" s="35">
+        <v>44562</v>
+      </c>
+      <c r="F541" s="34"/>
+    </row>
+    <row r="542" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A542" s="135" t="s">
+        <v>154</v>
+      </c>
+      <c r="B542" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="C542" s="57" t="s">
+        <v>155</v>
+      </c>
+      <c r="D542" s="23"/>
+      <c r="E542" s="36"/>
+      <c r="F542" s="36"/>
+    </row>
+    <row r="543" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A543" s="136" t="s">
+        <v>416</v>
+      </c>
+      <c r="B543" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C543" s="22" t="s">
+        <v>585</v>
+      </c>
+      <c r="D543" s="22"/>
+      <c r="E543" s="22"/>
+      <c r="F543" s="22"/>
+    </row>
+    <row r="544" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A544" s="117" t="s">
+        <v>156</v>
+      </c>
+      <c r="B544" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C544" s="22" t="s">
         <v>393</v>
       </c>
-      <c r="D511" s="17" t="s">
+      <c r="D544" s="17" t="s">
         <v>224</v>
       </c>
-      <c r="E511" s="34" t="s">
+      <c r="E544" s="34" t="s">
         <v>235</v>
       </c>
-      <c r="F511" s="34"/>
-    </row>
-    <row r="512" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A512" s="117" t="s">
+      <c r="F544" s="34"/>
+    </row>
+    <row r="545" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A545" s="117" t="s">
         <v>111</v>
       </c>
-      <c r="B512" s="18" t="s">
+      <c r="B545" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="C512" s="22" t="s">
+      <c r="C545" s="22" t="s">
         <v>657</v>
       </c>
-      <c r="D512" s="17" t="s">
+      <c r="D545" s="17" t="s">
         <v>164</v>
       </c>
-      <c r="E512" s="34" t="s">
+      <c r="E545" s="34" t="s">
         <v>225</v>
       </c>
-      <c r="F512" s="34"/>
-    </row>
-    <row r="513" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A513" s="117" t="s">
+      <c r="F545" s="34"/>
+    </row>
+    <row r="546" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A546" s="117" t="s">
         <v>157</v>
       </c>
-      <c r="B513" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="C513" s="22" t="s">
+      <c r="B546" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C546" s="22" t="s">
         <v>158</v>
       </c>
-      <c r="D513" s="17" t="s">
+      <c r="D546" s="17" t="s">
         <v>230</v>
       </c>
-      <c r="E513" s="34">
+      <c r="E546" s="34">
         <v>1</v>
       </c>
-      <c r="F513" s="34"/>
-    </row>
-    <row r="514" spans="1:6" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A514" s="117" t="s">
+      <c r="F546" s="34"/>
+    </row>
+    <row r="547" spans="1:6" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A547" s="117" t="s">
         <v>134</v>
       </c>
-      <c r="B514" s="18" t="s">
+      <c r="B547" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="C514" s="22" t="s">
+      <c r="C547" s="22" t="s">
         <v>658</v>
       </c>
-      <c r="D514" s="17"/>
-      <c r="E514" s="34" t="s">
+      <c r="D547" s="17"/>
+      <c r="E547" s="34" t="s">
         <v>231</v>
       </c>
-      <c r="F514" s="34"/>
-    </row>
-    <row r="515" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A515" s="122" t="s">
+      <c r="F547" s="34"/>
+    </row>
+    <row r="548" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A548" s="122" t="s">
         <v>104</v>
       </c>
-      <c r="B515" s="103" t="s">
+      <c r="B548" s="103" t="s">
         <v>283</v>
       </c>
-      <c r="C515" s="112" t="s">
+      <c r="C548" s="112" t="s">
         <v>691</v>
       </c>
-      <c r="D515" s="104"/>
-      <c r="E515" s="105"/>
-      <c r="F515" s="61"/>
-    </row>
-    <row r="516" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A516" s="119" t="s">
+      <c r="D548" s="104"/>
+      <c r="E548" s="105"/>
+      <c r="F548" s="61"/>
+    </row>
+    <row r="549" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A549" s="119" t="s">
         <v>105</v>
       </c>
-      <c r="B516" s="18" t="s">
+      <c r="B549" s="18" t="s">
         <v>283</v>
       </c>
-      <c r="C516" s="22" t="s">
+      <c r="C549" s="22" t="s">
         <v>659</v>
       </c>
-      <c r="D516" s="17" t="s">
+      <c r="D549" s="17" t="s">
         <v>164</v>
       </c>
-      <c r="E516" s="22" t="s">
+      <c r="E549" s="22" t="s">
         <v>622</v>
       </c>
-      <c r="F516" s="17" t="s">
+      <c r="F549" s="17" t="s">
         <v>622</v>
       </c>
     </row>
-    <row r="517" spans="1:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="A517" s="119" t="s">
+    <row r="550" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A550" s="119" t="s">
         <v>109</v>
       </c>
-      <c r="B517" s="18" t="s">
+      <c r="B550" s="18" t="s">
         <v>285</v>
       </c>
-      <c r="C517" s="22" t="s">
+      <c r="C550" s="22" t="s">
         <v>660</v>
       </c>
-      <c r="D517" s="17" t="s">
+      <c r="D550" s="17" t="s">
         <v>224</v>
       </c>
-      <c r="E517" s="34" t="s">
+      <c r="E550" s="34" t="s">
         <v>248</v>
       </c>
-      <c r="F517" s="17"/>
-    </row>
-    <row r="518" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A518" s="119" t="s">
+      <c r="F550" s="17"/>
+    </row>
+    <row r="551" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A551" s="119" t="s">
         <v>111</v>
       </c>
-      <c r="B518" s="18" t="s">
+      <c r="B551" s="18" t="s">
         <v>285</v>
       </c>
-      <c r="C518" s="22" t="s">
+      <c r="C551" s="22" t="s">
         <v>661</v>
       </c>
-      <c r="D518" s="17" t="s">
+      <c r="D551" s="17" t="s">
         <v>164</v>
       </c>
-      <c r="E518" s="34" t="s">
+      <c r="E551" s="34" t="s">
         <v>225</v>
       </c>
-      <c r="F518" s="17"/>
-    </row>
-    <row r="519" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A519" s="119" t="s">
+      <c r="F551" s="17"/>
+    </row>
+    <row r="552" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A552" s="119" t="s">
         <v>112</v>
       </c>
-      <c r="B519" s="18" t="s">
+      <c r="B552" s="18" t="s">
         <v>283</v>
       </c>
-      <c r="C519" s="22" t="s">
+      <c r="C552" s="22" t="s">
         <v>662</v>
       </c>
-      <c r="D519" s="17" t="s">
+      <c r="D552" s="17" t="s">
         <v>224</v>
       </c>
-      <c r="E519" s="34" t="s">
+      <c r="E552" s="34" t="s">
         <v>250</v>
       </c>
-      <c r="F519" s="17"/>
-    </row>
-    <row r="520" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A520" s="119" t="s">
+      <c r="F552" s="17"/>
+    </row>
+    <row r="553" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A553" s="119" t="s">
         <v>111</v>
       </c>
-      <c r="B520" s="18" t="s">
+      <c r="B553" s="18" t="s">
         <v>285</v>
       </c>
-      <c r="C520" s="22" t="s">
+      <c r="C553" s="22" t="s">
         <v>663</v>
       </c>
-      <c r="D520" s="17" t="s">
+      <c r="D553" s="17" t="s">
         <v>164</v>
       </c>
-      <c r="E520" s="34" t="s">
+      <c r="E553" s="34" t="s">
         <v>225</v>
       </c>
-      <c r="F520" s="17"/>
+      <c r="F553" s="17"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F520" xr:uid="{FDB56CEA-A5F9-42A4-9956-612B841F9EA3}"/>
+  <autoFilter ref="A1:F553" xr:uid="{FDB56CEA-A5F9-42A4-9956-612B841F9EA3}"/>
   <hyperlinks>
     <hyperlink ref="E144" r:id="rId1" xr:uid="{DC86665A-695B-47C7-A818-F422C1F11636}"/>
     <hyperlink ref="A3" r:id="rId2" location="_extublextensions" xr:uid="{9531FFDF-372C-4676-833B-DAB9A8A93F85}"/>
@@ -12682,32 +13273,34 @@
     <hyperlink ref="A339" r:id="rId35" location="_cacallowancecharge" xr:uid="{80D22635-8F22-45B1-8C34-1716E9E26DE8}"/>
     <hyperlink ref="A359" r:id="rId36" location="_cactaxexchangerate" xr:uid="{BCD141C2-4004-4CBB-B0BC-78234B52536F}"/>
     <hyperlink ref="A365" r:id="rId37" location="_cactaxtotal" xr:uid="{F590367A-A414-4836-B877-B45CAAC6831A}"/>
-    <hyperlink ref="A382" r:id="rId38" location="_caclegalmonetarytotal" xr:uid="{8210054B-4866-4E0B-927B-112720F5333A}"/>
-    <hyperlink ref="A400" r:id="rId39" location="_cacinvoiceline" xr:uid="{3369C0DE-B96E-467C-ACCE-5A15AF093960}"/>
-    <hyperlink ref="A401" r:id="rId40" location="line-extension" xr:uid="{B0885766-A5C8-4695-92B2-C7145CD1F1E9}"/>
-    <hyperlink ref="A402" r:id="rId41" location="_cbcid_2" xr:uid="{71781B25-853D-4EFB-8F44-A9D3625850D0}"/>
-    <hyperlink ref="A403" r:id="rId42" location="_cbcnote_2" xr:uid="{98D33551-D2FB-41A5-A4E1-AEE90E145BA9}"/>
-    <hyperlink ref="A404" r:id="rId43" location="_cbcinvoicedquantity" xr:uid="{87EF7BBA-1B13-4007-9095-8AE85F5F1008}"/>
-    <hyperlink ref="A406" r:id="rId44" location="_cbclineextensionamount" xr:uid="{D40231D1-E253-47C4-B5B9-B84EB5F6F50F}"/>
-    <hyperlink ref="A408" r:id="rId45" location="_cbcaccountingcost_2" xr:uid="{309B2CF2-FC9E-489D-8994-EB8FAC53C8FC}"/>
-    <hyperlink ref="A409" r:id="rId46" location="_cacinvoiceperiod_2" xr:uid="{A9EFAE24-A87A-48DF-9825-6EAE0A819597}"/>
-    <hyperlink ref="A412" r:id="rId47" location="_cacorderlinereference" xr:uid="{EA537A80-55AC-4040-AC1B-EAAE9B5C5833}"/>
-    <hyperlink ref="A413" r:id="rId48" location="line-extension" xr:uid="{43385FB3-6E8C-479C-90A3-4E2457151E6A}"/>
-    <hyperlink ref="A420" r:id="rId49" location="_cacdespatchlinereference" xr:uid="{5CA189E3-27B9-45A0-9E5C-68E190ECD76F}"/>
-    <hyperlink ref="A425" r:id="rId50" location="_cacdocumentreference" xr:uid="{A19B217D-77E4-425F-BDA5-5DF30BE8056A}"/>
-    <hyperlink ref="A431" r:id="rId51" location="_cacdelivery_2" xr:uid="{282BE4F7-2F74-4307-BEA0-8B99B6D0D072}"/>
-    <hyperlink ref="A450" r:id="rId52" location="_cacallowancecharge_2" xr:uid="{BBB5AC6A-295D-4CC8-9AB0-23254C334669}"/>
-    <hyperlink ref="A459" r:id="rId53" location="_cactaxtotal_2" xr:uid="{B39E2A67-C6B0-4C2A-BCB9-6F069B44CAE2}"/>
-    <hyperlink ref="A475" r:id="rId54" location="_cacitem" xr:uid="{B64D9D45-3490-4FEE-9419-FD0CA5A56103}"/>
-    <hyperlink ref="A476" r:id="rId55" location="_item" xr:uid="{6A80D8B8-C919-4E6A-BA08-40D3A5648119}"/>
-    <hyperlink ref="A509" r:id="rId56" location="_cacprice" xr:uid="{3BB354D5-3D7E-483C-A9EF-D83745606B59}"/>
-    <hyperlink ref="A510" r:id="rId57" location="_price" xr:uid="{F00AB999-534C-4AB0-AEB7-47167B304468}"/>
-    <hyperlink ref="A515" r:id="rId58" location="_cacallowancecharge_2" xr:uid="{EE4A92E6-5BEF-42BB-95BF-9A7B00B36F90}"/>
+    <hyperlink ref="A399" r:id="rId38" location="_caclegalmonetarytotal" xr:uid="{8210054B-4866-4E0B-927B-112720F5333A}"/>
+    <hyperlink ref="A417" r:id="rId39" location="_cacinvoiceline" xr:uid="{3369C0DE-B96E-467C-ACCE-5A15AF093960}"/>
+    <hyperlink ref="A418" r:id="rId40" location="line-extension" xr:uid="{B0885766-A5C8-4695-92B2-C7145CD1F1E9}"/>
+    <hyperlink ref="A419" r:id="rId41" location="_cbcid_2" xr:uid="{71781B25-853D-4EFB-8F44-A9D3625850D0}"/>
+    <hyperlink ref="A420" r:id="rId42" location="_cbcnote_2" xr:uid="{98D33551-D2FB-41A5-A4E1-AEE90E145BA9}"/>
+    <hyperlink ref="A421" r:id="rId43" location="_cbcinvoicedquantity" xr:uid="{87EF7BBA-1B13-4007-9095-8AE85F5F1008}"/>
+    <hyperlink ref="A423" r:id="rId44" location="_cbclineextensionamount" xr:uid="{D40231D1-E253-47C4-B5B9-B84EB5F6F50F}"/>
+    <hyperlink ref="A425" r:id="rId45" location="_cbcaccountingcost_2" xr:uid="{309B2CF2-FC9E-489D-8994-EB8FAC53C8FC}"/>
+    <hyperlink ref="A426" r:id="rId46" location="_cacinvoiceperiod_2" xr:uid="{A9EFAE24-A87A-48DF-9825-6EAE0A819597}"/>
+    <hyperlink ref="A429" r:id="rId47" location="_cacorderlinereference" xr:uid="{EA537A80-55AC-4040-AC1B-EAAE9B5C5833}"/>
+    <hyperlink ref="A430" r:id="rId48" location="line-extension" xr:uid="{43385FB3-6E8C-479C-90A3-4E2457151E6A}"/>
+    <hyperlink ref="A437" r:id="rId49" location="_cacdespatchlinereference" xr:uid="{5CA189E3-27B9-45A0-9E5C-68E190ECD76F}"/>
+    <hyperlink ref="A442" r:id="rId50" location="_cacdocumentreference" xr:uid="{A19B217D-77E4-425F-BDA5-5DF30BE8056A}"/>
+    <hyperlink ref="A448" r:id="rId51" location="_cacdelivery_2" xr:uid="{282BE4F7-2F74-4307-BEA0-8B99B6D0D072}"/>
+    <hyperlink ref="A467" r:id="rId52" location="_cacallowancecharge_2" xr:uid="{BBB5AC6A-295D-4CC8-9AB0-23254C334669}"/>
+    <hyperlink ref="A476" r:id="rId53" location="_cactaxtotal_2" xr:uid="{B39E2A67-C6B0-4C2A-BCB9-6F069B44CAE2}"/>
+    <hyperlink ref="A508" r:id="rId54" location="_cacitem" xr:uid="{B64D9D45-3490-4FEE-9419-FD0CA5A56103}"/>
+    <hyperlink ref="A509" r:id="rId55" location="_item" xr:uid="{6A80D8B8-C919-4E6A-BA08-40D3A5648119}"/>
+    <hyperlink ref="A542" r:id="rId56" location="_cacprice" xr:uid="{3BB354D5-3D7E-483C-A9EF-D83745606B59}"/>
+    <hyperlink ref="A543" r:id="rId57" location="_price" xr:uid="{F00AB999-534C-4AB0-AEB7-47167B304468}"/>
+    <hyperlink ref="A548" r:id="rId58" location="_cacallowancecharge_2" xr:uid="{EE4A92E6-5BEF-42BB-95BF-9A7B00B36F90}"/>
     <hyperlink ref="A335" r:id="rId59" location="_cacprepaidpayment" display="https://pagero.github.io/puf-billing/ - _cacprepaidpayment" xr:uid="{93904BDA-31E1-4B82-992D-F6F1FD7C9DE7}"/>
     <hyperlink ref="E284" r:id="rId60" xr:uid="{96DE9CC8-A74C-4283-88B5-21C225678470}"/>
+    <hyperlink ref="A382" r:id="rId61" location="_cactaxtotal" display="cac:TaxTotal" xr:uid="{79A56161-FFCF-47DC-AAC8-B1C196070793}"/>
+    <hyperlink ref="A492" r:id="rId62" location="_cactaxtotal_2" display="cac:TaxTotal" xr:uid="{A9EB48A3-FB05-44E0-8DD1-5609C8ACE462}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId61"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId63"/>
 </worksheet>
 </file>
 
@@ -12998,6 +13591,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008296D2E9439BF946A1501D3A497E974E" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9a8df56671683c60572e05043457fa7c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="222206e9-2590-4389-ac08-92b39e79291a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7a8e40c0b678fce4b7614ca76454760e" ns2:_="">
     <xsd:import namespace="222206e9-2590-4389-ac08-92b39e79291a"/>
@@ -13143,35 +13751,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58840883-6350-4B75-8993-54B5916E5251}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97BB75A6-1832-49A3-9C38-BF9FC8430A95}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="222206e9-2590-4389-ac08-92b39e79291a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -13193,9 +13776,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97BB75A6-1832-49A3-9C38-BF9FC8430A95}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58840883-6350-4B75-8993-54B5916E5251}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="222206e9-2590-4389-ac08-92b39e79291a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
1131621 - PUF excel specification - Update withholdingtaxtotal to optional
</commit_message>
<xml_diff>
--- a/specification/excel/Pagero Universal Format.xlsx
+++ b/specification/excel/Pagero Universal Format.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\development\format\puf-billing\specification\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EFF16C2-08BD-4C44-9345-E6BA623977AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7388564-3F19-48DB-815F-9738C3357B16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="54495" yWindow="-5250" windowWidth="26010" windowHeight="20985" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-5370" windowWidth="51840" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="8" r:id="rId1"/>
@@ -3519,12 +3519,6 @@
       <alignment horizontal="left" wrapText="1" indent="2"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
       <protection hidden="1"/>
@@ -3534,6 +3528,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -4056,46 +4056,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="137" t="s">
+      <c r="A1" s="140" t="s">
         <v>397</v>
       </c>
-      <c r="B1" s="137"/>
-      <c r="C1" s="137"/>
-      <c r="D1" s="137"/>
-      <c r="E1" s="137"/>
-      <c r="F1" s="137"/>
-      <c r="G1" s="137"/>
-      <c r="H1" s="137"/>
+      <c r="B1" s="140"/>
+      <c r="C1" s="140"/>
+      <c r="D1" s="140"/>
+      <c r="E1" s="140"/>
+      <c r="F1" s="140"/>
+      <c r="G1" s="140"/>
+      <c r="H1" s="140"/>
     </row>
     <row r="2" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="137"/>
-      <c r="B2" s="137"/>
-      <c r="C2" s="137"/>
-      <c r="D2" s="137"/>
-      <c r="E2" s="137"/>
-      <c r="F2" s="137"/>
-      <c r="G2" s="137"/>
-      <c r="H2" s="137"/>
+      <c r="A2" s="140"/>
+      <c r="B2" s="140"/>
+      <c r="C2" s="140"/>
+      <c r="D2" s="140"/>
+      <c r="E2" s="140"/>
+      <c r="F2" s="140"/>
+      <c r="G2" s="140"/>
+      <c r="H2" s="140"/>
     </row>
     <row r="3" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="137"/>
-      <c r="B3" s="137"/>
-      <c r="C3" s="137"/>
-      <c r="D3" s="137"/>
-      <c r="E3" s="137"/>
-      <c r="F3" s="137"/>
-      <c r="G3" s="137"/>
-      <c r="H3" s="137"/>
+      <c r="A3" s="140"/>
+      <c r="B3" s="140"/>
+      <c r="C3" s="140"/>
+      <c r="D3" s="140"/>
+      <c r="E3" s="140"/>
+      <c r="F3" s="140"/>
+      <c r="G3" s="140"/>
+      <c r="H3" s="140"/>
     </row>
     <row r="4" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="138"/>
-      <c r="B4" s="138"/>
-      <c r="C4" s="138"/>
-      <c r="D4" s="138"/>
-      <c r="E4" s="138"/>
-      <c r="F4" s="138"/>
-      <c r="G4" s="138"/>
-      <c r="H4" s="138"/>
+      <c r="A4" s="141"/>
+      <c r="B4" s="141"/>
+      <c r="C4" s="141"/>
+      <c r="D4" s="141"/>
+      <c r="E4" s="141"/>
+      <c r="F4" s="141"/>
+      <c r="G4" s="141"/>
+      <c r="H4" s="141"/>
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.4">
       <c r="A5" s="73"/>
@@ -4159,8 +4159,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDB56CEA-A5F9-42A4-9956-612B841F9EA3}">
   <dimension ref="A1:F553"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A479" workbookViewId="0">
-      <selection activeCell="A501" sqref="A501"/>
+    <sheetView tabSelected="1" topLeftCell="A471" workbookViewId="0">
+      <selection activeCell="B492" sqref="B492"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -10385,7 +10385,7 @@
         <v>738</v>
       </c>
       <c r="B382" s="62" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C382" s="28" t="s">
         <v>712</v>
@@ -10431,18 +10431,18 @@
       <c r="F384" s="17"/>
     </row>
     <row r="385" spans="1:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="A385" s="139" t="s">
+      <c r="A385" s="137" t="s">
         <v>117</v>
       </c>
-      <c r="B385" s="140" t="s">
+      <c r="B385" s="138" t="s">
         <v>45</v>
       </c>
       <c r="C385" s="57" t="s">
         <v>741</v>
       </c>
       <c r="D385" s="58"/>
-      <c r="E385" s="141"/>
-      <c r="F385" s="141"/>
+      <c r="E385" s="139"/>
+      <c r="F385" s="139"/>
     </row>
     <row r="386" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A386" s="117" t="s">
@@ -12230,15 +12230,15 @@
       <c r="F491" s="17"/>
     </row>
     <row r="492" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A492" s="141" t="s">
+      <c r="A492" s="139" t="s">
         <v>738</v>
       </c>
-      <c r="B492" s="140" t="s">
-        <v>45</v>
+      <c r="B492" s="138" t="s">
+        <v>39</v>
       </c>
       <c r="C492" s="57"/>
       <c r="D492" s="58"/>
-      <c r="E492" s="141"/>
+      <c r="E492" s="139"/>
       <c r="F492" s="58"/>
     </row>
     <row r="493" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
@@ -13591,21 +13591,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008296D2E9439BF946A1501D3A497E974E" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9a8df56671683c60572e05043457fa7c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="222206e9-2590-4389-ac08-92b39e79291a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7a8e40c0b678fce4b7614ca76454760e" ns2:_="">
     <xsd:import namespace="222206e9-2590-4389-ac08-92b39e79291a"/>
@@ -13751,10 +13736,35 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97BB75A6-1832-49A3-9C38-BF9FC8430A95}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58840883-6350-4B75-8993-54B5916E5251}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="222206e9-2590-4389-ac08-92b39e79291a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -13776,19 +13786,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58840883-6350-4B75-8993-54B5916E5251}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97BB75A6-1832-49A3-9C38-BF9FC8430A95}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="222206e9-2590-4389-ac08-92b39e79291a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
1612400 - PUF Excel Specification - Add withholding amount for credit invoices.
</commit_message>
<xml_diff>
--- a/specification/excel/Pagero Universal Format.xlsx
+++ b/specification/excel/Pagero Universal Format.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\development\puf-billing\specification\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\development\format\puf-billing\specification\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{535AC171-E03B-444D-BF6F-CE7C09022044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AB015E4-FCB2-4978-8B2A-7409EAD0349E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7185" yWindow="315" windowWidth="31500" windowHeight="19380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="6" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4682" uniqueCount="866">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4755" uniqueCount="867">
   <si>
     <t>Comments</t>
   </si>
@@ -3154,6 +3154,9 @@
   </si>
   <si>
     <t>cbc:WebsiteURI</t>
+  </si>
+  <si>
+    <t>Added withholding amount for credit</t>
   </si>
 </sst>
 </file>
@@ -3763,7 +3766,7 @@
     <cellStyle name="Pagero Green" xfId="2" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
     <cellStyle name="Pagero Grey" xfId="9" xr:uid="{1C805717-4869-43EB-8A4F-0A7959EA5D60}"/>
     <cellStyle name="Pagero Light Green" xfId="8" xr:uid="{69640978-6259-4509-B932-3F75A4F5FBA6}"/>
-    <cellStyle name="Percent" xfId="10" builtinId="5"/>
+    <cellStyle name="Per cent" xfId="10" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -4135,8 +4138,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:E47"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4306,8 +4309,12 @@
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B38" s="20"/>
-      <c r="C38" s="16"/>
+      <c r="B38" s="20">
+        <v>45866</v>
+      </c>
+      <c r="C38" s="16" t="s">
+        <v>866</v>
+      </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B39" s="20"/>
@@ -4362,8 +4369,8 @@
   <dimension ref="A1:E586"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A67" sqref="A67:XFD67"/>
+      <pane ySplit="2" topLeftCell="A412" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A415" sqref="A415:XFD431"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -13448,10 +13455,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41A28953-D494-4CBC-9080-60B98492A541}">
-  <dimension ref="A1:E550"/>
+  <dimension ref="A1:E567"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="E64" sqref="E64"/>
+    <sheetView topLeftCell="A410" workbookViewId="0">
+      <selection activeCell="F407" sqref="F407"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -19806,2174 +19813,2439 @@
         <v>549</v>
       </c>
     </row>
-    <row r="412" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="412" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A412" s="33" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B412" s="37" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="C412" s="34" t="s">
-        <v>854</v>
+        <v>497</v>
       </c>
       <c r="D412" s="33"/>
       <c r="E412" s="40"/>
     </row>
-    <row r="413" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="413" spans="1:5" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A413" s="65" t="s">
+        <v>171</v>
+      </c>
+      <c r="B413" s="36" t="s">
+        <v>720</v>
+      </c>
+      <c r="C413" s="22" t="s">
+        <v>576</v>
+      </c>
+      <c r="D413" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E413" s="28" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="414" spans="1:5" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A414" s="66" t="s">
+        <v>822</v>
+      </c>
+      <c r="B414" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C414" s="24" t="s">
+        <v>577</v>
+      </c>
+      <c r="D414" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="E414" s="28" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="415" spans="1:5" s="2" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A415" s="68" t="s">
+        <v>178</v>
+      </c>
+      <c r="B415" s="50" t="s">
+        <v>719</v>
+      </c>
+      <c r="C415" s="60" t="s">
+        <v>716</v>
+      </c>
+      <c r="D415" s="57"/>
+      <c r="E415" s="58"/>
+    </row>
+    <row r="416" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A416" s="66" t="s">
         <v>21</v>
       </c>
-      <c r="B413" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C413" s="22" t="s">
-        <v>226</v>
-      </c>
-      <c r="D413" s="22"/>
-      <c r="E413" s="27"/>
-    </row>
-    <row r="414" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A414" s="65" t="s">
-        <v>183</v>
-      </c>
-      <c r="B414" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C414" s="22" t="s">
-        <v>582</v>
-      </c>
-      <c r="D414" s="16" t="s">
+      <c r="B416" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C416" s="22" t="s">
+        <v>578</v>
+      </c>
+      <c r="D416" s="22"/>
+      <c r="E416" s="27"/>
+    </row>
+    <row r="417" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A417" s="66" t="s">
+        <v>179</v>
+      </c>
+      <c r="B417" s="36" t="s">
+        <v>720</v>
+      </c>
+      <c r="C417" s="22" t="s">
+        <v>579</v>
+      </c>
+      <c r="D417" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E414" s="30" t="s">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="415" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A415" s="66" t="s">
+      <c r="E417" s="27" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="418" spans="1:5" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A418" s="71" t="s">
         <v>822</v>
       </c>
-      <c r="B415" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C415" s="22" t="s">
-        <v>584</v>
-      </c>
-      <c r="D415" s="16" t="s">
+      <c r="B418" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C418" s="24" t="s">
+        <v>567</v>
+      </c>
+      <c r="D418" s="16" t="s">
         <v>234</v>
       </c>
-      <c r="E415" s="28" t="s">
+      <c r="E418" s="27" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="416" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A416" s="65" t="s">
-        <v>184</v>
-      </c>
-      <c r="B416" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C416" s="22" t="s">
-        <v>855</v>
-      </c>
-      <c r="D416" s="16" t="s">
+    <row r="419" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A419" s="66" t="s">
+        <v>171</v>
+      </c>
+      <c r="B419" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C419" s="22" t="s">
+        <v>568</v>
+      </c>
+      <c r="D419" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E416" s="30" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="417" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A417" s="66" t="s">
+      <c r="E419" s="27" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="420" spans="1:5" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A420" s="71" t="s">
         <v>822</v>
       </c>
-      <c r="B417" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C417" s="22" t="s">
-        <v>831</v>
-      </c>
-      <c r="D417" s="16" t="s">
+      <c r="B420" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C420" s="24" t="s">
+        <v>569</v>
+      </c>
+      <c r="D420" s="16" t="s">
         <v>234</v>
       </c>
-      <c r="E417" s="28" t="s">
+      <c r="E420" s="28" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="418" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A418" s="65" t="s">
-        <v>185</v>
-      </c>
-      <c r="B418" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C418" s="22" t="s">
-        <v>856</v>
-      </c>
-      <c r="D418" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="E418" s="30" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="419" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A419" s="66" t="s">
-        <v>822</v>
-      </c>
-      <c r="B419" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C419" s="22" t="s">
-        <v>832</v>
-      </c>
-      <c r="D419" s="16" t="s">
+    <row r="421" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A421" s="70" t="s">
+        <v>166</v>
+      </c>
+      <c r="B421" s="50" t="s">
+        <v>720</v>
+      </c>
+      <c r="C421" s="60"/>
+      <c r="D421" s="57"/>
+      <c r="E421" s="58"/>
+    </row>
+    <row r="422" spans="1:5" s="2" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A422" s="71" t="s">
+        <v>24</v>
+      </c>
+      <c r="B422" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C422" s="22" t="s">
+        <v>580</v>
+      </c>
+      <c r="D422" s="16" t="s">
         <v>234</v>
       </c>
-      <c r="E419" s="28" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="420" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A420" s="65" t="s">
-        <v>186</v>
-      </c>
-      <c r="B420" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C420" s="22" t="s">
-        <v>829</v>
-      </c>
-      <c r="D420" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="E420" s="28" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="421" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A421" s="66" t="s">
-        <v>822</v>
-      </c>
-      <c r="B421" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C421" s="22" t="s">
-        <v>593</v>
-      </c>
-      <c r="D421" s="16" t="s">
-        <v>234</v>
-      </c>
-      <c r="E421" s="28" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="422" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A422" s="65" t="s">
-        <v>187</v>
-      </c>
-      <c r="B422" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C422" s="22" t="s">
-        <v>830</v>
-      </c>
-      <c r="D422" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="E422" s="30" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="423" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A423" s="66" t="s">
-        <v>822</v>
+      <c r="E422" s="28" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="423" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A423" s="71" t="s">
+        <v>167</v>
       </c>
       <c r="B423" s="36" t="s">
         <v>719</v>
       </c>
       <c r="C423" s="22" t="s">
-        <v>596</v>
+        <v>571</v>
       </c>
       <c r="D423" s="16" t="s">
-        <v>234</v>
-      </c>
-      <c r="E423" s="28" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="424" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A424" s="65" t="s">
-        <v>188</v>
+        <v>535</v>
+      </c>
+      <c r="E423" s="28">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="424" spans="1:5" s="2" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A424" s="71" t="s">
+        <v>168</v>
       </c>
       <c r="B424" s="36" t="s">
         <v>719</v>
       </c>
       <c r="C424" s="22" t="s">
-        <v>597</v>
+        <v>572</v>
       </c>
       <c r="D424" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="E424" s="30" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="425" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A425" s="66" t="s">
-        <v>822</v>
+        <v>230</v>
+      </c>
+      <c r="E424" s="28" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="425" spans="1:5" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A425" s="71" t="s">
+        <v>180</v>
       </c>
       <c r="B425" s="36" t="s">
         <v>719</v>
       </c>
       <c r="C425" s="22" t="s">
-        <v>599</v>
+        <v>574</v>
       </c>
       <c r="D425" s="16" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="E425" s="28" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="426" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A426" s="65" t="s">
-        <v>189</v>
-      </c>
-      <c r="B426" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C426" s="22" t="s">
-        <v>600</v>
-      </c>
-      <c r="D426" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="E426" s="30" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="427" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A427" s="66" t="s">
-        <v>822</v>
+        <v>575</v>
+      </c>
+    </row>
+    <row r="426" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A426" s="73" t="s">
+        <v>75</v>
+      </c>
+      <c r="B426" s="50" t="s">
+        <v>720</v>
+      </c>
+      <c r="C426" s="60"/>
+      <c r="D426" s="57"/>
+      <c r="E426" s="58"/>
+    </row>
+    <row r="427" spans="1:5" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A427" s="72" t="s">
+        <v>24</v>
       </c>
       <c r="B427" s="36" t="s">
         <v>719</v>
       </c>
       <c r="C427" s="22" t="s">
-        <v>601</v>
+        <v>547</v>
       </c>
       <c r="D427" s="16" t="s">
         <v>234</v>
       </c>
-      <c r="E427" s="28" t="s">
+      <c r="E427" s="27" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="428" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A428" s="72" t="s">
+        <v>57</v>
+      </c>
+      <c r="B428" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C428" s="22" t="s">
+        <v>548</v>
+      </c>
+      <c r="D428" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="E428" s="27" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="429" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A429" s="33" t="s">
+        <v>182</v>
+      </c>
+      <c r="B429" s="37" t="s">
+        <v>720</v>
+      </c>
+      <c r="C429" s="34" t="s">
+        <v>854</v>
+      </c>
+      <c r="D429" s="33"/>
+      <c r="E429" s="40"/>
+    </row>
+    <row r="430" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A430" s="65" t="s">
+        <v>21</v>
+      </c>
+      <c r="B430" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C430" s="22" t="s">
+        <v>226</v>
+      </c>
+      <c r="D430" s="22"/>
+      <c r="E430" s="27"/>
+    </row>
+    <row r="431" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A431" s="65" t="s">
+        <v>183</v>
+      </c>
+      <c r="B431" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C431" s="22" t="s">
+        <v>582</v>
+      </c>
+      <c r="D431" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E431" s="30" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="432" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A432" s="66" t="s">
+        <v>822</v>
+      </c>
+      <c r="B432" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C432" s="22" t="s">
+        <v>584</v>
+      </c>
+      <c r="D432" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="E432" s="28" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="428" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A428" s="65" t="s">
+    <row r="433" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A433" s="65" t="s">
+        <v>184</v>
+      </c>
+      <c r="B433" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C433" s="22" t="s">
+        <v>855</v>
+      </c>
+      <c r="D433" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E433" s="30" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="434" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A434" s="66" t="s">
+        <v>822</v>
+      </c>
+      <c r="B434" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C434" s="22" t="s">
+        <v>831</v>
+      </c>
+      <c r="D434" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="E434" s="28" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="435" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A435" s="65" t="s">
+        <v>185</v>
+      </c>
+      <c r="B435" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C435" s="22" t="s">
+        <v>856</v>
+      </c>
+      <c r="D435" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E435" s="30" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="436" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A436" s="66" t="s">
+        <v>822</v>
+      </c>
+      <c r="B436" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C436" s="22" t="s">
+        <v>832</v>
+      </c>
+      <c r="D436" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="E436" s="28" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="437" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A437" s="65" t="s">
+        <v>186</v>
+      </c>
+      <c r="B437" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C437" s="22" t="s">
+        <v>829</v>
+      </c>
+      <c r="D437" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E437" s="28" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="438" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A438" s="66" t="s">
+        <v>822</v>
+      </c>
+      <c r="B438" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C438" s="22" t="s">
+        <v>593</v>
+      </c>
+      <c r="D438" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="E438" s="28" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="439" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A439" s="65" t="s">
+        <v>187</v>
+      </c>
+      <c r="B439" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C439" s="22" t="s">
+        <v>830</v>
+      </c>
+      <c r="D439" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E439" s="30" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="440" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A440" s="66" t="s">
+        <v>822</v>
+      </c>
+      <c r="B440" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C440" s="22" t="s">
+        <v>596</v>
+      </c>
+      <c r="D440" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="E440" s="28" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="441" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A441" s="65" t="s">
+        <v>188</v>
+      </c>
+      <c r="B441" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C441" s="22" t="s">
+        <v>597</v>
+      </c>
+      <c r="D441" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E441" s="30" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="442" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A442" s="66" t="s">
+        <v>822</v>
+      </c>
+      <c r="B442" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C442" s="22" t="s">
+        <v>599</v>
+      </c>
+      <c r="D442" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="E442" s="28" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="443" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A443" s="65" t="s">
+        <v>189</v>
+      </c>
+      <c r="B443" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C443" s="22" t="s">
+        <v>600</v>
+      </c>
+      <c r="D443" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E443" s="30" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="444" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A444" s="66" t="s">
+        <v>822</v>
+      </c>
+      <c r="B444" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C444" s="22" t="s">
+        <v>601</v>
+      </c>
+      <c r="D444" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="E444" s="28" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="445" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A445" s="65" t="s">
         <v>190</v>
       </c>
-      <c r="B428" s="36" t="s">
+      <c r="B445" s="36" t="s">
         <v>720</v>
       </c>
-      <c r="C428" s="22" t="s">
+      <c r="C445" s="22" t="s">
         <v>828</v>
       </c>
-      <c r="D428" s="16" t="s">
+      <c r="D445" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E428" s="30" t="s">
+      <c r="E445" s="30" t="s">
         <v>603</v>
       </c>
     </row>
-    <row r="429" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A429" s="66" t="s">
+    <row r="446" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A446" s="66" t="s">
         <v>822</v>
       </c>
-      <c r="B429" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C429" s="22" t="s">
+      <c r="B446" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C446" s="22" t="s">
         <v>604</v>
       </c>
-      <c r="D429" s="16" t="s">
+      <c r="D446" s="16" t="s">
         <v>234</v>
       </c>
-      <c r="E429" s="28" t="s">
+      <c r="E446" s="28" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="430" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A430" s="34" t="s">
+    <row r="447" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A447" s="34" t="s">
         <v>787</v>
       </c>
-      <c r="B430" s="55" t="s">
+      <c r="B447" s="55" t="s">
         <v>764</v>
       </c>
-      <c r="C430" s="34" t="s">
+      <c r="C447" s="34" t="s">
         <v>790</v>
       </c>
-      <c r="D430" s="34"/>
-      <c r="E430" s="40"/>
-    </row>
-    <row r="431" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A431" s="87" t="s">
+      <c r="D447" s="34"/>
+      <c r="E447" s="40"/>
+    </row>
+    <row r="448" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A448" s="87" t="s">
         <v>21</v>
       </c>
-      <c r="B431" s="54" t="s">
-        <v>719</v>
-      </c>
-      <c r="C431" s="22" t="s">
+      <c r="B448" s="54" t="s">
+        <v>719</v>
+      </c>
+      <c r="C448" s="22" t="s">
         <v>605</v>
       </c>
-      <c r="D431" s="22"/>
-      <c r="E431" s="27"/>
-    </row>
-    <row r="432" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A432" s="87" t="s">
+      <c r="D448" s="22"/>
+      <c r="E448" s="27"/>
+    </row>
+    <row r="449" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A449" s="87" t="s">
         <v>24</v>
       </c>
-      <c r="B432" s="54" t="s">
+      <c r="B449" s="54" t="s">
         <v>720</v>
       </c>
-      <c r="C432" s="22" t="s">
+      <c r="C449" s="22" t="s">
         <v>606</v>
       </c>
-      <c r="D432" s="22" t="s">
+      <c r="D449" s="22" t="s">
         <v>228</v>
       </c>
-      <c r="E432" s="28">
+      <c r="E449" s="28">
         <v>1</v>
       </c>
     </row>
-    <row r="433" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A433" s="87" t="s">
+    <row r="450" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A450" s="87" t="s">
         <v>29</v>
       </c>
-      <c r="B433" s="54" t="s">
-        <v>719</v>
-      </c>
-      <c r="C433" s="22" t="s">
+      <c r="B450" s="54" t="s">
+        <v>719</v>
+      </c>
+      <c r="C450" s="22" t="s">
         <v>607</v>
       </c>
-      <c r="D433" s="22" t="s">
-        <v>230</v>
-      </c>
-      <c r="E433" s="28" t="s">
+      <c r="D450" s="22" t="s">
+        <v>230</v>
+      </c>
+      <c r="E450" s="28" t="s">
         <v>608</v>
       </c>
     </row>
-    <row r="434" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A434" s="87" t="s">
+    <row r="451" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A451" s="87" t="s">
         <v>789</v>
       </c>
-      <c r="B434" s="54" t="s">
-        <v>719</v>
-      </c>
-      <c r="C434" s="22" t="s">
+      <c r="B451" s="54" t="s">
+        <v>719</v>
+      </c>
+      <c r="C451" s="22" t="s">
         <v>791</v>
       </c>
-      <c r="D434" s="22" t="s">
+      <c r="D451" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="E434" s="28">
+      <c r="E451" s="28">
         <v>100</v>
       </c>
     </row>
-    <row r="435" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A435" s="88" t="s">
+    <row r="452" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A452" s="88" t="s">
         <v>823</v>
       </c>
-      <c r="B435" s="54" t="s">
-        <v>719</v>
-      </c>
-      <c r="C435" s="22" t="s">
+      <c r="B452" s="54" t="s">
+        <v>719</v>
+      </c>
+      <c r="C452" s="22" t="s">
         <v>792</v>
       </c>
-      <c r="D435" s="22" t="s">
+      <c r="D452" s="22" t="s">
         <v>234</v>
       </c>
-      <c r="E435" s="28" t="s">
+      <c r="E452" s="28" t="s">
         <v>609</v>
       </c>
     </row>
-    <row r="436" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A436" s="87" t="s">
+    <row r="453" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A453" s="87" t="s">
         <v>183</v>
-      </c>
-      <c r="B436" s="54" t="s">
-        <v>720</v>
-      </c>
-      <c r="C436" s="22" t="s">
-        <v>833</v>
-      </c>
-      <c r="D436" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="E436" s="30" t="s">
-        <v>611</v>
-      </c>
-    </row>
-    <row r="437" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A437" s="88" t="s">
-        <v>822</v>
-      </c>
-      <c r="B437" s="54" t="s">
-        <v>719</v>
-      </c>
-      <c r="C437" s="22" t="s">
-        <v>612</v>
-      </c>
-      <c r="D437" s="22" t="s">
-        <v>234</v>
-      </c>
-      <c r="E437" s="28" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="438" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A438" s="87" t="s">
-        <v>33</v>
-      </c>
-      <c r="B438" s="54" t="s">
-        <v>719</v>
-      </c>
-      <c r="C438" s="22" t="s">
-        <v>613</v>
-      </c>
-      <c r="D438" s="22" t="s">
-        <v>228</v>
-      </c>
-      <c r="E438" s="28" t="s">
-        <v>614</v>
-      </c>
-    </row>
-    <row r="439" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A439" s="68" t="s">
-        <v>193</v>
-      </c>
-      <c r="B439" s="62" t="s">
-        <v>719</v>
-      </c>
-      <c r="C439" s="60" t="s">
-        <v>834</v>
-      </c>
-      <c r="D439" s="60"/>
-      <c r="E439" s="58"/>
-    </row>
-    <row r="440" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A440" s="80" t="s">
-        <v>194</v>
-      </c>
-      <c r="B440" s="54" t="s">
-        <v>719</v>
-      </c>
-      <c r="C440" s="22" t="s">
-        <v>616</v>
-      </c>
-      <c r="D440" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="E440" s="28">
-        <v>43013</v>
-      </c>
-    </row>
-    <row r="441" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A441" s="80" t="s">
-        <v>195</v>
-      </c>
-      <c r="B441" s="54" t="s">
-        <v>719</v>
-      </c>
-      <c r="C441" s="22" t="s">
-        <v>617</v>
-      </c>
-      <c r="D441" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="E441" s="28">
-        <v>43023</v>
-      </c>
-    </row>
-    <row r="442" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A442" s="68" t="s">
-        <v>196</v>
-      </c>
-      <c r="B442" s="62" t="s">
-        <v>719</v>
-      </c>
-      <c r="C442" s="60"/>
-      <c r="D442" s="60"/>
-      <c r="E442" s="58"/>
-    </row>
-    <row r="443" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A443" s="80" t="s">
-        <v>197</v>
-      </c>
-      <c r="B443" s="54" t="s">
-        <v>719</v>
-      </c>
-      <c r="C443" s="22" t="s">
-        <v>618</v>
-      </c>
-      <c r="D443" s="22" t="s">
-        <v>228</v>
-      </c>
-      <c r="E443" s="28">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="444" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A444" s="80" t="s">
-        <v>198</v>
-      </c>
-      <c r="B444" s="54" t="s">
-        <v>719</v>
-      </c>
-      <c r="C444" s="22" t="s">
-        <v>619</v>
-      </c>
-      <c r="D444" s="22" t="s">
-        <v>228</v>
-      </c>
-      <c r="E444" s="28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="445" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A445" s="70" t="s">
-        <v>35</v>
-      </c>
-      <c r="B445" s="62" t="s">
-        <v>719</v>
-      </c>
-      <c r="C445" s="60"/>
-      <c r="D445" s="60"/>
-      <c r="E445" s="58"/>
-    </row>
-    <row r="446" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A446" s="89" t="s">
-        <v>21</v>
-      </c>
-      <c r="B446" s="54" t="s">
-        <v>719</v>
-      </c>
-      <c r="C446" s="22" t="s">
-        <v>605</v>
-      </c>
-      <c r="D446" s="22"/>
-      <c r="E446" s="27"/>
-    </row>
-    <row r="447" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A447" s="71" t="s">
-        <v>24</v>
-      </c>
-      <c r="B447" s="54" t="s">
-        <v>719</v>
-      </c>
-      <c r="C447" s="22" t="s">
-        <v>620</v>
-      </c>
-      <c r="D447" s="22" t="s">
-        <v>230</v>
-      </c>
-      <c r="E447" s="28" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="448" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A448" s="71" t="s">
-        <v>36</v>
-      </c>
-      <c r="B448" s="54" t="s">
-        <v>719</v>
-      </c>
-      <c r="C448" s="22" t="s">
-        <v>622</v>
-      </c>
-      <c r="D448" s="22" t="s">
-        <v>230</v>
-      </c>
-      <c r="E448" s="28" t="s">
-        <v>623</v>
-      </c>
-    </row>
-    <row r="449" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A449" s="71" t="s">
-        <v>25</v>
-      </c>
-      <c r="B449" s="54" t="s">
-        <v>719</v>
-      </c>
-      <c r="C449" s="22" t="s">
-        <v>624</v>
-      </c>
-      <c r="D449" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="E449" s="28" t="s">
-        <v>733</v>
-      </c>
-    </row>
-    <row r="450" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A450" s="68" t="s">
-        <v>199</v>
-      </c>
-      <c r="B450" s="62" t="s">
-        <v>719</v>
-      </c>
-      <c r="C450" s="60"/>
-      <c r="D450" s="60"/>
-      <c r="E450" s="58"/>
-    </row>
-    <row r="451" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A451" s="66" t="s">
-        <v>197</v>
-      </c>
-      <c r="B451" s="54" t="s">
-        <v>720</v>
-      </c>
-      <c r="C451" s="22" t="s">
-        <v>625</v>
-      </c>
-      <c r="D451" s="22" t="s">
-        <v>228</v>
-      </c>
-      <c r="E451" s="28">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="452" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A452" s="68" t="s">
-        <v>200</v>
-      </c>
-      <c r="B452" s="62" t="s">
-        <v>719</v>
-      </c>
-      <c r="C452" s="60"/>
-      <c r="D452" s="60"/>
-      <c r="E452" s="58"/>
-    </row>
-    <row r="453" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A453" s="66" t="s">
-        <v>24</v>
       </c>
       <c r="B453" s="54" t="s">
         <v>720</v>
       </c>
       <c r="C453" s="22" t="s">
-        <v>626</v>
+        <v>833</v>
       </c>
       <c r="D453" s="22" t="s">
-        <v>230</v>
-      </c>
-      <c r="E453" s="28" t="s">
-        <v>765</v>
+        <v>15</v>
+      </c>
+      <c r="E453" s="30" t="s">
+        <v>611</v>
       </c>
     </row>
     <row r="454" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A454" s="66" t="s">
-        <v>25</v>
+      <c r="A454" s="88" t="s">
+        <v>822</v>
       </c>
       <c r="B454" s="54" t="s">
         <v>719</v>
       </c>
       <c r="C454" s="22" t="s">
-        <v>627</v>
+        <v>612</v>
       </c>
       <c r="D454" s="22" t="s">
+        <v>234</v>
+      </c>
+      <c r="E454" s="28" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="455" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A455" s="87" t="s">
+        <v>33</v>
+      </c>
+      <c r="B455" s="54" t="s">
+        <v>719</v>
+      </c>
+      <c r="C455" s="22" t="s">
+        <v>613</v>
+      </c>
+      <c r="D455" s="22" t="s">
+        <v>228</v>
+      </c>
+      <c r="E455" s="28" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="456" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A456" s="68" t="s">
+        <v>193</v>
+      </c>
+      <c r="B456" s="62" t="s">
+        <v>719</v>
+      </c>
+      <c r="C456" s="60" t="s">
+        <v>834</v>
+      </c>
+      <c r="D456" s="60"/>
+      <c r="E456" s="58"/>
+    </row>
+    <row r="457" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A457" s="80" t="s">
+        <v>194</v>
+      </c>
+      <c r="B457" s="54" t="s">
+        <v>719</v>
+      </c>
+      <c r="C457" s="22" t="s">
+        <v>616</v>
+      </c>
+      <c r="D457" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="E454" s="28" t="s">
-        <v>733</v>
-      </c>
-    </row>
-    <row r="455" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A455" s="68" t="s">
-        <v>200</v>
-      </c>
-      <c r="B455" s="62" t="s">
-        <v>721</v>
-      </c>
-      <c r="C455" s="60"/>
-      <c r="D455" s="60"/>
-      <c r="E455" s="58"/>
-    </row>
-    <row r="456" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A456" s="66" t="s">
-        <v>24</v>
-      </c>
-      <c r="B456" s="54" t="s">
-        <v>720</v>
-      </c>
-      <c r="C456" s="22" t="s">
-        <v>628</v>
-      </c>
-      <c r="D456" s="22" t="s">
-        <v>230</v>
-      </c>
-      <c r="E456" s="28" t="s">
-        <v>629</v>
-      </c>
-    </row>
-    <row r="457" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A457" s="66" t="s">
-        <v>24</v>
-      </c>
-      <c r="B457" s="54" t="s">
-        <v>719</v>
-      </c>
-      <c r="C457" s="22" t="s">
-        <v>630</v>
-      </c>
-      <c r="D457" s="22" t="s">
-        <v>234</v>
-      </c>
-      <c r="E457" s="28" t="s">
-        <v>631</v>
-      </c>
-    </row>
-    <row r="458" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A458" s="66" t="s">
-        <v>25</v>
+      <c r="E457" s="28">
+        <v>43013</v>
+      </c>
+    </row>
+    <row r="458" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A458" s="80" t="s">
+        <v>195</v>
       </c>
       <c r="B458" s="54" t="s">
         <v>719</v>
       </c>
       <c r="C458" s="22" t="s">
-        <v>632</v>
+        <v>617</v>
       </c>
       <c r="D458" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="E458" s="28" t="s">
+      <c r="E458" s="28">
+        <v>43023</v>
+      </c>
+    </row>
+    <row r="459" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A459" s="68" t="s">
+        <v>196</v>
+      </c>
+      <c r="B459" s="62" t="s">
+        <v>719</v>
+      </c>
+      <c r="C459" s="60"/>
+      <c r="D459" s="60"/>
+      <c r="E459" s="58"/>
+    </row>
+    <row r="460" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A460" s="80" t="s">
+        <v>197</v>
+      </c>
+      <c r="B460" s="54" t="s">
+        <v>719</v>
+      </c>
+      <c r="C460" s="22" t="s">
+        <v>618</v>
+      </c>
+      <c r="D460" s="22" t="s">
+        <v>228</v>
+      </c>
+      <c r="E460" s="28">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="461" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A461" s="80" t="s">
+        <v>198</v>
+      </c>
+      <c r="B461" s="54" t="s">
+        <v>719</v>
+      </c>
+      <c r="C461" s="22" t="s">
+        <v>619</v>
+      </c>
+      <c r="D461" s="22" t="s">
+        <v>228</v>
+      </c>
+      <c r="E461" s="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="462" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A462" s="70" t="s">
+        <v>35</v>
+      </c>
+      <c r="B462" s="62" t="s">
+        <v>719</v>
+      </c>
+      <c r="C462" s="60"/>
+      <c r="D462" s="60"/>
+      <c r="E462" s="58"/>
+    </row>
+    <row r="463" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A463" s="89" t="s">
+        <v>21</v>
+      </c>
+      <c r="B463" s="54" t="s">
+        <v>719</v>
+      </c>
+      <c r="C463" s="22" t="s">
+        <v>605</v>
+      </c>
+      <c r="D463" s="22"/>
+      <c r="E463" s="27"/>
+    </row>
+    <row r="464" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A464" s="71" t="s">
+        <v>24</v>
+      </c>
+      <c r="B464" s="54" t="s">
+        <v>719</v>
+      </c>
+      <c r="C464" s="22" t="s">
+        <v>620</v>
+      </c>
+      <c r="D464" s="22" t="s">
+        <v>230</v>
+      </c>
+      <c r="E464" s="28" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="465" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A465" s="71" t="s">
+        <v>36</v>
+      </c>
+      <c r="B465" s="54" t="s">
+        <v>719</v>
+      </c>
+      <c r="C465" s="22" t="s">
+        <v>622</v>
+      </c>
+      <c r="D465" s="22" t="s">
+        <v>230</v>
+      </c>
+      <c r="E465" s="28" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="466" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A466" s="71" t="s">
+        <v>25</v>
+      </c>
+      <c r="B466" s="54" t="s">
+        <v>719</v>
+      </c>
+      <c r="C466" s="22" t="s">
+        <v>624</v>
+      </c>
+      <c r="D466" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E466" s="28" t="s">
         <v>733</v>
       </c>
     </row>
-    <row r="459" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A459" s="66" t="s">
+    <row r="467" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A467" s="68" t="s">
+        <v>199</v>
+      </c>
+      <c r="B467" s="62" t="s">
+        <v>719</v>
+      </c>
+      <c r="C467" s="60"/>
+      <c r="D467" s="60"/>
+      <c r="E467" s="58"/>
+    </row>
+    <row r="468" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A468" s="66" t="s">
+        <v>197</v>
+      </c>
+      <c r="B468" s="54" t="s">
+        <v>720</v>
+      </c>
+      <c r="C468" s="22" t="s">
+        <v>625</v>
+      </c>
+      <c r="D468" s="22" t="s">
+        <v>228</v>
+      </c>
+      <c r="E468" s="28">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="469" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A469" s="68" t="s">
+        <v>200</v>
+      </c>
+      <c r="B469" s="62" t="s">
+        <v>719</v>
+      </c>
+      <c r="C469" s="60"/>
+      <c r="D469" s="60"/>
+      <c r="E469" s="58"/>
+    </row>
+    <row r="470" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A470" s="66" t="s">
+        <v>24</v>
+      </c>
+      <c r="B470" s="54" t="s">
+        <v>720</v>
+      </c>
+      <c r="C470" s="22" t="s">
+        <v>626</v>
+      </c>
+      <c r="D470" s="22" t="s">
+        <v>230</v>
+      </c>
+      <c r="E470" s="28" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="471" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A471" s="66" t="s">
+        <v>25</v>
+      </c>
+      <c r="B471" s="54" t="s">
+        <v>719</v>
+      </c>
+      <c r="C471" s="22" t="s">
+        <v>627</v>
+      </c>
+      <c r="D471" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E471" s="28" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="472" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A472" s="68" t="s">
+        <v>200</v>
+      </c>
+      <c r="B472" s="62" t="s">
+        <v>721</v>
+      </c>
+      <c r="C472" s="60"/>
+      <c r="D472" s="60"/>
+      <c r="E472" s="58"/>
+    </row>
+    <row r="473" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A473" s="66" t="s">
+        <v>24</v>
+      </c>
+      <c r="B473" s="54" t="s">
+        <v>720</v>
+      </c>
+      <c r="C473" s="22" t="s">
+        <v>628</v>
+      </c>
+      <c r="D473" s="22" t="s">
+        <v>230</v>
+      </c>
+      <c r="E473" s="28" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="474" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A474" s="66" t="s">
+        <v>24</v>
+      </c>
+      <c r="B474" s="54" t="s">
+        <v>719</v>
+      </c>
+      <c r="C474" s="22" t="s">
+        <v>630</v>
+      </c>
+      <c r="D474" s="22" t="s">
+        <v>234</v>
+      </c>
+      <c r="E474" s="28" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="475" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A475" s="66" t="s">
+        <v>25</v>
+      </c>
+      <c r="B475" s="54" t="s">
+        <v>719</v>
+      </c>
+      <c r="C475" s="22" t="s">
+        <v>632</v>
+      </c>
+      <c r="D475" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E475" s="28" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="476" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A476" s="66" t="s">
         <v>26</v>
       </c>
-      <c r="B459" s="54" t="s">
-        <v>719</v>
-      </c>
-      <c r="C459" s="22" t="s">
+      <c r="B476" s="54" t="s">
+        <v>719</v>
+      </c>
+      <c r="C476" s="22" t="s">
         <v>633</v>
       </c>
-      <c r="D459" s="22" t="s">
+      <c r="D476" s="22" t="s">
         <v>634</v>
       </c>
-      <c r="E459" s="28" t="s">
+      <c r="E476" s="28" t="s">
         <v>635</v>
       </c>
     </row>
-    <row r="460" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A460" s="66" t="s">
+    <row r="477" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A477" s="66" t="s">
         <v>44</v>
       </c>
-      <c r="B460" s="54" t="s">
-        <v>719</v>
-      </c>
-      <c r="C460" s="22" t="s">
+      <c r="B477" s="54" t="s">
+        <v>719</v>
+      </c>
+      <c r="C477" s="22" t="s">
         <v>835</v>
       </c>
-      <c r="D460" s="22" t="s">
+      <c r="D477" s="22" t="s">
         <v>234</v>
       </c>
-      <c r="E460" s="28" t="s">
+      <c r="E477" s="28" t="s">
         <v>637</v>
       </c>
     </row>
-    <row r="461" spans="1:5" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A461" s="61" t="s">
+    <row r="478" spans="1:5" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A478" s="61" t="s">
         <v>122</v>
       </c>
-      <c r="B461" s="50" t="s">
-        <v>719</v>
-      </c>
-      <c r="C461" s="60" t="s">
+      <c r="B478" s="50" t="s">
+        <v>719</v>
+      </c>
+      <c r="C478" s="60" t="s">
         <v>836</v>
       </c>
-      <c r="D461" s="57"/>
-      <c r="E461" s="58"/>
-    </row>
-    <row r="462" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A462" s="66" t="s">
+      <c r="D478" s="57"/>
+      <c r="E478" s="58"/>
+    </row>
+    <row r="479" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A479" s="66" t="s">
         <v>201</v>
       </c>
-      <c r="B462" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C462" s="22" t="s">
+      <c r="B479" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C479" s="22" t="s">
         <v>638</v>
       </c>
-      <c r="D462" s="22" t="s">
+      <c r="D479" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="E462" s="27">
+      <c r="E479" s="27">
         <v>1</v>
       </c>
     </row>
-    <row r="463" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A463" s="71" t="s">
+    <row r="480" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A480" s="71" t="s">
         <v>823</v>
       </c>
-      <c r="B463" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C463" s="22" t="s">
+      <c r="B480" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C480" s="22" t="s">
         <v>639</v>
       </c>
-      <c r="D463" s="16" t="s">
+      <c r="D480" s="16" t="s">
         <v>234</v>
       </c>
-      <c r="E463" s="28" t="s">
+      <c r="E480" s="28" t="s">
         <v>609</v>
       </c>
     </row>
-    <row r="464" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A464" s="66" t="s">
+    <row r="481" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A481" s="66" t="s">
         <v>123</v>
       </c>
-      <c r="B464" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C464" s="22" t="s">
+      <c r="B481" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C481" s="22" t="s">
         <v>640</v>
       </c>
-      <c r="D464" s="16" t="s">
+      <c r="D481" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="E464" s="28" t="s">
+      <c r="E481" s="28" t="s">
         <v>733</v>
       </c>
     </row>
-    <row r="465" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A465" s="70" t="s">
+    <row r="482" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A482" s="70" t="s">
         <v>125</v>
       </c>
-      <c r="B465" s="50" t="s">
-        <v>719</v>
-      </c>
-      <c r="C465" s="60"/>
-      <c r="D465" s="57"/>
-      <c r="E465" s="58"/>
-    </row>
-    <row r="466" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A466" s="71" t="s">
+      <c r="B482" s="50" t="s">
+        <v>719</v>
+      </c>
+      <c r="C482" s="60"/>
+      <c r="D482" s="57"/>
+      <c r="E482" s="58"/>
+    </row>
+    <row r="483" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A483" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="B466" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C466" s="22" t="s">
+      <c r="B483" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C483" s="22" t="s">
         <v>435</v>
       </c>
-      <c r="D466" s="16" t="s">
+      <c r="D483" s="16" t="s">
         <v>228</v>
       </c>
-      <c r="E466" s="28" t="s">
+      <c r="E483" s="28" t="s">
         <v>750</v>
       </c>
     </row>
-    <row r="467" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A467" s="72" t="s">
+    <row r="484" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A484" s="72" t="s">
         <v>820</v>
       </c>
-      <c r="B467" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C467" s="22" t="s">
+      <c r="B484" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C484" s="22" t="s">
         <v>641</v>
       </c>
-      <c r="D467" s="16" t="s">
+      <c r="D484" s="16" t="s">
         <v>234</v>
       </c>
-      <c r="E467" s="30" t="s">
+      <c r="E484" s="30" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="468" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A468" s="70" t="s">
+    <row r="485" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A485" s="70" t="s">
         <v>127</v>
       </c>
-      <c r="B468" s="50" t="s">
-        <v>719</v>
-      </c>
-      <c r="C468" s="60" t="s">
+      <c r="B485" s="50" t="s">
+        <v>719</v>
+      </c>
+      <c r="C485" s="60" t="s">
         <v>439</v>
       </c>
-      <c r="D468" s="57"/>
-      <c r="E468" s="58"/>
-    </row>
-    <row r="469" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A469" s="71" t="s">
-        <v>60</v>
-      </c>
-      <c r="B469" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C469" s="22" t="s">
-        <v>642</v>
-      </c>
-      <c r="D469" s="16" t="s">
-        <v>230</v>
-      </c>
-      <c r="E469" s="28" t="s">
-        <v>643</v>
-      </c>
-    </row>
-    <row r="470" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A470" s="71" t="s">
-        <v>61</v>
-      </c>
-      <c r="B470" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C470" s="22" t="s">
-        <v>644</v>
-      </c>
-      <c r="D470" s="16" t="s">
-        <v>230</v>
-      </c>
-      <c r="E470" s="28" t="s">
-        <v>645</v>
-      </c>
-    </row>
-    <row r="471" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A471" s="71" t="s">
-        <v>63</v>
-      </c>
-      <c r="B471" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C471" s="22" t="s">
-        <v>444</v>
-      </c>
-      <c r="D471" s="16" t="s">
-        <v>230</v>
-      </c>
-      <c r="E471" s="28"/>
-    </row>
-    <row r="472" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A472" s="71" t="s">
-        <v>64</v>
-      </c>
-      <c r="B472" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C472" s="22" t="s">
-        <v>646</v>
-      </c>
-      <c r="D472" s="16" t="s">
-        <v>230</v>
-      </c>
-      <c r="E472" s="28" t="s">
-        <v>769</v>
-      </c>
-    </row>
-    <row r="473" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A473" s="71" t="s">
-        <v>65</v>
-      </c>
-      <c r="B473" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C473" s="22" t="s">
-        <v>647</v>
-      </c>
-      <c r="D473" s="16" t="s">
-        <v>230</v>
-      </c>
-      <c r="E473" s="28" t="s">
-        <v>770</v>
-      </c>
-    </row>
-    <row r="474" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A474" s="71" t="s">
-        <v>66</v>
-      </c>
-      <c r="B474" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C474" s="22" t="s">
-        <v>648</v>
-      </c>
-      <c r="D474" s="16" t="s">
-        <v>230</v>
-      </c>
-      <c r="E474" s="28" t="s">
-        <v>768</v>
-      </c>
-    </row>
-    <row r="475" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A475" s="71" t="s">
-        <v>67</v>
-      </c>
-      <c r="B475" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C475" s="22" t="s">
-        <v>649</v>
-      </c>
-      <c r="D475" s="16" t="s">
-        <v>230</v>
-      </c>
-      <c r="E475" s="28">
-        <v>86756</v>
-      </c>
-    </row>
-    <row r="476" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A476" s="71" t="s">
-        <v>68</v>
-      </c>
-      <c r="B476" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C476" s="22" t="s">
-        <v>650</v>
-      </c>
-      <c r="D476" s="16" t="s">
-        <v>230</v>
-      </c>
-      <c r="E476" s="28" t="s">
-        <v>651</v>
-      </c>
-    </row>
-    <row r="477" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A477" s="73" t="s">
-        <v>71</v>
-      </c>
-      <c r="B477" s="50" t="s">
-        <v>719</v>
-      </c>
-      <c r="C477" s="60"/>
-      <c r="D477" s="57"/>
-      <c r="E477" s="58"/>
-    </row>
-    <row r="478" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A478" s="72" t="s">
-        <v>72</v>
-      </c>
-      <c r="B478" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C478" s="22" t="s">
-        <v>652</v>
-      </c>
-      <c r="D478" s="16" t="s">
-        <v>234</v>
-      </c>
-      <c r="E478" s="28" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="479" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A479" s="72" t="s">
-        <v>57</v>
-      </c>
-      <c r="B479" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C479" s="22" t="s">
-        <v>653</v>
-      </c>
-      <c r="D479" s="16" t="s">
-        <v>230</v>
-      </c>
-      <c r="E479" s="28" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="480" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A480" s="61" t="s">
-        <v>170</v>
-      </c>
-      <c r="B480" s="50" t="s">
-        <v>719</v>
-      </c>
-      <c r="C480" s="60"/>
-      <c r="D480" s="57"/>
-      <c r="E480" s="58"/>
-    </row>
-    <row r="481" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A481" s="66" t="s">
-        <v>171</v>
-      </c>
-      <c r="B481" s="36" t="s">
-        <v>720</v>
-      </c>
-      <c r="C481" s="22" t="s">
-        <v>662</v>
-      </c>
-      <c r="D481" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="E481" s="28" t="s">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="482" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A482" s="71" t="s">
-        <v>822</v>
-      </c>
-      <c r="B482" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C482" s="24" t="s">
-        <v>663</v>
-      </c>
-      <c r="D482" s="16" t="s">
-        <v>234</v>
-      </c>
-      <c r="E482" s="28" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="483" spans="1:5" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A483" s="70" t="s">
-        <v>178</v>
-      </c>
-      <c r="B483" s="50" t="s">
-        <v>719</v>
-      </c>
-      <c r="C483" s="60" t="s">
-        <v>837</v>
-      </c>
-      <c r="D483" s="57"/>
-      <c r="E483" s="58"/>
-    </row>
-    <row r="484" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A484" s="71" t="s">
-        <v>179</v>
-      </c>
-      <c r="B484" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C484" s="22" t="s">
-        <v>665</v>
-      </c>
-      <c r="D484" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="E484" s="27" t="s">
-        <v>566</v>
-      </c>
-    </row>
-    <row r="485" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A485" s="72" t="s">
-        <v>822</v>
-      </c>
-      <c r="B485" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C485" s="24" t="s">
-        <v>666</v>
-      </c>
-      <c r="D485" s="16" t="s">
-        <v>234</v>
-      </c>
-      <c r="E485" s="27" t="s">
-        <v>237</v>
-      </c>
+      <c r="D485" s="57"/>
+      <c r="E485" s="58"/>
     </row>
     <row r="486" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A486" s="71" t="s">
+        <v>60</v>
+      </c>
+      <c r="B486" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C486" s="22" t="s">
+        <v>642</v>
+      </c>
+      <c r="D486" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="E486" s="28" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="487" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A487" s="71" t="s">
+        <v>61</v>
+      </c>
+      <c r="B487" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C487" s="22" t="s">
+        <v>644</v>
+      </c>
+      <c r="D487" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="E487" s="28" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="488" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A488" s="71" t="s">
+        <v>63</v>
+      </c>
+      <c r="B488" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C488" s="22" t="s">
+        <v>444</v>
+      </c>
+      <c r="D488" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="E488" s="28"/>
+    </row>
+    <row r="489" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A489" s="71" t="s">
+        <v>64</v>
+      </c>
+      <c r="B489" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C489" s="22" t="s">
+        <v>646</v>
+      </c>
+      <c r="D489" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="E489" s="28" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="490" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A490" s="71" t="s">
+        <v>65</v>
+      </c>
+      <c r="B490" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C490" s="22" t="s">
+        <v>647</v>
+      </c>
+      <c r="D490" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="E490" s="28" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="491" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A491" s="71" t="s">
+        <v>66</v>
+      </c>
+      <c r="B491" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C491" s="22" t="s">
+        <v>648</v>
+      </c>
+      <c r="D491" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="E491" s="28" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="492" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A492" s="71" t="s">
+        <v>67</v>
+      </c>
+      <c r="B492" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C492" s="22" t="s">
+        <v>649</v>
+      </c>
+      <c r="D492" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="E492" s="28">
+        <v>86756</v>
+      </c>
+    </row>
+    <row r="493" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A493" s="71" t="s">
+        <v>68</v>
+      </c>
+      <c r="B493" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C493" s="22" t="s">
+        <v>650</v>
+      </c>
+      <c r="D493" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="E493" s="28" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="494" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A494" s="73" t="s">
+        <v>71</v>
+      </c>
+      <c r="B494" s="50" t="s">
+        <v>719</v>
+      </c>
+      <c r="C494" s="60"/>
+      <c r="D494" s="57"/>
+      <c r="E494" s="58"/>
+    </row>
+    <row r="495" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A495" s="72" t="s">
+        <v>72</v>
+      </c>
+      <c r="B495" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C495" s="22" t="s">
+        <v>652</v>
+      </c>
+      <c r="D495" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="E495" s="28" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="496" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A496" s="72" t="s">
+        <v>57</v>
+      </c>
+      <c r="B496" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C496" s="22" t="s">
+        <v>653</v>
+      </c>
+      <c r="D496" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="E496" s="28" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="497" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A497" s="61" t="s">
+        <v>170</v>
+      </c>
+      <c r="B497" s="50" t="s">
+        <v>719</v>
+      </c>
+      <c r="C497" s="60"/>
+      <c r="D497" s="57"/>
+      <c r="E497" s="58"/>
+    </row>
+    <row r="498" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A498" s="66" t="s">
         <v>171</v>
       </c>
-      <c r="B486" s="36" t="s">
+      <c r="B498" s="36" t="s">
         <v>720</v>
       </c>
-      <c r="C486" s="22" t="s">
+      <c r="C498" s="22" t="s">
+        <v>662</v>
+      </c>
+      <c r="D498" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E498" s="28" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="499" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A499" s="71" t="s">
+        <v>822</v>
+      </c>
+      <c r="B499" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C499" s="24" t="s">
+        <v>663</v>
+      </c>
+      <c r="D499" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="E499" s="28" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="500" spans="1:5" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A500" s="70" t="s">
+        <v>178</v>
+      </c>
+      <c r="B500" s="50" t="s">
+        <v>719</v>
+      </c>
+      <c r="C500" s="60" t="s">
+        <v>837</v>
+      </c>
+      <c r="D500" s="57"/>
+      <c r="E500" s="58"/>
+    </row>
+    <row r="501" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A501" s="71" t="s">
+        <v>179</v>
+      </c>
+      <c r="B501" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C501" s="22" t="s">
+        <v>665</v>
+      </c>
+      <c r="D501" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E501" s="27" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="502" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A502" s="72" t="s">
+        <v>822</v>
+      </c>
+      <c r="B502" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C502" s="24" t="s">
+        <v>666</v>
+      </c>
+      <c r="D502" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="E502" s="27" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="503" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A503" s="71" t="s">
+        <v>171</v>
+      </c>
+      <c r="B503" s="36" t="s">
+        <v>720</v>
+      </c>
+      <c r="C503" s="22" t="s">
         <v>667</v>
       </c>
-      <c r="D486" s="16" t="s">
+      <c r="D503" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E486" s="27" t="s">
+      <c r="E503" s="27" t="s">
         <v>563</v>
       </c>
     </row>
-    <row r="487" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A487" s="72" t="s">
+    <row r="504" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A504" s="72" t="s">
         <v>822</v>
       </c>
-      <c r="B487" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C487" s="24" t="s">
+      <c r="B504" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C504" s="24" t="s">
         <v>668</v>
       </c>
-      <c r="D487" s="16" t="s">
-        <v>234</v>
-      </c>
-      <c r="E487" s="28" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="488" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A488" s="73" t="s">
-        <v>166</v>
-      </c>
-      <c r="B488" s="50" t="s">
-        <v>720</v>
-      </c>
-      <c r="C488" s="60"/>
-      <c r="D488" s="57"/>
-      <c r="E488" s="58"/>
-    </row>
-    <row r="489" spans="1:5" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A489" s="72" t="s">
-        <v>24</v>
-      </c>
-      <c r="B489" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C489" s="22" t="s">
-        <v>580</v>
-      </c>
-      <c r="D489" s="16" t="s">
-        <v>234</v>
-      </c>
-      <c r="E489" s="28" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="490" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A490" s="72" t="s">
-        <v>167</v>
-      </c>
-      <c r="B490" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C490" s="22" t="s">
-        <v>571</v>
-      </c>
-      <c r="D490" s="16" t="s">
-        <v>535</v>
-      </c>
-      <c r="E490" s="28">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="491" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A491" s="72" t="s">
-        <v>168</v>
-      </c>
-      <c r="B491" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C491" s="22" t="s">
-        <v>669</v>
-      </c>
-      <c r="D491" s="16" t="s">
-        <v>230</v>
-      </c>
-      <c r="E491" s="28"/>
-    </row>
-    <row r="492" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A492" s="72" t="s">
-        <v>180</v>
-      </c>
-      <c r="B492" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C492" s="22" t="s">
-        <v>670</v>
-      </c>
-      <c r="D492" s="16" t="s">
-        <v>230</v>
-      </c>
-      <c r="E492" s="28" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="493" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A493" s="75" t="s">
-        <v>75</v>
-      </c>
-      <c r="B493" s="50" t="s">
-        <v>720</v>
-      </c>
-      <c r="C493" s="60"/>
-      <c r="D493" s="57"/>
-      <c r="E493" s="58"/>
-    </row>
-    <row r="494" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A494" s="76" t="s">
-        <v>24</v>
-      </c>
-      <c r="B494" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C494" s="22" t="s">
-        <v>547</v>
-      </c>
-      <c r="D494" s="16" t="s">
-        <v>234</v>
-      </c>
-      <c r="E494" s="27" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="495" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A495" s="76" t="s">
-        <v>57</v>
-      </c>
-      <c r="B495" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C495" s="22" t="s">
-        <v>548</v>
-      </c>
-      <c r="D495" s="16" t="s">
-        <v>230</v>
-      </c>
-      <c r="E495" s="27" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="496" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A496" s="68" t="s">
-        <v>159</v>
-      </c>
-      <c r="B496" s="62" t="s">
-        <v>721</v>
-      </c>
-      <c r="C496" s="60" t="s">
-        <v>838</v>
-      </c>
-      <c r="D496" s="60"/>
-      <c r="E496" s="58"/>
-    </row>
-    <row r="497" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A497" s="65" t="s">
-        <v>160</v>
-      </c>
-      <c r="B497" s="54" t="s">
-        <v>720</v>
-      </c>
-      <c r="C497" s="22" t="s">
-        <v>655</v>
-      </c>
-      <c r="D497" s="22" t="s">
-        <v>234</v>
-      </c>
-      <c r="E497" s="27" t="s">
-        <v>656</v>
-      </c>
-    </row>
-    <row r="498" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A498" s="65" t="s">
-        <v>161</v>
-      </c>
-      <c r="B498" s="54" t="s">
-        <v>719</v>
-      </c>
-      <c r="C498" s="22" t="s">
-        <v>657</v>
-      </c>
-      <c r="D498" s="22" t="s">
-        <v>234</v>
-      </c>
-      <c r="E498" s="28">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="499" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A499" s="65" t="s">
-        <v>162</v>
-      </c>
-      <c r="B499" s="54" t="s">
-        <v>719</v>
-      </c>
-      <c r="C499" s="22" t="s">
-        <v>532</v>
-      </c>
-      <c r="D499" s="22" t="s">
-        <v>230</v>
-      </c>
-      <c r="E499" s="28" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="500" spans="1:5" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A500" s="65" t="s">
-        <v>163</v>
-      </c>
-      <c r="B500" s="54" t="s">
-        <v>719</v>
-      </c>
-      <c r="C500" s="22" t="s">
-        <v>658</v>
-      </c>
-      <c r="D500" s="22" t="s">
-        <v>535</v>
-      </c>
-      <c r="E500" s="28">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="501" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A501" s="65" t="s">
-        <v>164</v>
-      </c>
-      <c r="B501" s="54" t="s">
-        <v>720</v>
-      </c>
-      <c r="C501" s="22" t="s">
-        <v>659</v>
-      </c>
-      <c r="D501" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="E501" s="28" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="502" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A502" s="65" t="s">
-        <v>822</v>
-      </c>
-      <c r="B502" s="54" t="s">
-        <v>719</v>
-      </c>
-      <c r="C502" s="22" t="s">
-        <v>660</v>
-      </c>
-      <c r="D502" s="22" t="s">
-        <v>234</v>
-      </c>
-      <c r="E502" s="28" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="503" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A503" s="65" t="s">
-        <v>165</v>
-      </c>
-      <c r="B503" s="54" t="s">
-        <v>719</v>
-      </c>
-      <c r="C503" s="22" t="s">
-        <v>661</v>
-      </c>
-      <c r="D503" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="E503" s="28" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="504" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A504" s="65" t="s">
-        <v>822</v>
-      </c>
-      <c r="B504" s="54" t="s">
-        <v>719</v>
-      </c>
-      <c r="C504" s="22" t="s">
-        <v>539</v>
-      </c>
-      <c r="D504" s="22" t="s">
+      <c r="D504" s="16" t="s">
         <v>234</v>
       </c>
       <c r="E504" s="28" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="505" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A505" s="61" t="s">
-        <v>202</v>
+    <row r="505" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A505" s="73" t="s">
+        <v>166</v>
       </c>
       <c r="B505" s="50" t="s">
         <v>720</v>
       </c>
-      <c r="C505" s="60" t="s">
-        <v>839</v>
-      </c>
+      <c r="C505" s="60"/>
       <c r="D505" s="57"/>
       <c r="E505" s="58"/>
     </row>
-    <row r="506" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A506" s="81" t="s">
+    <row r="506" spans="1:5" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A506" s="72" t="s">
+        <v>24</v>
+      </c>
+      <c r="B506" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C506" s="22" t="s">
+        <v>580</v>
+      </c>
+      <c r="D506" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="E506" s="28" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="507" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A507" s="72" t="s">
+        <v>167</v>
+      </c>
+      <c r="B507" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C507" s="22" t="s">
+        <v>571</v>
+      </c>
+      <c r="D507" s="16" t="s">
+        <v>535</v>
+      </c>
+      <c r="E507" s="28">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="508" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A508" s="72" t="s">
+        <v>168</v>
+      </c>
+      <c r="B508" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C508" s="22" t="s">
+        <v>669</v>
+      </c>
+      <c r="D508" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="E508" s="28"/>
+    </row>
+    <row r="509" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A509" s="72" t="s">
+        <v>180</v>
+      </c>
+      <c r="B509" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C509" s="22" t="s">
+        <v>670</v>
+      </c>
+      <c r="D509" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="E509" s="28" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="510" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A510" s="75" t="s">
+        <v>75</v>
+      </c>
+      <c r="B510" s="50" t="s">
+        <v>720</v>
+      </c>
+      <c r="C510" s="60"/>
+      <c r="D510" s="57"/>
+      <c r="E510" s="58"/>
+    </row>
+    <row r="511" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A511" s="76" t="s">
+        <v>24</v>
+      </c>
+      <c r="B511" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C511" s="22" t="s">
+        <v>547</v>
+      </c>
+      <c r="D511" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="E511" s="27" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="512" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A512" s="76" t="s">
+        <v>57</v>
+      </c>
+      <c r="B512" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C512" s="22" t="s">
+        <v>548</v>
+      </c>
+      <c r="D512" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="E512" s="27" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="513" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A513" s="68" t="s">
+        <v>159</v>
+      </c>
+      <c r="B513" s="62" t="s">
+        <v>721</v>
+      </c>
+      <c r="C513" s="60" t="s">
+        <v>838</v>
+      </c>
+      <c r="D513" s="60"/>
+      <c r="E513" s="58"/>
+    </row>
+    <row r="514" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A514" s="65" t="s">
+        <v>160</v>
+      </c>
+      <c r="B514" s="54" t="s">
+        <v>720</v>
+      </c>
+      <c r="C514" s="22" t="s">
+        <v>655</v>
+      </c>
+      <c r="D514" s="22" t="s">
+        <v>234</v>
+      </c>
+      <c r="E514" s="27" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="515" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A515" s="65" t="s">
+        <v>161</v>
+      </c>
+      <c r="B515" s="54" t="s">
+        <v>719</v>
+      </c>
+      <c r="C515" s="22" t="s">
+        <v>657</v>
+      </c>
+      <c r="D515" s="22" t="s">
+        <v>234</v>
+      </c>
+      <c r="E515" s="28">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="516" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A516" s="65" t="s">
+        <v>162</v>
+      </c>
+      <c r="B516" s="54" t="s">
+        <v>719</v>
+      </c>
+      <c r="C516" s="22" t="s">
+        <v>532</v>
+      </c>
+      <c r="D516" s="22" t="s">
+        <v>230</v>
+      </c>
+      <c r="E516" s="28" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="517" spans="1:5" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A517" s="65" t="s">
+        <v>163</v>
+      </c>
+      <c r="B517" s="54" t="s">
+        <v>719</v>
+      </c>
+      <c r="C517" s="22" t="s">
+        <v>658</v>
+      </c>
+      <c r="D517" s="22" t="s">
+        <v>535</v>
+      </c>
+      <c r="E517" s="28">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="518" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A518" s="65" t="s">
+        <v>164</v>
+      </c>
+      <c r="B518" s="54" t="s">
+        <v>720</v>
+      </c>
+      <c r="C518" s="22" t="s">
+        <v>659</v>
+      </c>
+      <c r="D518" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="E518" s="28" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="519" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A519" s="65" t="s">
+        <v>822</v>
+      </c>
+      <c r="B519" s="54" t="s">
+        <v>719</v>
+      </c>
+      <c r="C519" s="22" t="s">
+        <v>660</v>
+      </c>
+      <c r="D519" s="22" t="s">
+        <v>234</v>
+      </c>
+      <c r="E519" s="28" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="520" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A520" s="65" t="s">
+        <v>165</v>
+      </c>
+      <c r="B520" s="54" t="s">
+        <v>719</v>
+      </c>
+      <c r="C520" s="22" t="s">
+        <v>661</v>
+      </c>
+      <c r="D520" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="E520" s="28" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="521" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A521" s="65" t="s">
+        <v>822</v>
+      </c>
+      <c r="B521" s="54" t="s">
+        <v>719</v>
+      </c>
+      <c r="C521" s="22" t="s">
+        <v>539</v>
+      </c>
+      <c r="D521" s="22" t="s">
+        <v>234</v>
+      </c>
+      <c r="E521" s="28" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="522" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A522" s="61" t="s">
+        <v>202</v>
+      </c>
+      <c r="B522" s="50" t="s">
+        <v>720</v>
+      </c>
+      <c r="C522" s="60" t="s">
+        <v>839</v>
+      </c>
+      <c r="D522" s="57"/>
+      <c r="E522" s="58"/>
+    </row>
+    <row r="523" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A523" s="81" t="s">
         <v>21</v>
       </c>
-      <c r="B506" s="50" t="s">
-        <v>719</v>
-      </c>
-      <c r="C506" s="60" t="s">
+      <c r="B523" s="50" t="s">
+        <v>719</v>
+      </c>
+      <c r="C523" s="60" t="s">
         <v>605</v>
       </c>
-      <c r="D506" s="60"/>
-      <c r="E506" s="60"/>
-    </row>
-    <row r="507" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A507" s="66" t="s">
+      <c r="D523" s="60"/>
+      <c r="E523" s="60"/>
+    </row>
+    <row r="524" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A524" s="66" t="s">
         <v>126</v>
       </c>
-      <c r="B507" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C507" s="22" t="s">
+      <c r="B524" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C524" s="22" t="s">
         <v>673</v>
       </c>
-      <c r="D507" s="22" t="s">
-        <v>230</v>
-      </c>
-      <c r="E507" s="28" t="s">
+      <c r="D524" s="22" t="s">
+        <v>230</v>
+      </c>
+      <c r="E524" s="28" t="s">
         <v>840</v>
       </c>
     </row>
-    <row r="508" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A508" s="66" t="s">
+    <row r="525" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A525" s="66" t="s">
         <v>57</v>
       </c>
-      <c r="B508" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C508" s="22" t="s">
+      <c r="B525" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C525" s="22" t="s">
         <v>674</v>
       </c>
-      <c r="D508" s="22" t="s">
-        <v>230</v>
-      </c>
-      <c r="E508" s="28" t="s">
+      <c r="D525" s="22" t="s">
+        <v>230</v>
+      </c>
+      <c r="E525" s="28" t="s">
         <v>675</v>
       </c>
     </row>
-    <row r="509" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A509" s="70" t="s">
+    <row r="526" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A526" s="70" t="s">
         <v>203</v>
       </c>
-      <c r="B509" s="50" t="s">
-        <v>719</v>
-      </c>
-      <c r="C509" s="60"/>
-      <c r="D509" s="57"/>
-      <c r="E509" s="58"/>
-    </row>
-    <row r="510" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A510" s="71" t="s">
+      <c r="B526" s="50" t="s">
+        <v>719</v>
+      </c>
+      <c r="C526" s="60"/>
+      <c r="D526" s="57"/>
+      <c r="E526" s="58"/>
+    </row>
+    <row r="527" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A527" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="B510" s="36" t="s">
+      <c r="B527" s="36" t="s">
         <v>720</v>
       </c>
-      <c r="C510" s="22" t="s">
+      <c r="C527" s="22" t="s">
         <v>676</v>
       </c>
-      <c r="D510" s="16" t="s">
+      <c r="D527" s="16" t="s">
         <v>228</v>
       </c>
-      <c r="E510" s="28">
+      <c r="E527" s="28">
         <v>123455</v>
       </c>
     </row>
-    <row r="511" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A511" s="70" t="s">
+    <row r="528" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A528" s="70" t="s">
         <v>204</v>
       </c>
-      <c r="B511" s="50" t="s">
-        <v>719</v>
-      </c>
-      <c r="C511" s="60"/>
-      <c r="D511" s="57"/>
-      <c r="E511" s="58"/>
-    </row>
-    <row r="512" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A512" s="71" t="s">
+      <c r="B528" s="50" t="s">
+        <v>719</v>
+      </c>
+      <c r="C528" s="60"/>
+      <c r="D528" s="57"/>
+      <c r="E528" s="58"/>
+    </row>
+    <row r="529" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A529" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="B512" s="36" t="s">
+      <c r="B529" s="36" t="s">
         <v>720</v>
       </c>
-      <c r="C512" s="22" t="s">
+      <c r="C529" s="22" t="s">
         <v>677</v>
       </c>
-      <c r="D512" s="16" t="s">
+      <c r="D529" s="16" t="s">
         <v>228</v>
       </c>
-      <c r="E512" s="28">
+      <c r="E529" s="28">
         <v>987342</v>
       </c>
     </row>
-    <row r="513" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A513" s="70" t="s">
+    <row r="530" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A530" s="70" t="s">
         <v>205</v>
       </c>
-      <c r="B513" s="50" t="s">
-        <v>719</v>
-      </c>
-      <c r="C513" s="60"/>
-      <c r="D513" s="57"/>
-      <c r="E513" s="58"/>
-    </row>
-    <row r="514" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A514" s="71" t="s">
+      <c r="B530" s="50" t="s">
+        <v>719</v>
+      </c>
+      <c r="C530" s="60"/>
+      <c r="D530" s="57"/>
+      <c r="E530" s="58"/>
+    </row>
+    <row r="531" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A531" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="B514" s="36" t="s">
+      <c r="B531" s="36" t="s">
         <v>720</v>
       </c>
-      <c r="C514" s="22" t="s">
+      <c r="C531" s="22" t="s">
         <v>678</v>
       </c>
-      <c r="D514" s="16" t="s">
+      <c r="D531" s="16" t="s">
         <v>228</v>
       </c>
-      <c r="E514" s="28" t="s">
+      <c r="E531" s="28" t="s">
         <v>679</v>
       </c>
     </row>
-    <row r="515" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A515" s="70" t="s">
+    <row r="532" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A532" s="70" t="s">
         <v>206</v>
       </c>
-      <c r="B515" s="50" t="s">
-        <v>719</v>
-      </c>
-      <c r="C515" s="60"/>
-      <c r="D515" s="57"/>
-      <c r="E515" s="58"/>
-    </row>
-    <row r="516" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A516" s="71" t="s">
-        <v>24</v>
-      </c>
-      <c r="B516" s="36" t="s">
-        <v>720</v>
-      </c>
-      <c r="C516" s="22" t="s">
-        <v>680</v>
-      </c>
-      <c r="D516" s="16" t="s">
-        <v>228</v>
-      </c>
-      <c r="E516" s="28">
-        <v>10986700</v>
-      </c>
-    </row>
-    <row r="517" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A517" s="72" t="s">
-        <v>820</v>
-      </c>
-      <c r="B517" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C517" s="22" t="s">
-        <v>681</v>
-      </c>
-      <c r="D517" s="16"/>
-      <c r="E517" s="30" t="s">
-        <v>682</v>
-      </c>
-    </row>
-    <row r="518" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A518" s="70" t="s">
-        <v>207</v>
-      </c>
-      <c r="B518" s="50" t="s">
-        <v>719</v>
-      </c>
-      <c r="C518" s="60"/>
-      <c r="D518" s="57"/>
-      <c r="E518" s="58"/>
-    </row>
-    <row r="519" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A519" s="71" t="s">
-        <v>72</v>
-      </c>
-      <c r="B519" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C519" s="22" t="s">
-        <v>683</v>
-      </c>
-      <c r="D519" s="16" t="s">
-        <v>234</v>
-      </c>
-      <c r="E519" s="28" t="s">
-        <v>684</v>
-      </c>
-    </row>
-    <row r="520" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A520" s="70" t="s">
-        <v>208</v>
-      </c>
-      <c r="B520" s="50" t="s">
-        <v>721</v>
-      </c>
-      <c r="C520" s="60"/>
-      <c r="D520" s="57"/>
-      <c r="E520" s="58"/>
-    </row>
-    <row r="521" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A521" s="71" t="s">
-        <v>209</v>
-      </c>
-      <c r="B521" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C521" s="22" t="s">
-        <v>685</v>
-      </c>
-      <c r="D521" s="16" t="s">
-        <v>228</v>
-      </c>
-      <c r="E521" s="28">
-        <v>9873242</v>
-      </c>
-    </row>
-    <row r="522" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A522" s="72" t="s">
-        <v>824</v>
-      </c>
-      <c r="B522" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C522" s="22" t="s">
-        <v>686</v>
-      </c>
-      <c r="D522" s="16" t="s">
-        <v>234</v>
-      </c>
-      <c r="E522" s="28" t="s">
-        <v>687</v>
-      </c>
-    </row>
-    <row r="523" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A523" s="72" t="s">
-        <v>825</v>
-      </c>
-      <c r="B523" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C523" s="22" t="s">
-        <v>688</v>
-      </c>
-      <c r="D523" s="16" t="s">
-        <v>234</v>
-      </c>
-      <c r="E523" s="28"/>
-    </row>
-    <row r="524" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A524" s="70" t="s">
-        <v>210</v>
-      </c>
-      <c r="B524" s="50" t="s">
-        <v>719</v>
-      </c>
-      <c r="C524" s="60" t="s">
-        <v>841</v>
-      </c>
-      <c r="D524" s="57"/>
-      <c r="E524" s="58"/>
-    </row>
-    <row r="525" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A525" s="71" t="s">
-        <v>24</v>
-      </c>
-      <c r="B525" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C525" s="22" t="s">
-        <v>690</v>
-      </c>
-      <c r="D525" s="16" t="s">
-        <v>234</v>
-      </c>
-      <c r="E525" s="28" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="526" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A526" s="71" t="s">
-        <v>167</v>
-      </c>
-      <c r="B526" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C526" s="22" t="s">
-        <v>691</v>
-      </c>
-      <c r="D526" s="16" t="s">
-        <v>535</v>
-      </c>
-      <c r="E526" s="28">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="527" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A527" s="73" t="s">
-        <v>75</v>
-      </c>
-      <c r="B527" s="50" t="s">
-        <v>720</v>
-      </c>
-      <c r="C527" s="60"/>
-      <c r="D527" s="57"/>
-      <c r="E527" s="58"/>
-    </row>
-    <row r="528" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A528" s="72" t="s">
-        <v>24</v>
-      </c>
-      <c r="B528" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C528" s="22" t="s">
-        <v>547</v>
-      </c>
-      <c r="D528" s="16"/>
-      <c r="E528" s="28" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="529" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A529" s="70" t="s">
-        <v>211</v>
-      </c>
-      <c r="B529" s="50" t="s">
-        <v>721</v>
-      </c>
-      <c r="C529" s="60" t="s">
-        <v>842</v>
-      </c>
-      <c r="D529" s="57"/>
-      <c r="E529" s="58"/>
-    </row>
-    <row r="530" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A530" s="71" t="s">
-        <v>57</v>
-      </c>
-      <c r="B530" s="36" t="s">
-        <v>720</v>
-      </c>
-      <c r="C530" s="22" t="s">
-        <v>693</v>
-      </c>
-      <c r="D530" s="16" t="s">
-        <v>230</v>
-      </c>
-      <c r="E530" s="28" t="s">
-        <v>694</v>
-      </c>
-    </row>
-    <row r="531" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A531" s="71" t="s">
-        <v>212</v>
-      </c>
-      <c r="B531" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C531" s="22" t="s">
-        <v>695</v>
-      </c>
-      <c r="D531" s="16" t="s">
-        <v>230</v>
-      </c>
-      <c r="E531" s="28" t="s">
-        <v>696</v>
-      </c>
-    </row>
-    <row r="532" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A532" s="70" t="s">
-        <v>213</v>
-      </c>
       <c r="B532" s="50" t="s">
         <v>719</v>
       </c>
-      <c r="C532" s="60" t="s">
-        <v>697</v>
-      </c>
+      <c r="C532" s="60"/>
       <c r="D532" s="57"/>
       <c r="E532" s="58"/>
     </row>
-    <row r="533" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="533" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A533" s="71" t="s">
-        <v>214</v>
+        <v>24</v>
       </c>
       <c r="B533" s="36" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="C533" s="22" t="s">
-        <v>698</v>
+        <v>680</v>
       </c>
       <c r="D533" s="16" t="s">
-        <v>10</v>
+        <v>228</v>
       </c>
       <c r="E533" s="28">
-        <v>36161</v>
-      </c>
-    </row>
-    <row r="534" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A534" s="71" t="s">
-        <v>215</v>
+        <v>10986700</v>
+      </c>
+    </row>
+    <row r="534" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A534" s="72" t="s">
+        <v>820</v>
       </c>
       <c r="B534" s="36" t="s">
         <v>719</v>
       </c>
       <c r="C534" s="22" t="s">
-        <v>699</v>
-      </c>
-      <c r="D534" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E534" s="28">
-        <v>36161</v>
+        <v>681</v>
+      </c>
+      <c r="D534" s="16"/>
+      <c r="E534" s="30" t="s">
+        <v>682</v>
       </c>
     </row>
     <row r="535" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A535" s="71" t="s">
-        <v>216</v>
-      </c>
-      <c r="B535" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C535" s="22" t="s">
-        <v>700</v>
-      </c>
-      <c r="D535" s="16" t="s">
-        <v>230</v>
-      </c>
-      <c r="E535" s="28">
-        <v>123456</v>
-      </c>
+      <c r="A535" s="70" t="s">
+        <v>207</v>
+      </c>
+      <c r="B535" s="50" t="s">
+        <v>719</v>
+      </c>
+      <c r="C535" s="60"/>
+      <c r="D535" s="57"/>
+      <c r="E535" s="58"/>
     </row>
     <row r="536" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A536" s="73" t="s">
-        <v>217</v>
-      </c>
-      <c r="B536" s="50" t="s">
-        <v>719</v>
-      </c>
-      <c r="C536" s="60"/>
-      <c r="D536" s="57"/>
-      <c r="E536" s="58"/>
+      <c r="A536" s="71" t="s">
+        <v>72</v>
+      </c>
+      <c r="B536" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C536" s="22" t="s">
+        <v>683</v>
+      </c>
+      <c r="D536" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="E536" s="28" t="s">
+        <v>684</v>
+      </c>
     </row>
     <row r="537" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A537" s="72" t="s">
-        <v>218</v>
-      </c>
-      <c r="B537" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C537" s="22" t="s">
-        <v>701</v>
-      </c>
-      <c r="D537" s="16" t="s">
-        <v>230</v>
-      </c>
-      <c r="E537" s="28" t="s">
-        <v>629</v>
-      </c>
+      <c r="A537" s="70" t="s">
+        <v>208</v>
+      </c>
+      <c r="B537" s="50" t="s">
+        <v>721</v>
+      </c>
+      <c r="C537" s="60"/>
+      <c r="D537" s="57"/>
+      <c r="E537" s="58"/>
     </row>
     <row r="538" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A538" s="72" t="s">
-        <v>219</v>
+      <c r="A538" s="71" t="s">
+        <v>209</v>
       </c>
       <c r="B538" s="36" t="s">
         <v>719</v>
       </c>
       <c r="C538" s="22" t="s">
-        <v>702</v>
+        <v>685</v>
       </c>
       <c r="D538" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E538" s="28" t="s">
-        <v>766</v>
-      </c>
-    </row>
-    <row r="539" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A539" s="61" t="s">
-        <v>220</v>
-      </c>
-      <c r="B539" s="50" t="s">
-        <v>719</v>
-      </c>
-      <c r="C539" s="60" t="s">
-        <v>843</v>
-      </c>
-      <c r="D539" s="57"/>
-      <c r="E539" s="58"/>
-    </row>
-    <row r="540" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A540" s="78" t="s">
-        <v>21</v>
-      </c>
-      <c r="B540" s="35" t="s">
+        <v>228</v>
+      </c>
+      <c r="E538" s="28">
+        <v>9873242</v>
+      </c>
+    </row>
+    <row r="539" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A539" s="72" t="s">
+        <v>824</v>
+      </c>
+      <c r="B539" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C539" s="22" t="s">
+        <v>686</v>
+      </c>
+      <c r="D539" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="E539" s="28" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="540" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A540" s="72" t="s">
+        <v>825</v>
+      </c>
+      <c r="B540" s="36" t="s">
         <v>719</v>
       </c>
       <c r="C540" s="22" t="s">
-        <v>605</v>
-      </c>
-      <c r="D540" s="22"/>
-      <c r="E540" s="27"/>
-    </row>
-    <row r="541" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A541" s="66" t="s">
-        <v>221</v>
-      </c>
-      <c r="B541" s="36" t="s">
-        <v>720</v>
-      </c>
-      <c r="C541" s="22" t="s">
-        <v>704</v>
-      </c>
-      <c r="D541" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="E541" s="28" t="s">
-        <v>705</v>
-      </c>
-    </row>
-    <row r="542" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+        <v>688</v>
+      </c>
+      <c r="D540" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="E540" s="28"/>
+    </row>
+    <row r="541" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A541" s="70" t="s">
+        <v>210</v>
+      </c>
+      <c r="B541" s="50" t="s">
+        <v>719</v>
+      </c>
+      <c r="C541" s="60" t="s">
+        <v>841</v>
+      </c>
+      <c r="D541" s="57"/>
+      <c r="E541" s="58"/>
+    </row>
+    <row r="542" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A542" s="71" t="s">
-        <v>822</v>
-      </c>
-      <c r="B542" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="B542" s="36" t="s">
         <v>719</v>
       </c>
       <c r="C542" s="22" t="s">
-        <v>706</v>
+        <v>690</v>
       </c>
       <c r="D542" s="16" t="s">
         <v>234</v>
       </c>
       <c r="E542" s="28" t="s">
-        <v>237</v>
+        <v>541</v>
       </c>
     </row>
     <row r="543" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A543" s="66" t="s">
-        <v>222</v>
-      </c>
-      <c r="B543" s="35" t="s">
+      <c r="A543" s="71" t="s">
+        <v>167</v>
+      </c>
+      <c r="B543" s="36" t="s">
         <v>719</v>
       </c>
       <c r="C543" s="22" t="s">
-        <v>707</v>
+        <v>691</v>
       </c>
       <c r="D543" s="16" t="s">
-        <v>1</v>
+        <v>535</v>
       </c>
       <c r="E543" s="28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="544" spans="1:5" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A544" s="71" t="s">
-        <v>823</v>
-      </c>
-      <c r="B544" s="35" t="s">
-        <v>719</v>
-      </c>
-      <c r="C544" s="22" t="s">
-        <v>708</v>
-      </c>
-      <c r="D544" s="16"/>
-      <c r="E544" s="28" t="s">
-        <v>609</v>
-      </c>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="544" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A544" s="73" t="s">
+        <v>75</v>
+      </c>
+      <c r="B544" s="50" t="s">
+        <v>720</v>
+      </c>
+      <c r="C544" s="60"/>
+      <c r="D544" s="57"/>
+      <c r="E544" s="58"/>
     </row>
     <row r="545" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A545" s="61" t="s">
-        <v>159</v>
-      </c>
-      <c r="B545" s="50" t="s">
+      <c r="A545" s="72" t="s">
+        <v>24</v>
+      </c>
+      <c r="B545" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C545" s="22" t="s">
+        <v>547</v>
+      </c>
+      <c r="D545" s="16"/>
+      <c r="E545" s="28" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="546" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A546" s="70" t="s">
+        <v>211</v>
+      </c>
+      <c r="B546" s="50" t="s">
         <v>721</v>
       </c>
-      <c r="C545" s="60" t="s">
-        <v>844</v>
-      </c>
-      <c r="D545" s="57"/>
-      <c r="E545" s="58"/>
-    </row>
-    <row r="546" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A546" s="66" t="s">
-        <v>160</v>
-      </c>
-      <c r="B546" s="36" t="s">
-        <v>720</v>
-      </c>
-      <c r="C546" s="22" t="s">
-        <v>709</v>
-      </c>
-      <c r="D546" s="16" t="s">
-        <v>234</v>
-      </c>
-      <c r="E546" s="27" t="s">
-        <v>656</v>
-      </c>
-    </row>
-    <row r="547" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A547" s="66" t="s">
-        <v>164</v>
+      <c r="C546" s="60" t="s">
+        <v>842</v>
+      </c>
+      <c r="D546" s="57"/>
+      <c r="E546" s="58"/>
+    </row>
+    <row r="547" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A547" s="71" t="s">
+        <v>57</v>
       </c>
       <c r="B547" s="36" t="s">
         <v>720</v>
       </c>
       <c r="C547" s="22" t="s">
+        <v>693</v>
+      </c>
+      <c r="D547" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="E547" s="28" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="548" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A548" s="71" t="s">
+        <v>212</v>
+      </c>
+      <c r="B548" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C548" s="22" t="s">
+        <v>695</v>
+      </c>
+      <c r="D548" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="E548" s="28" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="549" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A549" s="70" t="s">
+        <v>213</v>
+      </c>
+      <c r="B549" s="50" t="s">
+        <v>719</v>
+      </c>
+      <c r="C549" s="60" t="s">
+        <v>697</v>
+      </c>
+      <c r="D549" s="57"/>
+      <c r="E549" s="58"/>
+    </row>
+    <row r="550" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A550" s="71" t="s">
+        <v>214</v>
+      </c>
+      <c r="B550" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C550" s="22" t="s">
+        <v>698</v>
+      </c>
+      <c r="D550" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E550" s="28">
+        <v>36161</v>
+      </c>
+    </row>
+    <row r="551" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A551" s="71" t="s">
+        <v>215</v>
+      </c>
+      <c r="B551" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C551" s="22" t="s">
+        <v>699</v>
+      </c>
+      <c r="D551" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E551" s="28">
+        <v>36161</v>
+      </c>
+    </row>
+    <row r="552" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A552" s="71" t="s">
+        <v>216</v>
+      </c>
+      <c r="B552" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C552" s="22" t="s">
+        <v>700</v>
+      </c>
+      <c r="D552" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="E552" s="28">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="553" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A553" s="73" t="s">
+        <v>217</v>
+      </c>
+      <c r="B553" s="50" t="s">
+        <v>719</v>
+      </c>
+      <c r="C553" s="60"/>
+      <c r="D553" s="57"/>
+      <c r="E553" s="58"/>
+    </row>
+    <row r="554" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A554" s="72" t="s">
+        <v>218</v>
+      </c>
+      <c r="B554" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C554" s="22" t="s">
+        <v>701</v>
+      </c>
+      <c r="D554" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="E554" s="28" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="555" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A555" s="72" t="s">
+        <v>219</v>
+      </c>
+      <c r="B555" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C555" s="22" t="s">
+        <v>702</v>
+      </c>
+      <c r="D555" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E555" s="28" t="s">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="556" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A556" s="61" t="s">
+        <v>220</v>
+      </c>
+      <c r="B556" s="50" t="s">
+        <v>719</v>
+      </c>
+      <c r="C556" s="60" t="s">
+        <v>843</v>
+      </c>
+      <c r="D556" s="57"/>
+      <c r="E556" s="58"/>
+    </row>
+    <row r="557" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A557" s="78" t="s">
+        <v>21</v>
+      </c>
+      <c r="B557" s="35" t="s">
+        <v>719</v>
+      </c>
+      <c r="C557" s="22" t="s">
+        <v>605</v>
+      </c>
+      <c r="D557" s="22"/>
+      <c r="E557" s="27"/>
+    </row>
+    <row r="558" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A558" s="66" t="s">
+        <v>221</v>
+      </c>
+      <c r="B558" s="36" t="s">
+        <v>720</v>
+      </c>
+      <c r="C558" s="22" t="s">
+        <v>704</v>
+      </c>
+      <c r="D558" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E558" s="28" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="559" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A559" s="71" t="s">
+        <v>822</v>
+      </c>
+      <c r="B559" s="35" t="s">
+        <v>719</v>
+      </c>
+      <c r="C559" s="22" t="s">
+        <v>706</v>
+      </c>
+      <c r="D559" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="E559" s="28" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="560" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A560" s="66" t="s">
+        <v>222</v>
+      </c>
+      <c r="B560" s="35" t="s">
+        <v>719</v>
+      </c>
+      <c r="C560" s="22" t="s">
+        <v>707</v>
+      </c>
+      <c r="D560" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E560" s="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="561" spans="1:5" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A561" s="71" t="s">
+        <v>823</v>
+      </c>
+      <c r="B561" s="35" t="s">
+        <v>719</v>
+      </c>
+      <c r="C561" s="22" t="s">
+        <v>708</v>
+      </c>
+      <c r="D561" s="16"/>
+      <c r="E561" s="28" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="562" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A562" s="61" t="s">
+        <v>159</v>
+      </c>
+      <c r="B562" s="50" t="s">
+        <v>721</v>
+      </c>
+      <c r="C562" s="60" t="s">
+        <v>844</v>
+      </c>
+      <c r="D562" s="57"/>
+      <c r="E562" s="58"/>
+    </row>
+    <row r="563" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A563" s="66" t="s">
+        <v>160</v>
+      </c>
+      <c r="B563" s="36" t="s">
+        <v>720</v>
+      </c>
+      <c r="C563" s="22" t="s">
+        <v>709</v>
+      </c>
+      <c r="D563" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="E563" s="27" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="564" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A564" s="66" t="s">
+        <v>164</v>
+      </c>
+      <c r="B564" s="36" t="s">
+        <v>720</v>
+      </c>
+      <c r="C564" s="22" t="s">
         <v>710</v>
       </c>
-      <c r="D547" s="16" t="s">
+      <c r="D564" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E547" s="28" t="s">
+      <c r="E564" s="28" t="s">
         <v>592</v>
       </c>
     </row>
-    <row r="548" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A548" s="71" t="s">
+    <row r="565" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A565" s="71" t="s">
         <v>822</v>
       </c>
-      <c r="B548" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C548" s="22" t="s">
+      <c r="B565" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C565" s="22" t="s">
         <v>711</v>
       </c>
-      <c r="D548" s="16" t="s">
+      <c r="D565" s="16" t="s">
         <v>234</v>
       </c>
-      <c r="E548" s="28" t="s">
+      <c r="E565" s="28" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="549" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A549" s="66" t="s">
+    <row r="566" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A566" s="66" t="s">
         <v>165</v>
       </c>
-      <c r="B549" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C549" s="22" t="s">
+      <c r="B566" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C566" s="22" t="s">
         <v>712</v>
       </c>
-      <c r="D549" s="16" t="s">
+      <c r="D566" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E549" s="28" t="s">
+      <c r="E566" s="28" t="s">
         <v>598</v>
       </c>
     </row>
-    <row r="550" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A550" s="71" t="s">
+    <row r="567" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A567" s="71" t="s">
         <v>822</v>
       </c>
-      <c r="B550" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C550" s="22" t="s">
+      <c r="B567" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C567" s="22" t="s">
         <v>713</v>
       </c>
-      <c r="D550" s="16" t="s">
+      <c r="D567" s="16" t="s">
         <v>234</v>
       </c>
-      <c r="E550" s="28" t="s">
+      <c r="E567" s="28" t="s">
         <v>237</v>
       </c>
     </row>

</xml_diff>

<commit_message>
1612400 - PUF Excel Specification - Add withholding amount for credit invoices. (#108)
</commit_message>
<xml_diff>
--- a/specification/excel/Pagero Universal Format.xlsx
+++ b/specification/excel/Pagero Universal Format.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\development\puf-billing\specification\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\development\format\puf-billing\specification\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{535AC171-E03B-444D-BF6F-CE7C09022044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AB015E4-FCB2-4978-8B2A-7409EAD0349E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7185" yWindow="315" windowWidth="31500" windowHeight="19380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="6" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4682" uniqueCount="866">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4755" uniqueCount="867">
   <si>
     <t>Comments</t>
   </si>
@@ -3154,6 +3154,9 @@
   </si>
   <si>
     <t>cbc:WebsiteURI</t>
+  </si>
+  <si>
+    <t>Added withholding amount for credit</t>
   </si>
 </sst>
 </file>
@@ -3763,7 +3766,7 @@
     <cellStyle name="Pagero Green" xfId="2" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
     <cellStyle name="Pagero Grey" xfId="9" xr:uid="{1C805717-4869-43EB-8A4F-0A7959EA5D60}"/>
     <cellStyle name="Pagero Light Green" xfId="8" xr:uid="{69640978-6259-4509-B932-3F75A4F5FBA6}"/>
-    <cellStyle name="Percent" xfId="10" builtinId="5"/>
+    <cellStyle name="Per cent" xfId="10" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -4135,8 +4138,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:E47"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4306,8 +4309,12 @@
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B38" s="20"/>
-      <c r="C38" s="16"/>
+      <c r="B38" s="20">
+        <v>45866</v>
+      </c>
+      <c r="C38" s="16" t="s">
+        <v>866</v>
+      </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B39" s="20"/>
@@ -4362,8 +4369,8 @@
   <dimension ref="A1:E586"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A67" sqref="A67:XFD67"/>
+      <pane ySplit="2" topLeftCell="A412" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A415" sqref="A415:XFD431"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -13448,10 +13455,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41A28953-D494-4CBC-9080-60B98492A541}">
-  <dimension ref="A1:E550"/>
+  <dimension ref="A1:E567"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="E64" sqref="E64"/>
+    <sheetView topLeftCell="A410" workbookViewId="0">
+      <selection activeCell="F407" sqref="F407"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -19806,2174 +19813,2439 @@
         <v>549</v>
       </c>
     </row>
-    <row r="412" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="412" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A412" s="33" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B412" s="37" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="C412" s="34" t="s">
-        <v>854</v>
+        <v>497</v>
       </c>
       <c r="D412" s="33"/>
       <c r="E412" s="40"/>
     </row>
-    <row r="413" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="413" spans="1:5" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A413" s="65" t="s">
+        <v>171</v>
+      </c>
+      <c r="B413" s="36" t="s">
+        <v>720</v>
+      </c>
+      <c r="C413" s="22" t="s">
+        <v>576</v>
+      </c>
+      <c r="D413" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E413" s="28" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="414" spans="1:5" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A414" s="66" t="s">
+        <v>822</v>
+      </c>
+      <c r="B414" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C414" s="24" t="s">
+        <v>577</v>
+      </c>
+      <c r="D414" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="E414" s="28" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="415" spans="1:5" s="2" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A415" s="68" t="s">
+        <v>178</v>
+      </c>
+      <c r="B415" s="50" t="s">
+        <v>719</v>
+      </c>
+      <c r="C415" s="60" t="s">
+        <v>716</v>
+      </c>
+      <c r="D415" s="57"/>
+      <c r="E415" s="58"/>
+    </row>
+    <row r="416" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A416" s="66" t="s">
         <v>21</v>
       </c>
-      <c r="B413" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C413" s="22" t="s">
-        <v>226</v>
-      </c>
-      <c r="D413" s="22"/>
-      <c r="E413" s="27"/>
-    </row>
-    <row r="414" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A414" s="65" t="s">
-        <v>183</v>
-      </c>
-      <c r="B414" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C414" s="22" t="s">
-        <v>582</v>
-      </c>
-      <c r="D414" s="16" t="s">
+      <c r="B416" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C416" s="22" t="s">
+        <v>578</v>
+      </c>
+      <c r="D416" s="22"/>
+      <c r="E416" s="27"/>
+    </row>
+    <row r="417" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A417" s="66" t="s">
+        <v>179</v>
+      </c>
+      <c r="B417" s="36" t="s">
+        <v>720</v>
+      </c>
+      <c r="C417" s="22" t="s">
+        <v>579</v>
+      </c>
+      <c r="D417" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E414" s="30" t="s">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="415" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A415" s="66" t="s">
+      <c r="E417" s="27" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="418" spans="1:5" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A418" s="71" t="s">
         <v>822</v>
       </c>
-      <c r="B415" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C415" s="22" t="s">
-        <v>584</v>
-      </c>
-      <c r="D415" s="16" t="s">
+      <c r="B418" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C418" s="24" t="s">
+        <v>567</v>
+      </c>
+      <c r="D418" s="16" t="s">
         <v>234</v>
       </c>
-      <c r="E415" s="28" t="s">
+      <c r="E418" s="27" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="416" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A416" s="65" t="s">
-        <v>184</v>
-      </c>
-      <c r="B416" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C416" s="22" t="s">
-        <v>855</v>
-      </c>
-      <c r="D416" s="16" t="s">
+    <row r="419" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A419" s="66" t="s">
+        <v>171</v>
+      </c>
+      <c r="B419" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C419" s="22" t="s">
+        <v>568</v>
+      </c>
+      <c r="D419" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E416" s="30" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="417" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A417" s="66" t="s">
+      <c r="E419" s="27" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="420" spans="1:5" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A420" s="71" t="s">
         <v>822</v>
       </c>
-      <c r="B417" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C417" s="22" t="s">
-        <v>831</v>
-      </c>
-      <c r="D417" s="16" t="s">
+      <c r="B420" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C420" s="24" t="s">
+        <v>569</v>
+      </c>
+      <c r="D420" s="16" t="s">
         <v>234</v>
       </c>
-      <c r="E417" s="28" t="s">
+      <c r="E420" s="28" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="418" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A418" s="65" t="s">
-        <v>185</v>
-      </c>
-      <c r="B418" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C418" s="22" t="s">
-        <v>856</v>
-      </c>
-      <c r="D418" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="E418" s="30" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="419" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A419" s="66" t="s">
-        <v>822</v>
-      </c>
-      <c r="B419" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C419" s="22" t="s">
-        <v>832</v>
-      </c>
-      <c r="D419" s="16" t="s">
+    <row r="421" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A421" s="70" t="s">
+        <v>166</v>
+      </c>
+      <c r="B421" s="50" t="s">
+        <v>720</v>
+      </c>
+      <c r="C421" s="60"/>
+      <c r="D421" s="57"/>
+      <c r="E421" s="58"/>
+    </row>
+    <row r="422" spans="1:5" s="2" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A422" s="71" t="s">
+        <v>24</v>
+      </c>
+      <c r="B422" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C422" s="22" t="s">
+        <v>580</v>
+      </c>
+      <c r="D422" s="16" t="s">
         <v>234</v>
       </c>
-      <c r="E419" s="28" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="420" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A420" s="65" t="s">
-        <v>186</v>
-      </c>
-      <c r="B420" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C420" s="22" t="s">
-        <v>829</v>
-      </c>
-      <c r="D420" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="E420" s="28" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="421" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A421" s="66" t="s">
-        <v>822</v>
-      </c>
-      <c r="B421" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C421" s="22" t="s">
-        <v>593</v>
-      </c>
-      <c r="D421" s="16" t="s">
-        <v>234</v>
-      </c>
-      <c r="E421" s="28" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="422" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A422" s="65" t="s">
-        <v>187</v>
-      </c>
-      <c r="B422" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C422" s="22" t="s">
-        <v>830</v>
-      </c>
-      <c r="D422" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="E422" s="30" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="423" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A423" s="66" t="s">
-        <v>822</v>
+      <c r="E422" s="28" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="423" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A423" s="71" t="s">
+        <v>167</v>
       </c>
       <c r="B423" s="36" t="s">
         <v>719</v>
       </c>
       <c r="C423" s="22" t="s">
-        <v>596</v>
+        <v>571</v>
       </c>
       <c r="D423" s="16" t="s">
-        <v>234</v>
-      </c>
-      <c r="E423" s="28" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="424" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A424" s="65" t="s">
-        <v>188</v>
+        <v>535</v>
+      </c>
+      <c r="E423" s="28">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="424" spans="1:5" s="2" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A424" s="71" t="s">
+        <v>168</v>
       </c>
       <c r="B424" s="36" t="s">
         <v>719</v>
       </c>
       <c r="C424" s="22" t="s">
-        <v>597</v>
+        <v>572</v>
       </c>
       <c r="D424" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="E424" s="30" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="425" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A425" s="66" t="s">
-        <v>822</v>
+        <v>230</v>
+      </c>
+      <c r="E424" s="28" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="425" spans="1:5" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A425" s="71" t="s">
+        <v>180</v>
       </c>
       <c r="B425" s="36" t="s">
         <v>719</v>
       </c>
       <c r="C425" s="22" t="s">
-        <v>599</v>
+        <v>574</v>
       </c>
       <c r="D425" s="16" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="E425" s="28" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="426" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A426" s="65" t="s">
-        <v>189</v>
-      </c>
-      <c r="B426" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C426" s="22" t="s">
-        <v>600</v>
-      </c>
-      <c r="D426" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="E426" s="30" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="427" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A427" s="66" t="s">
-        <v>822</v>
+        <v>575</v>
+      </c>
+    </row>
+    <row r="426" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A426" s="73" t="s">
+        <v>75</v>
+      </c>
+      <c r="B426" s="50" t="s">
+        <v>720</v>
+      </c>
+      <c r="C426" s="60"/>
+      <c r="D426" s="57"/>
+      <c r="E426" s="58"/>
+    </row>
+    <row r="427" spans="1:5" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A427" s="72" t="s">
+        <v>24</v>
       </c>
       <c r="B427" s="36" t="s">
         <v>719</v>
       </c>
       <c r="C427" s="22" t="s">
-        <v>601</v>
+        <v>547</v>
       </c>
       <c r="D427" s="16" t="s">
         <v>234</v>
       </c>
-      <c r="E427" s="28" t="s">
+      <c r="E427" s="27" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="428" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A428" s="72" t="s">
+        <v>57</v>
+      </c>
+      <c r="B428" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C428" s="22" t="s">
+        <v>548</v>
+      </c>
+      <c r="D428" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="E428" s="27" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="429" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A429" s="33" t="s">
+        <v>182</v>
+      </c>
+      <c r="B429" s="37" t="s">
+        <v>720</v>
+      </c>
+      <c r="C429" s="34" t="s">
+        <v>854</v>
+      </c>
+      <c r="D429" s="33"/>
+      <c r="E429" s="40"/>
+    </row>
+    <row r="430" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A430" s="65" t="s">
+        <v>21</v>
+      </c>
+      <c r="B430" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C430" s="22" t="s">
+        <v>226</v>
+      </c>
+      <c r="D430" s="22"/>
+      <c r="E430" s="27"/>
+    </row>
+    <row r="431" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A431" s="65" t="s">
+        <v>183</v>
+      </c>
+      <c r="B431" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C431" s="22" t="s">
+        <v>582</v>
+      </c>
+      <c r="D431" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E431" s="30" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="432" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A432" s="66" t="s">
+        <v>822</v>
+      </c>
+      <c r="B432" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C432" s="22" t="s">
+        <v>584</v>
+      </c>
+      <c r="D432" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="E432" s="28" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="428" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A428" s="65" t="s">
+    <row r="433" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A433" s="65" t="s">
+        <v>184</v>
+      </c>
+      <c r="B433" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C433" s="22" t="s">
+        <v>855</v>
+      </c>
+      <c r="D433" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E433" s="30" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="434" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A434" s="66" t="s">
+        <v>822</v>
+      </c>
+      <c r="B434" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C434" s="22" t="s">
+        <v>831</v>
+      </c>
+      <c r="D434" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="E434" s="28" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="435" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A435" s="65" t="s">
+        <v>185</v>
+      </c>
+      <c r="B435" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C435" s="22" t="s">
+        <v>856</v>
+      </c>
+      <c r="D435" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E435" s="30" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="436" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A436" s="66" t="s">
+        <v>822</v>
+      </c>
+      <c r="B436" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C436" s="22" t="s">
+        <v>832</v>
+      </c>
+      <c r="D436" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="E436" s="28" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="437" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A437" s="65" t="s">
+        <v>186</v>
+      </c>
+      <c r="B437" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C437" s="22" t="s">
+        <v>829</v>
+      </c>
+      <c r="D437" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E437" s="28" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="438" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A438" s="66" t="s">
+        <v>822</v>
+      </c>
+      <c r="B438" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C438" s="22" t="s">
+        <v>593</v>
+      </c>
+      <c r="D438" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="E438" s="28" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="439" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A439" s="65" t="s">
+        <v>187</v>
+      </c>
+      <c r="B439" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C439" s="22" t="s">
+        <v>830</v>
+      </c>
+      <c r="D439" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E439" s="30" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="440" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A440" s="66" t="s">
+        <v>822</v>
+      </c>
+      <c r="B440" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C440" s="22" t="s">
+        <v>596</v>
+      </c>
+      <c r="D440" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="E440" s="28" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="441" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A441" s="65" t="s">
+        <v>188</v>
+      </c>
+      <c r="B441" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C441" s="22" t="s">
+        <v>597</v>
+      </c>
+      <c r="D441" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E441" s="30" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="442" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A442" s="66" t="s">
+        <v>822</v>
+      </c>
+      <c r="B442" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C442" s="22" t="s">
+        <v>599</v>
+      </c>
+      <c r="D442" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="E442" s="28" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="443" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A443" s="65" t="s">
+        <v>189</v>
+      </c>
+      <c r="B443" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C443" s="22" t="s">
+        <v>600</v>
+      </c>
+      <c r="D443" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E443" s="30" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="444" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A444" s="66" t="s">
+        <v>822</v>
+      </c>
+      <c r="B444" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C444" s="22" t="s">
+        <v>601</v>
+      </c>
+      <c r="D444" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="E444" s="28" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="445" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A445" s="65" t="s">
         <v>190</v>
       </c>
-      <c r="B428" s="36" t="s">
+      <c r="B445" s="36" t="s">
         <v>720</v>
       </c>
-      <c r="C428" s="22" t="s">
+      <c r="C445" s="22" t="s">
         <v>828</v>
       </c>
-      <c r="D428" s="16" t="s">
+      <c r="D445" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E428" s="30" t="s">
+      <c r="E445" s="30" t="s">
         <v>603</v>
       </c>
     </row>
-    <row r="429" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A429" s="66" t="s">
+    <row r="446" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A446" s="66" t="s">
         <v>822</v>
       </c>
-      <c r="B429" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C429" s="22" t="s">
+      <c r="B446" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C446" s="22" t="s">
         <v>604</v>
       </c>
-      <c r="D429" s="16" t="s">
+      <c r="D446" s="16" t="s">
         <v>234</v>
       </c>
-      <c r="E429" s="28" t="s">
+      <c r="E446" s="28" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="430" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A430" s="34" t="s">
+    <row r="447" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A447" s="34" t="s">
         <v>787</v>
       </c>
-      <c r="B430" s="55" t="s">
+      <c r="B447" s="55" t="s">
         <v>764</v>
       </c>
-      <c r="C430" s="34" t="s">
+      <c r="C447" s="34" t="s">
         <v>790</v>
       </c>
-      <c r="D430" s="34"/>
-      <c r="E430" s="40"/>
-    </row>
-    <row r="431" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A431" s="87" t="s">
+      <c r="D447" s="34"/>
+      <c r="E447" s="40"/>
+    </row>
+    <row r="448" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A448" s="87" t="s">
         <v>21</v>
       </c>
-      <c r="B431" s="54" t="s">
-        <v>719</v>
-      </c>
-      <c r="C431" s="22" t="s">
+      <c r="B448" s="54" t="s">
+        <v>719</v>
+      </c>
+      <c r="C448" s="22" t="s">
         <v>605</v>
       </c>
-      <c r="D431" s="22"/>
-      <c r="E431" s="27"/>
-    </row>
-    <row r="432" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A432" s="87" t="s">
+      <c r="D448" s="22"/>
+      <c r="E448" s="27"/>
+    </row>
+    <row r="449" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A449" s="87" t="s">
         <v>24</v>
       </c>
-      <c r="B432" s="54" t="s">
+      <c r="B449" s="54" t="s">
         <v>720</v>
       </c>
-      <c r="C432" s="22" t="s">
+      <c r="C449" s="22" t="s">
         <v>606</v>
       </c>
-      <c r="D432" s="22" t="s">
+      <c r="D449" s="22" t="s">
         <v>228</v>
       </c>
-      <c r="E432" s="28">
+      <c r="E449" s="28">
         <v>1</v>
       </c>
     </row>
-    <row r="433" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A433" s="87" t="s">
+    <row r="450" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A450" s="87" t="s">
         <v>29</v>
       </c>
-      <c r="B433" s="54" t="s">
-        <v>719</v>
-      </c>
-      <c r="C433" s="22" t="s">
+      <c r="B450" s="54" t="s">
+        <v>719</v>
+      </c>
+      <c r="C450" s="22" t="s">
         <v>607</v>
       </c>
-      <c r="D433" s="22" t="s">
-        <v>230</v>
-      </c>
-      <c r="E433" s="28" t="s">
+      <c r="D450" s="22" t="s">
+        <v>230</v>
+      </c>
+      <c r="E450" s="28" t="s">
         <v>608</v>
       </c>
     </row>
-    <row r="434" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A434" s="87" t="s">
+    <row r="451" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A451" s="87" t="s">
         <v>789</v>
       </c>
-      <c r="B434" s="54" t="s">
-        <v>719</v>
-      </c>
-      <c r="C434" s="22" t="s">
+      <c r="B451" s="54" t="s">
+        <v>719</v>
+      </c>
+      <c r="C451" s="22" t="s">
         <v>791</v>
       </c>
-      <c r="D434" s="22" t="s">
+      <c r="D451" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="E434" s="28">
+      <c r="E451" s="28">
         <v>100</v>
       </c>
     </row>
-    <row r="435" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A435" s="88" t="s">
+    <row r="452" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A452" s="88" t="s">
         <v>823</v>
       </c>
-      <c r="B435" s="54" t="s">
-        <v>719</v>
-      </c>
-      <c r="C435" s="22" t="s">
+      <c r="B452" s="54" t="s">
+        <v>719</v>
+      </c>
+      <c r="C452" s="22" t="s">
         <v>792</v>
       </c>
-      <c r="D435" s="22" t="s">
+      <c r="D452" s="22" t="s">
         <v>234</v>
       </c>
-      <c r="E435" s="28" t="s">
+      <c r="E452" s="28" t="s">
         <v>609</v>
       </c>
     </row>
-    <row r="436" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A436" s="87" t="s">
+    <row r="453" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A453" s="87" t="s">
         <v>183</v>
-      </c>
-      <c r="B436" s="54" t="s">
-        <v>720</v>
-      </c>
-      <c r="C436" s="22" t="s">
-        <v>833</v>
-      </c>
-      <c r="D436" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="E436" s="30" t="s">
-        <v>611</v>
-      </c>
-    </row>
-    <row r="437" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A437" s="88" t="s">
-        <v>822</v>
-      </c>
-      <c r="B437" s="54" t="s">
-        <v>719</v>
-      </c>
-      <c r="C437" s="22" t="s">
-        <v>612</v>
-      </c>
-      <c r="D437" s="22" t="s">
-        <v>234</v>
-      </c>
-      <c r="E437" s="28" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="438" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A438" s="87" t="s">
-        <v>33</v>
-      </c>
-      <c r="B438" s="54" t="s">
-        <v>719</v>
-      </c>
-      <c r="C438" s="22" t="s">
-        <v>613</v>
-      </c>
-      <c r="D438" s="22" t="s">
-        <v>228</v>
-      </c>
-      <c r="E438" s="28" t="s">
-        <v>614</v>
-      </c>
-    </row>
-    <row r="439" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A439" s="68" t="s">
-        <v>193</v>
-      </c>
-      <c r="B439" s="62" t="s">
-        <v>719</v>
-      </c>
-      <c r="C439" s="60" t="s">
-        <v>834</v>
-      </c>
-      <c r="D439" s="60"/>
-      <c r="E439" s="58"/>
-    </row>
-    <row r="440" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A440" s="80" t="s">
-        <v>194</v>
-      </c>
-      <c r="B440" s="54" t="s">
-        <v>719</v>
-      </c>
-      <c r="C440" s="22" t="s">
-        <v>616</v>
-      </c>
-      <c r="D440" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="E440" s="28">
-        <v>43013</v>
-      </c>
-    </row>
-    <row r="441" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A441" s="80" t="s">
-        <v>195</v>
-      </c>
-      <c r="B441" s="54" t="s">
-        <v>719</v>
-      </c>
-      <c r="C441" s="22" t="s">
-        <v>617</v>
-      </c>
-      <c r="D441" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="E441" s="28">
-        <v>43023</v>
-      </c>
-    </row>
-    <row r="442" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A442" s="68" t="s">
-        <v>196</v>
-      </c>
-      <c r="B442" s="62" t="s">
-        <v>719</v>
-      </c>
-      <c r="C442" s="60"/>
-      <c r="D442" s="60"/>
-      <c r="E442" s="58"/>
-    </row>
-    <row r="443" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A443" s="80" t="s">
-        <v>197</v>
-      </c>
-      <c r="B443" s="54" t="s">
-        <v>719</v>
-      </c>
-      <c r="C443" s="22" t="s">
-        <v>618</v>
-      </c>
-      <c r="D443" s="22" t="s">
-        <v>228</v>
-      </c>
-      <c r="E443" s="28">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="444" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A444" s="80" t="s">
-        <v>198</v>
-      </c>
-      <c r="B444" s="54" t="s">
-        <v>719</v>
-      </c>
-      <c r="C444" s="22" t="s">
-        <v>619</v>
-      </c>
-      <c r="D444" s="22" t="s">
-        <v>228</v>
-      </c>
-      <c r="E444" s="28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="445" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A445" s="70" t="s">
-        <v>35</v>
-      </c>
-      <c r="B445" s="62" t="s">
-        <v>719</v>
-      </c>
-      <c r="C445" s="60"/>
-      <c r="D445" s="60"/>
-      <c r="E445" s="58"/>
-    </row>
-    <row r="446" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A446" s="89" t="s">
-        <v>21</v>
-      </c>
-      <c r="B446" s="54" t="s">
-        <v>719</v>
-      </c>
-      <c r="C446" s="22" t="s">
-        <v>605</v>
-      </c>
-      <c r="D446" s="22"/>
-      <c r="E446" s="27"/>
-    </row>
-    <row r="447" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A447" s="71" t="s">
-        <v>24</v>
-      </c>
-      <c r="B447" s="54" t="s">
-        <v>719</v>
-      </c>
-      <c r="C447" s="22" t="s">
-        <v>620</v>
-      </c>
-      <c r="D447" s="22" t="s">
-        <v>230</v>
-      </c>
-      <c r="E447" s="28" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="448" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A448" s="71" t="s">
-        <v>36</v>
-      </c>
-      <c r="B448" s="54" t="s">
-        <v>719</v>
-      </c>
-      <c r="C448" s="22" t="s">
-        <v>622</v>
-      </c>
-      <c r="D448" s="22" t="s">
-        <v>230</v>
-      </c>
-      <c r="E448" s="28" t="s">
-        <v>623</v>
-      </c>
-    </row>
-    <row r="449" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A449" s="71" t="s">
-        <v>25</v>
-      </c>
-      <c r="B449" s="54" t="s">
-        <v>719</v>
-      </c>
-      <c r="C449" s="22" t="s">
-        <v>624</v>
-      </c>
-      <c r="D449" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="E449" s="28" t="s">
-        <v>733</v>
-      </c>
-    </row>
-    <row r="450" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A450" s="68" t="s">
-        <v>199</v>
-      </c>
-      <c r="B450" s="62" t="s">
-        <v>719</v>
-      </c>
-      <c r="C450" s="60"/>
-      <c r="D450" s="60"/>
-      <c r="E450" s="58"/>
-    </row>
-    <row r="451" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A451" s="66" t="s">
-        <v>197</v>
-      </c>
-      <c r="B451" s="54" t="s">
-        <v>720</v>
-      </c>
-      <c r="C451" s="22" t="s">
-        <v>625</v>
-      </c>
-      <c r="D451" s="22" t="s">
-        <v>228</v>
-      </c>
-      <c r="E451" s="28">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="452" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A452" s="68" t="s">
-        <v>200</v>
-      </c>
-      <c r="B452" s="62" t="s">
-        <v>719</v>
-      </c>
-      <c r="C452" s="60"/>
-      <c r="D452" s="60"/>
-      <c r="E452" s="58"/>
-    </row>
-    <row r="453" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A453" s="66" t="s">
-        <v>24</v>
       </c>
       <c r="B453" s="54" t="s">
         <v>720</v>
       </c>
       <c r="C453" s="22" t="s">
-        <v>626</v>
+        <v>833</v>
       </c>
       <c r="D453" s="22" t="s">
-        <v>230</v>
-      </c>
-      <c r="E453" s="28" t="s">
-        <v>765</v>
+        <v>15</v>
+      </c>
+      <c r="E453" s="30" t="s">
+        <v>611</v>
       </c>
     </row>
     <row r="454" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A454" s="66" t="s">
-        <v>25</v>
+      <c r="A454" s="88" t="s">
+        <v>822</v>
       </c>
       <c r="B454" s="54" t="s">
         <v>719</v>
       </c>
       <c r="C454" s="22" t="s">
-        <v>627</v>
+        <v>612</v>
       </c>
       <c r="D454" s="22" t="s">
+        <v>234</v>
+      </c>
+      <c r="E454" s="28" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="455" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A455" s="87" t="s">
+        <v>33</v>
+      </c>
+      <c r="B455" s="54" t="s">
+        <v>719</v>
+      </c>
+      <c r="C455" s="22" t="s">
+        <v>613</v>
+      </c>
+      <c r="D455" s="22" t="s">
+        <v>228</v>
+      </c>
+      <c r="E455" s="28" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="456" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A456" s="68" t="s">
+        <v>193</v>
+      </c>
+      <c r="B456" s="62" t="s">
+        <v>719</v>
+      </c>
+      <c r="C456" s="60" t="s">
+        <v>834</v>
+      </c>
+      <c r="D456" s="60"/>
+      <c r="E456" s="58"/>
+    </row>
+    <row r="457" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A457" s="80" t="s">
+        <v>194</v>
+      </c>
+      <c r="B457" s="54" t="s">
+        <v>719</v>
+      </c>
+      <c r="C457" s="22" t="s">
+        <v>616</v>
+      </c>
+      <c r="D457" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="E454" s="28" t="s">
-        <v>733</v>
-      </c>
-    </row>
-    <row r="455" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A455" s="68" t="s">
-        <v>200</v>
-      </c>
-      <c r="B455" s="62" t="s">
-        <v>721</v>
-      </c>
-      <c r="C455" s="60"/>
-      <c r="D455" s="60"/>
-      <c r="E455" s="58"/>
-    </row>
-    <row r="456" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A456" s="66" t="s">
-        <v>24</v>
-      </c>
-      <c r="B456" s="54" t="s">
-        <v>720</v>
-      </c>
-      <c r="C456" s="22" t="s">
-        <v>628</v>
-      </c>
-      <c r="D456" s="22" t="s">
-        <v>230</v>
-      </c>
-      <c r="E456" s="28" t="s">
-        <v>629</v>
-      </c>
-    </row>
-    <row r="457" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A457" s="66" t="s">
-        <v>24</v>
-      </c>
-      <c r="B457" s="54" t="s">
-        <v>719</v>
-      </c>
-      <c r="C457" s="22" t="s">
-        <v>630</v>
-      </c>
-      <c r="D457" s="22" t="s">
-        <v>234</v>
-      </c>
-      <c r="E457" s="28" t="s">
-        <v>631</v>
-      </c>
-    </row>
-    <row r="458" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A458" s="66" t="s">
-        <v>25</v>
+      <c r="E457" s="28">
+        <v>43013</v>
+      </c>
+    </row>
+    <row r="458" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A458" s="80" t="s">
+        <v>195</v>
       </c>
       <c r="B458" s="54" t="s">
         <v>719</v>
       </c>
       <c r="C458" s="22" t="s">
-        <v>632</v>
+        <v>617</v>
       </c>
       <c r="D458" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="E458" s="28" t="s">
+      <c r="E458" s="28">
+        <v>43023</v>
+      </c>
+    </row>
+    <row r="459" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A459" s="68" t="s">
+        <v>196</v>
+      </c>
+      <c r="B459" s="62" t="s">
+        <v>719</v>
+      </c>
+      <c r="C459" s="60"/>
+      <c r="D459" s="60"/>
+      <c r="E459" s="58"/>
+    </row>
+    <row r="460" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A460" s="80" t="s">
+        <v>197</v>
+      </c>
+      <c r="B460" s="54" t="s">
+        <v>719</v>
+      </c>
+      <c r="C460" s="22" t="s">
+        <v>618</v>
+      </c>
+      <c r="D460" s="22" t="s">
+        <v>228</v>
+      </c>
+      <c r="E460" s="28">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="461" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A461" s="80" t="s">
+        <v>198</v>
+      </c>
+      <c r="B461" s="54" t="s">
+        <v>719</v>
+      </c>
+      <c r="C461" s="22" t="s">
+        <v>619</v>
+      </c>
+      <c r="D461" s="22" t="s">
+        <v>228</v>
+      </c>
+      <c r="E461" s="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="462" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A462" s="70" t="s">
+        <v>35</v>
+      </c>
+      <c r="B462" s="62" t="s">
+        <v>719</v>
+      </c>
+      <c r="C462" s="60"/>
+      <c r="D462" s="60"/>
+      <c r="E462" s="58"/>
+    </row>
+    <row r="463" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A463" s="89" t="s">
+        <v>21</v>
+      </c>
+      <c r="B463" s="54" t="s">
+        <v>719</v>
+      </c>
+      <c r="C463" s="22" t="s">
+        <v>605</v>
+      </c>
+      <c r="D463" s="22"/>
+      <c r="E463" s="27"/>
+    </row>
+    <row r="464" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A464" s="71" t="s">
+        <v>24</v>
+      </c>
+      <c r="B464" s="54" t="s">
+        <v>719</v>
+      </c>
+      <c r="C464" s="22" t="s">
+        <v>620</v>
+      </c>
+      <c r="D464" s="22" t="s">
+        <v>230</v>
+      </c>
+      <c r="E464" s="28" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="465" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A465" s="71" t="s">
+        <v>36</v>
+      </c>
+      <c r="B465" s="54" t="s">
+        <v>719</v>
+      </c>
+      <c r="C465" s="22" t="s">
+        <v>622</v>
+      </c>
+      <c r="D465" s="22" t="s">
+        <v>230</v>
+      </c>
+      <c r="E465" s="28" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="466" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A466" s="71" t="s">
+        <v>25</v>
+      </c>
+      <c r="B466" s="54" t="s">
+        <v>719</v>
+      </c>
+      <c r="C466" s="22" t="s">
+        <v>624</v>
+      </c>
+      <c r="D466" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E466" s="28" t="s">
         <v>733</v>
       </c>
     </row>
-    <row r="459" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A459" s="66" t="s">
+    <row r="467" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A467" s="68" t="s">
+        <v>199</v>
+      </c>
+      <c r="B467" s="62" t="s">
+        <v>719</v>
+      </c>
+      <c r="C467" s="60"/>
+      <c r="D467" s="60"/>
+      <c r="E467" s="58"/>
+    </row>
+    <row r="468" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A468" s="66" t="s">
+        <v>197</v>
+      </c>
+      <c r="B468" s="54" t="s">
+        <v>720</v>
+      </c>
+      <c r="C468" s="22" t="s">
+        <v>625</v>
+      </c>
+      <c r="D468" s="22" t="s">
+        <v>228</v>
+      </c>
+      <c r="E468" s="28">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="469" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A469" s="68" t="s">
+        <v>200</v>
+      </c>
+      <c r="B469" s="62" t="s">
+        <v>719</v>
+      </c>
+      <c r="C469" s="60"/>
+      <c r="D469" s="60"/>
+      <c r="E469" s="58"/>
+    </row>
+    <row r="470" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A470" s="66" t="s">
+        <v>24</v>
+      </c>
+      <c r="B470" s="54" t="s">
+        <v>720</v>
+      </c>
+      <c r="C470" s="22" t="s">
+        <v>626</v>
+      </c>
+      <c r="D470" s="22" t="s">
+        <v>230</v>
+      </c>
+      <c r="E470" s="28" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="471" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A471" s="66" t="s">
+        <v>25</v>
+      </c>
+      <c r="B471" s="54" t="s">
+        <v>719</v>
+      </c>
+      <c r="C471" s="22" t="s">
+        <v>627</v>
+      </c>
+      <c r="D471" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E471" s="28" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="472" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A472" s="68" t="s">
+        <v>200</v>
+      </c>
+      <c r="B472" s="62" t="s">
+        <v>721</v>
+      </c>
+      <c r="C472" s="60"/>
+      <c r="D472" s="60"/>
+      <c r="E472" s="58"/>
+    </row>
+    <row r="473" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A473" s="66" t="s">
+        <v>24</v>
+      </c>
+      <c r="B473" s="54" t="s">
+        <v>720</v>
+      </c>
+      <c r="C473" s="22" t="s">
+        <v>628</v>
+      </c>
+      <c r="D473" s="22" t="s">
+        <v>230</v>
+      </c>
+      <c r="E473" s="28" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="474" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A474" s="66" t="s">
+        <v>24</v>
+      </c>
+      <c r="B474" s="54" t="s">
+        <v>719</v>
+      </c>
+      <c r="C474" s="22" t="s">
+        <v>630</v>
+      </c>
+      <c r="D474" s="22" t="s">
+        <v>234</v>
+      </c>
+      <c r="E474" s="28" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="475" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A475" s="66" t="s">
+        <v>25</v>
+      </c>
+      <c r="B475" s="54" t="s">
+        <v>719</v>
+      </c>
+      <c r="C475" s="22" t="s">
+        <v>632</v>
+      </c>
+      <c r="D475" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E475" s="28" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="476" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A476" s="66" t="s">
         <v>26</v>
       </c>
-      <c r="B459" s="54" t="s">
-        <v>719</v>
-      </c>
-      <c r="C459" s="22" t="s">
+      <c r="B476" s="54" t="s">
+        <v>719</v>
+      </c>
+      <c r="C476" s="22" t="s">
         <v>633</v>
       </c>
-      <c r="D459" s="22" t="s">
+      <c r="D476" s="22" t="s">
         <v>634</v>
       </c>
-      <c r="E459" s="28" t="s">
+      <c r="E476" s="28" t="s">
         <v>635</v>
       </c>
     </row>
-    <row r="460" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A460" s="66" t="s">
+    <row r="477" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A477" s="66" t="s">
         <v>44</v>
       </c>
-      <c r="B460" s="54" t="s">
-        <v>719</v>
-      </c>
-      <c r="C460" s="22" t="s">
+      <c r="B477" s="54" t="s">
+        <v>719</v>
+      </c>
+      <c r="C477" s="22" t="s">
         <v>835</v>
       </c>
-      <c r="D460" s="22" t="s">
+      <c r="D477" s="22" t="s">
         <v>234</v>
       </c>
-      <c r="E460" s="28" t="s">
+      <c r="E477" s="28" t="s">
         <v>637</v>
       </c>
     </row>
-    <row r="461" spans="1:5" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A461" s="61" t="s">
+    <row r="478" spans="1:5" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A478" s="61" t="s">
         <v>122</v>
       </c>
-      <c r="B461" s="50" t="s">
-        <v>719</v>
-      </c>
-      <c r="C461" s="60" t="s">
+      <c r="B478" s="50" t="s">
+        <v>719</v>
+      </c>
+      <c r="C478" s="60" t="s">
         <v>836</v>
       </c>
-      <c r="D461" s="57"/>
-      <c r="E461" s="58"/>
-    </row>
-    <row r="462" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A462" s="66" t="s">
+      <c r="D478" s="57"/>
+      <c r="E478" s="58"/>
+    </row>
+    <row r="479" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A479" s="66" t="s">
         <v>201</v>
       </c>
-      <c r="B462" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C462" s="22" t="s">
+      <c r="B479" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C479" s="22" t="s">
         <v>638</v>
       </c>
-      <c r="D462" s="22" t="s">
+      <c r="D479" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="E462" s="27">
+      <c r="E479" s="27">
         <v>1</v>
       </c>
     </row>
-    <row r="463" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A463" s="71" t="s">
+    <row r="480" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A480" s="71" t="s">
         <v>823</v>
       </c>
-      <c r="B463" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C463" s="22" t="s">
+      <c r="B480" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C480" s="22" t="s">
         <v>639</v>
       </c>
-      <c r="D463" s="16" t="s">
+      <c r="D480" s="16" t="s">
         <v>234</v>
       </c>
-      <c r="E463" s="28" t="s">
+      <c r="E480" s="28" t="s">
         <v>609</v>
       </c>
     </row>
-    <row r="464" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A464" s="66" t="s">
+    <row r="481" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A481" s="66" t="s">
         <v>123</v>
       </c>
-      <c r="B464" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C464" s="22" t="s">
+      <c r="B481" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C481" s="22" t="s">
         <v>640</v>
       </c>
-      <c r="D464" s="16" t="s">
+      <c r="D481" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="E464" s="28" t="s">
+      <c r="E481" s="28" t="s">
         <v>733</v>
       </c>
     </row>
-    <row r="465" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A465" s="70" t="s">
+    <row r="482" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A482" s="70" t="s">
         <v>125</v>
       </c>
-      <c r="B465" s="50" t="s">
-        <v>719</v>
-      </c>
-      <c r="C465" s="60"/>
-      <c r="D465" s="57"/>
-      <c r="E465" s="58"/>
-    </row>
-    <row r="466" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A466" s="71" t="s">
+      <c r="B482" s="50" t="s">
+        <v>719</v>
+      </c>
+      <c r="C482" s="60"/>
+      <c r="D482" s="57"/>
+      <c r="E482" s="58"/>
+    </row>
+    <row r="483" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A483" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="B466" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C466" s="22" t="s">
+      <c r="B483" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C483" s="22" t="s">
         <v>435</v>
       </c>
-      <c r="D466" s="16" t="s">
+      <c r="D483" s="16" t="s">
         <v>228</v>
       </c>
-      <c r="E466" s="28" t="s">
+      <c r="E483" s="28" t="s">
         <v>750</v>
       </c>
     </row>
-    <row r="467" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A467" s="72" t="s">
+    <row r="484" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A484" s="72" t="s">
         <v>820</v>
       </c>
-      <c r="B467" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C467" s="22" t="s">
+      <c r="B484" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C484" s="22" t="s">
         <v>641</v>
       </c>
-      <c r="D467" s="16" t="s">
+      <c r="D484" s="16" t="s">
         <v>234</v>
       </c>
-      <c r="E467" s="30" t="s">
+      <c r="E484" s="30" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="468" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A468" s="70" t="s">
+    <row r="485" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A485" s="70" t="s">
         <v>127</v>
       </c>
-      <c r="B468" s="50" t="s">
-        <v>719</v>
-      </c>
-      <c r="C468" s="60" t="s">
+      <c r="B485" s="50" t="s">
+        <v>719</v>
+      </c>
+      <c r="C485" s="60" t="s">
         <v>439</v>
       </c>
-      <c r="D468" s="57"/>
-      <c r="E468" s="58"/>
-    </row>
-    <row r="469" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A469" s="71" t="s">
-        <v>60</v>
-      </c>
-      <c r="B469" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C469" s="22" t="s">
-        <v>642</v>
-      </c>
-      <c r="D469" s="16" t="s">
-        <v>230</v>
-      </c>
-      <c r="E469" s="28" t="s">
-        <v>643</v>
-      </c>
-    </row>
-    <row r="470" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A470" s="71" t="s">
-        <v>61</v>
-      </c>
-      <c r="B470" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C470" s="22" t="s">
-        <v>644</v>
-      </c>
-      <c r="D470" s="16" t="s">
-        <v>230</v>
-      </c>
-      <c r="E470" s="28" t="s">
-        <v>645</v>
-      </c>
-    </row>
-    <row r="471" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A471" s="71" t="s">
-        <v>63</v>
-      </c>
-      <c r="B471" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C471" s="22" t="s">
-        <v>444</v>
-      </c>
-      <c r="D471" s="16" t="s">
-        <v>230</v>
-      </c>
-      <c r="E471" s="28"/>
-    </row>
-    <row r="472" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A472" s="71" t="s">
-        <v>64</v>
-      </c>
-      <c r="B472" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C472" s="22" t="s">
-        <v>646</v>
-      </c>
-      <c r="D472" s="16" t="s">
-        <v>230</v>
-      </c>
-      <c r="E472" s="28" t="s">
-        <v>769</v>
-      </c>
-    </row>
-    <row r="473" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A473" s="71" t="s">
-        <v>65</v>
-      </c>
-      <c r="B473" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C473" s="22" t="s">
-        <v>647</v>
-      </c>
-      <c r="D473" s="16" t="s">
-        <v>230</v>
-      </c>
-      <c r="E473" s="28" t="s">
-        <v>770</v>
-      </c>
-    </row>
-    <row r="474" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A474" s="71" t="s">
-        <v>66</v>
-      </c>
-      <c r="B474" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C474" s="22" t="s">
-        <v>648</v>
-      </c>
-      <c r="D474" s="16" t="s">
-        <v>230</v>
-      </c>
-      <c r="E474" s="28" t="s">
-        <v>768</v>
-      </c>
-    </row>
-    <row r="475" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A475" s="71" t="s">
-        <v>67</v>
-      </c>
-      <c r="B475" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C475" s="22" t="s">
-        <v>649</v>
-      </c>
-      <c r="D475" s="16" t="s">
-        <v>230</v>
-      </c>
-      <c r="E475" s="28">
-        <v>86756</v>
-      </c>
-    </row>
-    <row r="476" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A476" s="71" t="s">
-        <v>68</v>
-      </c>
-      <c r="B476" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C476" s="22" t="s">
-        <v>650</v>
-      </c>
-      <c r="D476" s="16" t="s">
-        <v>230</v>
-      </c>
-      <c r="E476" s="28" t="s">
-        <v>651</v>
-      </c>
-    </row>
-    <row r="477" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A477" s="73" t="s">
-        <v>71</v>
-      </c>
-      <c r="B477" s="50" t="s">
-        <v>719</v>
-      </c>
-      <c r="C477" s="60"/>
-      <c r="D477" s="57"/>
-      <c r="E477" s="58"/>
-    </row>
-    <row r="478" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A478" s="72" t="s">
-        <v>72</v>
-      </c>
-      <c r="B478" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C478" s="22" t="s">
-        <v>652</v>
-      </c>
-      <c r="D478" s="16" t="s">
-        <v>234</v>
-      </c>
-      <c r="E478" s="28" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="479" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A479" s="72" t="s">
-        <v>57</v>
-      </c>
-      <c r="B479" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C479" s="22" t="s">
-        <v>653</v>
-      </c>
-      <c r="D479" s="16" t="s">
-        <v>230</v>
-      </c>
-      <c r="E479" s="28" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="480" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A480" s="61" t="s">
-        <v>170</v>
-      </c>
-      <c r="B480" s="50" t="s">
-        <v>719</v>
-      </c>
-      <c r="C480" s="60"/>
-      <c r="D480" s="57"/>
-      <c r="E480" s="58"/>
-    </row>
-    <row r="481" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A481" s="66" t="s">
-        <v>171</v>
-      </c>
-      <c r="B481" s="36" t="s">
-        <v>720</v>
-      </c>
-      <c r="C481" s="22" t="s">
-        <v>662</v>
-      </c>
-      <c r="D481" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="E481" s="28" t="s">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="482" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A482" s="71" t="s">
-        <v>822</v>
-      </c>
-      <c r="B482" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C482" s="24" t="s">
-        <v>663</v>
-      </c>
-      <c r="D482" s="16" t="s">
-        <v>234</v>
-      </c>
-      <c r="E482" s="28" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="483" spans="1:5" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A483" s="70" t="s">
-        <v>178</v>
-      </c>
-      <c r="B483" s="50" t="s">
-        <v>719</v>
-      </c>
-      <c r="C483" s="60" t="s">
-        <v>837</v>
-      </c>
-      <c r="D483" s="57"/>
-      <c r="E483" s="58"/>
-    </row>
-    <row r="484" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A484" s="71" t="s">
-        <v>179</v>
-      </c>
-      <c r="B484" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C484" s="22" t="s">
-        <v>665</v>
-      </c>
-      <c r="D484" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="E484" s="27" t="s">
-        <v>566</v>
-      </c>
-    </row>
-    <row r="485" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A485" s="72" t="s">
-        <v>822</v>
-      </c>
-      <c r="B485" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C485" s="24" t="s">
-        <v>666</v>
-      </c>
-      <c r="D485" s="16" t="s">
-        <v>234</v>
-      </c>
-      <c r="E485" s="27" t="s">
-        <v>237</v>
-      </c>
+      <c r="D485" s="57"/>
+      <c r="E485" s="58"/>
     </row>
     <row r="486" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A486" s="71" t="s">
+        <v>60</v>
+      </c>
+      <c r="B486" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C486" s="22" t="s">
+        <v>642</v>
+      </c>
+      <c r="D486" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="E486" s="28" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="487" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A487" s="71" t="s">
+        <v>61</v>
+      </c>
+      <c r="B487" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C487" s="22" t="s">
+        <v>644</v>
+      </c>
+      <c r="D487" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="E487" s="28" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="488" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A488" s="71" t="s">
+        <v>63</v>
+      </c>
+      <c r="B488" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C488" s="22" t="s">
+        <v>444</v>
+      </c>
+      <c r="D488" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="E488" s="28"/>
+    </row>
+    <row r="489" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A489" s="71" t="s">
+        <v>64</v>
+      </c>
+      <c r="B489" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C489" s="22" t="s">
+        <v>646</v>
+      </c>
+      <c r="D489" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="E489" s="28" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="490" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A490" s="71" t="s">
+        <v>65</v>
+      </c>
+      <c r="B490" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C490" s="22" t="s">
+        <v>647</v>
+      </c>
+      <c r="D490" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="E490" s="28" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="491" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A491" s="71" t="s">
+        <v>66</v>
+      </c>
+      <c r="B491" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C491" s="22" t="s">
+        <v>648</v>
+      </c>
+      <c r="D491" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="E491" s="28" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="492" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A492" s="71" t="s">
+        <v>67</v>
+      </c>
+      <c r="B492" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C492" s="22" t="s">
+        <v>649</v>
+      </c>
+      <c r="D492" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="E492" s="28">
+        <v>86756</v>
+      </c>
+    </row>
+    <row r="493" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A493" s="71" t="s">
+        <v>68</v>
+      </c>
+      <c r="B493" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C493" s="22" t="s">
+        <v>650</v>
+      </c>
+      <c r="D493" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="E493" s="28" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="494" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A494" s="73" t="s">
+        <v>71</v>
+      </c>
+      <c r="B494" s="50" t="s">
+        <v>719</v>
+      </c>
+      <c r="C494" s="60"/>
+      <c r="D494" s="57"/>
+      <c r="E494" s="58"/>
+    </row>
+    <row r="495" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A495" s="72" t="s">
+        <v>72</v>
+      </c>
+      <c r="B495" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C495" s="22" t="s">
+        <v>652</v>
+      </c>
+      <c r="D495" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="E495" s="28" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="496" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A496" s="72" t="s">
+        <v>57</v>
+      </c>
+      <c r="B496" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C496" s="22" t="s">
+        <v>653</v>
+      </c>
+      <c r="D496" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="E496" s="28" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="497" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A497" s="61" t="s">
+        <v>170</v>
+      </c>
+      <c r="B497" s="50" t="s">
+        <v>719</v>
+      </c>
+      <c r="C497" s="60"/>
+      <c r="D497" s="57"/>
+      <c r="E497" s="58"/>
+    </row>
+    <row r="498" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A498" s="66" t="s">
         <v>171</v>
       </c>
-      <c r="B486" s="36" t="s">
+      <c r="B498" s="36" t="s">
         <v>720</v>
       </c>
-      <c r="C486" s="22" t="s">
+      <c r="C498" s="22" t="s">
+        <v>662</v>
+      </c>
+      <c r="D498" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E498" s="28" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="499" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A499" s="71" t="s">
+        <v>822</v>
+      </c>
+      <c r="B499" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C499" s="24" t="s">
+        <v>663</v>
+      </c>
+      <c r="D499" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="E499" s="28" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="500" spans="1:5" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A500" s="70" t="s">
+        <v>178</v>
+      </c>
+      <c r="B500" s="50" t="s">
+        <v>719</v>
+      </c>
+      <c r="C500" s="60" t="s">
+        <v>837</v>
+      </c>
+      <c r="D500" s="57"/>
+      <c r="E500" s="58"/>
+    </row>
+    <row r="501" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A501" s="71" t="s">
+        <v>179</v>
+      </c>
+      <c r="B501" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C501" s="22" t="s">
+        <v>665</v>
+      </c>
+      <c r="D501" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E501" s="27" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="502" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A502" s="72" t="s">
+        <v>822</v>
+      </c>
+      <c r="B502" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C502" s="24" t="s">
+        <v>666</v>
+      </c>
+      <c r="D502" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="E502" s="27" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="503" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A503" s="71" t="s">
+        <v>171</v>
+      </c>
+      <c r="B503" s="36" t="s">
+        <v>720</v>
+      </c>
+      <c r="C503" s="22" t="s">
         <v>667</v>
       </c>
-      <c r="D486" s="16" t="s">
+      <c r="D503" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E486" s="27" t="s">
+      <c r="E503" s="27" t="s">
         <v>563</v>
       </c>
     </row>
-    <row r="487" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A487" s="72" t="s">
+    <row r="504" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A504" s="72" t="s">
         <v>822</v>
       </c>
-      <c r="B487" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C487" s="24" t="s">
+      <c r="B504" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C504" s="24" t="s">
         <v>668</v>
       </c>
-      <c r="D487" s="16" t="s">
-        <v>234</v>
-      </c>
-      <c r="E487" s="28" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="488" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A488" s="73" t="s">
-        <v>166</v>
-      </c>
-      <c r="B488" s="50" t="s">
-        <v>720</v>
-      </c>
-      <c r="C488" s="60"/>
-      <c r="D488" s="57"/>
-      <c r="E488" s="58"/>
-    </row>
-    <row r="489" spans="1:5" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A489" s="72" t="s">
-        <v>24</v>
-      </c>
-      <c r="B489" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C489" s="22" t="s">
-        <v>580</v>
-      </c>
-      <c r="D489" s="16" t="s">
-        <v>234</v>
-      </c>
-      <c r="E489" s="28" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="490" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A490" s="72" t="s">
-        <v>167</v>
-      </c>
-      <c r="B490" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C490" s="22" t="s">
-        <v>571</v>
-      </c>
-      <c r="D490" s="16" t="s">
-        <v>535</v>
-      </c>
-      <c r="E490" s="28">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="491" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A491" s="72" t="s">
-        <v>168</v>
-      </c>
-      <c r="B491" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C491" s="22" t="s">
-        <v>669</v>
-      </c>
-      <c r="D491" s="16" t="s">
-        <v>230</v>
-      </c>
-      <c r="E491" s="28"/>
-    </row>
-    <row r="492" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A492" s="72" t="s">
-        <v>180</v>
-      </c>
-      <c r="B492" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C492" s="22" t="s">
-        <v>670</v>
-      </c>
-      <c r="D492" s="16" t="s">
-        <v>230</v>
-      </c>
-      <c r="E492" s="28" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="493" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A493" s="75" t="s">
-        <v>75</v>
-      </c>
-      <c r="B493" s="50" t="s">
-        <v>720</v>
-      </c>
-      <c r="C493" s="60"/>
-      <c r="D493" s="57"/>
-      <c r="E493" s="58"/>
-    </row>
-    <row r="494" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A494" s="76" t="s">
-        <v>24</v>
-      </c>
-      <c r="B494" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C494" s="22" t="s">
-        <v>547</v>
-      </c>
-      <c r="D494" s="16" t="s">
-        <v>234</v>
-      </c>
-      <c r="E494" s="27" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="495" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A495" s="76" t="s">
-        <v>57</v>
-      </c>
-      <c r="B495" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C495" s="22" t="s">
-        <v>548</v>
-      </c>
-      <c r="D495" s="16" t="s">
-        <v>230</v>
-      </c>
-      <c r="E495" s="27" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="496" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A496" s="68" t="s">
-        <v>159</v>
-      </c>
-      <c r="B496" s="62" t="s">
-        <v>721</v>
-      </c>
-      <c r="C496" s="60" t="s">
-        <v>838</v>
-      </c>
-      <c r="D496" s="60"/>
-      <c r="E496" s="58"/>
-    </row>
-    <row r="497" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A497" s="65" t="s">
-        <v>160</v>
-      </c>
-      <c r="B497" s="54" t="s">
-        <v>720</v>
-      </c>
-      <c r="C497" s="22" t="s">
-        <v>655</v>
-      </c>
-      <c r="D497" s="22" t="s">
-        <v>234</v>
-      </c>
-      <c r="E497" s="27" t="s">
-        <v>656</v>
-      </c>
-    </row>
-    <row r="498" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A498" s="65" t="s">
-        <v>161</v>
-      </c>
-      <c r="B498" s="54" t="s">
-        <v>719</v>
-      </c>
-      <c r="C498" s="22" t="s">
-        <v>657</v>
-      </c>
-      <c r="D498" s="22" t="s">
-        <v>234</v>
-      </c>
-      <c r="E498" s="28">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="499" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A499" s="65" t="s">
-        <v>162</v>
-      </c>
-      <c r="B499" s="54" t="s">
-        <v>719</v>
-      </c>
-      <c r="C499" s="22" t="s">
-        <v>532</v>
-      </c>
-      <c r="D499" s="22" t="s">
-        <v>230</v>
-      </c>
-      <c r="E499" s="28" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="500" spans="1:5" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A500" s="65" t="s">
-        <v>163</v>
-      </c>
-      <c r="B500" s="54" t="s">
-        <v>719</v>
-      </c>
-      <c r="C500" s="22" t="s">
-        <v>658</v>
-      </c>
-      <c r="D500" s="22" t="s">
-        <v>535</v>
-      </c>
-      <c r="E500" s="28">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="501" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A501" s="65" t="s">
-        <v>164</v>
-      </c>
-      <c r="B501" s="54" t="s">
-        <v>720</v>
-      </c>
-      <c r="C501" s="22" t="s">
-        <v>659</v>
-      </c>
-      <c r="D501" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="E501" s="28" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="502" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A502" s="65" t="s">
-        <v>822</v>
-      </c>
-      <c r="B502" s="54" t="s">
-        <v>719</v>
-      </c>
-      <c r="C502" s="22" t="s">
-        <v>660</v>
-      </c>
-      <c r="D502" s="22" t="s">
-        <v>234</v>
-      </c>
-      <c r="E502" s="28" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="503" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A503" s="65" t="s">
-        <v>165</v>
-      </c>
-      <c r="B503" s="54" t="s">
-        <v>719</v>
-      </c>
-      <c r="C503" s="22" t="s">
-        <v>661</v>
-      </c>
-      <c r="D503" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="E503" s="28" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="504" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A504" s="65" t="s">
-        <v>822</v>
-      </c>
-      <c r="B504" s="54" t="s">
-        <v>719</v>
-      </c>
-      <c r="C504" s="22" t="s">
-        <v>539</v>
-      </c>
-      <c r="D504" s="22" t="s">
+      <c r="D504" s="16" t="s">
         <v>234</v>
       </c>
       <c r="E504" s="28" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="505" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A505" s="61" t="s">
-        <v>202</v>
+    <row r="505" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A505" s="73" t="s">
+        <v>166</v>
       </c>
       <c r="B505" s="50" t="s">
         <v>720</v>
       </c>
-      <c r="C505" s="60" t="s">
-        <v>839</v>
-      </c>
+      <c r="C505" s="60"/>
       <c r="D505" s="57"/>
       <c r="E505" s="58"/>
     </row>
-    <row r="506" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A506" s="81" t="s">
+    <row r="506" spans="1:5" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A506" s="72" t="s">
+        <v>24</v>
+      </c>
+      <c r="B506" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C506" s="22" t="s">
+        <v>580</v>
+      </c>
+      <c r="D506" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="E506" s="28" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="507" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A507" s="72" t="s">
+        <v>167</v>
+      </c>
+      <c r="B507" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C507" s="22" t="s">
+        <v>571</v>
+      </c>
+      <c r="D507" s="16" t="s">
+        <v>535</v>
+      </c>
+      <c r="E507" s="28">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="508" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A508" s="72" t="s">
+        <v>168</v>
+      </c>
+      <c r="B508" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C508" s="22" t="s">
+        <v>669</v>
+      </c>
+      <c r="D508" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="E508" s="28"/>
+    </row>
+    <row r="509" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A509" s="72" t="s">
+        <v>180</v>
+      </c>
+      <c r="B509" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C509" s="22" t="s">
+        <v>670</v>
+      </c>
+      <c r="D509" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="E509" s="28" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="510" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A510" s="75" t="s">
+        <v>75</v>
+      </c>
+      <c r="B510" s="50" t="s">
+        <v>720</v>
+      </c>
+      <c r="C510" s="60"/>
+      <c r="D510" s="57"/>
+      <c r="E510" s="58"/>
+    </row>
+    <row r="511" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A511" s="76" t="s">
+        <v>24</v>
+      </c>
+      <c r="B511" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C511" s="22" t="s">
+        <v>547</v>
+      </c>
+      <c r="D511" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="E511" s="27" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="512" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A512" s="76" t="s">
+        <v>57</v>
+      </c>
+      <c r="B512" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C512" s="22" t="s">
+        <v>548</v>
+      </c>
+      <c r="D512" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="E512" s="27" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="513" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A513" s="68" t="s">
+        <v>159</v>
+      </c>
+      <c r="B513" s="62" t="s">
+        <v>721</v>
+      </c>
+      <c r="C513" s="60" t="s">
+        <v>838</v>
+      </c>
+      <c r="D513" s="60"/>
+      <c r="E513" s="58"/>
+    </row>
+    <row r="514" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A514" s="65" t="s">
+        <v>160</v>
+      </c>
+      <c r="B514" s="54" t="s">
+        <v>720</v>
+      </c>
+      <c r="C514" s="22" t="s">
+        <v>655</v>
+      </c>
+      <c r="D514" s="22" t="s">
+        <v>234</v>
+      </c>
+      <c r="E514" s="27" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="515" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A515" s="65" t="s">
+        <v>161</v>
+      </c>
+      <c r="B515" s="54" t="s">
+        <v>719</v>
+      </c>
+      <c r="C515" s="22" t="s">
+        <v>657</v>
+      </c>
+      <c r="D515" s="22" t="s">
+        <v>234</v>
+      </c>
+      <c r="E515" s="28">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="516" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A516" s="65" t="s">
+        <v>162</v>
+      </c>
+      <c r="B516" s="54" t="s">
+        <v>719</v>
+      </c>
+      <c r="C516" s="22" t="s">
+        <v>532</v>
+      </c>
+      <c r="D516" s="22" t="s">
+        <v>230</v>
+      </c>
+      <c r="E516" s="28" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="517" spans="1:5" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A517" s="65" t="s">
+        <v>163</v>
+      </c>
+      <c r="B517" s="54" t="s">
+        <v>719</v>
+      </c>
+      <c r="C517" s="22" t="s">
+        <v>658</v>
+      </c>
+      <c r="D517" s="22" t="s">
+        <v>535</v>
+      </c>
+      <c r="E517" s="28">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="518" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A518" s="65" t="s">
+        <v>164</v>
+      </c>
+      <c r="B518" s="54" t="s">
+        <v>720</v>
+      </c>
+      <c r="C518" s="22" t="s">
+        <v>659</v>
+      </c>
+      <c r="D518" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="E518" s="28" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="519" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A519" s="65" t="s">
+        <v>822</v>
+      </c>
+      <c r="B519" s="54" t="s">
+        <v>719</v>
+      </c>
+      <c r="C519" s="22" t="s">
+        <v>660</v>
+      </c>
+      <c r="D519" s="22" t="s">
+        <v>234</v>
+      </c>
+      <c r="E519" s="28" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="520" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A520" s="65" t="s">
+        <v>165</v>
+      </c>
+      <c r="B520" s="54" t="s">
+        <v>719</v>
+      </c>
+      <c r="C520" s="22" t="s">
+        <v>661</v>
+      </c>
+      <c r="D520" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="E520" s="28" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="521" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A521" s="65" t="s">
+        <v>822</v>
+      </c>
+      <c r="B521" s="54" t="s">
+        <v>719</v>
+      </c>
+      <c r="C521" s="22" t="s">
+        <v>539</v>
+      </c>
+      <c r="D521" s="22" t="s">
+        <v>234</v>
+      </c>
+      <c r="E521" s="28" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="522" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A522" s="61" t="s">
+        <v>202</v>
+      </c>
+      <c r="B522" s="50" t="s">
+        <v>720</v>
+      </c>
+      <c r="C522" s="60" t="s">
+        <v>839</v>
+      </c>
+      <c r="D522" s="57"/>
+      <c r="E522" s="58"/>
+    </row>
+    <row r="523" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A523" s="81" t="s">
         <v>21</v>
       </c>
-      <c r="B506" s="50" t="s">
-        <v>719</v>
-      </c>
-      <c r="C506" s="60" t="s">
+      <c r="B523" s="50" t="s">
+        <v>719</v>
+      </c>
+      <c r="C523" s="60" t="s">
         <v>605</v>
       </c>
-      <c r="D506" s="60"/>
-      <c r="E506" s="60"/>
-    </row>
-    <row r="507" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A507" s="66" t="s">
+      <c r="D523" s="60"/>
+      <c r="E523" s="60"/>
+    </row>
+    <row r="524" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A524" s="66" t="s">
         <v>126</v>
       </c>
-      <c r="B507" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C507" s="22" t="s">
+      <c r="B524" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C524" s="22" t="s">
         <v>673</v>
       </c>
-      <c r="D507" s="22" t="s">
-        <v>230</v>
-      </c>
-      <c r="E507" s="28" t="s">
+      <c r="D524" s="22" t="s">
+        <v>230</v>
+      </c>
+      <c r="E524" s="28" t="s">
         <v>840</v>
       </c>
     </row>
-    <row r="508" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A508" s="66" t="s">
+    <row r="525" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A525" s="66" t="s">
         <v>57</v>
       </c>
-      <c r="B508" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C508" s="22" t="s">
+      <c r="B525" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C525" s="22" t="s">
         <v>674</v>
       </c>
-      <c r="D508" s="22" t="s">
-        <v>230</v>
-      </c>
-      <c r="E508" s="28" t="s">
+      <c r="D525" s="22" t="s">
+        <v>230</v>
+      </c>
+      <c r="E525" s="28" t="s">
         <v>675</v>
       </c>
     </row>
-    <row r="509" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A509" s="70" t="s">
+    <row r="526" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A526" s="70" t="s">
         <v>203</v>
       </c>
-      <c r="B509" s="50" t="s">
-        <v>719</v>
-      </c>
-      <c r="C509" s="60"/>
-      <c r="D509" s="57"/>
-      <c r="E509" s="58"/>
-    </row>
-    <row r="510" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A510" s="71" t="s">
+      <c r="B526" s="50" t="s">
+        <v>719</v>
+      </c>
+      <c r="C526" s="60"/>
+      <c r="D526" s="57"/>
+      <c r="E526" s="58"/>
+    </row>
+    <row r="527" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A527" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="B510" s="36" t="s">
+      <c r="B527" s="36" t="s">
         <v>720</v>
       </c>
-      <c r="C510" s="22" t="s">
+      <c r="C527" s="22" t="s">
         <v>676</v>
       </c>
-      <c r="D510" s="16" t="s">
+      <c r="D527" s="16" t="s">
         <v>228</v>
       </c>
-      <c r="E510" s="28">
+      <c r="E527" s="28">
         <v>123455</v>
       </c>
     </row>
-    <row r="511" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A511" s="70" t="s">
+    <row r="528" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A528" s="70" t="s">
         <v>204</v>
       </c>
-      <c r="B511" s="50" t="s">
-        <v>719</v>
-      </c>
-      <c r="C511" s="60"/>
-      <c r="D511" s="57"/>
-      <c r="E511" s="58"/>
-    </row>
-    <row r="512" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A512" s="71" t="s">
+      <c r="B528" s="50" t="s">
+        <v>719</v>
+      </c>
+      <c r="C528" s="60"/>
+      <c r="D528" s="57"/>
+      <c r="E528" s="58"/>
+    </row>
+    <row r="529" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A529" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="B512" s="36" t="s">
+      <c r="B529" s="36" t="s">
         <v>720</v>
       </c>
-      <c r="C512" s="22" t="s">
+      <c r="C529" s="22" t="s">
         <v>677</v>
       </c>
-      <c r="D512" s="16" t="s">
+      <c r="D529" s="16" t="s">
         <v>228</v>
       </c>
-      <c r="E512" s="28">
+      <c r="E529" s="28">
         <v>987342</v>
       </c>
     </row>
-    <row r="513" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A513" s="70" t="s">
+    <row r="530" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A530" s="70" t="s">
         <v>205</v>
       </c>
-      <c r="B513" s="50" t="s">
-        <v>719</v>
-      </c>
-      <c r="C513" s="60"/>
-      <c r="D513" s="57"/>
-      <c r="E513" s="58"/>
-    </row>
-    <row r="514" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A514" s="71" t="s">
+      <c r="B530" s="50" t="s">
+        <v>719</v>
+      </c>
+      <c r="C530" s="60"/>
+      <c r="D530" s="57"/>
+      <c r="E530" s="58"/>
+    </row>
+    <row r="531" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A531" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="B514" s="36" t="s">
+      <c r="B531" s="36" t="s">
         <v>720</v>
       </c>
-      <c r="C514" s="22" t="s">
+      <c r="C531" s="22" t="s">
         <v>678</v>
       </c>
-      <c r="D514" s="16" t="s">
+      <c r="D531" s="16" t="s">
         <v>228</v>
       </c>
-      <c r="E514" s="28" t="s">
+      <c r="E531" s="28" t="s">
         <v>679</v>
       </c>
     </row>
-    <row r="515" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A515" s="70" t="s">
+    <row r="532" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A532" s="70" t="s">
         <v>206</v>
       </c>
-      <c r="B515" s="50" t="s">
-        <v>719</v>
-      </c>
-      <c r="C515" s="60"/>
-      <c r="D515" s="57"/>
-      <c r="E515" s="58"/>
-    </row>
-    <row r="516" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A516" s="71" t="s">
-        <v>24</v>
-      </c>
-      <c r="B516" s="36" t="s">
-        <v>720</v>
-      </c>
-      <c r="C516" s="22" t="s">
-        <v>680</v>
-      </c>
-      <c r="D516" s="16" t="s">
-        <v>228</v>
-      </c>
-      <c r="E516" s="28">
-        <v>10986700</v>
-      </c>
-    </row>
-    <row r="517" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A517" s="72" t="s">
-        <v>820</v>
-      </c>
-      <c r="B517" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C517" s="22" t="s">
-        <v>681</v>
-      </c>
-      <c r="D517" s="16"/>
-      <c r="E517" s="30" t="s">
-        <v>682</v>
-      </c>
-    </row>
-    <row r="518" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A518" s="70" t="s">
-        <v>207</v>
-      </c>
-      <c r="B518" s="50" t="s">
-        <v>719</v>
-      </c>
-      <c r="C518" s="60"/>
-      <c r="D518" s="57"/>
-      <c r="E518" s="58"/>
-    </row>
-    <row r="519" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A519" s="71" t="s">
-        <v>72</v>
-      </c>
-      <c r="B519" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C519" s="22" t="s">
-        <v>683</v>
-      </c>
-      <c r="D519" s="16" t="s">
-        <v>234</v>
-      </c>
-      <c r="E519" s="28" t="s">
-        <v>684</v>
-      </c>
-    </row>
-    <row r="520" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A520" s="70" t="s">
-        <v>208</v>
-      </c>
-      <c r="B520" s="50" t="s">
-        <v>721</v>
-      </c>
-      <c r="C520" s="60"/>
-      <c r="D520" s="57"/>
-      <c r="E520" s="58"/>
-    </row>
-    <row r="521" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A521" s="71" t="s">
-        <v>209</v>
-      </c>
-      <c r="B521" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C521" s="22" t="s">
-        <v>685</v>
-      </c>
-      <c r="D521" s="16" t="s">
-        <v>228</v>
-      </c>
-      <c r="E521" s="28">
-        <v>9873242</v>
-      </c>
-    </row>
-    <row r="522" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A522" s="72" t="s">
-        <v>824</v>
-      </c>
-      <c r="B522" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C522" s="22" t="s">
-        <v>686</v>
-      </c>
-      <c r="D522" s="16" t="s">
-        <v>234</v>
-      </c>
-      <c r="E522" s="28" t="s">
-        <v>687</v>
-      </c>
-    </row>
-    <row r="523" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A523" s="72" t="s">
-        <v>825</v>
-      </c>
-      <c r="B523" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C523" s="22" t="s">
-        <v>688</v>
-      </c>
-      <c r="D523" s="16" t="s">
-        <v>234</v>
-      </c>
-      <c r="E523" s="28"/>
-    </row>
-    <row r="524" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A524" s="70" t="s">
-        <v>210</v>
-      </c>
-      <c r="B524" s="50" t="s">
-        <v>719</v>
-      </c>
-      <c r="C524" s="60" t="s">
-        <v>841</v>
-      </c>
-      <c r="D524" s="57"/>
-      <c r="E524" s="58"/>
-    </row>
-    <row r="525" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A525" s="71" t="s">
-        <v>24</v>
-      </c>
-      <c r="B525" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C525" s="22" t="s">
-        <v>690</v>
-      </c>
-      <c r="D525" s="16" t="s">
-        <v>234</v>
-      </c>
-      <c r="E525" s="28" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="526" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A526" s="71" t="s">
-        <v>167</v>
-      </c>
-      <c r="B526" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C526" s="22" t="s">
-        <v>691</v>
-      </c>
-      <c r="D526" s="16" t="s">
-        <v>535</v>
-      </c>
-      <c r="E526" s="28">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="527" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A527" s="73" t="s">
-        <v>75</v>
-      </c>
-      <c r="B527" s="50" t="s">
-        <v>720</v>
-      </c>
-      <c r="C527" s="60"/>
-      <c r="D527" s="57"/>
-      <c r="E527" s="58"/>
-    </row>
-    <row r="528" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A528" s="72" t="s">
-        <v>24</v>
-      </c>
-      <c r="B528" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C528" s="22" t="s">
-        <v>547</v>
-      </c>
-      <c r="D528" s="16"/>
-      <c r="E528" s="28" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="529" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A529" s="70" t="s">
-        <v>211</v>
-      </c>
-      <c r="B529" s="50" t="s">
-        <v>721</v>
-      </c>
-      <c r="C529" s="60" t="s">
-        <v>842</v>
-      </c>
-      <c r="D529" s="57"/>
-      <c r="E529" s="58"/>
-    </row>
-    <row r="530" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A530" s="71" t="s">
-        <v>57</v>
-      </c>
-      <c r="B530" s="36" t="s">
-        <v>720</v>
-      </c>
-      <c r="C530" s="22" t="s">
-        <v>693</v>
-      </c>
-      <c r="D530" s="16" t="s">
-        <v>230</v>
-      </c>
-      <c r="E530" s="28" t="s">
-        <v>694</v>
-      </c>
-    </row>
-    <row r="531" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A531" s="71" t="s">
-        <v>212</v>
-      </c>
-      <c r="B531" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C531" s="22" t="s">
-        <v>695</v>
-      </c>
-      <c r="D531" s="16" t="s">
-        <v>230</v>
-      </c>
-      <c r="E531" s="28" t="s">
-        <v>696</v>
-      </c>
-    </row>
-    <row r="532" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A532" s="70" t="s">
-        <v>213</v>
-      </c>
       <c r="B532" s="50" t="s">
         <v>719</v>
       </c>
-      <c r="C532" s="60" t="s">
-        <v>697</v>
-      </c>
+      <c r="C532" s="60"/>
       <c r="D532" s="57"/>
       <c r="E532" s="58"/>
     </row>
-    <row r="533" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="533" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A533" s="71" t="s">
-        <v>214</v>
+        <v>24</v>
       </c>
       <c r="B533" s="36" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="C533" s="22" t="s">
-        <v>698</v>
+        <v>680</v>
       </c>
       <c r="D533" s="16" t="s">
-        <v>10</v>
+        <v>228</v>
       </c>
       <c r="E533" s="28">
-        <v>36161</v>
-      </c>
-    </row>
-    <row r="534" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A534" s="71" t="s">
-        <v>215</v>
+        <v>10986700</v>
+      </c>
+    </row>
+    <row r="534" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A534" s="72" t="s">
+        <v>820</v>
       </c>
       <c r="B534" s="36" t="s">
         <v>719</v>
       </c>
       <c r="C534" s="22" t="s">
-        <v>699</v>
-      </c>
-      <c r="D534" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E534" s="28">
-        <v>36161</v>
+        <v>681</v>
+      </c>
+      <c r="D534" s="16"/>
+      <c r="E534" s="30" t="s">
+        <v>682</v>
       </c>
     </row>
     <row r="535" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A535" s="71" t="s">
-        <v>216</v>
-      </c>
-      <c r="B535" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C535" s="22" t="s">
-        <v>700</v>
-      </c>
-      <c r="D535" s="16" t="s">
-        <v>230</v>
-      </c>
-      <c r="E535" s="28">
-        <v>123456</v>
-      </c>
+      <c r="A535" s="70" t="s">
+        <v>207</v>
+      </c>
+      <c r="B535" s="50" t="s">
+        <v>719</v>
+      </c>
+      <c r="C535" s="60"/>
+      <c r="D535" s="57"/>
+      <c r="E535" s="58"/>
     </row>
     <row r="536" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A536" s="73" t="s">
-        <v>217</v>
-      </c>
-      <c r="B536" s="50" t="s">
-        <v>719</v>
-      </c>
-      <c r="C536" s="60"/>
-      <c r="D536" s="57"/>
-      <c r="E536" s="58"/>
+      <c r="A536" s="71" t="s">
+        <v>72</v>
+      </c>
+      <c r="B536" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C536" s="22" t="s">
+        <v>683</v>
+      </c>
+      <c r="D536" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="E536" s="28" t="s">
+        <v>684</v>
+      </c>
     </row>
     <row r="537" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A537" s="72" t="s">
-        <v>218</v>
-      </c>
-      <c r="B537" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C537" s="22" t="s">
-        <v>701</v>
-      </c>
-      <c r="D537" s="16" t="s">
-        <v>230</v>
-      </c>
-      <c r="E537" s="28" t="s">
-        <v>629</v>
-      </c>
+      <c r="A537" s="70" t="s">
+        <v>208</v>
+      </c>
+      <c r="B537" s="50" t="s">
+        <v>721</v>
+      </c>
+      <c r="C537" s="60"/>
+      <c r="D537" s="57"/>
+      <c r="E537" s="58"/>
     </row>
     <row r="538" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A538" s="72" t="s">
-        <v>219</v>
+      <c r="A538" s="71" t="s">
+        <v>209</v>
       </c>
       <c r="B538" s="36" t="s">
         <v>719</v>
       </c>
       <c r="C538" s="22" t="s">
-        <v>702</v>
+        <v>685</v>
       </c>
       <c r="D538" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E538" s="28" t="s">
-        <v>766</v>
-      </c>
-    </row>
-    <row r="539" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A539" s="61" t="s">
-        <v>220</v>
-      </c>
-      <c r="B539" s="50" t="s">
-        <v>719</v>
-      </c>
-      <c r="C539" s="60" t="s">
-        <v>843</v>
-      </c>
-      <c r="D539" s="57"/>
-      <c r="E539" s="58"/>
-    </row>
-    <row r="540" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A540" s="78" t="s">
-        <v>21</v>
-      </c>
-      <c r="B540" s="35" t="s">
+        <v>228</v>
+      </c>
+      <c r="E538" s="28">
+        <v>9873242</v>
+      </c>
+    </row>
+    <row r="539" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A539" s="72" t="s">
+        <v>824</v>
+      </c>
+      <c r="B539" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C539" s="22" t="s">
+        <v>686</v>
+      </c>
+      <c r="D539" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="E539" s="28" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="540" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A540" s="72" t="s">
+        <v>825</v>
+      </c>
+      <c r="B540" s="36" t="s">
         <v>719</v>
       </c>
       <c r="C540" s="22" t="s">
-        <v>605</v>
-      </c>
-      <c r="D540" s="22"/>
-      <c r="E540" s="27"/>
-    </row>
-    <row r="541" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A541" s="66" t="s">
-        <v>221</v>
-      </c>
-      <c r="B541" s="36" t="s">
-        <v>720</v>
-      </c>
-      <c r="C541" s="22" t="s">
-        <v>704</v>
-      </c>
-      <c r="D541" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="E541" s="28" t="s">
-        <v>705</v>
-      </c>
-    </row>
-    <row r="542" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+        <v>688</v>
+      </c>
+      <c r="D540" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="E540" s="28"/>
+    </row>
+    <row r="541" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A541" s="70" t="s">
+        <v>210</v>
+      </c>
+      <c r="B541" s="50" t="s">
+        <v>719</v>
+      </c>
+      <c r="C541" s="60" t="s">
+        <v>841</v>
+      </c>
+      <c r="D541" s="57"/>
+      <c r="E541" s="58"/>
+    </row>
+    <row r="542" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A542" s="71" t="s">
-        <v>822</v>
-      </c>
-      <c r="B542" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="B542" s="36" t="s">
         <v>719</v>
       </c>
       <c r="C542" s="22" t="s">
-        <v>706</v>
+        <v>690</v>
       </c>
       <c r="D542" s="16" t="s">
         <v>234</v>
       </c>
       <c r="E542" s="28" t="s">
-        <v>237</v>
+        <v>541</v>
       </c>
     </row>
     <row r="543" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A543" s="66" t="s">
-        <v>222</v>
-      </c>
-      <c r="B543" s="35" t="s">
+      <c r="A543" s="71" t="s">
+        <v>167</v>
+      </c>
+      <c r="B543" s="36" t="s">
         <v>719</v>
       </c>
       <c r="C543" s="22" t="s">
-        <v>707</v>
+        <v>691</v>
       </c>
       <c r="D543" s="16" t="s">
-        <v>1</v>
+        <v>535</v>
       </c>
       <c r="E543" s="28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="544" spans="1:5" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A544" s="71" t="s">
-        <v>823</v>
-      </c>
-      <c r="B544" s="35" t="s">
-        <v>719</v>
-      </c>
-      <c r="C544" s="22" t="s">
-        <v>708</v>
-      </c>
-      <c r="D544" s="16"/>
-      <c r="E544" s="28" t="s">
-        <v>609</v>
-      </c>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="544" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A544" s="73" t="s">
+        <v>75</v>
+      </c>
+      <c r="B544" s="50" t="s">
+        <v>720</v>
+      </c>
+      <c r="C544" s="60"/>
+      <c r="D544" s="57"/>
+      <c r="E544" s="58"/>
     </row>
     <row r="545" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A545" s="61" t="s">
-        <v>159</v>
-      </c>
-      <c r="B545" s="50" t="s">
+      <c r="A545" s="72" t="s">
+        <v>24</v>
+      </c>
+      <c r="B545" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C545" s="22" t="s">
+        <v>547</v>
+      </c>
+      <c r="D545" s="16"/>
+      <c r="E545" s="28" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="546" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A546" s="70" t="s">
+        <v>211</v>
+      </c>
+      <c r="B546" s="50" t="s">
         <v>721</v>
       </c>
-      <c r="C545" s="60" t="s">
-        <v>844</v>
-      </c>
-      <c r="D545" s="57"/>
-      <c r="E545" s="58"/>
-    </row>
-    <row r="546" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A546" s="66" t="s">
-        <v>160</v>
-      </c>
-      <c r="B546" s="36" t="s">
-        <v>720</v>
-      </c>
-      <c r="C546" s="22" t="s">
-        <v>709</v>
-      </c>
-      <c r="D546" s="16" t="s">
-        <v>234</v>
-      </c>
-      <c r="E546" s="27" t="s">
-        <v>656</v>
-      </c>
-    </row>
-    <row r="547" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A547" s="66" t="s">
-        <v>164</v>
+      <c r="C546" s="60" t="s">
+        <v>842</v>
+      </c>
+      <c r="D546" s="57"/>
+      <c r="E546" s="58"/>
+    </row>
+    <row r="547" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A547" s="71" t="s">
+        <v>57</v>
       </c>
       <c r="B547" s="36" t="s">
         <v>720</v>
       </c>
       <c r="C547" s="22" t="s">
+        <v>693</v>
+      </c>
+      <c r="D547" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="E547" s="28" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="548" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A548" s="71" t="s">
+        <v>212</v>
+      </c>
+      <c r="B548" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C548" s="22" t="s">
+        <v>695</v>
+      </c>
+      <c r="D548" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="E548" s="28" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="549" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A549" s="70" t="s">
+        <v>213</v>
+      </c>
+      <c r="B549" s="50" t="s">
+        <v>719</v>
+      </c>
+      <c r="C549" s="60" t="s">
+        <v>697</v>
+      </c>
+      <c r="D549" s="57"/>
+      <c r="E549" s="58"/>
+    </row>
+    <row r="550" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A550" s="71" t="s">
+        <v>214</v>
+      </c>
+      <c r="B550" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C550" s="22" t="s">
+        <v>698</v>
+      </c>
+      <c r="D550" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E550" s="28">
+        <v>36161</v>
+      </c>
+    </row>
+    <row r="551" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A551" s="71" t="s">
+        <v>215</v>
+      </c>
+      <c r="B551" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C551" s="22" t="s">
+        <v>699</v>
+      </c>
+      <c r="D551" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E551" s="28">
+        <v>36161</v>
+      </c>
+    </row>
+    <row r="552" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A552" s="71" t="s">
+        <v>216</v>
+      </c>
+      <c r="B552" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C552" s="22" t="s">
+        <v>700</v>
+      </c>
+      <c r="D552" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="E552" s="28">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="553" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A553" s="73" t="s">
+        <v>217</v>
+      </c>
+      <c r="B553" s="50" t="s">
+        <v>719</v>
+      </c>
+      <c r="C553" s="60"/>
+      <c r="D553" s="57"/>
+      <c r="E553" s="58"/>
+    </row>
+    <row r="554" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A554" s="72" t="s">
+        <v>218</v>
+      </c>
+      <c r="B554" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C554" s="22" t="s">
+        <v>701</v>
+      </c>
+      <c r="D554" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="E554" s="28" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="555" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A555" s="72" t="s">
+        <v>219</v>
+      </c>
+      <c r="B555" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C555" s="22" t="s">
+        <v>702</v>
+      </c>
+      <c r="D555" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E555" s="28" t="s">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="556" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A556" s="61" t="s">
+        <v>220</v>
+      </c>
+      <c r="B556" s="50" t="s">
+        <v>719</v>
+      </c>
+      <c r="C556" s="60" t="s">
+        <v>843</v>
+      </c>
+      <c r="D556" s="57"/>
+      <c r="E556" s="58"/>
+    </row>
+    <row r="557" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A557" s="78" t="s">
+        <v>21</v>
+      </c>
+      <c r="B557" s="35" t="s">
+        <v>719</v>
+      </c>
+      <c r="C557" s="22" t="s">
+        <v>605</v>
+      </c>
+      <c r="D557" s="22"/>
+      <c r="E557" s="27"/>
+    </row>
+    <row r="558" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A558" s="66" t="s">
+        <v>221</v>
+      </c>
+      <c r="B558" s="36" t="s">
+        <v>720</v>
+      </c>
+      <c r="C558" s="22" t="s">
+        <v>704</v>
+      </c>
+      <c r="D558" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E558" s="28" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="559" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A559" s="71" t="s">
+        <v>822</v>
+      </c>
+      <c r="B559" s="35" t="s">
+        <v>719</v>
+      </c>
+      <c r="C559" s="22" t="s">
+        <v>706</v>
+      </c>
+      <c r="D559" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="E559" s="28" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="560" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A560" s="66" t="s">
+        <v>222</v>
+      </c>
+      <c r="B560" s="35" t="s">
+        <v>719</v>
+      </c>
+      <c r="C560" s="22" t="s">
+        <v>707</v>
+      </c>
+      <c r="D560" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E560" s="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="561" spans="1:5" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A561" s="71" t="s">
+        <v>823</v>
+      </c>
+      <c r="B561" s="35" t="s">
+        <v>719</v>
+      </c>
+      <c r="C561" s="22" t="s">
+        <v>708</v>
+      </c>
+      <c r="D561" s="16"/>
+      <c r="E561" s="28" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="562" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A562" s="61" t="s">
+        <v>159</v>
+      </c>
+      <c r="B562" s="50" t="s">
+        <v>721</v>
+      </c>
+      <c r="C562" s="60" t="s">
+        <v>844</v>
+      </c>
+      <c r="D562" s="57"/>
+      <c r="E562" s="58"/>
+    </row>
+    <row r="563" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A563" s="66" t="s">
+        <v>160</v>
+      </c>
+      <c r="B563" s="36" t="s">
+        <v>720</v>
+      </c>
+      <c r="C563" s="22" t="s">
+        <v>709</v>
+      </c>
+      <c r="D563" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="E563" s="27" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="564" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A564" s="66" t="s">
+        <v>164</v>
+      </c>
+      <c r="B564" s="36" t="s">
+        <v>720</v>
+      </c>
+      <c r="C564" s="22" t="s">
         <v>710</v>
       </c>
-      <c r="D547" s="16" t="s">
+      <c r="D564" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E547" s="28" t="s">
+      <c r="E564" s="28" t="s">
         <v>592</v>
       </c>
     </row>
-    <row r="548" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A548" s="71" t="s">
+    <row r="565" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A565" s="71" t="s">
         <v>822</v>
       </c>
-      <c r="B548" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C548" s="22" t="s">
+      <c r="B565" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C565" s="22" t="s">
         <v>711</v>
       </c>
-      <c r="D548" s="16" t="s">
+      <c r="D565" s="16" t="s">
         <v>234</v>
       </c>
-      <c r="E548" s="28" t="s">
+      <c r="E565" s="28" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="549" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A549" s="66" t="s">
+    <row r="566" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A566" s="66" t="s">
         <v>165</v>
       </c>
-      <c r="B549" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C549" s="22" t="s">
+      <c r="B566" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C566" s="22" t="s">
         <v>712</v>
       </c>
-      <c r="D549" s="16" t="s">
+      <c r="D566" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E549" s="28" t="s">
+      <c r="E566" s="28" t="s">
         <v>598</v>
       </c>
     </row>
-    <row r="550" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A550" s="71" t="s">
+    <row r="567" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A567" s="71" t="s">
         <v>822</v>
       </c>
-      <c r="B550" s="36" t="s">
-        <v>719</v>
-      </c>
-      <c r="C550" s="22" t="s">
+      <c r="B567" s="36" t="s">
+        <v>719</v>
+      </c>
+      <c r="C567" s="22" t="s">
         <v>713</v>
       </c>
-      <c r="D550" s="16" t="s">
+      <c r="D567" s="16" t="s">
         <v>234</v>
       </c>
-      <c r="E550" s="28" t="s">
+      <c r="E567" s="28" t="s">
         <v>237</v>
       </c>
     </row>

</xml_diff>